<commit_message>
start creating option for absolue value mapping.
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g_del\Documents\R\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E2311B-FA92-4C68-BBC4-AB22B0F73769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A00EA3D-D419-48C4-A681-6E1C2EF523C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="435">
   <si>
     <t>id</t>
   </si>
@@ -1329,6 +1329,15 @@
   </si>
   <si>
     <t>Deux paramètres</t>
+  </si>
+  <si>
+    <t>map_latest_measurements</t>
+  </si>
+  <si>
+    <t>Latest measurements</t>
+  </si>
+  <si>
+    <t>Plus récentes mesures</t>
   </si>
 </sst>
 </file>
@@ -2263,10 +2272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D143"/>
+  <dimension ref="A1:D144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+      <selection activeCell="D82" sqref="A82:XFD82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3329,843 +3338,854 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" s="4" t="s">
+      <c r="A82" t="s">
+        <v>432</v>
+      </c>
+      <c r="C82" t="s">
+        <v>433</v>
+      </c>
+      <c r="D82" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" t="s">
-        <v>156</v>
-      </c>
-      <c r="B83" t="s">
-        <v>48</v>
-      </c>
-      <c r="C83" t="s">
-        <v>157</v>
-      </c>
-      <c r="D83" t="s">
-        <v>158</v>
-      </c>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B84" t="s">
-        <v>159</v>
+        <v>48</v>
       </c>
       <c r="C84" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D84" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B85" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C85" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="D85" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B86" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="C86" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="D86" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B87" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C87" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D87" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B88" t="s">
-        <v>170</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="D88" s="9" t="s">
-        <v>172</v>
+        <v>166</v>
+      </c>
+      <c r="C88" t="s">
+        <v>176</v>
+      </c>
+      <c r="D88" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
+        <v>168</v>
+      </c>
+      <c r="B89" t="s">
+        <v>170</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" t="s">
         <v>169</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>166</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>171</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D90" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" s="8" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B90" s="8"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" t="s">
-        <v>61</v>
-      </c>
-      <c r="B91" t="s">
-        <v>9</v>
-      </c>
-      <c r="C91" t="s">
-        <v>62</v>
-      </c>
-      <c r="D91" t="s">
-        <v>63</v>
-      </c>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="B92" t="s">
         <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="D92" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="D93" t="s">
-        <v>66</v>
+        <v>115</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
       </c>
       <c r="C94" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D94" t="s">
-        <v>252</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>247</v>
+        <v>67</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>248</v>
+        <v>68</v>
       </c>
       <c r="D95" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>389</v>
+        <v>247</v>
       </c>
       <c r="B96" t="s">
         <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>392</v>
+        <v>248</v>
       </c>
       <c r="D96" t="s">
-        <v>394</v>
+        <v>248</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B97" t="s">
         <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D97" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B98" t="s">
         <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D98" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>182</v>
+        <v>391</v>
       </c>
       <c r="B99" t="s">
         <v>9</v>
       </c>
       <c r="C99" t="s">
-        <v>183</v>
+        <v>396</v>
       </c>
       <c r="D99" t="s">
-        <v>184</v>
+        <v>397</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B100" t="s">
         <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D100" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
       </c>
       <c r="C101" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D101" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="B102" t="s">
         <v>9</v>
       </c>
       <c r="C102" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="D102" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>69</v>
+        <v>181</v>
       </c>
       <c r="B103" t="s">
         <v>9</v>
       </c>
       <c r="C103" t="s">
-        <v>70</v>
+        <v>220</v>
       </c>
       <c r="D103" t="s">
-        <v>71</v>
+        <v>221</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>190</v>
+        <v>69</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
       </c>
       <c r="C104" t="s">
-        <v>185</v>
+        <v>70</v>
       </c>
       <c r="D104" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
       </c>
       <c r="C105" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D105" t="s">
-        <v>198</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>72</v>
+        <v>196</v>
       </c>
       <c r="B106" t="s">
         <v>9</v>
       </c>
       <c r="C106" t="s">
-        <v>73</v>
+        <v>197</v>
       </c>
       <c r="D106" t="s">
-        <v>74</v>
+        <v>198</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>189</v>
+        <v>72</v>
       </c>
       <c r="B107" t="s">
         <v>9</v>
       </c>
       <c r="C107" t="s">
-        <v>191</v>
+        <v>73</v>
       </c>
       <c r="D107" t="s">
-        <v>192</v>
+        <v>74</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
       </c>
       <c r="C108" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D108" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>75</v>
+        <v>199</v>
       </c>
       <c r="B109" t="s">
         <v>9</v>
       </c>
       <c r="C109" t="s">
-        <v>76</v>
+        <v>200</v>
       </c>
       <c r="D109" t="s">
-        <v>77</v>
+        <v>201</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>188</v>
+        <v>75</v>
       </c>
       <c r="B110" t="s">
         <v>9</v>
       </c>
       <c r="C110" t="s">
-        <v>186</v>
+        <v>76</v>
       </c>
       <c r="D110" t="s">
-        <v>187</v>
+        <v>77</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B111" t="s">
         <v>9</v>
       </c>
       <c r="C111" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="D111" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="B112" t="s">
         <v>9</v>
       </c>
       <c r="C112" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="D112" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B113" t="s">
         <v>9</v>
       </c>
       <c r="C113" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D113" t="s">
-        <v>126</v>
+        <v>223</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B114" t="s">
         <v>9</v>
       </c>
       <c r="C114" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D114" t="s">
-        <v>229</v>
+        <v>126</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>320</v>
+        <v>227</v>
+      </c>
+      <c r="B115" t="s">
+        <v>9</v>
       </c>
       <c r="C115" t="s">
-        <v>321</v>
+        <v>228</v>
       </c>
       <c r="D115" t="s">
-        <v>322</v>
+        <v>229</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>81</v>
-      </c>
-      <c r="B116" t="s">
-        <v>9</v>
+        <v>320</v>
       </c>
       <c r="C116" t="s">
-        <v>82</v>
+        <v>321</v>
       </c>
       <c r="D116" t="s">
-        <v>83</v>
+        <v>322</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="B117" t="s">
         <v>9</v>
       </c>
       <c r="C117" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="D117" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
-        <v>230</v>
+        <v>8</v>
       </c>
       <c r="B118" t="s">
         <v>9</v>
       </c>
       <c r="C118" t="s">
-        <v>230</v>
+        <v>10</v>
       </c>
       <c r="D118" t="s">
-        <v>231</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="B119" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="C119" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="D119" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="B120" t="s">
-        <v>9</v>
+        <v>209</v>
       </c>
       <c r="C120" t="s">
-        <v>234</v>
+        <v>208</v>
       </c>
       <c r="D120" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B121" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="C121" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D121" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="B122" t="s">
-        <v>9</v>
+        <v>209</v>
       </c>
       <c r="C122" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="D122" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B123" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="C123" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D123" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="B124" t="s">
-        <v>9</v>
+        <v>209</v>
       </c>
       <c r="C124" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="D124" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B125" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="C125" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D125" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>127</v>
+        <v>242</v>
       </c>
       <c r="B126" t="s">
-        <v>9</v>
+        <v>209</v>
       </c>
       <c r="C126" t="s">
-        <v>128</v>
+        <v>244</v>
       </c>
       <c r="D126" t="s">
-        <v>129</v>
+        <v>246</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>238</v>
+        <v>127</v>
       </c>
       <c r="B127" t="s">
         <v>9</v>
       </c>
       <c r="C127" t="s">
-        <v>239</v>
+        <v>128</v>
       </c>
       <c r="D127" t="s">
-        <v>240</v>
+        <v>129</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>15</v>
+        <v>238</v>
       </c>
       <c r="B128" t="s">
         <v>9</v>
       </c>
       <c r="C128" t="s">
+        <v>239</v>
+      </c>
+      <c r="D128" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" t="s">
+        <v>15</v>
+      </c>
+      <c r="B129" t="s">
+        <v>9</v>
+      </c>
+      <c r="C129" t="s">
         <v>16</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D129" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="2" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B129" s="2"/>
-      <c r="C129" s="2"/>
-      <c r="D129" s="2"/>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130" t="s">
-        <v>131</v>
-      </c>
-      <c r="B130" t="s">
-        <v>130</v>
-      </c>
-      <c r="C130" t="s">
-        <v>150</v>
-      </c>
-      <c r="D130" t="s">
-        <v>149</v>
-      </c>
+      <c r="B130" s="2"/>
+      <c r="C130" s="2"/>
+      <c r="D130" s="2"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="B131" t="s">
         <v>130</v>
       </c>
       <c r="C131" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D131" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="B132" t="s">
         <v>130</v>
       </c>
       <c r="C132" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="D132" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B133" t="s">
         <v>130</v>
       </c>
       <c r="C133" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D133" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B134" t="s">
         <v>130</v>
       </c>
       <c r="C134" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D134" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B135" t="s">
         <v>130</v>
       </c>
       <c r="C135" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="D135" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B136" t="s">
         <v>130</v>
       </c>
       <c r="C136" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D136" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B137" t="s">
         <v>130</v>
       </c>
       <c r="C137" t="s">
+        <v>152</v>
+      </c>
+      <c r="D137" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" t="s">
+        <v>145</v>
+      </c>
+      <c r="B138" t="s">
+        <v>130</v>
+      </c>
+      <c r="C138" t="s">
         <v>146</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D138" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138" s="4" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B138" s="4"/>
-      <c r="C138" s="4"/>
-      <c r="D138" s="4"/>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A139" t="s">
-        <v>84</v>
-      </c>
-      <c r="B139" t="s">
-        <v>85</v>
-      </c>
-      <c r="C139" t="s">
-        <v>400</v>
-      </c>
-      <c r="D139" t="s">
-        <v>401</v>
-      </c>
+      <c r="B139" s="4"/>
+      <c r="C139" s="4"/>
+      <c r="D139" s="4"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="s">
-        <v>398</v>
+        <v>84</v>
       </c>
       <c r="B140" t="s">
         <v>85</v>
       </c>
       <c r="C140" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
       <c r="D140" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="s">
-        <v>180</v>
+        <v>398</v>
       </c>
       <c r="B141" t="s">
         <v>85</v>
       </c>
       <c r="C141" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="D141" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" t="s">
-        <v>404</v>
+        <v>180</v>
       </c>
       <c r="B142" t="s">
         <v>85</v>
       </c>
       <c r="C142" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D142" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" t="s">
-        <v>86</v>
+        <v>404</v>
       </c>
       <c r="B143" t="s">
         <v>85</v>
       </c>
       <c r="C143" t="s">
+        <v>405</v>
+      </c>
+      <c r="D143" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" t="s">
+        <v>86</v>
+      </c>
+      <c r="B144" t="s">
+        <v>85</v>
+      </c>
+      <c r="C144" t="s">
         <v>87</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D144" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
work on map for parameters
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g_del\Documents\R\YGwater\inst\apps\YGwater\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A00EA3D-D419-48C4-A681-6E1C2EF523C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F577C5-F58D-44D2-A90E-384863896B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="474">
   <si>
     <t>id</t>
   </si>
@@ -1097,9 +1097,6 @@
     <t>Login failed</t>
   </si>
   <si>
-    <t>login_close</t>
-  </si>
-  <si>
     <t>modal actionButton text</t>
   </si>
   <si>
@@ -1175,9 +1172,6 @@
     <t>Select a date</t>
   </si>
   <si>
-    <t>map_date_within_select</t>
-  </si>
-  <si>
     <t>With data within ... day(s) at most</t>
   </si>
   <si>
@@ -1280,12 +1274,6 @@
     <t>Date ciblée</t>
   </si>
   <si>
-    <t>Absolute value</t>
-  </si>
-  <si>
-    <t>Valeure absolue</t>
-  </si>
-  <si>
     <t>map_actual_date</t>
   </si>
   <si>
@@ -1338,6 +1326,135 @@
   </si>
   <si>
     <t>Plus récentes mesures</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Enregistrer</t>
+  </si>
+  <si>
+    <t>map_edit_primary_param</t>
+  </si>
+  <si>
+    <t>map_add_second_param</t>
+  </si>
+  <si>
+    <t>map_edit_second_param</t>
+  </si>
+  <si>
+    <t>map_edit_aes</t>
+  </si>
+  <si>
+    <t>Edit primary parameter</t>
+  </si>
+  <si>
+    <t>Ajouter paramètre secondaire</t>
+  </si>
+  <si>
+    <t>Modifier paramètre secondaire</t>
+  </si>
+  <si>
+    <t>Add scondary parameter</t>
+  </si>
+  <si>
+    <t>Edit secondary parameter</t>
+  </si>
+  <si>
+    <t>Edit map aesthetics</t>
+  </si>
+  <si>
+    <t>Modifier l'esthétique de la carte</t>
+  </si>
+  <si>
+    <t>map_rm_second_param</t>
+  </si>
+  <si>
+    <t>Remove secondary parameter</t>
+  </si>
+  <si>
+    <t>Enlever paramètre secondaire</t>
+  </si>
+  <si>
+    <t>Absolute values</t>
+  </si>
+  <si>
+    <t>Valeures absolue</t>
+  </si>
+  <si>
+    <t>map_primary_param</t>
+  </si>
+  <si>
+    <t>map_second_param</t>
+  </si>
+  <si>
+    <t>Secondary parameter</t>
+  </si>
+  <si>
+    <t>Paramètre secondaire</t>
+  </si>
+  <si>
+    <t>Paramètre primaire</t>
+  </si>
+  <si>
+    <t>Primary parameter</t>
+  </si>
+  <si>
+    <t>map_min_yrs_selected1</t>
+  </si>
+  <si>
+    <t>map_min_yrs_selected2</t>
+  </si>
+  <si>
+    <t>With at least</t>
+  </si>
+  <si>
+    <t>years of record</t>
+  </si>
+  <si>
+    <t>Avec au moins</t>
+  </si>
+  <si>
+    <t>années de mesures</t>
+  </si>
+  <si>
+    <t>map_date_within</t>
+  </si>
+  <si>
+    <t>map_date_within_selected1</t>
+  </si>
+  <si>
+    <t>map_date_within_selected2</t>
+  </si>
+  <si>
+    <t>jour(s) ou moins de la date ciblée</t>
+  </si>
+  <si>
+    <t>day(s) or less of target date</t>
+  </si>
+  <si>
+    <t>and data within</t>
+  </si>
+  <si>
+    <t>et données dans un délai de</t>
+  </si>
+  <si>
+    <t>map_mapType</t>
+  </si>
+  <si>
+    <t>Map type</t>
+  </si>
+  <si>
+    <t>Type de carte</t>
+  </si>
+  <si>
+    <t>Modifer paramètre primaire</t>
+  </si>
+  <si>
+    <t>close</t>
   </si>
 </sst>
 </file>
@@ -2272,22 +2389,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D144"/>
+  <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D82" sqref="A82:XFD82"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142:XFD142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.15625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="43.578125" customWidth="1"/>
-    <col min="4" max="4" width="49.83984375" customWidth="1"/>
-    <col min="5" max="5" width="54.41796875" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" customWidth="1"/>
+    <col min="5" max="5" width="54.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2301,7 +2418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2315,7 +2432,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -2329,7 +2446,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -2337,7 +2454,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2351,7 +2468,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2365,7 +2482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2379,7 +2496,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2393,7 +2510,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2407,7 +2524,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -2421,7 +2538,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2435,7 +2552,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>328</v>
       </c>
@@ -2443,7 +2560,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>327</v>
       </c>
@@ -2457,7 +2574,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>332</v>
       </c>
@@ -2471,7 +2588,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>333</v>
       </c>
@@ -2485,7 +2602,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>340</v>
       </c>
@@ -2499,7 +2616,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>344</v>
       </c>
@@ -2513,7 +2630,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>342</v>
       </c>
@@ -2527,7 +2644,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>345</v>
       </c>
@@ -2541,1651 +2658,1794 @@
         <v>348</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B20" t="s">
         <v>347</v>
       </c>
       <c r="C20" t="s">
+        <v>358</v>
+      </c>
+      <c r="D20" t="s">
         <v>359</v>
       </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>354</v>
+      </c>
+      <c r="C21" t="s">
         <v>361</v>
       </c>
-      <c r="B21" t="s">
-        <v>355</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>362</v>
       </c>
-      <c r="D21" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>354</v>
-      </c>
-      <c r="B22" t="s">
-        <v>355</v>
-      </c>
-      <c r="C22" t="s">
-        <v>356</v>
-      </c>
-      <c r="D22" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="2" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>179</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="3" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>47</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B26" t="s">
         <v>48</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C26" t="s">
         <v>49</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D26" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="4" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>263</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>261</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>271</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>263</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>261</v>
+        <v>215</v>
       </c>
       <c r="C30" t="s">
-        <v>271</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>273</v>
       </c>
       <c r="B31" t="s">
-        <v>215</v>
+        <v>276</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>274</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="B32" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C32" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="D32" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B33" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C33" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D33" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B34" t="s">
         <v>283</v>
       </c>
       <c r="C34" t="s">
-        <v>288</v>
+        <v>312</v>
       </c>
       <c r="D34" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B35" t="s">
         <v>283</v>
       </c>
       <c r="C35" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D35" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="B36" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C36" t="s">
-        <v>313</v>
+        <v>286</v>
       </c>
       <c r="D36" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>284</v>
+        <v>311</v>
       </c>
       <c r="B37" t="s">
         <v>285</v>
       </c>
       <c r="C37" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D37" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
       <c r="B38" t="s">
         <v>285</v>
       </c>
       <c r="C38" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D38" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B39" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C39" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D39" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B40" t="s">
         <v>282</v>
       </c>
       <c r="C40" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="D40" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>299</v>
+        <v>317</v>
       </c>
       <c r="B41" t="s">
         <v>282</v>
       </c>
       <c r="C41" t="s">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="D41" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="B42" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C42" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="D42" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B43" t="s">
         <v>283</v>
       </c>
       <c r="C43" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D43" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="B44" t="s">
         <v>283</v>
       </c>
       <c r="C44" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D44" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>308</v>
+        <v>323</v>
       </c>
       <c r="B45" t="s">
-        <v>283</v>
+        <v>324</v>
       </c>
       <c r="C45" t="s">
-        <v>309</v>
+        <v>325</v>
       </c>
       <c r="D45" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" t="s">
-        <v>323</v>
-      </c>
-      <c r="B46" t="s">
-        <v>324</v>
-      </c>
-      <c r="C46" t="s">
-        <v>325</v>
-      </c>
-      <c r="D46" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="10" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>213</v>
+      </c>
+      <c r="B47" t="s">
+        <v>214</v>
+      </c>
+      <c r="C47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>213</v>
+        <v>78</v>
       </c>
       <c r="B48" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C48" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="D48" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>211</v>
       </c>
       <c r="B49" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C49" t="s">
-        <v>79</v>
+        <v>218</v>
       </c>
       <c r="D49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>211</v>
+        <v>249</v>
       </c>
       <c r="B50" t="s">
-        <v>217</v>
+        <v>250</v>
       </c>
       <c r="C50" t="s">
-        <v>218</v>
+        <v>253</v>
       </c>
       <c r="D50" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B51" t="s">
         <v>250</v>
       </c>
       <c r="C51" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="D51" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="B52" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="C52" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D52" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B53" t="s">
         <v>262</v>
       </c>
       <c r="C53" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D53" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" t="s">
-        <v>267</v>
-      </c>
-      <c r="B54" t="s">
-        <v>262</v>
-      </c>
-      <c r="C54" t="s">
-        <v>268</v>
-      </c>
-      <c r="D54" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="5" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" t="s">
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>54</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B55" t="s">
         <v>48</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C55" t="s">
         <v>55</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D55" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="6" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57" t="s">
+        <v>57</v>
+      </c>
+      <c r="D57" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="C58" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="D58" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B59" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C59" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D59" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B60" t="s">
         <v>101</v>
       </c>
       <c r="C60" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D60" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="B61" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C61" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="D61" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C62" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="D62" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" t="s">
-        <v>109</v>
-      </c>
-      <c r="B63" t="s">
-        <v>110</v>
-      </c>
-      <c r="C63" t="s">
-        <v>111</v>
-      </c>
-      <c r="D63" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" t="s">
+        <v>59</v>
+      </c>
+      <c r="D64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>364</v>
       </c>
       <c r="B65" t="s">
-        <v>48</v>
+        <v>363</v>
       </c>
       <c r="C65" t="s">
-        <v>59</v>
+        <v>369</v>
       </c>
       <c r="D65" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>365</v>
       </c>
       <c r="B66" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C66" t="s">
         <v>370</v>
       </c>
       <c r="D66" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>372</v>
+      </c>
+      <c r="B67" t="s">
         <v>366</v>
       </c>
-      <c r="B67" t="s">
-        <v>364</v>
-      </c>
       <c r="C67" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D67" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>373</v>
       </c>
       <c r="B68" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C68" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="D68" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>374</v>
-      </c>
-      <c r="B69" t="s">
-        <v>367</v>
+        <v>469</v>
       </c>
       <c r="C69" t="s">
-        <v>375</v>
+        <v>470</v>
       </c>
       <c r="D69" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" t="s">
+      <c r="C70" t="s">
+        <v>378</v>
+      </c>
+      <c r="D70" t="s">
         <v>377</v>
       </c>
-      <c r="C70" t="s">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>462</v>
+      </c>
+      <c r="C71" t="s">
         <v>379</v>
       </c>
-      <c r="D70" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" t="s">
+      <c r="D71" t="s">
         <v>380</v>
       </c>
-      <c r="C71" t="s">
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>463</v>
+      </c>
+      <c r="C72" t="s">
+        <v>467</v>
+      </c>
+      <c r="D72" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>464</v>
+      </c>
+      <c r="C73" t="s">
+        <v>466</v>
+      </c>
+      <c r="D73" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>381</v>
       </c>
-      <c r="D71" t="s">
+      <c r="C74" t="s">
+        <v>383</v>
+      </c>
+      <c r="D74" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" t="s">
-        <v>383</v>
-      </c>
-      <c r="C72" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>405</v>
+      </c>
+      <c r="B75" t="s">
+        <v>406</v>
+      </c>
+      <c r="C75" t="s">
+        <v>407</v>
+      </c>
+      <c r="D75" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>456</v>
+      </c>
+      <c r="C76" t="s">
+        <v>458</v>
+      </c>
+      <c r="D76" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>457</v>
+      </c>
+      <c r="C77" t="s">
+        <v>459</v>
+      </c>
+      <c r="D77" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>409</v>
+      </c>
+      <c r="B78" t="s">
+        <v>410</v>
+      </c>
+      <c r="C78" t="s">
+        <v>411</v>
+      </c>
+      <c r="D78" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>384</v>
+      </c>
+      <c r="C79" t="s">
+        <v>448</v>
+      </c>
+      <c r="D79" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>385</v>
       </c>
-      <c r="D72" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" t="s">
-        <v>407</v>
-      </c>
-      <c r="B73" t="s">
-        <v>408</v>
-      </c>
-      <c r="C73" t="s">
-        <v>409</v>
-      </c>
-      <c r="D73" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" t="s">
-        <v>411</v>
-      </c>
-      <c r="B74" t="s">
-        <v>412</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="C80" t="s">
+        <v>421</v>
+      </c>
+      <c r="D80" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>413</v>
       </c>
-      <c r="D74" t="s">
+      <c r="C81" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" t="s">
-        <v>386</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="D81" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>415</v>
       </c>
-      <c r="D75" t="s">
+      <c r="C82" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" t="s">
-        <v>387</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="D82" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>418</v>
+      </c>
+      <c r="C83" t="s">
+        <v>419</v>
+      </c>
+      <c r="D83" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>422</v>
+      </c>
+      <c r="C84" t="s">
+        <v>423</v>
+      </c>
+      <c r="D84" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>425</v>
       </c>
-      <c r="D76" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" t="s">
-        <v>417</v>
-      </c>
-      <c r="C77" t="s">
-        <v>418</v>
-      </c>
-      <c r="D77" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" t="s">
-        <v>419</v>
-      </c>
-      <c r="C78" t="s">
-        <v>420</v>
-      </c>
-      <c r="D78" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" t="s">
-        <v>422</v>
-      </c>
-      <c r="C79" t="s">
-        <v>423</v>
-      </c>
-      <c r="D79" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" t="s">
+      <c r="C85" t="s">
         <v>426</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D85" t="s">
         <v>427</v>
       </c>
-      <c r="D80" t="s">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" t="s">
+      <c r="C86" t="s">
         <v>429</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D86" t="s">
         <v>430</v>
       </c>
-      <c r="D81" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" t="s">
-        <v>432</v>
-      </c>
-      <c r="C82" t="s">
-        <v>433</v>
-      </c>
-      <c r="D82" t="s">
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>450</v>
+      </c>
+      <c r="C87" t="s">
+        <v>455</v>
+      </c>
+      <c r="D87" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" s="4" t="s">
+      <c r="C88" t="s">
+        <v>438</v>
+      </c>
+      <c r="D88" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>451</v>
+      </c>
+      <c r="C89" t="s">
+        <v>452</v>
+      </c>
+      <c r="D89" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>435</v>
+      </c>
+      <c r="C90" t="s">
+        <v>441</v>
+      </c>
+      <c r="D90" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>436</v>
+      </c>
+      <c r="C91" t="s">
+        <v>442</v>
+      </c>
+      <c r="D91" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>445</v>
+      </c>
+      <c r="C92" t="s">
+        <v>446</v>
+      </c>
+      <c r="D92" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>437</v>
+      </c>
+      <c r="C93" t="s">
+        <v>443</v>
+      </c>
+      <c r="D93" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
-      <c r="D83" s="4"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" t="s">
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>156</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B95" t="s">
         <v>48</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C95" t="s">
         <v>157</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D95" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>162</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B96" t="s">
         <v>159</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C96" t="s">
         <v>160</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D96" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>165</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B97" t="s">
         <v>166</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C97" t="s">
         <v>177</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D97" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>174</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B98" t="s">
         <v>159</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C98" t="s">
         <v>163</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D98" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>167</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B99" t="s">
         <v>166</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C99" t="s">
         <v>176</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D99" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>168</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B100" t="s">
         <v>170</v>
       </c>
-      <c r="C89" s="9" t="s">
+      <c r="C100" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D89" s="9" t="s">
+      <c r="D100" s="9" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>169</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B101" t="s">
         <v>166</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C101" t="s">
         <v>171</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D101" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" s="8" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" t="s">
+      <c r="B102" s="8"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>61</v>
-      </c>
-      <c r="B92" t="s">
-        <v>9</v>
-      </c>
-      <c r="C92" t="s">
-        <v>62</v>
-      </c>
-      <c r="D92" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" t="s">
-        <v>113</v>
-      </c>
-      <c r="B93" t="s">
-        <v>9</v>
-      </c>
-      <c r="C93" t="s">
-        <v>114</v>
-      </c>
-      <c r="D93" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" t="s">
-        <v>64</v>
-      </c>
-      <c r="B94" t="s">
-        <v>9</v>
-      </c>
-      <c r="C94" t="s">
-        <v>65</v>
-      </c>
-      <c r="D94" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" t="s">
-        <v>67</v>
-      </c>
-      <c r="B95" t="s">
-        <v>9</v>
-      </c>
-      <c r="C95" t="s">
-        <v>68</v>
-      </c>
-      <c r="D95" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" t="s">
-        <v>247</v>
-      </c>
-      <c r="B96" t="s">
-        <v>9</v>
-      </c>
-      <c r="C96" t="s">
-        <v>248</v>
-      </c>
-      <c r="D96" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" t="s">
-        <v>389</v>
-      </c>
-      <c r="B97" t="s">
-        <v>9</v>
-      </c>
-      <c r="C97" t="s">
-        <v>392</v>
-      </c>
-      <c r="D97" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" t="s">
-        <v>390</v>
-      </c>
-      <c r="B98" t="s">
-        <v>9</v>
-      </c>
-      <c r="C98" t="s">
-        <v>393</v>
-      </c>
-      <c r="D98" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" t="s">
-        <v>391</v>
-      </c>
-      <c r="B99" t="s">
-        <v>9</v>
-      </c>
-      <c r="C99" t="s">
-        <v>396</v>
-      </c>
-      <c r="D99" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100" t="s">
-        <v>182</v>
-      </c>
-      <c r="B100" t="s">
-        <v>9</v>
-      </c>
-      <c r="C100" t="s">
-        <v>183</v>
-      </c>
-      <c r="D100" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" t="s">
-        <v>193</v>
-      </c>
-      <c r="B101" t="s">
-        <v>9</v>
-      </c>
-      <c r="C101" t="s">
-        <v>194</v>
-      </c>
-      <c r="D101" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" t="s">
-        <v>202</v>
-      </c>
-      <c r="B102" t="s">
-        <v>9</v>
-      </c>
-      <c r="C102" t="s">
-        <v>203</v>
-      </c>
-      <c r="D102" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" t="s">
-        <v>181</v>
       </c>
       <c r="B103" t="s">
         <v>9</v>
       </c>
       <c r="C103" t="s">
-        <v>220</v>
+        <v>62</v>
       </c>
       <c r="D103" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
       </c>
       <c r="C104" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="D104" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>190</v>
+        <v>64</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
       </c>
       <c r="C105" t="s">
-        <v>185</v>
+        <v>65</v>
       </c>
       <c r="D105" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>196</v>
+        <v>67</v>
       </c>
       <c r="B106" t="s">
         <v>9</v>
       </c>
       <c r="C106" t="s">
-        <v>197</v>
+        <v>68</v>
       </c>
       <c r="D106" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>72</v>
+        <v>247</v>
       </c>
       <c r="B107" t="s">
         <v>9</v>
       </c>
       <c r="C107" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="D107" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>189</v>
+        <v>387</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
       </c>
       <c r="C108" t="s">
-        <v>191</v>
+        <v>390</v>
       </c>
       <c r="D108" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>199</v>
+        <v>388</v>
       </c>
       <c r="B109" t="s">
         <v>9</v>
       </c>
       <c r="C109" t="s">
-        <v>200</v>
+        <v>391</v>
       </c>
       <c r="D109" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>75</v>
+        <v>389</v>
       </c>
       <c r="B110" t="s">
         <v>9</v>
       </c>
       <c r="C110" t="s">
-        <v>76</v>
+        <v>394</v>
       </c>
       <c r="D110" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B111" t="s">
         <v>9</v>
       </c>
       <c r="C111" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D111" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="B112" t="s">
         <v>9</v>
       </c>
       <c r="C112" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="D112" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
       <c r="B113" t="s">
         <v>9</v>
       </c>
       <c r="C113" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="D113" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>225</v>
+        <v>181</v>
       </c>
       <c r="B114" t="s">
         <v>9</v>
       </c>
       <c r="C114" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D114" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>227</v>
+        <v>69</v>
       </c>
       <c r="B115" t="s">
         <v>9</v>
       </c>
       <c r="C115" t="s">
-        <v>228</v>
+        <v>70</v>
       </c>
       <c r="D115" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>320</v>
+        <v>190</v>
+      </c>
+      <c r="B116" t="s">
+        <v>9</v>
       </c>
       <c r="C116" t="s">
-        <v>321</v>
+        <v>185</v>
       </c>
       <c r="D116" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>81</v>
+        <v>196</v>
       </c>
       <c r="B117" t="s">
         <v>9</v>
       </c>
       <c r="C117" t="s">
-        <v>82</v>
+        <v>197</v>
       </c>
       <c r="D117" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="B118" t="s">
         <v>9</v>
       </c>
       <c r="C118" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="D118" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>230</v>
+        <v>189</v>
       </c>
       <c r="B119" t="s">
         <v>9</v>
       </c>
       <c r="C119" t="s">
-        <v>230</v>
+        <v>191</v>
       </c>
       <c r="D119" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B120" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="C120" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D120" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>232</v>
+        <v>75</v>
       </c>
       <c r="B121" t="s">
         <v>9</v>
       </c>
       <c r="C121" t="s">
-        <v>234</v>
+        <v>76</v>
       </c>
       <c r="D121" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>233</v>
+        <v>188</v>
       </c>
       <c r="B122" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="C122" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
       <c r="D122" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>259</v>
+        <v>205</v>
       </c>
       <c r="B123" t="s">
         <v>9</v>
       </c>
       <c r="C123" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="D123" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>260</v>
+        <v>224</v>
       </c>
       <c r="B124" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="C124" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="D124" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="B125" t="s">
         <v>9</v>
       </c>
       <c r="C125" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="D125" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="B126" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="C126" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="D126" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>127</v>
-      </c>
-      <c r="B127" t="s">
-        <v>9</v>
+        <v>320</v>
       </c>
       <c r="C127" t="s">
-        <v>128</v>
+        <v>321</v>
       </c>
       <c r="D127" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>238</v>
+        <v>81</v>
       </c>
       <c r="B128" t="s">
         <v>9</v>
       </c>
       <c r="C128" t="s">
-        <v>239</v>
+        <v>82</v>
       </c>
       <c r="D128" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B129" t="s">
         <v>9</v>
       </c>
       <c r="C129" t="s">
+        <v>10</v>
+      </c>
+      <c r="D129" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>230</v>
+      </c>
+      <c r="B130" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130" t="s">
+        <v>230</v>
+      </c>
+      <c r="D130" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>208</v>
+      </c>
+      <c r="B131" t="s">
+        <v>209</v>
+      </c>
+      <c r="C131" t="s">
+        <v>208</v>
+      </c>
+      <c r="D131" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>232</v>
+      </c>
+      <c r="B132" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132" t="s">
+        <v>234</v>
+      </c>
+      <c r="D132" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>233</v>
+      </c>
+      <c r="B133" t="s">
+        <v>209</v>
+      </c>
+      <c r="C133" t="s">
+        <v>236</v>
+      </c>
+      <c r="D133" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>259</v>
+      </c>
+      <c r="B134" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134" t="s">
+        <v>255</v>
+      </c>
+      <c r="D134" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>260</v>
+      </c>
+      <c r="B135" t="s">
+        <v>209</v>
+      </c>
+      <c r="C135" t="s">
+        <v>256</v>
+      </c>
+      <c r="D135" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>241</v>
+      </c>
+      <c r="B136" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136" t="s">
+        <v>243</v>
+      </c>
+      <c r="D136" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>242</v>
+      </c>
+      <c r="B137" t="s">
+        <v>209</v>
+      </c>
+      <c r="C137" t="s">
+        <v>244</v>
+      </c>
+      <c r="D137" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>127</v>
+      </c>
+      <c r="B138" t="s">
+        <v>9</v>
+      </c>
+      <c r="C138" t="s">
+        <v>128</v>
+      </c>
+      <c r="D138" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>238</v>
+      </c>
+      <c r="B139" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139" t="s">
+        <v>239</v>
+      </c>
+      <c r="D139" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>15</v>
+      </c>
+      <c r="B140" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140" t="s">
         <v>16</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D140" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130" s="2" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>431</v>
+      </c>
+      <c r="C141" t="s">
+        <v>432</v>
+      </c>
+      <c r="D141" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>473</v>
+      </c>
+      <c r="B142" t="s">
+        <v>354</v>
+      </c>
+      <c r="C142" t="s">
+        <v>355</v>
+      </c>
+      <c r="D142" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="2"/>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131" t="s">
+      <c r="B143" s="2"/>
+      <c r="C143" s="2"/>
+      <c r="D143" s="2"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>131</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B144" t="s">
         <v>130</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C144" t="s">
         <v>150</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D144" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A132" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>148</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B145" t="s">
         <v>130</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C145" t="s">
         <v>151</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D145" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>132</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B146" t="s">
         <v>130</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C146" t="s">
         <v>133</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D146" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A134" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>137</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B147" t="s">
         <v>130</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C147" t="s">
         <v>138</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D147" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A135" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>134</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B148" t="s">
         <v>130</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C148" t="s">
         <v>135</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D148" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>141</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B149" t="s">
         <v>130</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C149" t="s">
         <v>153</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D149" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>143</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B150" t="s">
         <v>130</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C150" t="s">
         <v>152</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D150" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>145</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B151" t="s">
         <v>130</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C151" t="s">
         <v>146</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D151" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A139" s="4" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B139" s="4"/>
-      <c r="C139" s="4"/>
-      <c r="D139" s="4"/>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" t="s">
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="4"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>84</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B153" t="s">
         <v>85</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C153" t="s">
+        <v>398</v>
+      </c>
+      <c r="D153" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>396</v>
+      </c>
+      <c r="B154" t="s">
+        <v>85</v>
+      </c>
+      <c r="C154" t="s">
+        <v>387</v>
+      </c>
+      <c r="D154" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>180</v>
+      </c>
+      <c r="B155" t="s">
+        <v>85</v>
+      </c>
+      <c r="C155" t="s">
         <v>400</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D155" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A141" t="s">
-        <v>398</v>
-      </c>
-      <c r="B141" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>402</v>
+      </c>
+      <c r="B156" t="s">
         <v>85</v>
       </c>
-      <c r="C141" t="s">
-        <v>389</v>
-      </c>
-      <c r="D141" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A142" t="s">
-        <v>180</v>
-      </c>
-      <c r="B142" t="s">
+      <c r="C156" t="s">
+        <v>403</v>
+      </c>
+      <c r="D156" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>86</v>
+      </c>
+      <c r="B157" t="s">
         <v>85</v>
       </c>
-      <c r="C142" t="s">
-        <v>402</v>
-      </c>
-      <c r="D142" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A143" t="s">
-        <v>404</v>
-      </c>
-      <c r="B143" t="s">
-        <v>85</v>
-      </c>
-      <c r="C143" t="s">
-        <v>405</v>
-      </c>
-      <c r="D143" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A144" t="s">
-        <v>86</v>
-      </c>
-      <c r="B144" t="s">
-        <v>85</v>
-      </c>
-      <c r="C144" t="s">
+      <c r="C157" t="s">
         <v>87</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D157" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bunch of incremental improvements
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DA5DBB-19AA-4F7D-AF6F-7DDAD3CC5904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FE1923-5291-451D-9998-6CEE7B6F020D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="557">
   <si>
     <t>id</t>
   </si>
@@ -50,9 +50,6 @@
     <t>titleCase</t>
   </si>
   <si>
-    <t>Sets language in titleCase function</t>
-  </si>
-  <si>
     <t>en</t>
   </si>
   <si>
@@ -311,18 +308,6 @@
     <t>Télécharger les données</t>
   </si>
   <si>
-    <t>chg_lang</t>
-  </si>
-  <si>
-    <t>direct translation for language selection</t>
-  </si>
-  <si>
-    <t>Change Language</t>
-  </si>
-  <si>
-    <t>Changer de langue</t>
-  </si>
-  <si>
     <t>Filters affect each other by limiting subsequent options. Reset to clear all filters.</t>
   </si>
   <si>
@@ -1707,6 +1692,18 @@
   </si>
   <si>
     <t>generating_working</t>
+  </si>
+  <si>
+    <t>Sets language to use in titleCase function</t>
+  </si>
+  <si>
+    <t>the page/website title</t>
+  </si>
+  <si>
+    <t>Portail de données hydrométéorologiques du Yukon</t>
+  </si>
+  <si>
+    <t>Yukon Hydrometeorological Data Portal:</t>
   </si>
 </sst>
 </file>
@@ -2649,8 +2646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="A170" sqref="A170"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2681,32 +2678,32 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>553</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>554</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>556</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>555</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2714,105 +2711,105 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2820,133 +2817,133 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B13" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C13" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D13" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B14" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C14" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D14" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>328</v>
+      </c>
+      <c r="B15" t="s">
+        <v>334</v>
+      </c>
+      <c r="C15" t="s">
         <v>333</v>
       </c>
-      <c r="B15" t="s">
-        <v>339</v>
-      </c>
-      <c r="C15" t="s">
-        <v>338</v>
-      </c>
       <c r="D15" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B16" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C16" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D16" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B17" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C17" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D17" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B18" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C18" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D18" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B19" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C19" t="s">
+        <v>338</v>
+      </c>
+      <c r="D19" t="s">
         <v>343</v>
-      </c>
-      <c r="D19" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B20" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C20" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="D20" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B21" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C21" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="D21" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2954,35 +2951,35 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
         <v>40</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" t="s">
         <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>179</v>
-      </c>
-      <c r="D23" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
         <v>43</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>44</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>45</v>
-      </c>
-      <c r="D24" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2990,21 +2987,21 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>48</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>49</v>
-      </c>
-      <c r="D26" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -3012,259 +3009,259 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" t="s">
         <v>51</v>
       </c>
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>52</v>
-      </c>
-      <c r="D28" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B29" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C29" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D29" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" t="s">
+        <v>210</v>
+      </c>
+      <c r="C30" t="s">
         <v>89</v>
       </c>
-      <c r="B30" t="s">
-        <v>215</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>90</v>
-      </c>
-      <c r="D30" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B31" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C31" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D31" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B32" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C32" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D32" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B33" t="s">
+        <v>278</v>
+      </c>
+      <c r="C33" t="s">
         <v>283</v>
       </c>
-      <c r="C33" t="s">
-        <v>288</v>
-      </c>
       <c r="D33" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>273</v>
+      </c>
+      <c r="B34" t="s">
         <v>278</v>
       </c>
-      <c r="B34" t="s">
-        <v>283</v>
-      </c>
       <c r="C34" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D34" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B35" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C35" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D35" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>279</v>
+      </c>
+      <c r="B36" t="s">
+        <v>280</v>
+      </c>
+      <c r="C36" t="s">
+        <v>281</v>
+      </c>
+      <c r="D36" t="s">
         <v>284</v>
-      </c>
-      <c r="B36" t="s">
-        <v>285</v>
-      </c>
-      <c r="C36" t="s">
-        <v>286</v>
-      </c>
-      <c r="D36" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B37" t="s">
+        <v>280</v>
+      </c>
+      <c r="C37" t="s">
         <v>285</v>
       </c>
-      <c r="C37" t="s">
-        <v>290</v>
-      </c>
       <c r="D37" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B38" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C38" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D38" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B39" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C39" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D39" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B40" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C40" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D40" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B41" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C41" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D41" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B42" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C42" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D42" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B43" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C43" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D43" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B44" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C44" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D44" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B45" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C45" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D45" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -3272,105 +3269,105 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B47" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D47" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" t="s">
+        <v>211</v>
+      </c>
+      <c r="C48" t="s">
         <v>78</v>
       </c>
-      <c r="B48" t="s">
-        <v>216</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>79</v>
-      </c>
-      <c r="D48" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B49" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C49" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D49" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>244</v>
+      </c>
+      <c r="B50" t="s">
+        <v>245</v>
+      </c>
+      <c r="C50" t="s">
+        <v>248</v>
+      </c>
+      <c r="D50" t="s">
         <v>249</v>
-      </c>
-      <c r="B50" t="s">
-        <v>250</v>
-      </c>
-      <c r="C50" t="s">
-        <v>253</v>
-      </c>
-      <c r="D50" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B51" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C51" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D51" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B52" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C52" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D52" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B53" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C53" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D53" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -3378,21 +3375,21 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" t="s">
         <v>54</v>
       </c>
-      <c r="B55" t="s">
-        <v>48</v>
-      </c>
-      <c r="C55" t="s">
-        <v>55</v>
-      </c>
       <c r="D55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -3400,91 +3397,91 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" t="s">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
-        <v>48</v>
-      </c>
-      <c r="C57" t="s">
-        <v>57</v>
-      </c>
       <c r="D57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C58" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D58" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" t="s">
+        <v>98</v>
+      </c>
+      <c r="D59" t="s">
         <v>100</v>
-      </c>
-      <c r="B59" t="s">
-        <v>101</v>
-      </c>
-      <c r="C59" t="s">
-        <v>103</v>
-      </c>
-      <c r="D59" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B60" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" t="s">
+        <v>99</v>
+      </c>
+      <c r="D60" t="s">
         <v>101</v>
-      </c>
-      <c r="C60" t="s">
-        <v>104</v>
-      </c>
-      <c r="D60" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B61" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C61" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D61" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B62" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C62" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D62" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -3492,501 +3489,501 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" t="s">
         <v>58</v>
       </c>
-      <c r="B64" t="s">
-        <v>48</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>59</v>
-      </c>
-      <c r="D64" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>359</v>
+      </c>
+      <c r="B65" t="s">
+        <v>358</v>
+      </c>
+      <c r="C65" t="s">
         <v>364</v>
       </c>
-      <c r="B65" t="s">
-        <v>363</v>
-      </c>
-      <c r="C65" t="s">
-        <v>369</v>
-      </c>
       <c r="D65" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>360</v>
+      </c>
+      <c r="B66" t="s">
+        <v>358</v>
+      </c>
+      <c r="C66" t="s">
         <v>365</v>
       </c>
-      <c r="B66" t="s">
-        <v>363</v>
-      </c>
-      <c r="C66" t="s">
-        <v>370</v>
-      </c>
       <c r="D66" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B67" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C67" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D67" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B68" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C68" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D68" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C69" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D69" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C70" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D70" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="C71" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D71" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>457</v>
+      </c>
+      <c r="C72" t="s">
+        <v>461</v>
+      </c>
+      <c r="D72" t="s">
         <v>462</v>
-      </c>
-      <c r="C72" t="s">
-        <v>466</v>
-      </c>
-      <c r="D72" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="C73" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D73" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C74" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D74" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B75" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C75" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D75" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C76" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="D76" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C77" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="D77" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B78" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C78" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D78" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="C79" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="D79" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="C80" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="D80" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C81" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D81" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="C82" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D82" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C83" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D83" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C84" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D84" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="C85" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D85" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C86" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D86" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="C87" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D87" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>444</v>
+      </c>
+      <c r="C88" t="s">
         <v>449</v>
       </c>
-      <c r="C88" t="s">
-        <v>454</v>
-      </c>
       <c r="D88" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="C89" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D89" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="C90" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="D90" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C91" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D91" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="C92" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D92" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="C93" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D93" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="C94" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D94" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C95" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="D95" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="C96" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="D96" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="C97" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D97" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="C98" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="D98" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="C99" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="D99" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="C100" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="D100" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="C101" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="D101" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="C102" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="D102" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="C103" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="D103" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="C104" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D104" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="C105" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="D105" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="C106" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="D106" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -3994,105 +3991,105 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B108" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C108" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D108" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B109" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C109" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D109" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B110" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C110" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D110" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B111" t="s">
+        <v>154</v>
+      </c>
+      <c r="C111" t="s">
+        <v>158</v>
+      </c>
+      <c r="D111" t="s">
         <v>159</v>
-      </c>
-      <c r="C111" t="s">
-        <v>163</v>
-      </c>
-      <c r="D111" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B112" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C112" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D112" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B113" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B114" t="s">
+        <v>161</v>
+      </c>
+      <c r="C114" t="s">
         <v>166</v>
       </c>
-      <c r="C114" t="s">
-        <v>171</v>
-      </c>
       <c r="D114" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
@@ -4100,726 +4097,726 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>60</v>
+      </c>
+      <c r="B116" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116" t="s">
         <v>61</v>
       </c>
-      <c r="B116" t="s">
-        <v>9</v>
-      </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
         <v>62</v>
-      </c>
-      <c r="D116" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B117" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C117" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D117" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>63</v>
+      </c>
+      <c r="B118" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118" t="s">
         <v>64</v>
       </c>
-      <c r="B118" t="s">
-        <v>9</v>
-      </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
         <v>65</v>
-      </c>
-      <c r="D118" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>66</v>
+      </c>
+      <c r="B119" t="s">
+        <v>8</v>
+      </c>
+      <c r="C119" t="s">
         <v>67</v>
       </c>
-      <c r="B119" t="s">
-        <v>9</v>
-      </c>
-      <c r="C119" t="s">
-        <v>68</v>
-      </c>
       <c r="D119" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B120" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C120" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D120" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>381</v>
+      </c>
+      <c r="B121" t="s">
+        <v>8</v>
+      </c>
+      <c r="C121" t="s">
+        <v>384</v>
+      </c>
+      <c r="D121" t="s">
         <v>386</v>
-      </c>
-      <c r="B121" t="s">
-        <v>9</v>
-      </c>
-      <c r="C121" t="s">
-        <v>389</v>
-      </c>
-      <c r="D121" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>382</v>
+      </c>
+      <c r="B122" t="s">
+        <v>8</v>
+      </c>
+      <c r="C122" t="s">
+        <v>385</v>
+      </c>
+      <c r="D122" t="s">
         <v>387</v>
-      </c>
-      <c r="B122" t="s">
-        <v>9</v>
-      </c>
-      <c r="C122" t="s">
-        <v>390</v>
-      </c>
-      <c r="D122" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>383</v>
+      </c>
+      <c r="B123" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123" t="s">
         <v>388</v>
       </c>
-      <c r="B123" t="s">
-        <v>9</v>
-      </c>
-      <c r="C123" t="s">
-        <v>393</v>
-      </c>
       <c r="D123" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C124" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D124" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B125" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C125" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D125" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B126" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C126" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D126" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B127" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C127" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D127" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>68</v>
+      </c>
+      <c r="B128" t="s">
+        <v>8</v>
+      </c>
+      <c r="C128" t="s">
         <v>69</v>
       </c>
-      <c r="B128" t="s">
-        <v>9</v>
-      </c>
-      <c r="C128" t="s">
+      <c r="D128" t="s">
         <v>70</v>
-      </c>
-      <c r="D128" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B129" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C129" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D129" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B130" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C130" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D130" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>71</v>
+      </c>
+      <c r="B131" t="s">
+        <v>8</v>
+      </c>
+      <c r="C131" t="s">
         <v>72</v>
       </c>
-      <c r="B131" t="s">
-        <v>9</v>
-      </c>
-      <c r="C131" t="s">
+      <c r="D131" t="s">
         <v>73</v>
-      </c>
-      <c r="D131" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B132" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C132" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D132" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B133" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C133" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D133" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>74</v>
+      </c>
+      <c r="B134" t="s">
+        <v>8</v>
+      </c>
+      <c r="C134" t="s">
         <v>75</v>
       </c>
-      <c r="B134" t="s">
-        <v>9</v>
-      </c>
-      <c r="C134" t="s">
+      <c r="D134" t="s">
         <v>76</v>
-      </c>
-      <c r="D134" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B135" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C135" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D135" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B136" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C136" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D136" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B137" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C137" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D137" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B138" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C138" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D138" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B139" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C139" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D139" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C140" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D140" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>80</v>
+      </c>
+      <c r="B141" t="s">
+        <v>8</v>
+      </c>
+      <c r="C141" t="s">
         <v>81</v>
       </c>
-      <c r="B141" t="s">
-        <v>9</v>
-      </c>
-      <c r="C141" t="s">
+      <c r="D141" t="s">
         <v>82</v>
-      </c>
-      <c r="D141" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>7</v>
+      </c>
+      <c r="B142" t="s">
         <v>8</v>
       </c>
-      <c r="B142" t="s">
+      <c r="C142" t="s">
         <v>9</v>
       </c>
-      <c r="C142" t="s">
+      <c r="D142" t="s">
         <v>10</v>
-      </c>
-      <c r="D142" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="C143" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D143" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B144" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C144" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D144" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B145" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C145" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D145" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B146" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C146" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D146" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B147" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C147" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D147" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B148" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C148" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D148" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B149" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C149" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D149" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B150" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C150" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D150" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B151" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C151" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D151" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B152" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C152" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D152" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B153" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C153" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D153" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>14</v>
+      </c>
+      <c r="B154" t="s">
+        <v>8</v>
+      </c>
+      <c r="C154" t="s">
         <v>15</v>
       </c>
-      <c r="B154" t="s">
-        <v>9</v>
-      </c>
-      <c r="C154" t="s">
+      <c r="D154" t="s">
         <v>16</v>
-      </c>
-      <c r="D154" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="C155" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D155" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="C156" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="D156" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B157" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C157" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="D157" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="C158" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="D158" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="C159" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D159" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="C160" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="D160" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="C161" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D161" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="C162" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="D162" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="C163" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="D163" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="C164" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="D164" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="C165" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="D165" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="C166" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="D166" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="C167" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D167" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="C168" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="D168" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="C169" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="D169" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="C170" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="D170" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -4827,119 +4824,119 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B172" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C172" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D172" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B173" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C173" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D173" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B174" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C174" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D174" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B175" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C175" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D175" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B176" t="s">
+        <v>125</v>
+      </c>
+      <c r="C176" t="s">
         <v>130</v>
       </c>
-      <c r="C176" t="s">
-        <v>135</v>
-      </c>
       <c r="D176" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B177" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C177" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D177" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B178" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C178" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D178" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B179" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C179" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D179" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
@@ -4947,72 +4944,72 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
+        <v>83</v>
+      </c>
+      <c r="B181" t="s">
         <v>84</v>
       </c>
-      <c r="B181" t="s">
-        <v>85</v>
-      </c>
       <c r="C181" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="D181" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B182" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C182" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="D182" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B183" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C183" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D183" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B184" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C184" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D184" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>85</v>
+      </c>
+      <c r="B185" t="s">
+        <v>84</v>
+      </c>
+      <c r="C185" t="s">
         <v>86</v>
       </c>
-      <c r="B185" t="s">
-        <v>85</v>
-      </c>
-      <c r="C185" t="s">
+      <c r="D185" t="s">
         <v>87</v>
-      </c>
-      <c r="D185" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add UI for snowInfo report
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FE1923-5291-451D-9998-6CEE7B6F020D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D802FCD-D889-4896-8129-E1072ACD8D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="579">
   <si>
     <t>id</t>
   </si>
@@ -1478,9 +1478,6 @@
     <t>Tous les endroits</t>
   </si>
   <si>
-    <t>gen_waterInfo_loc_select</t>
-  </si>
-  <si>
     <t>Select one, many, or all locations</t>
   </si>
   <si>
@@ -1640,9 +1637,6 @@
     <t>Max % de données manquantes pour retenir une valeure annuelle (dans les mois d'intérêt)</t>
   </si>
   <si>
-    <t>gen_waterInfo_plots</t>
-  </si>
-  <si>
     <t>Generate plots?</t>
   </si>
   <si>
@@ -1673,9 +1667,6 @@
     <t>Separate</t>
   </si>
   <si>
-    <t>séparé</t>
-  </si>
-  <si>
     <t>create_report</t>
   </si>
   <si>
@@ -1704,13 +1695,88 @@
   </si>
   <si>
     <t>Yukon Hydrometeorological Data Portal:</t>
+  </si>
+  <si>
+    <t>gen_waterInfo_info</t>
+  </si>
+  <si>
+    <t>This function is intended to facilitate the reporting of hydrology data by compiling basic statistics (years of record, months of operation, min, max, etc.), trend information (Mann-Kendall direction and p-value, Sen's slope), and creating simple plots of level (for lakes) or flow for all requested locations. Please note that this isn't exactly a polished output, and is to be used strictly for informational purposes. In particular, note that very little of the data underlying the trends calculated has been cleaned or certified as correct by a human.</t>
+  </si>
+  <si>
+    <t>Cette fonction est conçue pour faciliter le rapport des données hydrologiques en compilant des statistiques de base (années de relevés, mois d’exploitation, minimum, maximum, etc.), des informations sur les tendances (direction de Mann-Kendall et valeur-p, pente de Sen) et en générant des graphiques simples du niveau (pour les lacs) ou du débit pour tous les emplacements demandés. Veuillez noter qu’il ne s’agit pas d’un résultat finalisé, mais d’un outil strictement destiné à des fins informatives. En particulier, il convient de souligner que très peu des données sous-jacentes aux tendances calculées ont été nettoyées ou certifiées comme correctes par un humain.</t>
+  </si>
+  <si>
+    <t>gen_snowInfo_info</t>
+  </si>
+  <si>
+    <t>This function is intended to facilitate the reporting of snowpack data by compiling basic statistics (years of record, months of sampling, min, max, etc.), trend information (Mann-Kendall direction and p-value, Sen's slope), and creating simple plots of snow depth, snow water equivalent (SWE), and density for all requested locations. Please note that this isn't exactly a polished output, and is to be used strictly for informational purposes.</t>
+  </si>
+  <si>
+    <t>Cette fonction est conçue pour faciliter le rapport des données sur le manteau neigeux en compilant des statistiques de base (années de relevés, mois d’échantillonnage, minimum, maximum, etc.), des informations sur les tendances (direction de Mann-Kendall et valeur-p, pente de Sen) et en générant des graphiques simples de la profondeur de neige, de l’équivalent en eau de neige (EEN) et de la densité pour tous les emplacements demandés. Veuillez noter qu’il ne s’agit pas d’un résultat finalisé, mais d’un outil strictement destiné à des fins informatives.</t>
+  </si>
+  <si>
+    <t>gen_loc_select</t>
+  </si>
+  <si>
+    <t>gen_snowInfo_inactive</t>
+  </si>
+  <si>
+    <t>Include inactive locations?</t>
+  </si>
+  <si>
+    <t>Inclure les parcours inactifs?</t>
+  </si>
+  <si>
+    <t>gen_generate_plots</t>
+  </si>
+  <si>
+    <t>gen_snowInfo_complete</t>
+  </si>
+  <si>
+    <t>Complete years only?</t>
+  </si>
+  <si>
+    <t>Années complètes seulement?</t>
+  </si>
+  <si>
+    <t>gen_snowInfo_ptype</t>
+  </si>
+  <si>
+    <t>Grahpiques séparés ou combinés?</t>
+  </si>
+  <si>
+    <t>Combined or separate plots?</t>
+  </si>
+  <si>
+    <t>séparés</t>
+  </si>
+  <si>
+    <t>Combined</t>
+  </si>
+  <si>
+    <t>combinés</t>
+  </si>
+  <si>
+    <t>gen_snowInfo_ptype_separate</t>
+  </si>
+  <si>
+    <t>gen_snowInfo_ptype_combine</t>
+  </si>
+  <si>
+    <t>Select at least one location.</t>
+  </si>
+  <si>
+    <t>Sélectionez au moins un endroit.</t>
+  </si>
+  <si>
+    <t>gen_no_loc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1858,6 +1924,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="42">
@@ -2256,7 +2328,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -2268,6 +2340,7 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2644,10 +2717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D185"/>
+  <dimension ref="A1:D193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2678,7 +2751,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -2692,13 +2765,13 @@
         <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C3" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="D3" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3851,1164 +3924,1252 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>472</v>
-      </c>
-      <c r="C95" t="s">
-        <v>473</v>
+        <v>554</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>555</v>
       </c>
       <c r="D95" t="s">
-        <v>474</v>
+        <v>556</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C96" t="s">
-        <v>531</v>
+        <v>473</v>
       </c>
       <c r="D96" t="s">
-        <v>529</v>
+        <v>474</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C97" t="s">
-        <v>476</v>
+        <v>530</v>
       </c>
       <c r="D97" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C98" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="D98" t="s">
-        <v>483</v>
+        <v>529</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>484</v>
+        <v>560</v>
       </c>
       <c r="C99" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D99" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>523</v>
+        <v>578</v>
       </c>
       <c r="C100" t="s">
-        <v>525</v>
+        <v>576</v>
       </c>
       <c r="D100" t="s">
-        <v>527</v>
+        <v>577</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>524</v>
+        <v>483</v>
       </c>
       <c r="C101" t="s">
-        <v>526</v>
+        <v>484</v>
       </c>
       <c r="D101" t="s">
-        <v>528</v>
+        <v>485</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="C102" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
       <c r="D102" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>535</v>
+        <v>523</v>
       </c>
       <c r="C103" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="D103" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="C104" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="D104" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>541</v>
+        <v>564</v>
       </c>
       <c r="C105" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
       <c r="D105" t="s">
-        <v>544</v>
+        <v>535</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>536</v>
+      </c>
+      <c r="C106" t="s">
+        <v>537</v>
+      </c>
+      <c r="D106" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>539</v>
+      </c>
+      <c r="C107" t="s">
+        <v>541</v>
+      </c>
+      <c r="D107" t="s">
         <v>542</v>
       </c>
-      <c r="C106" t="s">
-        <v>545</v>
-      </c>
-      <c r="D106" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>151</v>
-      </c>
-      <c r="B108" t="s">
-        <v>47</v>
+        <v>540</v>
       </c>
       <c r="C108" t="s">
-        <v>152</v>
+        <v>543</v>
       </c>
       <c r="D108" t="s">
-        <v>153</v>
+        <v>571</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>157</v>
-      </c>
-      <c r="B109" t="s">
-        <v>154</v>
-      </c>
-      <c r="C109" t="s">
-        <v>155</v>
+        <v>557</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>558</v>
       </c>
       <c r="D109" t="s">
-        <v>156</v>
+        <v>559</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>160</v>
-      </c>
-      <c r="B110" t="s">
-        <v>161</v>
-      </c>
-      <c r="C110" t="s">
-        <v>172</v>
+        <v>561</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>562</v>
       </c>
       <c r="D110" t="s">
-        <v>173</v>
+        <v>563</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>169</v>
-      </c>
-      <c r="B111" t="s">
-        <v>154</v>
-      </c>
-      <c r="C111" t="s">
-        <v>158</v>
+        <v>565</v>
+      </c>
+      <c r="C111" s="11" t="s">
+        <v>566</v>
       </c>
       <c r="D111" t="s">
-        <v>159</v>
+        <v>567</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>162</v>
-      </c>
-      <c r="B112" t="s">
-        <v>161</v>
-      </c>
-      <c r="C112" t="s">
-        <v>171</v>
+        <v>568</v>
+      </c>
+      <c r="C112" s="11" t="s">
+        <v>570</v>
       </c>
       <c r="D112" t="s">
-        <v>170</v>
+        <v>569</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>163</v>
-      </c>
-      <c r="B113" t="s">
-        <v>165</v>
-      </c>
-      <c r="C113" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D113" s="9" t="s">
-        <v>167</v>
+        <v>574</v>
+      </c>
+      <c r="C113" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="D113" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>164</v>
-      </c>
-      <c r="B114" t="s">
-        <v>161</v>
-      </c>
-      <c r="C114" t="s">
-        <v>166</v>
+        <v>575</v>
+      </c>
+      <c r="C114" s="11" t="s">
+        <v>572</v>
       </c>
       <c r="D114" t="s">
-        <v>168</v>
+        <v>573</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B115" s="8"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
+      <c r="A115" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>60</v>
+        <v>151</v>
       </c>
       <c r="B116" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="C116" t="s">
-        <v>61</v>
+        <v>152</v>
       </c>
       <c r="D116" t="s">
-        <v>62</v>
+        <v>153</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="B117" t="s">
-        <v>8</v>
+        <v>154</v>
       </c>
       <c r="C117" t="s">
-        <v>109</v>
+        <v>155</v>
       </c>
       <c r="D117" t="s">
-        <v>110</v>
+        <v>156</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>63</v>
+        <v>160</v>
       </c>
       <c r="B118" t="s">
-        <v>8</v>
+        <v>161</v>
       </c>
       <c r="C118" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="D118" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>66</v>
+        <v>169</v>
       </c>
       <c r="B119" t="s">
-        <v>8</v>
+        <v>154</v>
       </c>
       <c r="C119" t="s">
-        <v>67</v>
+        <v>158</v>
       </c>
       <c r="D119" t="s">
-        <v>247</v>
+        <v>159</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>242</v>
+        <v>162</v>
       </c>
       <c r="B120" t="s">
-        <v>8</v>
+        <v>161</v>
       </c>
       <c r="C120" t="s">
-        <v>243</v>
+        <v>171</v>
       </c>
       <c r="D120" t="s">
-        <v>243</v>
+        <v>170</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>381</v>
+        <v>163</v>
       </c>
       <c r="B121" t="s">
-        <v>8</v>
-      </c>
-      <c r="C121" t="s">
-        <v>384</v>
-      </c>
-      <c r="D121" t="s">
-        <v>386</v>
+        <v>165</v>
+      </c>
+      <c r="C121" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D121" s="9" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>382</v>
+        <v>164</v>
       </c>
       <c r="B122" t="s">
-        <v>8</v>
+        <v>161</v>
       </c>
       <c r="C122" t="s">
-        <v>385</v>
+        <v>166</v>
       </c>
       <c r="D122" t="s">
-        <v>387</v>
+        <v>168</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>383</v>
-      </c>
-      <c r="B123" t="s">
-        <v>8</v>
-      </c>
-      <c r="C123" t="s">
-        <v>388</v>
-      </c>
-      <c r="D123" t="s">
-        <v>389</v>
-      </c>
+      <c r="A123" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B123" s="8"/>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>177</v>
+        <v>60</v>
       </c>
       <c r="B124" t="s">
         <v>8</v>
       </c>
       <c r="C124" t="s">
-        <v>178</v>
+        <v>61</v>
       </c>
       <c r="D124" t="s">
-        <v>179</v>
+        <v>62</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>188</v>
+        <v>108</v>
       </c>
       <c r="B125" t="s">
         <v>8</v>
       </c>
       <c r="C125" t="s">
-        <v>189</v>
+        <v>109</v>
       </c>
       <c r="D125" t="s">
-        <v>190</v>
+        <v>110</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>197</v>
+        <v>63</v>
       </c>
       <c r="B126" t="s">
         <v>8</v>
       </c>
       <c r="C126" t="s">
-        <v>198</v>
+        <v>64</v>
       </c>
       <c r="D126" t="s">
-        <v>199</v>
+        <v>65</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>176</v>
+        <v>66</v>
       </c>
       <c r="B127" t="s">
         <v>8</v>
       </c>
       <c r="C127" t="s">
-        <v>215</v>
+        <v>67</v>
       </c>
       <c r="D127" t="s">
-        <v>216</v>
+        <v>247</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>68</v>
+        <v>242</v>
       </c>
       <c r="B128" t="s">
         <v>8</v>
       </c>
       <c r="C128" t="s">
-        <v>69</v>
+        <v>243</v>
       </c>
       <c r="D128" t="s">
-        <v>70</v>
+        <v>243</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>185</v>
+        <v>381</v>
       </c>
       <c r="B129" t="s">
         <v>8</v>
       </c>
       <c r="C129" t="s">
-        <v>180</v>
+        <v>384</v>
       </c>
       <c r="D129" t="s">
-        <v>16</v>
+        <v>386</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>191</v>
+        <v>382</v>
       </c>
       <c r="B130" t="s">
         <v>8</v>
       </c>
       <c r="C130" t="s">
-        <v>192</v>
+        <v>385</v>
       </c>
       <c r="D130" t="s">
-        <v>193</v>
+        <v>387</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>71</v>
+        <v>383</v>
       </c>
       <c r="B131" t="s">
         <v>8</v>
       </c>
       <c r="C131" t="s">
-        <v>72</v>
+        <v>388</v>
       </c>
       <c r="D131" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B132" t="s">
         <v>8</v>
       </c>
       <c r="C132" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D132" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B133" t="s">
         <v>8</v>
       </c>
       <c r="C133" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D133" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>74</v>
+        <v>197</v>
       </c>
       <c r="B134" t="s">
         <v>8</v>
       </c>
       <c r="C134" t="s">
-        <v>75</v>
+        <v>198</v>
       </c>
       <c r="D134" t="s">
-        <v>76</v>
+        <v>199</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B135" t="s">
         <v>8</v>
       </c>
       <c r="C135" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="D135" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>200</v>
+        <v>68</v>
       </c>
       <c r="B136" t="s">
         <v>8</v>
       </c>
       <c r="C136" t="s">
-        <v>201</v>
+        <v>69</v>
       </c>
       <c r="D136" t="s">
-        <v>202</v>
+        <v>70</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="B137" t="s">
         <v>8</v>
       </c>
       <c r="C137" t="s">
-        <v>217</v>
+        <v>180</v>
       </c>
       <c r="D137" t="s">
-        <v>218</v>
+        <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="B138" t="s">
         <v>8</v>
       </c>
       <c r="C138" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="D138" t="s">
-        <v>121</v>
+        <v>193</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>222</v>
+        <v>71</v>
       </c>
       <c r="B139" t="s">
         <v>8</v>
       </c>
       <c r="C139" t="s">
-        <v>223</v>
+        <v>72</v>
       </c>
       <c r="D139" t="s">
-        <v>224</v>
+        <v>73</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>315</v>
+        <v>184</v>
+      </c>
+      <c r="B140" t="s">
+        <v>8</v>
       </c>
       <c r="C140" t="s">
-        <v>316</v>
+        <v>186</v>
       </c>
       <c r="D140" t="s">
-        <v>317</v>
+        <v>187</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>80</v>
+        <v>194</v>
       </c>
       <c r="B141" t="s">
         <v>8</v>
       </c>
       <c r="C141" t="s">
-        <v>81</v>
+        <v>195</v>
       </c>
       <c r="D141" t="s">
-        <v>82</v>
+        <v>196</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="B142" t="s">
         <v>8</v>
       </c>
       <c r="C142" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="D142" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>478</v>
+        <v>183</v>
+      </c>
+      <c r="B143" t="s">
+        <v>8</v>
       </c>
       <c r="C143" t="s">
-        <v>479</v>
+        <v>181</v>
       </c>
       <c r="D143" t="s">
-        <v>480</v>
+        <v>182</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="B144" t="s">
         <v>8</v>
       </c>
       <c r="C144" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="D144" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="B145" t="s">
-        <v>204</v>
+        <v>8</v>
       </c>
       <c r="C145" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="D145" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B146" t="s">
         <v>8</v>
       </c>
       <c r="C146" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D146" t="s">
-        <v>230</v>
+        <v>121</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B147" t="s">
-        <v>204</v>
+        <v>8</v>
       </c>
       <c r="C147" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D147" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>254</v>
-      </c>
-      <c r="B148" t="s">
-        <v>8</v>
+        <v>315</v>
       </c>
       <c r="C148" t="s">
-        <v>250</v>
+        <v>316</v>
       </c>
       <c r="D148" t="s">
-        <v>252</v>
+        <v>317</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="B149" t="s">
-        <v>204</v>
+        <v>8</v>
       </c>
       <c r="C149" t="s">
-        <v>251</v>
+        <v>81</v>
       </c>
       <c r="D149" t="s">
-        <v>253</v>
+        <v>82</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>236</v>
+        <v>7</v>
       </c>
       <c r="B150" t="s">
         <v>8</v>
       </c>
       <c r="C150" t="s">
-        <v>238</v>
+        <v>9</v>
       </c>
       <c r="D150" t="s">
-        <v>240</v>
+        <v>10</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>237</v>
-      </c>
-      <c r="B151" t="s">
-        <v>204</v>
+        <v>478</v>
       </c>
       <c r="C151" t="s">
-        <v>239</v>
+        <v>479</v>
       </c>
       <c r="D151" t="s">
-        <v>241</v>
+        <v>480</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>122</v>
+        <v>225</v>
       </c>
       <c r="B152" t="s">
         <v>8</v>
       </c>
       <c r="C152" t="s">
-        <v>123</v>
+        <v>225</v>
       </c>
       <c r="D152" t="s">
-        <v>124</v>
+        <v>226</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="B153" t="s">
-        <v>8</v>
+        <v>204</v>
       </c>
       <c r="C153" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="D153" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>14</v>
+        <v>227</v>
       </c>
       <c r="B154" t="s">
         <v>8</v>
       </c>
       <c r="C154" t="s">
-        <v>15</v>
+        <v>229</v>
       </c>
       <c r="D154" t="s">
-        <v>16</v>
+        <v>230</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>425</v>
+        <v>228</v>
+      </c>
+      <c r="B155" t="s">
+        <v>204</v>
       </c>
       <c r="C155" t="s">
-        <v>426</v>
+        <v>231</v>
       </c>
       <c r="D155" t="s">
-        <v>427</v>
+        <v>232</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>547</v>
+        <v>254</v>
+      </c>
+      <c r="B156" t="s">
+        <v>8</v>
       </c>
       <c r="C156" t="s">
-        <v>548</v>
+        <v>250</v>
       </c>
       <c r="D156" t="s">
-        <v>549</v>
+        <v>252</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>467</v>
+        <v>255</v>
       </c>
       <c r="B157" t="s">
-        <v>349</v>
+        <v>204</v>
       </c>
       <c r="C157" t="s">
-        <v>350</v>
+        <v>251</v>
       </c>
       <c r="D157" t="s">
-        <v>351</v>
+        <v>253</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>487</v>
+        <v>236</v>
+      </c>
+      <c r="B158" t="s">
+        <v>8</v>
       </c>
       <c r="C158" t="s">
-        <v>499</v>
+        <v>238</v>
       </c>
       <c r="D158" t="s">
-        <v>511</v>
+        <v>240</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>488</v>
+        <v>237</v>
+      </c>
+      <c r="B159" t="s">
+        <v>204</v>
       </c>
       <c r="C159" t="s">
-        <v>500</v>
+        <v>239</v>
       </c>
       <c r="D159" t="s">
-        <v>512</v>
+        <v>241</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>489</v>
+        <v>122</v>
+      </c>
+      <c r="B160" t="s">
+        <v>8</v>
       </c>
       <c r="C160" t="s">
-        <v>501</v>
+        <v>123</v>
       </c>
       <c r="D160" t="s">
-        <v>513</v>
+        <v>124</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>490</v>
+        <v>233</v>
+      </c>
+      <c r="B161" t="s">
+        <v>8</v>
       </c>
       <c r="C161" t="s">
-        <v>502</v>
+        <v>234</v>
       </c>
       <c r="D161" t="s">
-        <v>514</v>
+        <v>235</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>491</v>
+        <v>14</v>
+      </c>
+      <c r="B162" t="s">
+        <v>8</v>
       </c>
       <c r="C162" t="s">
-        <v>503</v>
+        <v>15</v>
       </c>
       <c r="D162" t="s">
-        <v>516</v>
+        <v>16</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>492</v>
+        <v>425</v>
       </c>
       <c r="C163" t="s">
-        <v>504</v>
+        <v>426</v>
       </c>
       <c r="D163" t="s">
-        <v>515</v>
+        <v>427</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>493</v>
+        <v>544</v>
       </c>
       <c r="C164" t="s">
-        <v>505</v>
+        <v>545</v>
       </c>
       <c r="D164" t="s">
-        <v>517</v>
+        <v>546</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>494</v>
+        <v>467</v>
+      </c>
+      <c r="B165" t="s">
+        <v>349</v>
       </c>
       <c r="C165" t="s">
-        <v>506</v>
+        <v>350</v>
       </c>
       <c r="D165" t="s">
-        <v>518</v>
+        <v>351</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="C166" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="D166" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="C167" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="D167" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="C168" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="D168" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="C169" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D169" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>552</v>
+        <v>490</v>
       </c>
       <c r="C170" t="s">
-        <v>551</v>
+        <v>502</v>
       </c>
       <c r="D170" t="s">
-        <v>550</v>
+        <v>515</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B171" s="2"/>
-      <c r="C171" s="2"/>
-      <c r="D171" s="2"/>
+      <c r="A171" t="s">
+        <v>491</v>
+      </c>
+      <c r="C171" t="s">
+        <v>503</v>
+      </c>
+      <c r="D171" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>126</v>
-      </c>
-      <c r="B172" t="s">
-        <v>125</v>
+        <v>492</v>
       </c>
       <c r="C172" t="s">
-        <v>145</v>
+        <v>504</v>
       </c>
       <c r="D172" t="s">
-        <v>144</v>
+        <v>516</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>143</v>
-      </c>
-      <c r="B173" t="s">
-        <v>125</v>
+        <v>493</v>
       </c>
       <c r="C173" t="s">
-        <v>146</v>
+        <v>505</v>
       </c>
       <c r="D173" t="s">
-        <v>149</v>
+        <v>517</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>127</v>
-      </c>
-      <c r="B174" t="s">
-        <v>125</v>
+        <v>494</v>
       </c>
       <c r="C174" t="s">
-        <v>128</v>
+        <v>506</v>
       </c>
       <c r="D174" t="s">
-        <v>135</v>
+        <v>518</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>132</v>
-      </c>
-      <c r="B175" t="s">
-        <v>125</v>
+        <v>495</v>
       </c>
       <c r="C175" t="s">
-        <v>133</v>
+        <v>507</v>
       </c>
       <c r="D175" t="s">
-        <v>134</v>
+        <v>519</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>129</v>
-      </c>
-      <c r="B176" t="s">
-        <v>125</v>
+        <v>496</v>
       </c>
       <c r="C176" t="s">
-        <v>130</v>
+        <v>508</v>
       </c>
       <c r="D176" t="s">
-        <v>131</v>
+        <v>520</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>136</v>
-      </c>
-      <c r="B177" t="s">
-        <v>125</v>
+        <v>497</v>
       </c>
       <c r="C177" t="s">
-        <v>148</v>
+        <v>509</v>
       </c>
       <c r="D177" t="s">
-        <v>137</v>
+        <v>521</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>138</v>
-      </c>
-      <c r="B178" t="s">
+        <v>549</v>
+      </c>
+      <c r="C178" t="s">
+        <v>548</v>
+      </c>
+      <c r="D178" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C178" t="s">
-        <v>147</v>
-      </c>
-      <c r="D178" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>140</v>
-      </c>
-      <c r="B179" t="s">
+      <c r="B179" s="2"/>
+      <c r="C179" s="2"/>
+      <c r="D179" s="2"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>126</v>
+      </c>
+      <c r="B180" t="s">
         <v>125</v>
       </c>
-      <c r="C179" t="s">
-        <v>141</v>
-      </c>
-      <c r="D179" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B180" s="4"/>
-      <c r="C180" s="4"/>
-      <c r="D180" s="4"/>
+      <c r="C180" t="s">
+        <v>145</v>
+      </c>
+      <c r="D180" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="B181" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="C181" t="s">
-        <v>392</v>
+        <v>146</v>
       </c>
       <c r="D181" t="s">
-        <v>393</v>
+        <v>149</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>390</v>
+        <v>127</v>
       </c>
       <c r="B182" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="C182" t="s">
-        <v>381</v>
+        <v>128</v>
       </c>
       <c r="D182" t="s">
-        <v>391</v>
+        <v>135</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>175</v>
+        <v>132</v>
       </c>
       <c r="B183" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="C183" t="s">
-        <v>394</v>
+        <v>133</v>
       </c>
       <c r="D183" t="s">
-        <v>395</v>
+        <v>134</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>396</v>
+        <v>129</v>
       </c>
       <c r="B184" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="C184" t="s">
-        <v>397</v>
+        <v>130</v>
       </c>
       <c r="D184" t="s">
-        <v>398</v>
+        <v>131</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>136</v>
+      </c>
+      <c r="B185" t="s">
+        <v>125</v>
+      </c>
+      <c r="C185" t="s">
+        <v>148</v>
+      </c>
+      <c r="D185" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>138</v>
+      </c>
+      <c r="B186" t="s">
+        <v>125</v>
+      </c>
+      <c r="C186" t="s">
+        <v>147</v>
+      </c>
+      <c r="D186" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>140</v>
+      </c>
+      <c r="B187" t="s">
+        <v>125</v>
+      </c>
+      <c r="C187" t="s">
+        <v>141</v>
+      </c>
+      <c r="D187" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B188" s="4"/>
+      <c r="C188" s="4"/>
+      <c r="D188" s="4"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>83</v>
+      </c>
+      <c r="B189" t="s">
+        <v>84</v>
+      </c>
+      <c r="C189" t="s">
+        <v>392</v>
+      </c>
+      <c r="D189" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>390</v>
+      </c>
+      <c r="B190" t="s">
+        <v>84</v>
+      </c>
+      <c r="C190" t="s">
+        <v>381</v>
+      </c>
+      <c r="D190" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>175</v>
+      </c>
+      <c r="B191" t="s">
+        <v>84</v>
+      </c>
+      <c r="C191" t="s">
+        <v>394</v>
+      </c>
+      <c r="D191" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>396</v>
+      </c>
+      <c r="B192" t="s">
+        <v>84</v>
+      </c>
+      <c r="C192" t="s">
+        <v>397</v>
+      </c>
+      <c r="D192" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>85</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B193" t="s">
         <v>84</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C193" t="s">
         <v>86</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D193" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes to app layout, reactivate tests on plotly objects.
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE24336A-9081-4E10-9577-E472AB71108C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632415C9-3653-40F7-9439-6067AD5A6CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="631">
   <si>
     <t>id</t>
   </si>
@@ -1779,6 +1779,153 @@
   </si>
   <si>
     <t>Entrez un nom d'utilisateur et un mot de passe.</t>
+  </si>
+  <si>
+    <t>gen_snowBul_info</t>
+  </si>
+  <si>
+    <t>This function allows you to create Excel workbooks with the statistics used in creating the Snow Bulletin, or to create the entire Snow Bulletin Word document.</t>
+  </si>
+  <si>
+    <t>Cette fonction vous permet to créer des documents Excel qui contiennent les statistics utilisées lors de la création du bulletin de conditions de neige, ou de créer le bulletin de neige en document Word.</t>
+  </si>
+  <si>
+    <t>gen_snowBul_toggle_stats</t>
+  </si>
+  <si>
+    <t>gen_snowBul_toggle_bulletin</t>
+  </si>
+  <si>
+    <t>Statistiques</t>
+  </si>
+  <si>
+    <t>Bulletin</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>gen_snowBul_year</t>
+  </si>
+  <si>
+    <t>gen_snowBul_month</t>
+  </si>
+  <si>
+    <t>gen_snowBul_lang</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Mois</t>
+  </si>
+  <si>
+    <t>Année</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>gen_snowBul_basins</t>
+  </si>
+  <si>
+    <t>Basins</t>
+  </si>
+  <si>
+    <t>Basins versants</t>
+  </si>
+  <si>
+    <t>gen_snowBul_precip_period</t>
+  </si>
+  <si>
+    <t>gen_snowBul_cddf_period</t>
+  </si>
+  <si>
+    <t>Period of record for precip stats</t>
+  </si>
+  <si>
+    <t>Period of record for CDDF stats</t>
+  </si>
+  <si>
+    <t>Période a utiliser pour les statistiques de précipitation</t>
+  </si>
+  <si>
+    <t>Période à utiliser pour les statistiques de DJGC</t>
+  </si>
+  <si>
+    <t>Last 40 years</t>
+  </si>
+  <si>
+    <t>1981-2010</t>
+  </si>
+  <si>
+    <t>1991-2020</t>
+  </si>
+  <si>
+    <t>Derniers 40 ans</t>
+  </si>
+  <si>
+    <t>All years of record</t>
+  </si>
+  <si>
+    <t>Toutes les années disponibles</t>
+  </si>
+  <si>
+    <t>gen_snowBul_period1</t>
+  </si>
+  <si>
+    <t>gen_snowBul_period2</t>
+  </si>
+  <si>
+    <t>gen_snowBul_period3</t>
+  </si>
+  <si>
+    <t>gen_snowBul_period4</t>
+  </si>
+  <si>
+    <t>Bulletin language</t>
+  </si>
+  <si>
+    <t>Language du bulletin</t>
+  </si>
+  <si>
+    <t>gen_snowBul_scale</t>
+  </si>
+  <si>
+    <t>Plot scale</t>
+  </si>
+  <si>
+    <t>Échelle des graphiques</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>Anglais</t>
+  </si>
+  <si>
+    <t>francais</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>gen_snowBul_error_stats</t>
+  </si>
+  <si>
+    <t>gen_snowBul_error_report</t>
+  </si>
+  <si>
+    <t>Error generating snow bulletin Word document</t>
+  </si>
+  <si>
+    <t>Error generating snow bulletin stats Excel tables</t>
+  </si>
+  <si>
+    <t>Échec lors de la création des tableaux de statistiques</t>
+  </si>
+  <si>
+    <t>Échec lors de la création du rapport Word</t>
   </si>
 </sst>
 </file>
@@ -2726,10 +2873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D194"/>
+  <dimension ref="A1:D212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4166,1033 +4313,1231 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B116" s="4"/>
-      <c r="C116" s="4"/>
-      <c r="D116" s="4"/>
+      <c r="A116" t="s">
+        <v>582</v>
+      </c>
+      <c r="C116" s="11" t="s">
+        <v>583</v>
+      </c>
+      <c r="D116" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>149</v>
-      </c>
-      <c r="B117" t="s">
-        <v>45</v>
-      </c>
-      <c r="C117" t="s">
-        <v>150</v>
+        <v>585</v>
+      </c>
+      <c r="C117" s="11" t="s">
+        <v>589</v>
       </c>
       <c r="D117" t="s">
-        <v>151</v>
+        <v>587</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>155</v>
-      </c>
-      <c r="B118" t="s">
-        <v>152</v>
-      </c>
-      <c r="C118" t="s">
-        <v>153</v>
+        <v>586</v>
+      </c>
+      <c r="C118" s="11" t="s">
+        <v>588</v>
       </c>
       <c r="D118" t="s">
-        <v>154</v>
+        <v>588</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>158</v>
-      </c>
-      <c r="B119" t="s">
-        <v>159</v>
-      </c>
-      <c r="C119" t="s">
-        <v>170</v>
+        <v>590</v>
+      </c>
+      <c r="C119" s="11" t="s">
+        <v>596</v>
       </c>
       <c r="D119" t="s">
-        <v>171</v>
+        <v>595</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>167</v>
-      </c>
-      <c r="B120" t="s">
-        <v>152</v>
-      </c>
-      <c r="C120" t="s">
-        <v>156</v>
+        <v>591</v>
+      </c>
+      <c r="C120" s="11" t="s">
+        <v>593</v>
       </c>
       <c r="D120" t="s">
-        <v>157</v>
+        <v>594</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>160</v>
-      </c>
-      <c r="B121" t="s">
-        <v>159</v>
-      </c>
-      <c r="C121" t="s">
-        <v>169</v>
+        <v>597</v>
+      </c>
+      <c r="C121" s="11" t="s">
+        <v>598</v>
       </c>
       <c r="D121" t="s">
-        <v>168</v>
+        <v>599</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>161</v>
-      </c>
-      <c r="B122" t="s">
-        <v>163</v>
-      </c>
-      <c r="C122" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D122" s="9" t="s">
-        <v>165</v>
+        <v>592</v>
+      </c>
+      <c r="C122" s="11" t="s">
+        <v>616</v>
+      </c>
+      <c r="D122" t="s">
+        <v>617</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>162</v>
-      </c>
-      <c r="B123" t="s">
-        <v>159</v>
-      </c>
-      <c r="C123" t="s">
-        <v>164</v>
+        <v>600</v>
+      </c>
+      <c r="C123" s="11" t="s">
+        <v>602</v>
       </c>
       <c r="D123" t="s">
-        <v>166</v>
+        <v>604</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B124" s="8"/>
-      <c r="C124" s="8"/>
-      <c r="D124" s="8"/>
+      <c r="A124" t="s">
+        <v>601</v>
+      </c>
+      <c r="C124" s="11" t="s">
+        <v>603</v>
+      </c>
+      <c r="D124" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>58</v>
-      </c>
-      <c r="B125" t="s">
-        <v>8</v>
-      </c>
-      <c r="C125" t="s">
-        <v>59</v>
+        <v>612</v>
+      </c>
+      <c r="C125" s="11" t="s">
+        <v>606</v>
       </c>
       <c r="D125" t="s">
-        <v>60</v>
+        <v>609</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>106</v>
-      </c>
-      <c r="B126" t="s">
-        <v>8</v>
-      </c>
-      <c r="C126" t="s">
-        <v>107</v>
+        <v>613</v>
+      </c>
+      <c r="C126" s="11" t="s">
+        <v>610</v>
       </c>
       <c r="D126" t="s">
-        <v>108</v>
+        <v>611</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>61</v>
-      </c>
-      <c r="B127" t="s">
-        <v>8</v>
-      </c>
-      <c r="C127" t="s">
-        <v>62</v>
-      </c>
-      <c r="D127" t="s">
-        <v>63</v>
+        <v>614</v>
+      </c>
+      <c r="C127" s="11" t="s">
+        <v>607</v>
+      </c>
+      <c r="D127" s="11" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>64</v>
-      </c>
-      <c r="B128" t="s">
-        <v>8</v>
-      </c>
-      <c r="C128" t="s">
-        <v>65</v>
-      </c>
-      <c r="D128" t="s">
-        <v>245</v>
+        <v>615</v>
+      </c>
+      <c r="C128" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="D128" s="11" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>240</v>
-      </c>
-      <c r="B129" t="s">
-        <v>8</v>
-      </c>
-      <c r="C129" t="s">
-        <v>241</v>
-      </c>
-      <c r="D129" t="s">
-        <v>241</v>
+        <v>618</v>
+      </c>
+      <c r="C129" s="11" t="s">
+        <v>619</v>
+      </c>
+      <c r="D129" s="11" t="s">
+        <v>620</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>377</v>
-      </c>
-      <c r="B130" t="s">
-        <v>8</v>
-      </c>
-      <c r="C130" t="s">
-        <v>380</v>
-      </c>
-      <c r="D130" t="s">
-        <v>382</v>
+        <v>625</v>
+      </c>
+      <c r="C130" s="11" t="s">
+        <v>628</v>
+      </c>
+      <c r="D130" s="11" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>378</v>
-      </c>
-      <c r="B131" t="s">
-        <v>8</v>
-      </c>
-      <c r="C131" t="s">
-        <v>381</v>
-      </c>
-      <c r="D131" t="s">
-        <v>383</v>
+        <v>626</v>
+      </c>
+      <c r="C131" s="11" t="s">
+        <v>627</v>
+      </c>
+      <c r="D131" s="11" t="s">
+        <v>630</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>379</v>
-      </c>
-      <c r="B132" t="s">
-        <v>8</v>
-      </c>
-      <c r="C132" t="s">
-        <v>384</v>
-      </c>
-      <c r="D132" t="s">
-        <v>385</v>
-      </c>
+      <c r="A132" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B132" s="4"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="4"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="B133" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="C133" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="D133" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="B134" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
       <c r="C134" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="D134" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="B135" t="s">
-        <v>8</v>
+        <v>159</v>
       </c>
       <c r="C135" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="D135" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B136" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
       <c r="C136" t="s">
-        <v>213</v>
+        <v>156</v>
       </c>
       <c r="D136" t="s">
-        <v>214</v>
+        <v>157</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>66</v>
+        <v>160</v>
       </c>
       <c r="B137" t="s">
-        <v>8</v>
+        <v>159</v>
       </c>
       <c r="C137" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="D137" t="s">
-        <v>68</v>
+        <v>168</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="B138" t="s">
-        <v>8</v>
-      </c>
-      <c r="C138" t="s">
-        <v>178</v>
-      </c>
-      <c r="D138" t="s">
-        <v>16</v>
+        <v>163</v>
+      </c>
+      <c r="C138" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D138" s="9" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="B139" t="s">
-        <v>8</v>
+        <v>159</v>
       </c>
       <c r="C139" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
       <c r="D139" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>69</v>
-      </c>
-      <c r="B140" t="s">
-        <v>8</v>
-      </c>
-      <c r="C140" t="s">
-        <v>70</v>
-      </c>
-      <c r="D140" t="s">
-        <v>71</v>
-      </c>
+      <c r="A140" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B140" s="8"/>
+      <c r="C140" s="8"/>
+      <c r="D140" s="8"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>182</v>
+        <v>58</v>
       </c>
       <c r="B141" t="s">
         <v>8</v>
       </c>
       <c r="C141" t="s">
-        <v>184</v>
+        <v>59</v>
       </c>
       <c r="D141" t="s">
-        <v>185</v>
+        <v>60</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>192</v>
+        <v>106</v>
       </c>
       <c r="B142" t="s">
         <v>8</v>
       </c>
       <c r="C142" t="s">
-        <v>193</v>
+        <v>107</v>
       </c>
       <c r="D142" t="s">
-        <v>194</v>
+        <v>108</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B143" t="s">
         <v>8</v>
       </c>
       <c r="C143" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D143" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>181</v>
+        <v>64</v>
       </c>
       <c r="B144" t="s">
         <v>8</v>
       </c>
       <c r="C144" t="s">
-        <v>179</v>
+        <v>65</v>
       </c>
       <c r="D144" t="s">
-        <v>180</v>
+        <v>245</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>198</v>
+        <v>240</v>
       </c>
       <c r="B145" t="s">
         <v>8</v>
       </c>
       <c r="C145" t="s">
-        <v>199</v>
+        <v>241</v>
       </c>
       <c r="D145" t="s">
-        <v>200</v>
+        <v>241</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>217</v>
+        <v>377</v>
       </c>
       <c r="B146" t="s">
         <v>8</v>
       </c>
       <c r="C146" t="s">
-        <v>215</v>
+        <v>380</v>
       </c>
       <c r="D146" t="s">
-        <v>216</v>
+        <v>382</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>218</v>
+        <v>378</v>
       </c>
       <c r="B147" t="s">
         <v>8</v>
       </c>
       <c r="C147" t="s">
-        <v>219</v>
+        <v>381</v>
       </c>
       <c r="D147" t="s">
-        <v>119</v>
+        <v>383</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>220</v>
+        <v>379</v>
       </c>
       <c r="B148" t="s">
         <v>8</v>
       </c>
       <c r="C148" t="s">
-        <v>221</v>
+        <v>384</v>
       </c>
       <c r="D148" t="s">
-        <v>222</v>
+        <v>385</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>313</v>
+        <v>175</v>
+      </c>
+      <c r="B149" t="s">
+        <v>8</v>
       </c>
       <c r="C149" t="s">
-        <v>314</v>
+        <v>176</v>
       </c>
       <c r="D149" t="s">
-        <v>315</v>
+        <v>177</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>78</v>
+        <v>186</v>
       </c>
       <c r="B150" t="s">
         <v>8</v>
       </c>
       <c r="C150" t="s">
-        <v>79</v>
+        <v>187</v>
       </c>
       <c r="D150" t="s">
-        <v>80</v>
+        <v>188</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="B151" t="s">
         <v>8</v>
       </c>
       <c r="C151" t="s">
-        <v>9</v>
+        <v>196</v>
       </c>
       <c r="D151" t="s">
-        <v>10</v>
+        <v>197</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>474</v>
+        <v>174</v>
+      </c>
+      <c r="B152" t="s">
+        <v>8</v>
       </c>
       <c r="C152" t="s">
-        <v>475</v>
+        <v>213</v>
       </c>
       <c r="D152" t="s">
-        <v>476</v>
+        <v>214</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>223</v>
+        <v>66</v>
       </c>
       <c r="B153" t="s">
         <v>8</v>
       </c>
       <c r="C153" t="s">
-        <v>223</v>
+        <v>67</v>
       </c>
       <c r="D153" t="s">
-        <v>224</v>
+        <v>68</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="B154" t="s">
-        <v>202</v>
+        <v>8</v>
       </c>
       <c r="C154" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="D154" t="s">
-        <v>203</v>
+        <v>16</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="B155" t="s">
         <v>8</v>
       </c>
       <c r="C155" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="D155" t="s">
-        <v>228</v>
+        <v>191</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>226</v>
+        <v>69</v>
       </c>
       <c r="B156" t="s">
-        <v>202</v>
+        <v>8</v>
       </c>
       <c r="C156" t="s">
-        <v>229</v>
+        <v>70</v>
       </c>
       <c r="D156" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>252</v>
+        <v>182</v>
       </c>
       <c r="B157" t="s">
         <v>8</v>
       </c>
       <c r="C157" t="s">
-        <v>248</v>
+        <v>184</v>
       </c>
       <c r="D157" t="s">
-        <v>250</v>
+        <v>185</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>253</v>
+        <v>192</v>
       </c>
       <c r="B158" t="s">
-        <v>202</v>
+        <v>8</v>
       </c>
       <c r="C158" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
       <c r="D158" t="s">
-        <v>251</v>
+        <v>194</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>234</v>
+        <v>72</v>
       </c>
       <c r="B159" t="s">
         <v>8</v>
       </c>
       <c r="C159" t="s">
-        <v>236</v>
+        <v>73</v>
       </c>
       <c r="D159" t="s">
-        <v>238</v>
+        <v>74</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>235</v>
+        <v>181</v>
       </c>
       <c r="B160" t="s">
-        <v>202</v>
+        <v>8</v>
       </c>
       <c r="C160" t="s">
-        <v>237</v>
+        <v>179</v>
       </c>
       <c r="D160" t="s">
-        <v>239</v>
+        <v>180</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>120</v>
+        <v>198</v>
       </c>
       <c r="B161" t="s">
         <v>8</v>
       </c>
       <c r="C161" t="s">
-        <v>121</v>
+        <v>199</v>
       </c>
       <c r="D161" t="s">
-        <v>122</v>
+        <v>200</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B162" t="s">
         <v>8</v>
       </c>
       <c r="C162" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="D162" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>14</v>
+        <v>218</v>
       </c>
       <c r="B163" t="s">
         <v>8</v>
       </c>
       <c r="C163" t="s">
-        <v>15</v>
+        <v>219</v>
       </c>
       <c r="D163" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>421</v>
+        <v>220</v>
+      </c>
+      <c r="B164" t="s">
+        <v>8</v>
       </c>
       <c r="C164" t="s">
-        <v>422</v>
+        <v>221</v>
       </c>
       <c r="D164" t="s">
-        <v>423</v>
+        <v>222</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>540</v>
+        <v>313</v>
       </c>
       <c r="C165" t="s">
-        <v>541</v>
+        <v>314</v>
       </c>
       <c r="D165" t="s">
-        <v>542</v>
+        <v>315</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>463</v>
+        <v>78</v>
       </c>
       <c r="B166" t="s">
-        <v>345</v>
+        <v>8</v>
       </c>
       <c r="C166" t="s">
-        <v>346</v>
+        <v>79</v>
       </c>
       <c r="D166" t="s">
-        <v>347</v>
+        <v>80</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>482</v>
+        <v>7</v>
+      </c>
+      <c r="B167" t="s">
+        <v>8</v>
       </c>
       <c r="C167" t="s">
-        <v>494</v>
+        <v>9</v>
       </c>
       <c r="D167" t="s">
-        <v>506</v>
+        <v>10</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="C168" t="s">
-        <v>495</v>
+        <v>475</v>
       </c>
       <c r="D168" t="s">
-        <v>507</v>
+        <v>476</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>484</v>
+        <v>223</v>
+      </c>
+      <c r="B169" t="s">
+        <v>8</v>
       </c>
       <c r="C169" t="s">
-        <v>496</v>
+        <v>223</v>
       </c>
       <c r="D169" t="s">
-        <v>508</v>
+        <v>224</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>485</v>
+        <v>201</v>
+      </c>
+      <c r="B170" t="s">
+        <v>202</v>
       </c>
       <c r="C170" t="s">
-        <v>497</v>
+        <v>201</v>
       </c>
       <c r="D170" t="s">
-        <v>509</v>
+        <v>203</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>486</v>
+        <v>225</v>
+      </c>
+      <c r="B171" t="s">
+        <v>8</v>
       </c>
       <c r="C171" t="s">
-        <v>498</v>
+        <v>227</v>
       </c>
       <c r="D171" t="s">
-        <v>511</v>
+        <v>228</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>487</v>
+        <v>226</v>
+      </c>
+      <c r="B172" t="s">
+        <v>202</v>
       </c>
       <c r="C172" t="s">
-        <v>499</v>
+        <v>229</v>
       </c>
       <c r="D172" t="s">
-        <v>510</v>
+        <v>230</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>488</v>
+        <v>252</v>
+      </c>
+      <c r="B173" t="s">
+        <v>8</v>
       </c>
       <c r="C173" t="s">
-        <v>500</v>
+        <v>248</v>
       </c>
       <c r="D173" t="s">
-        <v>512</v>
+        <v>250</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>489</v>
+        <v>253</v>
+      </c>
+      <c r="B174" t="s">
+        <v>202</v>
       </c>
       <c r="C174" t="s">
-        <v>501</v>
+        <v>249</v>
       </c>
       <c r="D174" t="s">
-        <v>513</v>
+        <v>251</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>490</v>
+        <v>234</v>
+      </c>
+      <c r="B175" t="s">
+        <v>8</v>
       </c>
       <c r="C175" t="s">
-        <v>502</v>
+        <v>236</v>
       </c>
       <c r="D175" t="s">
-        <v>514</v>
+        <v>238</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>491</v>
+        <v>235</v>
+      </c>
+      <c r="B176" t="s">
+        <v>202</v>
       </c>
       <c r="C176" t="s">
-        <v>503</v>
+        <v>237</v>
       </c>
       <c r="D176" t="s">
-        <v>515</v>
+        <v>239</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>492</v>
+        <v>120</v>
+      </c>
+      <c r="B177" t="s">
+        <v>8</v>
       </c>
       <c r="C177" t="s">
-        <v>504</v>
+        <v>121</v>
       </c>
       <c r="D177" t="s">
-        <v>516</v>
+        <v>122</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>493</v>
+        <v>231</v>
+      </c>
+      <c r="B178" t="s">
+        <v>8</v>
       </c>
       <c r="C178" t="s">
-        <v>505</v>
+        <v>232</v>
       </c>
       <c r="D178" t="s">
-        <v>517</v>
+        <v>233</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>545</v>
+        <v>14</v>
+      </c>
+      <c r="B179" t="s">
+        <v>8</v>
       </c>
       <c r="C179" t="s">
-        <v>544</v>
+        <v>15</v>
       </c>
       <c r="D179" t="s">
-        <v>543</v>
+        <v>16</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B180" s="2"/>
-      <c r="C180" s="2"/>
-      <c r="D180" s="2"/>
+      <c r="A180" t="s">
+        <v>421</v>
+      </c>
+      <c r="C180" t="s">
+        <v>422</v>
+      </c>
+      <c r="D180" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>124</v>
-      </c>
-      <c r="B181" t="s">
-        <v>123</v>
+        <v>540</v>
       </c>
       <c r="C181" t="s">
-        <v>143</v>
+        <v>541</v>
       </c>
       <c r="D181" t="s">
-        <v>142</v>
+        <v>542</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>141</v>
+        <v>463</v>
       </c>
       <c r="B182" t="s">
-        <v>123</v>
+        <v>345</v>
       </c>
       <c r="C182" t="s">
-        <v>144</v>
+        <v>346</v>
       </c>
       <c r="D182" t="s">
-        <v>147</v>
+        <v>347</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>125</v>
-      </c>
-      <c r="B183" t="s">
-        <v>123</v>
+        <v>482</v>
       </c>
       <c r="C183" t="s">
-        <v>126</v>
+        <v>494</v>
       </c>
       <c r="D183" t="s">
-        <v>133</v>
+        <v>506</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>130</v>
-      </c>
-      <c r="B184" t="s">
-        <v>123</v>
+        <v>483</v>
       </c>
       <c r="C184" t="s">
-        <v>131</v>
+        <v>495</v>
       </c>
       <c r="D184" t="s">
-        <v>132</v>
+        <v>507</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>127</v>
-      </c>
-      <c r="B185" t="s">
-        <v>123</v>
+        <v>484</v>
       </c>
       <c r="C185" t="s">
-        <v>128</v>
+        <v>496</v>
       </c>
       <c r="D185" t="s">
-        <v>129</v>
+        <v>508</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>134</v>
-      </c>
-      <c r="B186" t="s">
-        <v>123</v>
+        <v>485</v>
       </c>
       <c r="C186" t="s">
-        <v>146</v>
+        <v>497</v>
       </c>
       <c r="D186" t="s">
-        <v>135</v>
+        <v>509</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>136</v>
-      </c>
-      <c r="B187" t="s">
-        <v>123</v>
+        <v>486</v>
       </c>
       <c r="C187" t="s">
-        <v>145</v>
+        <v>498</v>
       </c>
       <c r="D187" t="s">
-        <v>137</v>
+        <v>511</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>138</v>
-      </c>
-      <c r="B188" t="s">
-        <v>123</v>
+        <v>487</v>
       </c>
       <c r="C188" t="s">
-        <v>139</v>
+        <v>499</v>
       </c>
       <c r="D188" t="s">
-        <v>140</v>
+        <v>510</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B189" s="4"/>
-      <c r="C189" s="4"/>
-      <c r="D189" s="4"/>
+      <c r="A189" t="s">
+        <v>488</v>
+      </c>
+      <c r="C189" t="s">
+        <v>500</v>
+      </c>
+      <c r="D189" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>81</v>
-      </c>
-      <c r="B190" t="s">
-        <v>82</v>
+        <v>489</v>
       </c>
       <c r="C190" t="s">
-        <v>388</v>
+        <v>501</v>
       </c>
       <c r="D190" t="s">
-        <v>389</v>
+        <v>513</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>386</v>
-      </c>
-      <c r="B191" t="s">
-        <v>82</v>
+        <v>490</v>
       </c>
       <c r="C191" t="s">
-        <v>377</v>
+        <v>502</v>
       </c>
       <c r="D191" t="s">
-        <v>387</v>
+        <v>514</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>173</v>
-      </c>
-      <c r="B192" t="s">
-        <v>82</v>
+        <v>491</v>
       </c>
       <c r="C192" t="s">
-        <v>390</v>
+        <v>503</v>
       </c>
       <c r="D192" t="s">
-        <v>391</v>
+        <v>515</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>392</v>
-      </c>
-      <c r="B193" t="s">
-        <v>82</v>
+        <v>492</v>
       </c>
       <c r="C193" t="s">
-        <v>393</v>
+        <v>504</v>
       </c>
       <c r="D193" t="s">
-        <v>394</v>
+        <v>516</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
+        <v>493</v>
+      </c>
+      <c r="C194" t="s">
+        <v>505</v>
+      </c>
+      <c r="D194" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>545</v>
+      </c>
+      <c r="C195" t="s">
+        <v>544</v>
+      </c>
+      <c r="D195" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>621</v>
+      </c>
+      <c r="C196" t="s">
+        <v>2</v>
+      </c>
+      <c r="D196" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>623</v>
+      </c>
+      <c r="C197" t="s">
+        <v>624</v>
+      </c>
+      <c r="D197" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B198" s="2"/>
+      <c r="C198" s="2"/>
+      <c r="D198" s="2"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>124</v>
+      </c>
+      <c r="B199" t="s">
+        <v>123</v>
+      </c>
+      <c r="C199" t="s">
+        <v>143</v>
+      </c>
+      <c r="D199" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>141</v>
+      </c>
+      <c r="B200" t="s">
+        <v>123</v>
+      </c>
+      <c r="C200" t="s">
+        <v>144</v>
+      </c>
+      <c r="D200" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>125</v>
+      </c>
+      <c r="B201" t="s">
+        <v>123</v>
+      </c>
+      <c r="C201" t="s">
+        <v>126</v>
+      </c>
+      <c r="D201" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>130</v>
+      </c>
+      <c r="B202" t="s">
+        <v>123</v>
+      </c>
+      <c r="C202" t="s">
+        <v>131</v>
+      </c>
+      <c r="D202" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>127</v>
+      </c>
+      <c r="B203" t="s">
+        <v>123</v>
+      </c>
+      <c r="C203" t="s">
+        <v>128</v>
+      </c>
+      <c r="D203" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>134</v>
+      </c>
+      <c r="B204" t="s">
+        <v>123</v>
+      </c>
+      <c r="C204" t="s">
+        <v>146</v>
+      </c>
+      <c r="D204" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>136</v>
+      </c>
+      <c r="B205" t="s">
+        <v>123</v>
+      </c>
+      <c r="C205" t="s">
+        <v>145</v>
+      </c>
+      <c r="D205" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>138</v>
+      </c>
+      <c r="B206" t="s">
+        <v>123</v>
+      </c>
+      <c r="C206" t="s">
+        <v>139</v>
+      </c>
+      <c r="D206" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B207" s="4"/>
+      <c r="C207" s="4"/>
+      <c r="D207" s="4"/>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>81</v>
+      </c>
+      <c r="B208" t="s">
+        <v>82</v>
+      </c>
+      <c r="C208" t="s">
+        <v>388</v>
+      </c>
+      <c r="D208" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>386</v>
+      </c>
+      <c r="B209" t="s">
+        <v>82</v>
+      </c>
+      <c r="C209" t="s">
+        <v>377</v>
+      </c>
+      <c r="D209" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>173</v>
+      </c>
+      <c r="B210" t="s">
+        <v>82</v>
+      </c>
+      <c r="C210" t="s">
+        <v>390</v>
+      </c>
+      <c r="D210" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>392</v>
+      </c>
+      <c r="B211" t="s">
+        <v>82</v>
+      </c>
+      <c r="C211" t="s">
+        <v>393</v>
+      </c>
+      <c r="D211" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>83</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B212" t="s">
         <v>82</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C212" t="s">
         <v>84</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D212" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rejig files in app, snow bulletin tweaks
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632415C9-3653-40F7-9439-6067AD5A6CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79C035D-6236-4E70-A810-1C3EFBFD7223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="647">
   <si>
     <t>id</t>
   </si>
@@ -563,9 +563,6 @@
     <t>param_group</t>
   </si>
   <si>
-    <t>Parameter Group</t>
-  </si>
-  <si>
     <t>Groupe de paramètre</t>
   </si>
   <si>
@@ -596,9 +593,6 @@
     <t>param_groups</t>
   </si>
   <si>
-    <t>Parameter Groups</t>
-  </si>
-  <si>
     <t>Groupes de paramètres</t>
   </si>
   <si>
@@ -623,9 +617,6 @@
     <t>param_group(s)</t>
   </si>
   <si>
-    <t>Parameter Group(s)</t>
-  </si>
-  <si>
     <t>Groupe(s) de paramètre(s)</t>
   </si>
   <si>
@@ -1169,30 +1160,9 @@
     <t>media_type</t>
   </si>
   <si>
-    <t>media_types</t>
-  </si>
-  <si>
     <t>media_type(s)</t>
   </si>
   <si>
-    <t>Sample Media Type</t>
-  </si>
-  <si>
-    <t>Sample Media Types</t>
-  </si>
-  <si>
-    <t>Type de média d'échantillonage</t>
-  </si>
-  <si>
-    <t>Types de médias d'échantillonage</t>
-  </si>
-  <si>
-    <t>Sample Media Type(s)</t>
-  </si>
-  <si>
-    <t>Type(s) de médias(s) d'échantillonage</t>
-  </si>
-  <si>
     <t>media_type_col</t>
   </si>
   <si>
@@ -1926,6 +1896,84 @@
   </si>
   <si>
     <t>Échec lors de la création du rapport Word</t>
+  </si>
+  <si>
+    <t>Parameter group</t>
+  </si>
+  <si>
+    <t>Parameter groups</t>
+  </si>
+  <si>
+    <t>Parameter group(s)</t>
+  </si>
+  <si>
+    <t>locs</t>
+  </si>
+  <si>
+    <t>Locations</t>
+  </si>
+  <si>
+    <t>Endroits</t>
+  </si>
+  <si>
+    <t>loc(s)</t>
+  </si>
+  <si>
+    <t>Location(s)</t>
+  </si>
+  <si>
+    <t>Endroit(s)</t>
+  </si>
+  <si>
+    <t>param_sub_group</t>
+  </si>
+  <si>
+    <t>Parameter sub-group</t>
+  </si>
+  <si>
+    <t>Sous-groupe de paramètre</t>
+  </si>
+  <si>
+    <t>Sous-roupes de paramètres</t>
+  </si>
+  <si>
+    <t>Sous-groupe(s) de paramètre(s)</t>
+  </si>
+  <si>
+    <t>Parameter sub-groups</t>
+  </si>
+  <si>
+    <t>Parameter sub-group(s)</t>
+  </si>
+  <si>
+    <t>param_sub_groups</t>
+  </si>
+  <si>
+    <t>param_sub_group(s)</t>
+  </si>
+  <si>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>Sample type(s)</t>
+  </si>
+  <si>
+    <t>Sample media(s)</t>
+  </si>
+  <si>
+    <t>sample_type(s)</t>
+  </si>
+  <si>
+    <t>Média(s) d'échantillonage</t>
+  </si>
+  <si>
+    <t>Type d'échantillon</t>
+  </si>
+  <si>
+    <t>sample_type_col</t>
+  </si>
+  <si>
+    <t>sample_type_fr</t>
   </si>
 </sst>
 </file>
@@ -2873,10 +2921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D212"/>
+  <dimension ref="A1:D217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="D217" sqref="D217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2907,7 +2955,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -2921,13 +2969,13 @@
         <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="C3" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="D3" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2960,10 +3008,10 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="D6" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3038,7 +3086,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -3046,142 +3094,142 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B13" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C13" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="D13" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>320</v>
+      </c>
+      <c r="B14" t="s">
+        <v>322</v>
+      </c>
+      <c r="C14" t="s">
         <v>323</v>
       </c>
-      <c r="B14" t="s">
-        <v>325</v>
-      </c>
-      <c r="C14" t="s">
-        <v>326</v>
-      </c>
       <c r="D14" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B15" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C15" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D15" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B16" t="s">
+        <v>334</v>
+      </c>
+      <c r="C16" t="s">
         <v>337</v>
       </c>
-      <c r="C16" t="s">
-        <v>340</v>
-      </c>
       <c r="D16" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>332</v>
+      </c>
+      <c r="B17" t="s">
         <v>335</v>
       </c>
-      <c r="B17" t="s">
-        <v>338</v>
-      </c>
       <c r="C17" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D17" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B18" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C18" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D18" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>333</v>
+      </c>
+      <c r="B19" t="s">
+        <v>335</v>
+      </c>
+      <c r="C19" t="s">
+        <v>331</v>
+      </c>
+      <c r="D19" t="s">
         <v>336</v>
-      </c>
-      <c r="B19" t="s">
-        <v>338</v>
-      </c>
-      <c r="C19" t="s">
-        <v>334</v>
-      </c>
-      <c r="D19" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="B20" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C20" t="s">
-        <v>580</v>
+        <v>570</v>
       </c>
       <c r="D20" t="s">
-        <v>581</v>
+        <v>571</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B21" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C21" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D21" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B22" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C22" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D22" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3266,16 +3314,16 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B30" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C30" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D30" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3283,7 +3331,7 @@
         <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C31" t="s">
         <v>87</v>
@@ -3294,217 +3342,217 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>263</v>
+      </c>
+      <c r="B32" t="s">
         <v>266</v>
       </c>
-      <c r="B32" t="s">
-        <v>269</v>
-      </c>
       <c r="C32" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D32" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B33" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C33" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D33" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B34" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C34" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B35" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C35" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D35" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B36" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C36" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D36" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B37" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C37" t="s">
+        <v>276</v>
+      </c>
+      <c r="D37" t="s">
         <v>279</v>
-      </c>
-      <c r="D37" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B38" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C38" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D38" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B39" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C39" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D39" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B40" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C40" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D40" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B41" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C41" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D41" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B42" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C42" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D42" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>292</v>
+      </c>
+      <c r="B43" t="s">
+        <v>273</v>
+      </c>
+      <c r="C43" t="s">
+        <v>294</v>
+      </c>
+      <c r="D43" t="s">
         <v>295</v>
-      </c>
-      <c r="B43" t="s">
-        <v>276</v>
-      </c>
-      <c r="C43" t="s">
-        <v>297</v>
-      </c>
-      <c r="D43" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>293</v>
+      </c>
+      <c r="B44" t="s">
+        <v>273</v>
+      </c>
+      <c r="C44" t="s">
         <v>296</v>
       </c>
-      <c r="B44" t="s">
-        <v>276</v>
-      </c>
-      <c r="C44" t="s">
-        <v>299</v>
-      </c>
       <c r="D44" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B45" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C45" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D45" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>313</v>
+      </c>
+      <c r="B46" t="s">
+        <v>314</v>
+      </c>
+      <c r="C46" t="s">
+        <v>315</v>
+      </c>
+      <c r="D46" t="s">
         <v>316</v>
-      </c>
-      <c r="B46" t="s">
-        <v>317</v>
-      </c>
-      <c r="C46" t="s">
-        <v>318</v>
-      </c>
-      <c r="D46" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -3512,10 +3560,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B48" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C48" t="s">
         <v>89</v>
@@ -3529,7 +3577,7 @@
         <v>75</v>
       </c>
       <c r="B49" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C49" t="s">
         <v>76</v>
@@ -3540,72 +3588,72 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B50" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C50" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D50" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B51" t="s">
+        <v>240</v>
+      </c>
+      <c r="C51" t="s">
         <v>243</v>
       </c>
-      <c r="C51" t="s">
-        <v>246</v>
-      </c>
       <c r="D51" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B52" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C52" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D52" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B53" t="s">
+        <v>252</v>
+      </c>
+      <c r="C53" t="s">
         <v>255</v>
       </c>
-      <c r="C53" t="s">
-        <v>258</v>
-      </c>
       <c r="D53" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B54" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C54" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D54" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3705,7 +3753,7 @@
         <v>118</v>
       </c>
       <c r="D62" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3724,7 +3772,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -3746,746 +3794,746 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B66" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C66" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D66" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B67" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C67" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D67" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B68" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C68" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D68" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B69" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C69" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D69" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="C70" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="D70" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C71" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D71" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="C72" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D72" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="C73" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="D73" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="C74" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="D74" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C75" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D75" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="B76" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="C76" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="D76" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="C77" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="D77" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="C78" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
       <c r="D78" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="B79" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="C79" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="D79" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="C80" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="D80" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="C81" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="D81" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C82" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="D82" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="C83" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="D83" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C84" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="D84" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="C85" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="D85" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="C86" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="D86" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="C87" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="D87" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="C88" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="D88" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="C89" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="D89" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="C90" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="D90" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="C91" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="D91" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="C92" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="D92" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="C93" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="D93" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="C94" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="D94" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="C95" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="D95" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="D96" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="C97" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="D97" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="C98" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="D98" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="C99" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="D99" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="C100" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="D100" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
       <c r="C101" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
       <c r="D101" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="C102" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="D102" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="C103" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="D103" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="C104" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="D104" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="C105" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="D105" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="C106" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="D106" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="C107" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="D107" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="C108" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="D108" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="C109" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="D109" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
       <c r="D110" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
       <c r="D111" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>561</v>
+        <v>551</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>562</v>
+        <v>552</v>
       </c>
       <c r="D112" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="D113" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>570</v>
+        <v>560</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="D114" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="D115" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>582</v>
+        <v>572</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>583</v>
+        <v>573</v>
       </c>
       <c r="D116" t="s">
-        <v>584</v>
+        <v>574</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
       <c r="D117" t="s">
-        <v>587</v>
+        <v>577</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>588</v>
+        <v>578</v>
       </c>
       <c r="D118" t="s">
-        <v>588</v>
+        <v>578</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
       <c r="D119" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>593</v>
+        <v>583</v>
       </c>
       <c r="D120" t="s">
-        <v>594</v>
+        <v>584</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
       <c r="D121" t="s">
-        <v>599</v>
+        <v>589</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>592</v>
+        <v>582</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>616</v>
+        <v>606</v>
       </c>
       <c r="D122" t="s">
-        <v>617</v>
+        <v>607</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>602</v>
+        <v>592</v>
       </c>
       <c r="D123" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
       <c r="D124" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>606</v>
+        <v>596</v>
       </c>
       <c r="D125" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="D126" t="s">
-        <v>611</v>
+        <v>601</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="D127" s="11" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="D128" s="11" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>618</v>
+        <v>608</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>619</v>
+        <v>609</v>
       </c>
       <c r="D129" s="11" t="s">
-        <v>620</v>
+        <v>610</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="D130" s="11" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
       <c r="D131" s="11" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -4632,913 +4680,971 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>61</v>
-      </c>
-      <c r="B143" t="s">
-        <v>8</v>
+        <v>624</v>
       </c>
       <c r="C143" t="s">
-        <v>62</v>
+        <v>625</v>
       </c>
       <c r="D143" t="s">
-        <v>63</v>
+        <v>626</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>64</v>
-      </c>
-      <c r="B144" t="s">
-        <v>8</v>
+        <v>627</v>
       </c>
       <c r="C144" t="s">
-        <v>65</v>
+        <v>628</v>
       </c>
       <c r="D144" t="s">
-        <v>245</v>
+        <v>629</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>240</v>
+        <v>61</v>
       </c>
       <c r="B145" t="s">
         <v>8</v>
       </c>
       <c r="C145" t="s">
-        <v>241</v>
+        <v>62</v>
       </c>
       <c r="D145" t="s">
-        <v>241</v>
+        <v>63</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>377</v>
+        <v>64</v>
       </c>
       <c r="B146" t="s">
         <v>8</v>
       </c>
       <c r="C146" t="s">
-        <v>380</v>
+        <v>65</v>
       </c>
       <c r="D146" t="s">
-        <v>382</v>
+        <v>242</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>378</v>
+        <v>237</v>
       </c>
       <c r="B147" t="s">
         <v>8</v>
       </c>
       <c r="C147" t="s">
-        <v>381</v>
+        <v>238</v>
       </c>
       <c r="D147" t="s">
-        <v>383</v>
+        <v>238</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B148" t="s">
         <v>8</v>
       </c>
       <c r="C148" t="s">
-        <v>384</v>
+        <v>641</v>
       </c>
       <c r="D148" t="s">
-        <v>385</v>
+        <v>643</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>175</v>
-      </c>
-      <c r="B149" t="s">
-        <v>8</v>
+        <v>642</v>
       </c>
       <c r="C149" t="s">
-        <v>176</v>
+        <v>640</v>
       </c>
       <c r="D149" t="s">
-        <v>177</v>
+        <v>644</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B150" t="s">
         <v>8</v>
       </c>
       <c r="C150" t="s">
-        <v>187</v>
+        <v>621</v>
       </c>
       <c r="D150" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B151" t="s">
         <v>8</v>
       </c>
       <c r="C151" t="s">
-        <v>196</v>
+        <v>622</v>
       </c>
       <c r="D151" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="B152" t="s">
         <v>8</v>
       </c>
       <c r="C152" t="s">
-        <v>213</v>
+        <v>623</v>
       </c>
       <c r="D152" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>66</v>
+        <v>630</v>
       </c>
       <c r="B153" t="s">
         <v>8</v>
       </c>
       <c r="C153" t="s">
-        <v>67</v>
+        <v>631</v>
       </c>
       <c r="D153" t="s">
-        <v>68</v>
+        <v>632</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>183</v>
+        <v>637</v>
       </c>
       <c r="B154" t="s">
         <v>8</v>
       </c>
       <c r="C154" t="s">
-        <v>178</v>
+        <v>635</v>
       </c>
       <c r="D154" t="s">
-        <v>16</v>
+        <v>633</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>189</v>
+        <v>638</v>
       </c>
       <c r="B155" t="s">
         <v>8</v>
       </c>
       <c r="C155" t="s">
-        <v>190</v>
+        <v>636</v>
       </c>
       <c r="D155" t="s">
-        <v>191</v>
+        <v>634</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>69</v>
+        <v>174</v>
       </c>
       <c r="B156" t="s">
         <v>8</v>
       </c>
       <c r="C156" t="s">
-        <v>70</v>
+        <v>210</v>
       </c>
       <c r="D156" t="s">
-        <v>71</v>
+        <v>211</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>182</v>
+        <v>66</v>
       </c>
       <c r="B157" t="s">
         <v>8</v>
       </c>
       <c r="C157" t="s">
-        <v>184</v>
+        <v>67</v>
       </c>
       <c r="D157" t="s">
-        <v>185</v>
+        <v>68</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B158" t="s">
         <v>8</v>
       </c>
       <c r="C158" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="D158" t="s">
-        <v>194</v>
+        <v>16</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>72</v>
+        <v>187</v>
       </c>
       <c r="B159" t="s">
         <v>8</v>
       </c>
       <c r="C159" t="s">
-        <v>73</v>
+        <v>188</v>
       </c>
       <c r="D159" t="s">
-        <v>74</v>
+        <v>189</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>181</v>
+        <v>69</v>
       </c>
       <c r="B160" t="s">
         <v>8</v>
       </c>
       <c r="C160" t="s">
-        <v>179</v>
+        <v>70</v>
       </c>
       <c r="D160" t="s">
-        <v>180</v>
+        <v>71</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B161" t="s">
         <v>8</v>
       </c>
       <c r="C161" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="D161" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="B162" t="s">
         <v>8</v>
       </c>
       <c r="C162" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="D162" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>218</v>
+        <v>72</v>
       </c>
       <c r="B163" t="s">
         <v>8</v>
       </c>
       <c r="C163" t="s">
-        <v>219</v>
+        <v>73</v>
       </c>
       <c r="D163" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="B164" t="s">
         <v>8</v>
       </c>
       <c r="C164" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="D164" t="s">
-        <v>222</v>
+        <v>179</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>313</v>
+        <v>195</v>
+      </c>
+      <c r="B165" t="s">
+        <v>8</v>
       </c>
       <c r="C165" t="s">
-        <v>314</v>
+        <v>196</v>
       </c>
       <c r="D165" t="s">
-        <v>315</v>
+        <v>197</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>78</v>
+        <v>214</v>
       </c>
       <c r="B166" t="s">
         <v>8</v>
       </c>
       <c r="C166" t="s">
-        <v>79</v>
+        <v>212</v>
       </c>
       <c r="D166" t="s">
-        <v>80</v>
+        <v>213</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="B167" t="s">
         <v>8</v>
       </c>
       <c r="C167" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="D167" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>474</v>
+        <v>217</v>
+      </c>
+      <c r="B168" t="s">
+        <v>8</v>
       </c>
       <c r="C168" t="s">
-        <v>475</v>
+        <v>218</v>
       </c>
       <c r="D168" t="s">
-        <v>476</v>
+        <v>219</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>223</v>
-      </c>
-      <c r="B169" t="s">
-        <v>8</v>
+        <v>310</v>
       </c>
       <c r="C169" t="s">
-        <v>223</v>
+        <v>311</v>
       </c>
       <c r="D169" t="s">
-        <v>224</v>
+        <v>312</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>201</v>
+        <v>78</v>
       </c>
       <c r="B170" t="s">
-        <v>202</v>
+        <v>8</v>
       </c>
       <c r="C170" t="s">
-        <v>201</v>
+        <v>79</v>
       </c>
       <c r="D170" t="s">
-        <v>203</v>
+        <v>80</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>225</v>
+        <v>7</v>
       </c>
       <c r="B171" t="s">
         <v>8</v>
       </c>
       <c r="C171" t="s">
-        <v>227</v>
+        <v>9</v>
       </c>
       <c r="D171" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>226</v>
-      </c>
-      <c r="B172" t="s">
-        <v>202</v>
+        <v>464</v>
       </c>
       <c r="C172" t="s">
-        <v>229</v>
+        <v>465</v>
       </c>
       <c r="D172" t="s">
-        <v>230</v>
+        <v>466</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>252</v>
+        <v>220</v>
       </c>
       <c r="B173" t="s">
         <v>8</v>
       </c>
       <c r="C173" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="D173" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>253</v>
+        <v>198</v>
       </c>
       <c r="B174" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C174" t="s">
-        <v>249</v>
+        <v>198</v>
       </c>
       <c r="D174" t="s">
-        <v>251</v>
+        <v>200</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="B175" t="s">
         <v>8</v>
       </c>
       <c r="C175" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="D175" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="B176" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C176" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D176" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>120</v>
+        <v>249</v>
       </c>
       <c r="B177" t="s">
         <v>8</v>
       </c>
       <c r="C177" t="s">
-        <v>121</v>
+        <v>245</v>
       </c>
       <c r="D177" t="s">
-        <v>122</v>
+        <v>247</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="B178" t="s">
-        <v>8</v>
+        <v>199</v>
       </c>
       <c r="C178" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="D178" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="B179" t="s">
         <v>8</v>
       </c>
       <c r="C179" t="s">
-        <v>15</v>
+        <v>233</v>
       </c>
       <c r="D179" t="s">
-        <v>16</v>
+        <v>235</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>421</v>
+        <v>232</v>
+      </c>
+      <c r="B180" t="s">
+        <v>199</v>
       </c>
       <c r="C180" t="s">
-        <v>422</v>
+        <v>234</v>
       </c>
       <c r="D180" t="s">
-        <v>423</v>
+        <v>236</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>540</v>
+        <v>120</v>
+      </c>
+      <c r="B181" t="s">
+        <v>8</v>
       </c>
       <c r="C181" t="s">
-        <v>541</v>
+        <v>121</v>
       </c>
       <c r="D181" t="s">
-        <v>542</v>
+        <v>122</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>463</v>
+        <v>228</v>
       </c>
       <c r="B182" t="s">
-        <v>345</v>
+        <v>8</v>
       </c>
       <c r="C182" t="s">
-        <v>346</v>
+        <v>229</v>
       </c>
       <c r="D182" t="s">
-        <v>347</v>
+        <v>230</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>482</v>
+        <v>14</v>
+      </c>
+      <c r="B183" t="s">
+        <v>8</v>
       </c>
       <c r="C183" t="s">
-        <v>494</v>
+        <v>15</v>
       </c>
       <c r="D183" t="s">
-        <v>506</v>
+        <v>16</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>483</v>
+        <v>411</v>
       </c>
       <c r="C184" t="s">
-        <v>495</v>
+        <v>412</v>
       </c>
       <c r="D184" t="s">
-        <v>507</v>
+        <v>413</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>484</v>
+        <v>530</v>
       </c>
       <c r="C185" t="s">
-        <v>496</v>
+        <v>531</v>
       </c>
       <c r="D185" t="s">
-        <v>508</v>
+        <v>532</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>485</v>
+        <v>453</v>
+      </c>
+      <c r="B186" t="s">
+        <v>342</v>
       </c>
       <c r="C186" t="s">
-        <v>497</v>
+        <v>343</v>
       </c>
       <c r="D186" t="s">
-        <v>509</v>
+        <v>344</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="C187" t="s">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="D187" t="s">
-        <v>511</v>
+        <v>496</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="C188" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="D188" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="C189" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="D189" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="C190" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="D190" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="C191" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="D191" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="C192" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="D192" t="s">
-        <v>515</v>
+        <v>500</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="C193" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="D193" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="C194" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="D194" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>545</v>
+        <v>480</v>
       </c>
       <c r="C195" t="s">
-        <v>544</v>
+        <v>492</v>
       </c>
       <c r="D195" t="s">
-        <v>543</v>
+        <v>504</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>621</v>
+        <v>481</v>
       </c>
       <c r="C196" t="s">
-        <v>2</v>
+        <v>493</v>
       </c>
       <c r="D196" t="s">
-        <v>622</v>
+        <v>505</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>623</v>
+        <v>482</v>
       </c>
       <c r="C197" t="s">
-        <v>624</v>
+        <v>494</v>
       </c>
       <c r="D197" t="s">
-        <v>3</v>
+        <v>506</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B198" s="2"/>
-      <c r="C198" s="2"/>
-      <c r="D198" s="2"/>
+      <c r="A198" t="s">
+        <v>483</v>
+      </c>
+      <c r="C198" t="s">
+        <v>495</v>
+      </c>
+      <c r="D198" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>124</v>
-      </c>
-      <c r="B199" t="s">
-        <v>123</v>
+        <v>535</v>
       </c>
       <c r="C199" t="s">
-        <v>143</v>
+        <v>534</v>
       </c>
       <c r="D199" t="s">
-        <v>142</v>
+        <v>533</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>141</v>
-      </c>
-      <c r="B200" t="s">
-        <v>123</v>
+        <v>611</v>
       </c>
       <c r="C200" t="s">
-        <v>144</v>
+        <v>2</v>
       </c>
       <c r="D200" t="s">
-        <v>147</v>
+        <v>612</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>125</v>
-      </c>
-      <c r="B201" t="s">
+        <v>613</v>
+      </c>
+      <c r="C201" t="s">
+        <v>614</v>
+      </c>
+      <c r="D201" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C201" t="s">
-        <v>126</v>
-      </c>
-      <c r="D201" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>130</v>
-      </c>
-      <c r="B202" t="s">
-        <v>123</v>
-      </c>
-      <c r="C202" t="s">
-        <v>131</v>
-      </c>
-      <c r="D202" t="s">
-        <v>132</v>
-      </c>
+      <c r="B202" s="2"/>
+      <c r="C202" s="2"/>
+      <c r="D202" s="2"/>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B203" t="s">
         <v>123</v>
       </c>
       <c r="C203" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="D203" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B204" t="s">
         <v>123</v>
       </c>
       <c r="C204" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D204" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B205" t="s">
         <v>123</v>
       </c>
       <c r="C205" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="D205" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B206" t="s">
         <v>123</v>
       </c>
       <c r="C206" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D206" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B207" s="4"/>
-      <c r="C207" s="4"/>
-      <c r="D207" s="4"/>
+      <c r="A207" t="s">
+        <v>127</v>
+      </c>
+      <c r="B207" t="s">
+        <v>123</v>
+      </c>
+      <c r="C207" t="s">
+        <v>128</v>
+      </c>
+      <c r="D207" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="B208" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="C208" t="s">
-        <v>388</v>
+        <v>146</v>
       </c>
       <c r="D208" t="s">
-        <v>389</v>
+        <v>135</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>386</v>
+        <v>136</v>
       </c>
       <c r="B209" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="C209" t="s">
-        <v>377</v>
+        <v>145</v>
       </c>
       <c r="D209" t="s">
-        <v>387</v>
+        <v>137</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="B210" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="C210" t="s">
-        <v>390</v>
+        <v>139</v>
       </c>
       <c r="D210" t="s">
-        <v>391</v>
+        <v>140</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>392</v>
-      </c>
-      <c r="B211" t="s">
-        <v>82</v>
-      </c>
-      <c r="C211" t="s">
-        <v>393</v>
-      </c>
-      <c r="D211" t="s">
-        <v>394</v>
-      </c>
+      <c r="A211" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B211" s="4"/>
+      <c r="C211" s="4"/>
+      <c r="D211" s="4"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B212" t="s">
         <v>82</v>
       </c>
       <c r="C212" t="s">
+        <v>378</v>
+      </c>
+      <c r="D212" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>376</v>
+      </c>
+      <c r="B213" t="s">
+        <v>82</v>
+      </c>
+      <c r="C213" t="s">
+        <v>374</v>
+      </c>
+      <c r="D213" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>173</v>
+      </c>
+      <c r="B214" t="s">
+        <v>82</v>
+      </c>
+      <c r="C214" t="s">
+        <v>380</v>
+      </c>
+      <c r="D214" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>382</v>
+      </c>
+      <c r="B215" t="s">
+        <v>82</v>
+      </c>
+      <c r="C215" t="s">
+        <v>383</v>
+      </c>
+      <c r="D215" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>83</v>
+      </c>
+      <c r="B216" t="s">
+        <v>82</v>
+      </c>
+      <c r="C216" t="s">
         <v>84</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D216" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>645</v>
+      </c>
+      <c r="C217" t="s">
+        <v>639</v>
+      </c>
+      <c r="D217" t="s">
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
discrete data filter + download works!
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03113C5-E45C-4130-B19B-A84AB9BEB97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFC6FCA-EB27-4886-B345-EFE735BCF6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1755" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="680">
   <si>
     <t>id</t>
   </si>
@@ -797,15 +797,6 @@
     <t>view_data_instructions</t>
   </si>
   <si>
-    <t>view_data</t>
-  </si>
-  <si>
-    <t>View data</t>
-  </si>
-  <si>
-    <t>Voir les données</t>
-  </si>
-  <si>
     <t>view_plots</t>
   </si>
   <si>
@@ -857,9 +848,6 @@
     <t>modal selection</t>
   </si>
   <si>
-    <t>data_subset_msg</t>
-  </si>
-  <si>
     <t>modal message</t>
   </si>
   <si>
@@ -2037,6 +2025,54 @@
   </si>
   <si>
     <t>Appliquer</t>
+  </si>
+  <si>
+    <t>select_all</t>
+  </si>
+  <si>
+    <t>Select/deselect all</t>
+  </si>
+  <si>
+    <t>Sélectionner/dé-sélectionner tout</t>
+  </si>
+  <si>
+    <t>view_data1</t>
+  </si>
+  <si>
+    <t>view_data2</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>sample results</t>
+  </si>
+  <si>
+    <t>Voir les résultats de</t>
+  </si>
+  <si>
+    <t>échantillons</t>
+  </si>
+  <si>
+    <t>ts_subset_msg</t>
+  </si>
+  <si>
+    <t>discrete_subset_msg</t>
+  </si>
+  <si>
+    <t>Subset of data (max 3 results per sample)</t>
+  </si>
+  <si>
+    <t>Sous-ensemble de données (max 3 résultats par échantillon)</t>
+  </si>
+  <si>
+    <t>dl_num_results</t>
+  </si>
+  <si>
+    <t>Number of results that will be returned:</t>
+  </si>
+  <si>
+    <t>Nombre de résultats à télécharger:</t>
   </si>
 </sst>
 </file>
@@ -2984,10 +3020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D224"/>
+  <dimension ref="A1:D228"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3018,7 +3054,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -3032,13 +3068,13 @@
         <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C3" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D3" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3071,10 +3107,10 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="D6" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3149,7 +3185,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -3157,142 +3193,142 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B13" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C13" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D13" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>316</v>
+      </c>
+      <c r="B14" t="s">
+        <v>318</v>
+      </c>
+      <c r="C14" t="s">
+        <v>319</v>
+      </c>
+      <c r="D14" t="s">
         <v>320</v>
-      </c>
-      <c r="B14" t="s">
-        <v>322</v>
-      </c>
-      <c r="C14" t="s">
-        <v>323</v>
-      </c>
-      <c r="D14" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>317</v>
+      </c>
+      <c r="B15" t="s">
+        <v>323</v>
+      </c>
+      <c r="C15" t="s">
+        <v>322</v>
+      </c>
+      <c r="D15" t="s">
         <v>321</v>
-      </c>
-      <c r="B15" t="s">
-        <v>327</v>
-      </c>
-      <c r="C15" t="s">
-        <v>326</v>
-      </c>
-      <c r="D15" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B16" t="s">
+        <v>330</v>
+      </c>
+      <c r="C16" t="s">
+        <v>333</v>
+      </c>
+      <c r="D16" t="s">
         <v>334</v>
-      </c>
-      <c r="C16" t="s">
-        <v>337</v>
-      </c>
-      <c r="D16" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B17" t="s">
+        <v>331</v>
+      </c>
+      <c r="C17" t="s">
+        <v>325</v>
+      </c>
+      <c r="D17" t="s">
         <v>335</v>
-      </c>
-      <c r="C17" t="s">
-        <v>329</v>
-      </c>
-      <c r="D17" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>326</v>
+      </c>
+      <c r="B18" t="s">
         <v>330</v>
       </c>
-      <c r="B18" t="s">
-        <v>334</v>
-      </c>
       <c r="C18" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D18" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B19" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C19" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D19" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B20" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C20" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D20" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B21" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C21" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D21" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B22" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C22" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D22" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3383,10 +3419,10 @@
         <v>251</v>
       </c>
       <c r="C30" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D30" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3405,30 +3441,27 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>260</v>
+      </c>
+      <c r="B32" t="s">
         <v>263</v>
       </c>
-      <c r="B32" t="s">
-        <v>266</v>
-      </c>
       <c r="C32" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D32" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>270</v>
-      </c>
-      <c r="B33" t="s">
-        <v>272</v>
+        <v>677</v>
       </c>
       <c r="C33" t="s">
-        <v>271</v>
+        <v>678</v>
       </c>
       <c r="D33" t="s">
-        <v>306</v>
+        <v>679</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3436,622 +3469,631 @@
         <v>267</v>
       </c>
       <c r="B34" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C34" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="D34" t="s">
-        <v>277</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B35" t="s">
+        <v>270</v>
+      </c>
+      <c r="C35" t="s">
+        <v>274</v>
+      </c>
+      <c r="D35" t="s">
         <v>273</v>
-      </c>
-      <c r="C35" t="s">
-        <v>302</v>
-      </c>
-      <c r="D35" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B36" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C36" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D36" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B37" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C37" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="D37" t="s">
-        <v>279</v>
+        <v>301</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>301</v>
+        <v>673</v>
       </c>
       <c r="B38" t="s">
+        <v>271</v>
+      </c>
+      <c r="C38" t="s">
+        <v>272</v>
+      </c>
+      <c r="D38" t="s">
         <v>275</v>
-      </c>
-      <c r="C38" t="s">
-        <v>280</v>
-      </c>
-      <c r="D38" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>282</v>
+        <v>674</v>
       </c>
       <c r="B39" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C39" t="s">
-        <v>283</v>
+        <v>675</v>
       </c>
       <c r="D39" t="s">
-        <v>284</v>
+        <v>676</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="B40" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C40" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D40" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="B41" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C41" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="D41" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>307</v>
+        <v>281</v>
       </c>
       <c r="B42" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C42" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="D42" t="s">
-        <v>309</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B43" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C43" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D43" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="B44" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C44" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="D44" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="B45" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C45" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D45" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="B46" t="s">
-        <v>314</v>
+        <v>270</v>
       </c>
       <c r="C46" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="D46" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
+      <c r="A47" t="s">
+        <v>294</v>
+      </c>
+      <c r="B47" t="s">
+        <v>270</v>
+      </c>
+      <c r="C47" t="s">
+        <v>295</v>
+      </c>
+      <c r="D47" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>647</v>
+        <v>309</v>
+      </c>
+      <c r="B48" t="s">
+        <v>310</v>
       </c>
       <c r="C48" t="s">
-        <v>648</v>
+        <v>311</v>
       </c>
       <c r="D48" t="s">
-        <v>649</v>
+        <v>312</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>665</v>
-      </c>
-      <c r="C49" t="s">
-        <v>666</v>
-      </c>
-      <c r="D49" t="s">
-        <v>667</v>
-      </c>
+      <c r="A49" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="C50" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="D50" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>653</v>
+        <v>661</v>
       </c>
       <c r="C51" t="s">
-        <v>654</v>
+        <v>662</v>
       </c>
       <c r="D51" t="s">
-        <v>655</v>
+        <v>663</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>203</v>
-      </c>
-      <c r="B52" t="s">
-        <v>204</v>
+        <v>646</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>647</v>
       </c>
       <c r="D52" t="s">
-        <v>90</v>
+        <v>648</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>75</v>
-      </c>
-      <c r="B53" t="s">
-        <v>206</v>
+        <v>649</v>
       </c>
       <c r="C53" t="s">
-        <v>76</v>
+        <v>650</v>
       </c>
       <c r="D53" t="s">
-        <v>77</v>
+        <v>651</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B54" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C54" t="s">
-        <v>208</v>
+        <v>89</v>
       </c>
       <c r="D54" t="s">
-        <v>209</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>239</v>
+        <v>75</v>
       </c>
       <c r="B55" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
       <c r="C55" t="s">
-        <v>243</v>
+        <v>76</v>
       </c>
       <c r="D55" t="s">
-        <v>244</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>241</v>
+        <v>201</v>
       </c>
       <c r="B56" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
       <c r="C56" t="s">
-        <v>260</v>
+        <v>208</v>
       </c>
       <c r="D56" t="s">
-        <v>260</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B57" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="C57" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D57" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>241</v>
+      </c>
+      <c r="B58" t="s">
+        <v>240</v>
+      </c>
+      <c r="C58" t="s">
         <v>257</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>667</v>
+      </c>
+      <c r="B59" t="s">
         <v>252</v>
       </c>
-      <c r="C58" t="s">
-        <v>258</v>
-      </c>
-      <c r="D58" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="C59" t="s">
+        <v>669</v>
+      </c>
+      <c r="D59" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>668</v>
       </c>
       <c r="B60" t="s">
-        <v>45</v>
+        <v>252</v>
       </c>
       <c r="C60" t="s">
-        <v>52</v>
+        <v>670</v>
       </c>
       <c r="D60" t="s">
-        <v>52</v>
+        <v>672</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
+      <c r="A61" t="s">
+        <v>664</v>
+      </c>
+      <c r="B61" t="s">
+        <v>252</v>
+      </c>
+      <c r="C61" t="s">
+        <v>665</v>
+      </c>
+      <c r="D61" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>254</v>
       </c>
       <c r="B62" t="s">
-        <v>45</v>
+        <v>252</v>
       </c>
       <c r="C62" t="s">
-        <v>54</v>
+        <v>255</v>
       </c>
       <c r="D62" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>91</v>
-      </c>
-      <c r="B63" t="s">
-        <v>92</v>
-      </c>
-      <c r="C63" t="s">
-        <v>100</v>
-      </c>
-      <c r="D63" t="s">
-        <v>101</v>
-      </c>
+      <c r="A63" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="B64" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="C64" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="D64" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>95</v>
-      </c>
-      <c r="B65" t="s">
-        <v>94</v>
-      </c>
-      <c r="C65" t="s">
-        <v>97</v>
-      </c>
-      <c r="D65" t="s">
-        <v>99</v>
-      </c>
+      <c r="A65" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="C66" t="s">
-        <v>118</v>
+        <v>54</v>
       </c>
       <c r="D66" t="s">
-        <v>288</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B67" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C67" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D67" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
+      <c r="A68" t="s">
+        <v>93</v>
+      </c>
+      <c r="B68" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D68" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="B69" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="C69" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="D69" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>352</v>
+        <v>117</v>
       </c>
       <c r="B70" t="s">
-        <v>351</v>
+        <v>92</v>
       </c>
       <c r="C70" t="s">
-        <v>357</v>
+        <v>118</v>
       </c>
       <c r="D70" t="s">
-        <v>358</v>
+        <v>284</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>353</v>
+        <v>102</v>
       </c>
       <c r="B71" t="s">
-        <v>351</v>
+        <v>103</v>
       </c>
       <c r="C71" t="s">
-        <v>358</v>
+        <v>104</v>
       </c>
       <c r="D71" t="s">
-        <v>358</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>360</v>
-      </c>
-      <c r="B72" t="s">
-        <v>354</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="A72" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="D72" t="s">
-        <v>356</v>
-      </c>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>361</v>
+        <v>55</v>
       </c>
       <c r="B73" t="s">
-        <v>354</v>
+        <v>45</v>
       </c>
       <c r="C73" t="s">
-        <v>362</v>
+        <v>56</v>
       </c>
       <c r="D73" t="s">
-        <v>363</v>
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>449</v>
+        <v>348</v>
+      </c>
+      <c r="B74" t="s">
+        <v>347</v>
       </c>
       <c r="C74" t="s">
-        <v>450</v>
+        <v>353</v>
       </c>
       <c r="D74" t="s">
-        <v>451</v>
+        <v>354</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>364</v>
+        <v>349</v>
+      </c>
+      <c r="B75" t="s">
+        <v>347</v>
       </c>
       <c r="C75" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="D75" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>442</v>
+        <v>356</v>
+      </c>
+      <c r="B76" t="s">
+        <v>350</v>
       </c>
       <c r="C76" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="D76" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>443</v>
+        <v>357</v>
+      </c>
+      <c r="B77" t="s">
+        <v>350</v>
       </c>
       <c r="C77" t="s">
-        <v>447</v>
+        <v>358</v>
       </c>
       <c r="D77" t="s">
-        <v>448</v>
+        <v>359</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C78" t="s">
         <v>446</v>
       </c>
       <c r="D78" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="C79" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="D79" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>385</v>
-      </c>
-      <c r="B80" t="s">
-        <v>386</v>
+        <v>438</v>
       </c>
       <c r="C80" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="D80" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="C81" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="D81" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="C82" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="D82" t="s">
         <v>441</v>
@@ -4059,1732 +4101,1779 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>389</v>
-      </c>
-      <c r="B83" t="s">
-        <v>390</v>
+        <v>365</v>
       </c>
       <c r="C83" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="D83" t="s">
-        <v>392</v>
+        <v>366</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>454</v>
+        <v>381</v>
+      </c>
+      <c r="B84" t="s">
+        <v>382</v>
       </c>
       <c r="C84" t="s">
-        <v>428</v>
+        <v>383</v>
       </c>
       <c r="D84" t="s">
-        <v>429</v>
+        <v>384</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>455</v>
+        <v>432</v>
       </c>
       <c r="C85" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="D85" t="s">
-        <v>457</v>
+        <v>436</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>372</v>
+        <v>433</v>
       </c>
       <c r="C86" t="s">
-        <v>401</v>
+        <v>435</v>
       </c>
       <c r="D86" t="s">
-        <v>373</v>
+        <v>437</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>393</v>
+        <v>385</v>
+      </c>
+      <c r="B87" t="s">
+        <v>386</v>
       </c>
       <c r="C87" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="D87" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>395</v>
+        <v>450</v>
       </c>
       <c r="C88" t="s">
-        <v>396</v>
+        <v>424</v>
       </c>
       <c r="D88" t="s">
-        <v>397</v>
+        <v>425</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>398</v>
+        <v>451</v>
       </c>
       <c r="C89" t="s">
-        <v>399</v>
+        <v>452</v>
       </c>
       <c r="D89" t="s">
-        <v>400</v>
+        <v>453</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>402</v>
+        <v>368</v>
       </c>
       <c r="C90" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D90" t="s">
-        <v>404</v>
+        <v>369</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="C91" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="D91" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
       <c r="C92" t="s">
-        <v>409</v>
+        <v>392</v>
       </c>
       <c r="D92" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>430</v>
+        <v>394</v>
       </c>
       <c r="C93" t="s">
-        <v>435</v>
+        <v>395</v>
       </c>
       <c r="D93" t="s">
-        <v>434</v>
+        <v>396</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C94" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="D94" t="s">
-        <v>452</v>
+        <v>400</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>431</v>
+        <v>401</v>
       </c>
       <c r="C95" t="s">
-        <v>432</v>
+        <v>402</v>
       </c>
       <c r="D95" t="s">
-        <v>433</v>
+        <v>403</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="C96" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="D96" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="C97" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="D97" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="C98" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="D98" t="s">
-        <v>427</v>
+        <v>448</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="C99" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="D99" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>540</v>
-      </c>
-      <c r="C100" s="11" t="s">
-        <v>541</v>
+        <v>411</v>
+      </c>
+      <c r="C100" t="s">
+        <v>417</v>
       </c>
       <c r="D100" t="s">
-        <v>542</v>
+        <v>415</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>458</v>
+        <v>412</v>
       </c>
       <c r="C101" t="s">
-        <v>459</v>
+        <v>418</v>
       </c>
       <c r="D101" t="s">
-        <v>460</v>
+        <v>416</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="C102" t="s">
-        <v>516</v>
+        <v>422</v>
       </c>
       <c r="D102" t="s">
-        <v>514</v>
+        <v>423</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>463</v>
+        <v>413</v>
       </c>
       <c r="C103" t="s">
-        <v>462</v>
+        <v>419</v>
       </c>
       <c r="D103" t="s">
-        <v>515</v>
+        <v>420</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>546</v>
-      </c>
-      <c r="C104" t="s">
-        <v>467</v>
+        <v>536</v>
+      </c>
+      <c r="C104" s="11" t="s">
+        <v>537</v>
       </c>
       <c r="D104" t="s">
-        <v>468</v>
+        <v>538</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>564</v>
+        <v>454</v>
       </c>
       <c r="C105" t="s">
-        <v>562</v>
+        <v>455</v>
       </c>
       <c r="D105" t="s">
-        <v>563</v>
+        <v>456</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="C106" t="s">
-        <v>470</v>
+        <v>512</v>
       </c>
       <c r="D106" t="s">
-        <v>471</v>
+        <v>510</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>508</v>
+        <v>459</v>
       </c>
       <c r="C107" t="s">
-        <v>510</v>
+        <v>458</v>
       </c>
       <c r="D107" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>509</v>
+        <v>542</v>
       </c>
       <c r="C108" t="s">
-        <v>511</v>
+        <v>463</v>
       </c>
       <c r="D108" t="s">
-        <v>513</v>
+        <v>464</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>517</v>
+        <v>560</v>
       </c>
       <c r="C109" t="s">
-        <v>518</v>
+        <v>558</v>
       </c>
       <c r="D109" t="s">
-        <v>519</v>
+        <v>559</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>550</v>
+        <v>465</v>
       </c>
       <c r="C110" t="s">
-        <v>520</v>
+        <v>466</v>
       </c>
       <c r="D110" t="s">
-        <v>521</v>
+        <v>467</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="C111" t="s">
-        <v>523</v>
+        <v>506</v>
       </c>
       <c r="D111" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>525</v>
+        <v>505</v>
       </c>
       <c r="C112" t="s">
-        <v>527</v>
+        <v>507</v>
       </c>
       <c r="D112" t="s">
-        <v>528</v>
+        <v>509</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="C113" t="s">
-        <v>529</v>
+        <v>514</v>
       </c>
       <c r="D113" t="s">
-        <v>557</v>
+        <v>515</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>543</v>
-      </c>
-      <c r="C114" s="11" t="s">
-        <v>544</v>
+        <v>546</v>
+      </c>
+      <c r="C114" t="s">
+        <v>516</v>
       </c>
       <c r="D114" t="s">
-        <v>545</v>
+        <v>517</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>547</v>
-      </c>
-      <c r="C115" s="11" t="s">
-        <v>548</v>
+        <v>518</v>
+      </c>
+      <c r="C115" t="s">
+        <v>519</v>
       </c>
       <c r="D115" t="s">
-        <v>549</v>
+        <v>520</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>551</v>
-      </c>
-      <c r="C116" s="11" t="s">
-        <v>552</v>
+        <v>521</v>
+      </c>
+      <c r="C116" t="s">
+        <v>523</v>
       </c>
       <c r="D116" t="s">
-        <v>553</v>
+        <v>524</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>554</v>
-      </c>
-      <c r="C117" s="11" t="s">
-        <v>556</v>
+        <v>522</v>
+      </c>
+      <c r="C117" t="s">
+        <v>525</v>
       </c>
       <c r="D117" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>560</v>
+        <v>539</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>529</v>
+        <v>540</v>
       </c>
       <c r="D118" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="D119" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>572</v>
+        <v>547</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>573</v>
+        <v>548</v>
       </c>
       <c r="D120" t="s">
-        <v>574</v>
+        <v>549</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>575</v>
+        <v>550</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>579</v>
+        <v>552</v>
       </c>
       <c r="D121" t="s">
-        <v>577</v>
+        <v>551</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>576</v>
+        <v>556</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>578</v>
+        <v>525</v>
       </c>
       <c r="D122" t="s">
-        <v>578</v>
+        <v>553</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>580</v>
+        <v>557</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>586</v>
+        <v>554</v>
       </c>
       <c r="D123" t="s">
-        <v>585</v>
+        <v>555</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>581</v>
+        <v>568</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>583</v>
+        <v>569</v>
       </c>
       <c r="D124" t="s">
-        <v>584</v>
+        <v>570</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>587</v>
+        <v>571</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
       <c r="D125" t="s">
-        <v>589</v>
+        <v>573</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>582</v>
+        <v>572</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>606</v>
+        <v>574</v>
       </c>
       <c r="D126" t="s">
-        <v>607</v>
+        <v>574</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>590</v>
+        <v>576</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>592</v>
+        <v>582</v>
       </c>
       <c r="D127" t="s">
-        <v>594</v>
+        <v>581</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="D128" t="s">
-        <v>595</v>
+        <v>580</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>602</v>
+        <v>583</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>596</v>
+        <v>584</v>
       </c>
       <c r="D129" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>578</v>
+      </c>
+      <c r="C130" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="D130" t="s">
         <v>603</v>
-      </c>
-      <c r="C130" s="11" t="s">
-        <v>600</v>
-      </c>
-      <c r="D130" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>604</v>
+        <v>586</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>597</v>
-      </c>
-      <c r="D131" s="11" t="s">
-        <v>597</v>
+        <v>588</v>
+      </c>
+      <c r="D131" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>605</v>
+        <v>587</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>598</v>
-      </c>
-      <c r="D132" s="11" t="s">
-        <v>598</v>
+        <v>589</v>
+      </c>
+      <c r="D132" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="C133" s="11" t="s">
-        <v>609</v>
-      </c>
-      <c r="D133" s="11" t="s">
-        <v>610</v>
+        <v>592</v>
+      </c>
+      <c r="D133" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>615</v>
+        <v>599</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="D134" s="11" t="s">
-        <v>619</v>
+        <v>596</v>
+      </c>
+      <c r="D134" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>616</v>
+        <v>600</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>617</v>
+        <v>593</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>620</v>
+        <v>593</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B136" s="4"/>
-      <c r="C136" s="4"/>
-      <c r="D136" s="4"/>
+      <c r="A136" t="s">
+        <v>601</v>
+      </c>
+      <c r="C136" s="11" t="s">
+        <v>594</v>
+      </c>
+      <c r="D136" s="11" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>149</v>
-      </c>
-      <c r="B137" t="s">
-        <v>45</v>
-      </c>
-      <c r="C137" t="s">
-        <v>150</v>
-      </c>
-      <c r="D137" t="s">
-        <v>151</v>
+        <v>604</v>
+      </c>
+      <c r="C137" s="11" t="s">
+        <v>605</v>
+      </c>
+      <c r="D137" s="11" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>155</v>
-      </c>
-      <c r="B138" t="s">
-        <v>152</v>
-      </c>
-      <c r="C138" t="s">
-        <v>153</v>
-      </c>
-      <c r="D138" t="s">
-        <v>154</v>
+        <v>611</v>
+      </c>
+      <c r="C138" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="D138" s="11" t="s">
+        <v>615</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>158</v>
-      </c>
-      <c r="B139" t="s">
-        <v>159</v>
-      </c>
-      <c r="C139" t="s">
-        <v>170</v>
-      </c>
-      <c r="D139" t="s">
-        <v>171</v>
+        <v>612</v>
+      </c>
+      <c r="C139" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="D139" s="11" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>167</v>
-      </c>
-      <c r="B140" t="s">
-        <v>152</v>
-      </c>
-      <c r="C140" t="s">
-        <v>156</v>
-      </c>
-      <c r="D140" t="s">
-        <v>157</v>
-      </c>
+      <c r="A140" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B140" s="4"/>
+      <c r="C140" s="4"/>
+      <c r="D140" s="4"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B141" t="s">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="C141" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="D141" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B142" t="s">
-        <v>163</v>
-      </c>
-      <c r="C142" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D142" s="9" t="s">
-        <v>165</v>
+        <v>152</v>
+      </c>
+      <c r="C142" t="s">
+        <v>153</v>
+      </c>
+      <c r="D142" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B143" t="s">
         <v>159</v>
       </c>
       <c r="C143" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D143" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B144" s="8"/>
-      <c r="C144" s="8"/>
-      <c r="D144" s="8"/>
+      <c r="A144" t="s">
+        <v>167</v>
+      </c>
+      <c r="B144" t="s">
+        <v>152</v>
+      </c>
+      <c r="C144" t="s">
+        <v>156</v>
+      </c>
+      <c r="D144" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
       <c r="B145" t="s">
-        <v>8</v>
+        <v>159</v>
       </c>
       <c r="C145" t="s">
-        <v>59</v>
+        <v>169</v>
       </c>
       <c r="D145" t="s">
-        <v>60</v>
+        <v>168</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>106</v>
+        <v>161</v>
       </c>
       <c r="B146" t="s">
-        <v>8</v>
-      </c>
-      <c r="C146" t="s">
-        <v>107</v>
-      </c>
-      <c r="D146" t="s">
-        <v>108</v>
+        <v>163</v>
+      </c>
+      <c r="C146" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D146" s="9" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>624</v>
+        <v>162</v>
+      </c>
+      <c r="B147" t="s">
+        <v>159</v>
       </c>
       <c r="C147" t="s">
-        <v>625</v>
+        <v>164</v>
       </c>
       <c r="D147" t="s">
-        <v>626</v>
+        <v>166</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>627</v>
-      </c>
-      <c r="C148" t="s">
-        <v>628</v>
-      </c>
-      <c r="D148" t="s">
-        <v>629</v>
-      </c>
+      <c r="A148" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B148" s="8"/>
+      <c r="C148" s="8"/>
+      <c r="D148" s="8"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>659</v>
+        <v>58</v>
+      </c>
+      <c r="B149" t="s">
+        <v>8</v>
       </c>
       <c r="C149" t="s">
-        <v>661</v>
+        <v>59</v>
       </c>
       <c r="D149" t="s">
-        <v>662</v>
+        <v>60</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>660</v>
+        <v>106</v>
+      </c>
+      <c r="B150" t="s">
+        <v>8</v>
       </c>
       <c r="C150" t="s">
-        <v>664</v>
+        <v>107</v>
       </c>
       <c r="D150" t="s">
-        <v>663</v>
+        <v>108</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>61</v>
-      </c>
-      <c r="B151" t="s">
-        <v>8</v>
+        <v>620</v>
       </c>
       <c r="C151" t="s">
-        <v>62</v>
+        <v>621</v>
       </c>
       <c r="D151" t="s">
-        <v>63</v>
+        <v>622</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>64</v>
-      </c>
-      <c r="B152" t="s">
-        <v>8</v>
+        <v>623</v>
       </c>
       <c r="C152" t="s">
-        <v>65</v>
+        <v>624</v>
       </c>
       <c r="D152" t="s">
-        <v>242</v>
+        <v>625</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>237</v>
-      </c>
-      <c r="B153" t="s">
-        <v>8</v>
+        <v>655</v>
       </c>
       <c r="C153" t="s">
-        <v>238</v>
+        <v>657</v>
       </c>
       <c r="D153" t="s">
-        <v>238</v>
+        <v>658</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>375</v>
-      </c>
-      <c r="B154" t="s">
-        <v>8</v>
+        <v>656</v>
       </c>
       <c r="C154" t="s">
-        <v>641</v>
+        <v>660</v>
       </c>
       <c r="D154" t="s">
-        <v>643</v>
+        <v>659</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>642</v>
+        <v>61</v>
+      </c>
+      <c r="B155" t="s">
+        <v>8</v>
       </c>
       <c r="C155" t="s">
-        <v>640</v>
+        <v>62</v>
       </c>
       <c r="D155" t="s">
-        <v>644</v>
+        <v>63</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="B156" t="s">
         <v>8</v>
       </c>
       <c r="C156" t="s">
-        <v>621</v>
+        <v>65</v>
       </c>
       <c r="D156" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>185</v>
+        <v>237</v>
       </c>
       <c r="B157" t="s">
         <v>8</v>
       </c>
       <c r="C157" t="s">
-        <v>622</v>
+        <v>238</v>
       </c>
       <c r="D157" t="s">
-        <v>186</v>
+        <v>238</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>193</v>
+        <v>371</v>
       </c>
       <c r="B158" t="s">
         <v>8</v>
       </c>
       <c r="C158" t="s">
-        <v>623</v>
+        <v>637</v>
       </c>
       <c r="D158" t="s">
-        <v>194</v>
+        <v>639</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>630</v>
-      </c>
-      <c r="B159" t="s">
-        <v>8</v>
+        <v>638</v>
       </c>
       <c r="C159" t="s">
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="D159" t="s">
-        <v>632</v>
+        <v>640</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>637</v>
+        <v>175</v>
       </c>
       <c r="B160" t="s">
         <v>8</v>
       </c>
       <c r="C160" t="s">
-        <v>635</v>
+        <v>617</v>
       </c>
       <c r="D160" t="s">
-        <v>633</v>
+        <v>176</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>638</v>
+        <v>185</v>
       </c>
       <c r="B161" t="s">
         <v>8</v>
       </c>
       <c r="C161" t="s">
-        <v>636</v>
+        <v>618</v>
       </c>
       <c r="D161" t="s">
-        <v>634</v>
+        <v>186</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="B162" t="s">
         <v>8</v>
       </c>
       <c r="C162" t="s">
-        <v>210</v>
+        <v>619</v>
       </c>
       <c r="D162" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>66</v>
+        <v>626</v>
       </c>
       <c r="B163" t="s">
         <v>8</v>
       </c>
       <c r="C163" t="s">
-        <v>67</v>
+        <v>627</v>
       </c>
       <c r="D163" t="s">
-        <v>68</v>
+        <v>628</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>182</v>
+        <v>633</v>
       </c>
       <c r="B164" t="s">
         <v>8</v>
       </c>
       <c r="C164" t="s">
-        <v>177</v>
+        <v>631</v>
       </c>
       <c r="D164" t="s">
-        <v>16</v>
+        <v>629</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>187</v>
+        <v>634</v>
       </c>
       <c r="B165" t="s">
         <v>8</v>
       </c>
       <c r="C165" t="s">
-        <v>188</v>
+        <v>632</v>
       </c>
       <c r="D165" t="s">
-        <v>189</v>
+        <v>630</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>69</v>
+        <v>174</v>
       </c>
       <c r="B166" t="s">
         <v>8</v>
       </c>
       <c r="C166" t="s">
-        <v>70</v>
+        <v>210</v>
       </c>
       <c r="D166" t="s">
-        <v>71</v>
+        <v>211</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>181</v>
+        <v>66</v>
       </c>
       <c r="B167" t="s">
         <v>8</v>
       </c>
       <c r="C167" t="s">
-        <v>183</v>
+        <v>67</v>
       </c>
       <c r="D167" t="s">
-        <v>184</v>
+        <v>68</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B168" t="s">
         <v>8</v>
       </c>
       <c r="C168" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="D168" t="s">
-        <v>192</v>
+        <v>16</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>72</v>
+        <v>187</v>
       </c>
       <c r="B169" t="s">
         <v>8</v>
       </c>
       <c r="C169" t="s">
-        <v>73</v>
+        <v>188</v>
       </c>
       <c r="D169" t="s">
-        <v>74</v>
+        <v>189</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>180</v>
+        <v>69</v>
       </c>
       <c r="B170" t="s">
         <v>8</v>
       </c>
       <c r="C170" t="s">
-        <v>178</v>
+        <v>70</v>
       </c>
       <c r="D170" t="s">
-        <v>179</v>
+        <v>71</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="B171" t="s">
         <v>8</v>
       </c>
       <c r="C171" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="D171" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="B172" t="s">
         <v>8</v>
       </c>
       <c r="C172" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="D172" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>215</v>
+        <v>72</v>
       </c>
       <c r="B173" t="s">
         <v>8</v>
       </c>
       <c r="C173" t="s">
-        <v>216</v>
+        <v>73</v>
       </c>
       <c r="D173" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>217</v>
+        <v>180</v>
       </c>
       <c r="B174" t="s">
         <v>8</v>
       </c>
       <c r="C174" t="s">
-        <v>218</v>
+        <v>178</v>
       </c>
       <c r="D174" t="s">
-        <v>219</v>
+        <v>179</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>310</v>
+        <v>195</v>
+      </c>
+      <c r="B175" t="s">
+        <v>8</v>
       </c>
       <c r="C175" t="s">
-        <v>311</v>
+        <v>196</v>
       </c>
       <c r="D175" t="s">
-        <v>312</v>
+        <v>197</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>78</v>
+        <v>214</v>
       </c>
       <c r="B176" t="s">
         <v>8</v>
       </c>
       <c r="C176" t="s">
-        <v>79</v>
+        <v>212</v>
       </c>
       <c r="D176" t="s">
-        <v>80</v>
+        <v>213</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="B177" t="s">
         <v>8</v>
       </c>
       <c r="C177" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="D177" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>464</v>
+        <v>217</v>
+      </c>
+      <c r="B178" t="s">
+        <v>8</v>
       </c>
       <c r="C178" t="s">
-        <v>465</v>
+        <v>218</v>
       </c>
       <c r="D178" t="s">
-        <v>466</v>
+        <v>219</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>220</v>
-      </c>
-      <c r="B179" t="s">
-        <v>8</v>
+        <v>306</v>
       </c>
       <c r="C179" t="s">
-        <v>220</v>
+        <v>307</v>
       </c>
       <c r="D179" t="s">
-        <v>221</v>
+        <v>308</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>198</v>
+        <v>78</v>
       </c>
       <c r="B180" t="s">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="C180" t="s">
-        <v>198</v>
+        <v>79</v>
       </c>
       <c r="D180" t="s">
-        <v>200</v>
+        <v>80</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>222</v>
+        <v>7</v>
       </c>
       <c r="B181" t="s">
         <v>8</v>
       </c>
       <c r="C181" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="D181" t="s">
-        <v>225</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>223</v>
-      </c>
-      <c r="B182" t="s">
-        <v>199</v>
+        <v>460</v>
       </c>
       <c r="C182" t="s">
-        <v>226</v>
+        <v>461</v>
       </c>
       <c r="D182" t="s">
-        <v>227</v>
+        <v>462</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
       <c r="B183" t="s">
         <v>8</v>
       </c>
       <c r="C183" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="D183" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>250</v>
+        <v>198</v>
       </c>
       <c r="B184" t="s">
         <v>199</v>
       </c>
       <c r="C184" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="D184" t="s">
-        <v>248</v>
+        <v>200</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B185" t="s">
         <v>8</v>
       </c>
       <c r="C185" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D185" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B186" t="s">
         <v>199</v>
       </c>
       <c r="C186" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D186" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>120</v>
+        <v>249</v>
       </c>
       <c r="B187" t="s">
         <v>8</v>
       </c>
       <c r="C187" t="s">
-        <v>121</v>
+        <v>245</v>
       </c>
       <c r="D187" t="s">
-        <v>122</v>
+        <v>247</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="B188" t="s">
-        <v>8</v>
+        <v>199</v>
       </c>
       <c r="C188" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="D188" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="B189" t="s">
         <v>8</v>
       </c>
       <c r="C189" t="s">
-        <v>15</v>
+        <v>233</v>
       </c>
       <c r="D189" t="s">
-        <v>16</v>
+        <v>235</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>411</v>
+        <v>232</v>
+      </c>
+      <c r="B190" t="s">
+        <v>199</v>
       </c>
       <c r="C190" t="s">
-        <v>412</v>
+        <v>234</v>
       </c>
       <c r="D190" t="s">
-        <v>413</v>
+        <v>236</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>530</v>
+        <v>120</v>
+      </c>
+      <c r="B191" t="s">
+        <v>8</v>
       </c>
       <c r="C191" t="s">
-        <v>531</v>
+        <v>121</v>
       </c>
       <c r="D191" t="s">
-        <v>532</v>
+        <v>122</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>453</v>
+        <v>228</v>
       </c>
       <c r="B192" t="s">
-        <v>342</v>
+        <v>8</v>
       </c>
       <c r="C192" t="s">
-        <v>343</v>
+        <v>229</v>
       </c>
       <c r="D192" t="s">
-        <v>344</v>
+        <v>230</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>472</v>
+        <v>14</v>
+      </c>
+      <c r="B193" t="s">
+        <v>8</v>
       </c>
       <c r="C193" t="s">
-        <v>484</v>
+        <v>15</v>
       </c>
       <c r="D193" t="s">
-        <v>496</v>
+        <v>16</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>473</v>
+        <v>407</v>
       </c>
       <c r="C194" t="s">
-        <v>485</v>
+        <v>408</v>
       </c>
       <c r="D194" t="s">
-        <v>497</v>
+        <v>409</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>474</v>
+        <v>526</v>
       </c>
       <c r="C195" t="s">
-        <v>486</v>
+        <v>527</v>
       </c>
       <c r="D195" t="s">
-        <v>498</v>
+        <v>528</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>475</v>
+        <v>449</v>
+      </c>
+      <c r="B196" t="s">
+        <v>338</v>
       </c>
       <c r="C196" t="s">
-        <v>487</v>
+        <v>339</v>
       </c>
       <c r="D196" t="s">
-        <v>499</v>
+        <v>340</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="C197" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="D197" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="C198" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="D198" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="C199" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="D199" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="C200" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="D200" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="C201" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="D201" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="C202" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="D202" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="C203" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="D203" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="C204" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="D204" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>535</v>
+        <v>476</v>
       </c>
       <c r="C205" t="s">
-        <v>534</v>
+        <v>488</v>
       </c>
       <c r="D205" t="s">
-        <v>533</v>
+        <v>500</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>611</v>
+        <v>477</v>
       </c>
       <c r="C206" t="s">
-        <v>2</v>
+        <v>489</v>
       </c>
       <c r="D206" t="s">
-        <v>612</v>
+        <v>501</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>613</v>
+        <v>478</v>
       </c>
       <c r="C207" t="s">
-        <v>614</v>
+        <v>490</v>
       </c>
       <c r="D207" t="s">
-        <v>3</v>
+        <v>502</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B208" s="2"/>
-      <c r="C208" s="2"/>
-      <c r="D208" s="2"/>
+      <c r="A208" t="s">
+        <v>479</v>
+      </c>
+      <c r="C208" t="s">
+        <v>491</v>
+      </c>
+      <c r="D208" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>124</v>
-      </c>
-      <c r="B209" t="s">
-        <v>123</v>
+        <v>531</v>
       </c>
       <c r="C209" t="s">
-        <v>143</v>
+        <v>530</v>
       </c>
       <c r="D209" t="s">
-        <v>142</v>
+        <v>529</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>141</v>
-      </c>
-      <c r="B210" t="s">
-        <v>123</v>
+        <v>607</v>
       </c>
       <c r="C210" t="s">
-        <v>144</v>
+        <v>2</v>
       </c>
       <c r="D210" t="s">
-        <v>147</v>
+        <v>608</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>125</v>
-      </c>
-      <c r="B211" t="s">
+        <v>609</v>
+      </c>
+      <c r="C211" t="s">
+        <v>610</v>
+      </c>
+      <c r="D211" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C211" t="s">
-        <v>126</v>
-      </c>
-      <c r="D211" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>130</v>
-      </c>
-      <c r="B212" t="s">
-        <v>123</v>
-      </c>
-      <c r="C212" t="s">
-        <v>131</v>
-      </c>
-      <c r="D212" t="s">
-        <v>132</v>
-      </c>
+      <c r="B212" s="2"/>
+      <c r="C212" s="2"/>
+      <c r="D212" s="2"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B213" t="s">
         <v>123</v>
       </c>
       <c r="C213" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="D213" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B214" t="s">
         <v>123</v>
       </c>
       <c r="C214" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D214" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B215" t="s">
         <v>123</v>
       </c>
       <c r="C215" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="D215" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B216" t="s">
         <v>123</v>
       </c>
       <c r="C216" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D216" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B217" s="4"/>
-      <c r="C217" s="4"/>
-      <c r="D217" s="4"/>
+      <c r="A217" t="s">
+        <v>127</v>
+      </c>
+      <c r="B217" t="s">
+        <v>123</v>
+      </c>
+      <c r="C217" t="s">
+        <v>128</v>
+      </c>
+      <c r="D217" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="B218" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="C218" t="s">
-        <v>378</v>
+        <v>146</v>
       </c>
       <c r="D218" t="s">
-        <v>379</v>
+        <v>135</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>376</v>
+        <v>136</v>
       </c>
       <c r="B219" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="C219" t="s">
-        <v>374</v>
+        <v>145</v>
       </c>
       <c r="D219" t="s">
-        <v>377</v>
+        <v>137</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="B220" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="C220" t="s">
-        <v>380</v>
+        <v>139</v>
       </c>
       <c r="D220" t="s">
-        <v>381</v>
+        <v>140</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>382</v>
-      </c>
-      <c r="B221" t="s">
-        <v>82</v>
-      </c>
-      <c r="C221" t="s">
-        <v>383</v>
-      </c>
-      <c r="D221" t="s">
-        <v>384</v>
-      </c>
+      <c r="A221" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B221" s="4"/>
+      <c r="C221" s="4"/>
+      <c r="D221" s="4"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B222" t="s">
         <v>82</v>
       </c>
       <c r="C222" t="s">
-        <v>84</v>
+        <v>374</v>
       </c>
       <c r="D222" t="s">
-        <v>85</v>
+        <v>375</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>645</v>
+        <v>372</v>
+      </c>
+      <c r="B223" t="s">
+        <v>82</v>
       </c>
       <c r="C223" t="s">
-        <v>639</v>
+        <v>370</v>
       </c>
       <c r="D223" t="s">
-        <v>646</v>
+        <v>373</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>656</v>
+        <v>173</v>
+      </c>
+      <c r="B224" t="s">
+        <v>82</v>
       </c>
       <c r="C224" t="s">
-        <v>657</v>
+        <v>376</v>
       </c>
       <c r="D224" t="s">
-        <v>658</v>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>378</v>
+      </c>
+      <c r="B225" t="s">
+        <v>82</v>
+      </c>
+      <c r="C225" t="s">
+        <v>379</v>
+      </c>
+      <c r="D225" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>83</v>
+      </c>
+      <c r="B226" t="s">
+        <v>82</v>
+      </c>
+      <c r="C226" t="s">
+        <v>84</v>
+      </c>
+      <c r="D226" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>641</v>
+      </c>
+      <c r="C227" t="s">
+        <v>635</v>
+      </c>
+      <c r="D227" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>652</v>
+      </c>
+      <c r="C228" t="s">
+        <v>653</v>
+      </c>
+      <c r="D228" t="s">
+        <v>654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Beta version message.
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFC6FCA-EB27-4886-B345-EFE735BCF6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C3FA1C-9C75-46AD-8CFB-15C0DF0CBFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1755" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="694">
   <si>
     <t>id</t>
   </si>
@@ -383,9 +383,6 @@
     <t>Database columns and table names</t>
   </si>
   <si>
-    <t>Home view module</t>
-  </si>
-  <si>
     <t>date_range_lab</t>
   </si>
   <si>
@@ -2073,13 +2070,81 @@
   </si>
   <si>
     <t>Nombre de résultats à télécharger:</t>
+  </si>
+  <si>
+    <t>view_data</t>
+  </si>
+  <si>
+    <t>Voir les données</t>
+  </si>
+  <si>
+    <t>View data</t>
+  </si>
+  <si>
+    <t>text, part 1</t>
+  </si>
+  <si>
+    <t>text, part 2</t>
+  </si>
+  <si>
+    <t>text or button</t>
+  </si>
+  <si>
+    <t>button text for modal</t>
+  </si>
+  <si>
+    <t>Home module</t>
+  </si>
+  <si>
+    <t>betaTitle</t>
+  </si>
+  <si>
+    <t>beta version warning</t>
+  </si>
+  <si>
+    <t>betaText</t>
+  </si>
+  <si>
+    <t>🚧 Notice: this web site is under construction 🚧</t>
+  </si>
+  <si>
+    <t>🚧 Avis: ce site web est en état de construction. 🚧</t>
+  </si>
+  <si>
+    <t>Notez qu'en ce moment, plusieures sections n'ont pas de traductions francophones! On y est presque.&lt;br&gt;&lt;br&gt;Nous travaillons toujours à améliorer l'application en y ajoutant des fonctionnalités, en corrigeant des bugs et en finalisant les traductions français-anglais sur l'ensemble du site. Ne soyez pas surpris de tomber sur des éléments moins que soignés, ou (oh non!) de découvrir un bug. Si vous constatez des comportements étranges ou inattendus, merci d'envoyer un courriel à notre développeur principal à ghislain.delaplante@yukon.ca, et il s'en chargera.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Heads up: several sections do not have French translations yet.&lt;br&gt;&lt;br&gt;We're still working on things over here, building more functionality, fixing bugs, and completing French-English translations throughout the site. Don't be surprised if you come across some less than polished pieces, or (gasp!) find a bug. If you </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>do</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> find some strange stuff or unexpected behaviors, please email our main developer at ghislain.delaplante@yukon.ca and he'll fix it.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2233,6 +2298,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="42">
@@ -2631,7 +2704,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -2644,6 +2717,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3020,10 +3096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D228"/>
+  <dimension ref="A1:D231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3054,7 +3130,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -3065,21 +3141,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
+        <v>532</v>
+      </c>
+      <c r="C3" t="s">
+        <v>534</v>
+      </c>
+      <c r="D3" t="s">
         <v>533</v>
-      </c>
-      <c r="C3" t="s">
-        <v>535</v>
-      </c>
-      <c r="D3" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>116</v>
+        <v>686</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3101,2042 +3177,2048 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>687</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>688</v>
       </c>
       <c r="C6" t="s">
-        <v>561</v>
+        <v>690</v>
       </c>
       <c r="D6" t="s">
-        <v>562</v>
+        <v>691</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>689</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>688</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
+        <v>693</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>560</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>561</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B13" t="s">
-        <v>315</v>
-      </c>
-      <c r="C13" t="s">
-        <v>563</v>
-      </c>
-      <c r="D13" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>316</v>
-      </c>
-      <c r="B14" t="s">
-        <v>318</v>
-      </c>
-      <c r="C14" t="s">
-        <v>319</v>
-      </c>
-      <c r="D14" t="s">
-        <v>320</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B15" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="C15" t="s">
-        <v>322</v>
+        <v>562</v>
       </c>
       <c r="D15" t="s">
-        <v>321</v>
+        <v>563</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B16" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="C16" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="D16" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="B17" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="C17" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D17" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C18" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D18" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C19" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D19" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>565</v>
+        <v>325</v>
       </c>
       <c r="B20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C20" t="s">
-        <v>566</v>
+        <v>336</v>
       </c>
       <c r="D20" t="s">
-        <v>567</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="B21" t="s">
+        <v>330</v>
+      </c>
+      <c r="C21" t="s">
+        <v>326</v>
+      </c>
+      <c r="D21" t="s">
         <v>331</v>
-      </c>
-      <c r="C21" t="s">
-        <v>342</v>
-      </c>
-      <c r="D21" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>344</v>
+        <v>564</v>
       </c>
       <c r="B22" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C22" t="s">
-        <v>345</v>
+        <v>565</v>
       </c>
       <c r="D22" t="s">
-        <v>346</v>
+        <v>566</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="A23" t="s">
+        <v>340</v>
+      </c>
+      <c r="B23" t="s">
+        <v>330</v>
+      </c>
+      <c r="C23" t="s">
+        <v>341</v>
+      </c>
+      <c r="D23" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>343</v>
+      </c>
+      <c r="B24" t="s">
+        <v>337</v>
+      </c>
+      <c r="C24" t="s">
+        <v>344</v>
+      </c>
+      <c r="D24" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>38</v>
       </c>
-      <c r="C24" t="s">
-        <v>172</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C26" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+      <c r="A28" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
         <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>253</v>
-      </c>
-      <c r="B30" t="s">
-        <v>251</v>
-      </c>
-      <c r="C30" t="s">
-        <v>258</v>
-      </c>
-      <c r="D30" t="s">
-        <v>259</v>
-      </c>
+      <c r="A30" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>205</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="B32" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C32" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D32" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>677</v>
+        <v>86</v>
+      </c>
+      <c r="B33" t="s">
+        <v>204</v>
       </c>
       <c r="C33" t="s">
-        <v>678</v>
+        <v>87</v>
       </c>
       <c r="D33" t="s">
-        <v>679</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B34" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C34" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="D34" t="s">
-        <v>302</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>264</v>
-      </c>
-      <c r="B35" t="s">
-        <v>270</v>
+        <v>676</v>
       </c>
       <c r="C35" t="s">
-        <v>274</v>
+        <v>677</v>
       </c>
       <c r="D35" t="s">
-        <v>273</v>
+        <v>678</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B36" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C36" t="s">
-        <v>298</v>
+        <v>267</v>
       </c>
       <c r="D36" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B37" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C37" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="D37" t="s">
-        <v>301</v>
+        <v>272</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>673</v>
+        <v>264</v>
       </c>
       <c r="B38" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C38" t="s">
-        <v>272</v>
+        <v>297</v>
       </c>
       <c r="D38" t="s">
-        <v>275</v>
+        <v>299</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>674</v>
+        <v>265</v>
       </c>
       <c r="B39" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C39" t="s">
-        <v>675</v>
+        <v>298</v>
       </c>
       <c r="D39" t="s">
-        <v>676</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>297</v>
+        <v>672</v>
       </c>
       <c r="B40" t="s">
+        <v>270</v>
+      </c>
+      <c r="C40" t="s">
         <v>271</v>
       </c>
-      <c r="C40" t="s">
-        <v>276</v>
-      </c>
       <c r="D40" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>278</v>
+        <v>673</v>
       </c>
       <c r="B41" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C41" t="s">
-        <v>279</v>
+        <v>674</v>
       </c>
       <c r="D41" t="s">
-        <v>280</v>
+        <v>675</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="B42" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C42" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D42" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B43" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C43" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="D43" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="B44" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C44" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
       <c r="D44" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B45" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C45" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D45" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="B46" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C46" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="D46" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B47" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C47" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D47" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>309</v>
+        <v>288</v>
       </c>
       <c r="B48" t="s">
-        <v>310</v>
+        <v>269</v>
       </c>
       <c r="C48" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="D48" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
+      <c r="A49" t="s">
+        <v>293</v>
+      </c>
+      <c r="B49" t="s">
+        <v>269</v>
+      </c>
+      <c r="C49" t="s">
+        <v>294</v>
+      </c>
+      <c r="D49" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>643</v>
+        <v>308</v>
+      </c>
+      <c r="B50" t="s">
+        <v>309</v>
       </c>
       <c r="C50" t="s">
-        <v>644</v>
+        <v>310</v>
       </c>
       <c r="D50" t="s">
-        <v>645</v>
+        <v>311</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>661</v>
-      </c>
-      <c r="C51" t="s">
-        <v>662</v>
-      </c>
-      <c r="D51" t="s">
-        <v>663</v>
-      </c>
+      <c r="A51" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C52" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D52" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>649</v>
+        <v>660</v>
       </c>
       <c r="C53" t="s">
-        <v>650</v>
+        <v>661</v>
       </c>
       <c r="D53" t="s">
-        <v>651</v>
+        <v>662</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>203</v>
+        <v>645</v>
       </c>
       <c r="B54" t="s">
-        <v>204</v>
+        <v>685</v>
       </c>
       <c r="C54" t="s">
-        <v>89</v>
+        <v>646</v>
       </c>
       <c r="D54" t="s">
-        <v>90</v>
+        <v>647</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>75</v>
+        <v>648</v>
       </c>
       <c r="B55" t="s">
-        <v>206</v>
+        <v>685</v>
       </c>
       <c r="C55" t="s">
-        <v>76</v>
+        <v>649</v>
       </c>
       <c r="D55" t="s">
-        <v>77</v>
+        <v>650</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B56" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C56" t="s">
-        <v>208</v>
+        <v>89</v>
       </c>
       <c r="D56" t="s">
-        <v>209</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>239</v>
+        <v>75</v>
       </c>
       <c r="B57" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="C57" t="s">
-        <v>243</v>
+        <v>76</v>
       </c>
       <c r="D57" t="s">
-        <v>244</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="B58" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
       <c r="C58" t="s">
-        <v>257</v>
+        <v>207</v>
       </c>
       <c r="D58" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>667</v>
+        <v>238</v>
       </c>
       <c r="B59" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="C59" t="s">
-        <v>669</v>
+        <v>242</v>
       </c>
       <c r="D59" t="s">
-        <v>671</v>
+        <v>243</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>668</v>
+        <v>240</v>
       </c>
       <c r="B60" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="C60" t="s">
-        <v>670</v>
+        <v>256</v>
       </c>
       <c r="D60" t="s">
-        <v>672</v>
+        <v>256</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>664</v>
+        <v>679</v>
       </c>
       <c r="B61" t="s">
-        <v>252</v>
+        <v>684</v>
       </c>
       <c r="C61" t="s">
-        <v>665</v>
+        <v>681</v>
       </c>
       <c r="D61" t="s">
-        <v>666</v>
+        <v>680</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>254</v>
+        <v>666</v>
       </c>
       <c r="B62" t="s">
-        <v>252</v>
+        <v>682</v>
       </c>
       <c r="C62" t="s">
-        <v>255</v>
+        <v>668</v>
       </c>
       <c r="D62" t="s">
-        <v>256</v>
+        <v>670</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
+      <c r="A63" t="s">
+        <v>667</v>
+      </c>
+      <c r="B63" t="s">
+        <v>683</v>
+      </c>
+      <c r="C63" t="s">
+        <v>669</v>
+      </c>
+      <c r="D63" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>51</v>
+        <v>663</v>
       </c>
       <c r="B64" t="s">
-        <v>45</v>
+        <v>251</v>
       </c>
       <c r="C64" t="s">
-        <v>52</v>
+        <v>664</v>
       </c>
       <c r="D64" t="s">
-        <v>52</v>
+        <v>665</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B65" s="6"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
+      <c r="A65" t="s">
+        <v>253</v>
+      </c>
+      <c r="B65" t="s">
+        <v>251</v>
+      </c>
+      <c r="C65" t="s">
+        <v>254</v>
+      </c>
+      <c r="D65" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66" t="s">
-        <v>45</v>
-      </c>
-      <c r="C66" t="s">
-        <v>54</v>
-      </c>
-      <c r="D66" t="s">
-        <v>54</v>
-      </c>
+      <c r="A66" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="B67" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="C67" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="D67" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>93</v>
-      </c>
-      <c r="B68" t="s">
-        <v>94</v>
-      </c>
-      <c r="C68" t="s">
-        <v>96</v>
-      </c>
-      <c r="D68" t="s">
-        <v>98</v>
-      </c>
+      <c r="A68" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="B69" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="C69" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="D69" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="B70" t="s">
         <v>92</v>
       </c>
       <c r="C70" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="D70" t="s">
-        <v>284</v>
+        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B71" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C71" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D71" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
+      <c r="A72" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" t="s">
+        <v>97</v>
+      </c>
+      <c r="D72" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="B73" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="C73" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="D73" t="s">
-        <v>57</v>
+        <v>283</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>348</v>
+        <v>102</v>
       </c>
       <c r="B74" t="s">
-        <v>347</v>
+        <v>103</v>
       </c>
       <c r="C74" t="s">
-        <v>353</v>
+        <v>104</v>
       </c>
       <c r="D74" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>349</v>
-      </c>
-      <c r="B75" t="s">
-        <v>347</v>
-      </c>
-      <c r="C75" t="s">
-        <v>354</v>
-      </c>
-      <c r="D75" t="s">
-        <v>354</v>
-      </c>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>356</v>
+        <v>55</v>
       </c>
       <c r="B76" t="s">
-        <v>350</v>
+        <v>45</v>
       </c>
       <c r="C76" t="s">
-        <v>351</v>
+        <v>56</v>
       </c>
       <c r="D76" t="s">
-        <v>352</v>
+        <v>57</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B77" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C77" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D77" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>445</v>
+        <v>348</v>
+      </c>
+      <c r="B78" t="s">
+        <v>346</v>
       </c>
       <c r="C78" t="s">
-        <v>446</v>
+        <v>353</v>
       </c>
       <c r="D78" t="s">
-        <v>447</v>
+        <v>353</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>360</v>
+        <v>355</v>
+      </c>
+      <c r="B79" t="s">
+        <v>349</v>
       </c>
       <c r="C79" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="D79" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>438</v>
+        <v>356</v>
+      </c>
+      <c r="B80" t="s">
+        <v>349</v>
       </c>
       <c r="C80" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="D80" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="C81" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D81" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>440</v>
+        <v>359</v>
       </c>
       <c r="C82" t="s">
-        <v>442</v>
+        <v>361</v>
       </c>
       <c r="D82" t="s">
-        <v>441</v>
+        <v>360</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>365</v>
+        <v>437</v>
       </c>
       <c r="C83" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D83" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>381</v>
-      </c>
-      <c r="B84" t="s">
-        <v>382</v>
+        <v>438</v>
       </c>
       <c r="C84" t="s">
-        <v>383</v>
+        <v>442</v>
       </c>
       <c r="D84" t="s">
-        <v>384</v>
+        <v>443</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="C85" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="D85" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>433</v>
+        <v>364</v>
       </c>
       <c r="C86" t="s">
-        <v>435</v>
+        <v>366</v>
       </c>
       <c r="D86" t="s">
-        <v>437</v>
+        <v>365</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B87" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C87" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D87" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>450</v>
+        <v>431</v>
       </c>
       <c r="C88" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="D88" t="s">
-        <v>425</v>
+        <v>435</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="C89" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
       <c r="D89" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>368</v>
+        <v>384</v>
+      </c>
+      <c r="B90" t="s">
+        <v>385</v>
       </c>
       <c r="C90" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="D90" t="s">
-        <v>369</v>
+        <v>387</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>389</v>
+        <v>449</v>
       </c>
       <c r="C91" t="s">
-        <v>390</v>
+        <v>423</v>
       </c>
       <c r="D91" t="s">
-        <v>390</v>
+        <v>424</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>391</v>
+        <v>450</v>
       </c>
       <c r="C92" t="s">
-        <v>392</v>
+        <v>451</v>
       </c>
       <c r="D92" t="s">
-        <v>393</v>
+        <v>452</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="C93" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D93" t="s">
-        <v>396</v>
+        <v>368</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="C94" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="D94" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="C95" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="D95" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="C96" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="D96" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>426</v>
+        <v>397</v>
       </c>
       <c r="C97" t="s">
-        <v>431</v>
+        <v>398</v>
       </c>
       <c r="D97" t="s">
-        <v>430</v>
+        <v>399</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="C98" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="D98" t="s">
-        <v>448</v>
+        <v>402</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="C99" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
       <c r="D99" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
       <c r="C100" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="D100" t="s">
-        <v>415</v>
+        <v>429</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C101" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D101" t="s">
-        <v>416</v>
+        <v>447</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="C102" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="D102" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C103" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D103" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>536</v>
-      </c>
-      <c r="C104" s="11" t="s">
-        <v>537</v>
+        <v>411</v>
+      </c>
+      <c r="C104" t="s">
+        <v>417</v>
       </c>
       <c r="D104" t="s">
-        <v>538</v>
+        <v>415</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>454</v>
+        <v>420</v>
       </c>
       <c r="C105" t="s">
-        <v>455</v>
+        <v>421</v>
       </c>
       <c r="D105" t="s">
-        <v>456</v>
+        <v>422</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>457</v>
+        <v>412</v>
       </c>
       <c r="C106" t="s">
-        <v>512</v>
+        <v>418</v>
       </c>
       <c r="D106" t="s">
-        <v>510</v>
+        <v>419</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>459</v>
-      </c>
-      <c r="C107" t="s">
-        <v>458</v>
+        <v>535</v>
+      </c>
+      <c r="C107" s="11" t="s">
+        <v>536</v>
       </c>
       <c r="D107" t="s">
-        <v>511</v>
+        <v>537</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>542</v>
+        <v>453</v>
       </c>
       <c r="C108" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="D108" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>560</v>
+        <v>456</v>
       </c>
       <c r="C109" t="s">
-        <v>558</v>
+        <v>511</v>
       </c>
       <c r="D109" t="s">
-        <v>559</v>
+        <v>509</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="C110" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="D110" t="s">
-        <v>467</v>
+        <v>510</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>504</v>
+        <v>541</v>
       </c>
       <c r="C111" t="s">
-        <v>506</v>
+        <v>462</v>
       </c>
       <c r="D111" t="s">
-        <v>508</v>
+        <v>463</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>505</v>
+        <v>559</v>
       </c>
       <c r="C112" t="s">
-        <v>507</v>
+        <v>557</v>
       </c>
       <c r="D112" t="s">
-        <v>509</v>
+        <v>558</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>513</v>
+        <v>464</v>
       </c>
       <c r="C113" t="s">
-        <v>514</v>
+        <v>465</v>
       </c>
       <c r="D113" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>546</v>
+        <v>503</v>
       </c>
       <c r="C114" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="D114" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="C115" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
       <c r="D115" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="C116" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="D116" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>522</v>
+        <v>545</v>
       </c>
       <c r="C117" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
       <c r="D117" t="s">
-        <v>553</v>
+        <v>516</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>539</v>
-      </c>
-      <c r="C118" s="11" t="s">
-        <v>540</v>
+        <v>517</v>
+      </c>
+      <c r="C118" t="s">
+        <v>518</v>
       </c>
       <c r="D118" t="s">
-        <v>541</v>
+        <v>519</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>543</v>
-      </c>
-      <c r="C119" s="11" t="s">
-        <v>544</v>
+        <v>520</v>
+      </c>
+      <c r="C119" t="s">
+        <v>522</v>
       </c>
       <c r="D119" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>547</v>
-      </c>
-      <c r="C120" s="11" t="s">
-        <v>548</v>
+        <v>521</v>
+      </c>
+      <c r="C120" t="s">
+        <v>524</v>
       </c>
       <c r="D120" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>552</v>
+        <v>539</v>
       </c>
       <c r="D121" t="s">
-        <v>551</v>
+        <v>540</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>525</v>
+        <v>543</v>
       </c>
       <c r="D122" t="s">
-        <v>553</v>
+        <v>544</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="D123" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>568</v>
+        <v>549</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>569</v>
+        <v>551</v>
       </c>
       <c r="D124" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>571</v>
+        <v>555</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>575</v>
+        <v>524</v>
       </c>
       <c r="D125" t="s">
-        <v>573</v>
+        <v>552</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>574</v>
+        <v>553</v>
       </c>
       <c r="D126" t="s">
-        <v>574</v>
+        <v>554</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>582</v>
+        <v>568</v>
       </c>
       <c r="D127" t="s">
-        <v>581</v>
+        <v>569</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="D128" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>583</v>
+        <v>571</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
       <c r="D129" t="s">
-        <v>585</v>
+        <v>573</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>602</v>
+        <v>581</v>
       </c>
       <c r="D130" t="s">
-        <v>603</v>
+        <v>580</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>588</v>
+        <v>578</v>
       </c>
       <c r="D131" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="D132" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>598</v>
+        <v>577</v>
       </c>
       <c r="C133" s="11" t="s">
-        <v>592</v>
+        <v>601</v>
       </c>
       <c r="D133" t="s">
-        <v>595</v>
+        <v>602</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="D134" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>600</v>
+        <v>586</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>593</v>
-      </c>
-      <c r="D135" s="11" t="s">
-        <v>593</v>
+        <v>588</v>
+      </c>
+      <c r="D135" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C136" s="11" t="s">
-        <v>594</v>
-      </c>
-      <c r="D136" s="11" t="s">
+        <v>591</v>
+      </c>
+      <c r="D136" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="C137" s="11" t="s">
-        <v>605</v>
-      </c>
-      <c r="D137" s="11" t="s">
-        <v>606</v>
+        <v>595</v>
+      </c>
+      <c r="D137" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>611</v>
+        <v>599</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>614</v>
+        <v>592</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>615</v>
+        <v>592</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>616</v>
+        <v>593</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B140" s="4"/>
-      <c r="C140" s="4"/>
-      <c r="D140" s="4"/>
+      <c r="A140" t="s">
+        <v>603</v>
+      </c>
+      <c r="C140" s="11" t="s">
+        <v>604</v>
+      </c>
+      <c r="D140" s="11" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>149</v>
-      </c>
-      <c r="B141" t="s">
-        <v>45</v>
-      </c>
-      <c r="C141" t="s">
-        <v>150</v>
-      </c>
-      <c r="D141" t="s">
-        <v>151</v>
+        <v>610</v>
+      </c>
+      <c r="C141" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="D141" s="11" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>155</v>
-      </c>
-      <c r="B142" t="s">
-        <v>152</v>
-      </c>
-      <c r="C142" t="s">
-        <v>153</v>
-      </c>
-      <c r="D142" t="s">
-        <v>154</v>
+        <v>611</v>
+      </c>
+      <c r="C142" s="11" t="s">
+        <v>612</v>
+      </c>
+      <c r="D142" s="11" t="s">
+        <v>615</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>158</v>
-      </c>
-      <c r="B143" t="s">
-        <v>159</v>
-      </c>
-      <c r="C143" t="s">
-        <v>170</v>
-      </c>
-      <c r="D143" t="s">
-        <v>171</v>
-      </c>
+      <c r="A143" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B143" s="4"/>
+      <c r="C143" s="4"/>
+      <c r="D143" s="4"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="B144" t="s">
-        <v>152</v>
+        <v>45</v>
       </c>
       <c r="C144" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D144" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B145" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C145" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="D145" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B146" t="s">
-        <v>163</v>
-      </c>
-      <c r="C146" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D146" s="9" t="s">
-        <v>165</v>
+        <v>158</v>
+      </c>
+      <c r="C146" t="s">
+        <v>169</v>
+      </c>
+      <c r="D146" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B147" t="s">
+        <v>151</v>
+      </c>
+      <c r="C147" t="s">
+        <v>155</v>
+      </c>
+      <c r="D147" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>159</v>
       </c>
-      <c r="C147" t="s">
-        <v>164</v>
-      </c>
-      <c r="D147" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B148" s="8"/>
-      <c r="C148" s="8"/>
-      <c r="D148" s="8"/>
+      <c r="B148" t="s">
+        <v>158</v>
+      </c>
+      <c r="C148" t="s">
+        <v>168</v>
+      </c>
+      <c r="D148" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
       <c r="B149" t="s">
-        <v>8</v>
-      </c>
-      <c r="C149" t="s">
-        <v>59</v>
-      </c>
-      <c r="D149" t="s">
-        <v>60</v>
+        <v>162</v>
+      </c>
+      <c r="C149" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D149" s="9" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>106</v>
+        <v>161</v>
       </c>
       <c r="B150" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="C150" t="s">
-        <v>107</v>
+        <v>163</v>
       </c>
       <c r="D150" t="s">
-        <v>108</v>
+        <v>165</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>620</v>
-      </c>
-      <c r="C151" t="s">
-        <v>621</v>
-      </c>
-      <c r="D151" t="s">
-        <v>622</v>
-      </c>
+      <c r="A151" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B151" s="8"/>
+      <c r="C151" s="8"/>
+      <c r="D151" s="8"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>623</v>
+        <v>58</v>
+      </c>
+      <c r="B152" t="s">
+        <v>8</v>
       </c>
       <c r="C152" t="s">
-        <v>624</v>
+        <v>59</v>
       </c>
       <c r="D152" t="s">
-        <v>625</v>
+        <v>60</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>655</v>
+        <v>106</v>
+      </c>
+      <c r="B153" t="s">
+        <v>8</v>
       </c>
       <c r="C153" t="s">
-        <v>657</v>
+        <v>107</v>
       </c>
       <c r="D153" t="s">
-        <v>658</v>
+        <v>108</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>656</v>
+        <v>619</v>
       </c>
       <c r="C154" t="s">
-        <v>660</v>
+        <v>620</v>
       </c>
       <c r="D154" t="s">
-        <v>659</v>
+        <v>621</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>61</v>
-      </c>
-      <c r="B155" t="s">
-        <v>8</v>
+        <v>622</v>
       </c>
       <c r="C155" t="s">
-        <v>62</v>
+        <v>623</v>
       </c>
       <c r="D155" t="s">
-        <v>63</v>
+        <v>624</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>64</v>
-      </c>
-      <c r="B156" t="s">
-        <v>8</v>
+        <v>654</v>
       </c>
       <c r="C156" t="s">
-        <v>65</v>
+        <v>656</v>
       </c>
       <c r="D156" t="s">
-        <v>242</v>
+        <v>657</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>237</v>
-      </c>
-      <c r="B157" t="s">
-        <v>8</v>
+        <v>655</v>
       </c>
       <c r="C157" t="s">
-        <v>238</v>
+        <v>659</v>
       </c>
       <c r="D157" t="s">
-        <v>238</v>
+        <v>658</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>371</v>
+        <v>61</v>
       </c>
       <c r="B158" t="s">
         <v>8</v>
       </c>
       <c r="C158" t="s">
-        <v>637</v>
+        <v>62</v>
       </c>
       <c r="D158" t="s">
-        <v>639</v>
+        <v>63</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>638</v>
+        <v>64</v>
+      </c>
+      <c r="B159" t="s">
+        <v>8</v>
       </c>
       <c r="C159" t="s">
-        <v>636</v>
+        <v>65</v>
       </c>
       <c r="D159" t="s">
-        <v>640</v>
+        <v>241</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>175</v>
+        <v>236</v>
       </c>
       <c r="B160" t="s">
         <v>8</v>
       </c>
       <c r="C160" t="s">
-        <v>617</v>
+        <v>237</v>
       </c>
       <c r="D160" t="s">
-        <v>176</v>
+        <v>237</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>185</v>
+        <v>370</v>
       </c>
       <c r="B161" t="s">
         <v>8</v>
       </c>
       <c r="C161" t="s">
-        <v>618</v>
+        <v>636</v>
       </c>
       <c r="D161" t="s">
-        <v>186</v>
+        <v>638</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>193</v>
-      </c>
-      <c r="B162" t="s">
-        <v>8</v>
+        <v>637</v>
       </c>
       <c r="C162" t="s">
-        <v>619</v>
+        <v>635</v>
       </c>
       <c r="D162" t="s">
-        <v>194</v>
+        <v>639</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>626</v>
+        <v>174</v>
       </c>
       <c r="B163" t="s">
         <v>8</v>
       </c>
       <c r="C163" t="s">
-        <v>627</v>
+        <v>616</v>
       </c>
       <c r="D163" t="s">
-        <v>628</v>
+        <v>175</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>633</v>
+        <v>184</v>
       </c>
       <c r="B164" t="s">
         <v>8</v>
       </c>
       <c r="C164" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="D164" t="s">
-        <v>629</v>
+        <v>185</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>634</v>
+        <v>192</v>
       </c>
       <c r="B165" t="s">
         <v>8</v>
       </c>
       <c r="C165" t="s">
-        <v>632</v>
+        <v>618</v>
       </c>
       <c r="D165" t="s">
-        <v>630</v>
+        <v>193</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>174</v>
+        <v>625</v>
       </c>
       <c r="B166" t="s">
         <v>8</v>
       </c>
       <c r="C166" t="s">
-        <v>210</v>
+        <v>626</v>
       </c>
       <c r="D166" t="s">
-        <v>211</v>
+        <v>627</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>66</v>
+        <v>632</v>
       </c>
       <c r="B167" t="s">
         <v>8</v>
       </c>
       <c r="C167" t="s">
-        <v>67</v>
+        <v>630</v>
       </c>
       <c r="D167" t="s">
-        <v>68</v>
+        <v>628</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>182</v>
+        <v>633</v>
       </c>
       <c r="B168" t="s">
         <v>8</v>
       </c>
       <c r="C168" t="s">
-        <v>177</v>
+        <v>631</v>
       </c>
       <c r="D168" t="s">
-        <v>16</v>
+        <v>629</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="B169" t="s">
         <v>8</v>
       </c>
       <c r="C169" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="D169" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B170" t="s">
         <v>8</v>
       </c>
       <c r="C170" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D170" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -5147,38 +5229,38 @@
         <v>8</v>
       </c>
       <c r="C171" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D171" t="s">
-        <v>184</v>
+        <v>16</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B172" t="s">
         <v>8</v>
       </c>
       <c r="C172" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D172" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B173" t="s">
         <v>8</v>
       </c>
       <c r="C173" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D173" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -5189,695 +5271,738 @@
         <v>8</v>
       </c>
       <c r="C174" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D174" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B175" t="s">
         <v>8</v>
       </c>
       <c r="C175" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D175" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>214</v>
+        <v>72</v>
       </c>
       <c r="B176" t="s">
         <v>8</v>
       </c>
       <c r="C176" t="s">
-        <v>212</v>
+        <v>73</v>
       </c>
       <c r="D176" t="s">
-        <v>213</v>
+        <v>74</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="B177" t="s">
         <v>8</v>
       </c>
       <c r="C177" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="D177" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="B178" t="s">
         <v>8</v>
       </c>
       <c r="C178" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="D178" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>306</v>
+        <v>213</v>
+      </c>
+      <c r="B179" t="s">
+        <v>8</v>
       </c>
       <c r="C179" t="s">
-        <v>307</v>
+        <v>211</v>
       </c>
       <c r="D179" t="s">
-        <v>308</v>
+        <v>212</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>78</v>
+        <v>214</v>
       </c>
       <c r="B180" t="s">
         <v>8</v>
       </c>
       <c r="C180" t="s">
-        <v>79</v>
+        <v>215</v>
       </c>
       <c r="D180" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>7</v>
+        <v>216</v>
       </c>
       <c r="B181" t="s">
         <v>8</v>
       </c>
       <c r="C181" t="s">
-        <v>9</v>
+        <v>217</v>
       </c>
       <c r="D181" t="s">
-        <v>10</v>
+        <v>218</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>460</v>
+        <v>305</v>
       </c>
       <c r="C182" t="s">
-        <v>461</v>
+        <v>306</v>
       </c>
       <c r="D182" t="s">
-        <v>462</v>
+        <v>307</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>220</v>
+        <v>78</v>
       </c>
       <c r="B183" t="s">
         <v>8</v>
       </c>
       <c r="C183" t="s">
-        <v>220</v>
+        <v>79</v>
       </c>
       <c r="D183" t="s">
-        <v>221</v>
+        <v>80</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>198</v>
+        <v>7</v>
       </c>
       <c r="B184" t="s">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="C184" t="s">
-        <v>198</v>
+        <v>9</v>
       </c>
       <c r="D184" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>222</v>
-      </c>
-      <c r="B185" t="s">
-        <v>8</v>
+        <v>459</v>
       </c>
       <c r="C185" t="s">
-        <v>224</v>
+        <v>460</v>
       </c>
       <c r="D185" t="s">
-        <v>225</v>
+        <v>461</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B186" t="s">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="C186" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D186" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>249</v>
+        <v>197</v>
       </c>
       <c r="B187" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="C187" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="D187" t="s">
-        <v>247</v>
+        <v>199</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="B188" t="s">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="C188" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="D188" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B189" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="C189" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D189" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="B190" t="s">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="C190" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="D190" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>120</v>
+        <v>249</v>
       </c>
       <c r="B191" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="C191" t="s">
-        <v>121</v>
+        <v>245</v>
       </c>
       <c r="D191" t="s">
-        <v>122</v>
+        <v>247</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B192" t="s">
         <v>8</v>
       </c>
       <c r="C192" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D192" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="B193" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="C193" t="s">
-        <v>15</v>
+        <v>233</v>
       </c>
       <c r="D193" t="s">
-        <v>16</v>
+        <v>235</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>407</v>
+        <v>119</v>
+      </c>
+      <c r="B194" t="s">
+        <v>8</v>
       </c>
       <c r="C194" t="s">
-        <v>408</v>
+        <v>120</v>
       </c>
       <c r="D194" t="s">
-        <v>409</v>
+        <v>121</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>526</v>
+        <v>227</v>
+      </c>
+      <c r="B195" t="s">
+        <v>8</v>
       </c>
       <c r="C195" t="s">
-        <v>527</v>
+        <v>228</v>
       </c>
       <c r="D195" t="s">
-        <v>528</v>
+        <v>229</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>449</v>
+        <v>14</v>
       </c>
       <c r="B196" t="s">
-        <v>338</v>
+        <v>8</v>
       </c>
       <c r="C196" t="s">
-        <v>339</v>
+        <v>15</v>
       </c>
       <c r="D196" t="s">
-        <v>340</v>
+        <v>16</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>468</v>
+        <v>406</v>
       </c>
       <c r="C197" t="s">
-        <v>480</v>
+        <v>407</v>
       </c>
       <c r="D197" t="s">
-        <v>492</v>
+        <v>408</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>469</v>
+        <v>525</v>
       </c>
       <c r="C198" t="s">
-        <v>481</v>
+        <v>526</v>
       </c>
       <c r="D198" t="s">
-        <v>493</v>
+        <v>527</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>470</v>
+        <v>448</v>
+      </c>
+      <c r="B199" t="s">
+        <v>337</v>
       </c>
       <c r="C199" t="s">
-        <v>482</v>
+        <v>338</v>
       </c>
       <c r="D199" t="s">
-        <v>494</v>
+        <v>339</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C200" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D200" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C201" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D201" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C202" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D202" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C203" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="D203" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C204" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D204" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C205" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D205" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C206" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D206" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C207" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="D207" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C208" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="D208" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>531</v>
+        <v>476</v>
       </c>
       <c r="C209" t="s">
-        <v>530</v>
+        <v>488</v>
       </c>
       <c r="D209" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>607</v>
+        <v>477</v>
       </c>
       <c r="C210" t="s">
-        <v>2</v>
+        <v>489</v>
       </c>
       <c r="D210" t="s">
-        <v>608</v>
+        <v>501</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>609</v>
+        <v>478</v>
       </c>
       <c r="C211" t="s">
-        <v>610</v>
+        <v>490</v>
       </c>
       <c r="D211" t="s">
-        <v>3</v>
+        <v>502</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B212" s="2"/>
-      <c r="C212" s="2"/>
-      <c r="D212" s="2"/>
+      <c r="A212" t="s">
+        <v>530</v>
+      </c>
+      <c r="C212" t="s">
+        <v>529</v>
+      </c>
+      <c r="D212" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>124</v>
-      </c>
-      <c r="B213" t="s">
-        <v>123</v>
+        <v>606</v>
       </c>
       <c r="C213" t="s">
-        <v>143</v>
+        <v>2</v>
       </c>
       <c r="D213" t="s">
-        <v>142</v>
+        <v>607</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>141</v>
-      </c>
-      <c r="B214" t="s">
-        <v>123</v>
+        <v>608</v>
       </c>
       <c r="C214" t="s">
-        <v>144</v>
+        <v>609</v>
       </c>
       <c r="D214" t="s">
-        <v>147</v>
+        <v>3</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
-        <v>125</v>
-      </c>
-      <c r="B215" t="s">
-        <v>123</v>
-      </c>
-      <c r="C215" t="s">
-        <v>126</v>
-      </c>
-      <c r="D215" t="s">
-        <v>133</v>
-      </c>
+      <c r="A215" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B215" s="2"/>
+      <c r="C215" s="2"/>
+      <c r="D215" s="2"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B216" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C216" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="D216" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B217" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C217" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="D217" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B218" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C218" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="D218" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B219" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C219" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="D219" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B220" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C220" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D220" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B221" s="4"/>
-      <c r="C221" s="4"/>
-      <c r="D221" s="4"/>
+      <c r="A221" t="s">
+        <v>133</v>
+      </c>
+      <c r="B221" t="s">
+        <v>122</v>
+      </c>
+      <c r="C221" t="s">
+        <v>145</v>
+      </c>
+      <c r="D221" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="B222" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="C222" t="s">
-        <v>374</v>
+        <v>144</v>
       </c>
       <c r="D222" t="s">
-        <v>375</v>
+        <v>136</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>372</v>
+        <v>137</v>
       </c>
       <c r="B223" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="C223" t="s">
-        <v>370</v>
+        <v>138</v>
       </c>
       <c r="D223" t="s">
-        <v>373</v>
+        <v>139</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>173</v>
-      </c>
-      <c r="B224" t="s">
-        <v>82</v>
-      </c>
-      <c r="C224" t="s">
-        <v>376</v>
-      </c>
-      <c r="D224" t="s">
-        <v>377</v>
-      </c>
+      <c r="A224" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B224" s="4"/>
+      <c r="C224" s="4"/>
+      <c r="D224" s="4"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>378</v>
+        <v>81</v>
       </c>
       <c r="B225" t="s">
         <v>82</v>
       </c>
       <c r="C225" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D225" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>83</v>
+        <v>371</v>
       </c>
       <c r="B226" t="s">
         <v>82</v>
       </c>
       <c r="C226" t="s">
-        <v>84</v>
+        <v>369</v>
       </c>
       <c r="D226" t="s">
-        <v>85</v>
+        <v>372</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>641</v>
+        <v>172</v>
+      </c>
+      <c r="B227" t="s">
+        <v>82</v>
       </c>
       <c r="C227" t="s">
-        <v>635</v>
+        <v>375</v>
       </c>
       <c r="D227" t="s">
-        <v>642</v>
+        <v>376</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
+        <v>377</v>
+      </c>
+      <c r="B228" t="s">
+        <v>82</v>
+      </c>
+      <c r="C228" t="s">
+        <v>378</v>
+      </c>
+      <c r="D228" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>83</v>
+      </c>
+      <c r="B229" t="s">
+        <v>82</v>
+      </c>
+      <c r="C229" t="s">
+        <v>84</v>
+      </c>
+      <c r="D229" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>640</v>
+      </c>
+      <c r="C230" t="s">
+        <v>634</v>
+      </c>
+      <c r="D230" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>651</v>
+      </c>
+      <c r="C231" t="s">
         <v>652</v>
       </c>
-      <c r="C228" t="s">
+      <c r="D231" t="s">
         <v>653</v>
-      </c>
-      <c r="D228" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
migrate old translation setup to new function tr()
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C3FA1C-9C75-46AD-8CFB-15C0DF0CBFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286E4990-77A3-4F97-8A1B-5E76A345B509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="700">
   <si>
     <t>id</t>
   </si>
@@ -858,12 +858,6 @@
   </si>
   <si>
     <t>Sous-ensemble de données (3 lignes par série temporelle)</t>
-  </si>
-  <si>
-    <t>Location metadata (up to first three rows)</t>
-  </si>
-  <si>
-    <t>Métadonnées des sites (jusqu'aux trois premières lignes)</t>
   </si>
   <si>
     <t>extra_tbl_msg</t>
@@ -2138,6 +2132,30 @@
       </rPr>
       <t xml:space="preserve"> find some strange stuff or unexpected behaviors, please email our main developer at ghislain.delaplante@yukon.ca and he'll fix it.</t>
     </r>
+  </si>
+  <si>
+    <t>view_samples</t>
+  </si>
+  <si>
+    <t>Show samples</t>
+  </si>
+  <si>
+    <t>Voir les échantillons</t>
+  </si>
+  <si>
+    <t>reset_filters</t>
+  </si>
+  <si>
+    <t>Reset filters</t>
+  </si>
+  <si>
+    <t>Réinitialiser les filtres</t>
+  </si>
+  <si>
+    <t>Subset of location metadata (up to first three rows)</t>
+  </si>
+  <si>
+    <t>Sous-ensemble des métadonnées des sites (jusqu'aux trois premières lignes)</t>
   </si>
 </sst>
 </file>
@@ -3096,10 +3114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D231"/>
+  <dimension ref="A1:D233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3130,7 +3148,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -3144,18 +3162,18 @@
         <v>151</v>
       </c>
       <c r="B3" t="s">
+        <v>530</v>
+      </c>
+      <c r="C3" t="s">
         <v>532</v>
       </c>
-      <c r="C3" t="s">
-        <v>534</v>
-      </c>
       <c r="D3" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3177,30 +3195,30 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B6" t="s">
+        <v>686</v>
+      </c>
+      <c r="C6" t="s">
         <v>688</v>
       </c>
-      <c r="C6" t="s">
-        <v>690</v>
-      </c>
       <c r="D6" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B7" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C7" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3211,10 +3229,10 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D8" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3289,7 +3307,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -3297,142 +3315,142 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>310</v>
+      </c>
+      <c r="B15" t="s">
         <v>312</v>
       </c>
-      <c r="B15" t="s">
-        <v>314</v>
-      </c>
       <c r="C15" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D15" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>313</v>
+      </c>
+      <c r="B16" t="s">
         <v>315</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>316</v>
+      </c>
+      <c r="D16" t="s">
         <v>317</v>
-      </c>
-      <c r="C16" t="s">
-        <v>318</v>
-      </c>
-      <c r="D16" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C17" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B18" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C18" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D18" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B19" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C19" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D19" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B20" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C20" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D20" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>326</v>
+      </c>
+      <c r="B21" t="s">
         <v>328</v>
       </c>
-      <c r="B21" t="s">
-        <v>330</v>
-      </c>
       <c r="C21" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D21" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>562</v>
+      </c>
+      <c r="B22" t="s">
+        <v>328</v>
+      </c>
+      <c r="C22" t="s">
+        <v>563</v>
+      </c>
+      <c r="D22" t="s">
         <v>564</v>
-      </c>
-      <c r="B22" t="s">
-        <v>330</v>
-      </c>
-      <c r="C22" t="s">
-        <v>565</v>
-      </c>
-      <c r="D22" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>338</v>
+      </c>
+      <c r="B23" t="s">
+        <v>328</v>
+      </c>
+      <c r="C23" t="s">
+        <v>339</v>
+      </c>
+      <c r="D23" t="s">
         <v>340</v>
-      </c>
-      <c r="B23" t="s">
-        <v>330</v>
-      </c>
-      <c r="C23" t="s">
-        <v>341</v>
-      </c>
-      <c r="D23" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>341</v>
+      </c>
+      <c r="B24" t="s">
+        <v>335</v>
+      </c>
+      <c r="C24" t="s">
+        <v>342</v>
+      </c>
+      <c r="D24" t="s">
         <v>343</v>
-      </c>
-      <c r="B24" t="s">
-        <v>337</v>
-      </c>
-      <c r="C24" t="s">
-        <v>344</v>
-      </c>
-      <c r="D24" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3559,13 +3577,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>674</v>
+      </c>
+      <c r="C35" t="s">
+        <v>675</v>
+      </c>
+      <c r="D35" t="s">
         <v>676</v>
-      </c>
-      <c r="C35" t="s">
-        <v>677</v>
-      </c>
-      <c r="D35" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3579,7 +3597,7 @@
         <v>267</v>
       </c>
       <c r="D36" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3604,10 +3622,10 @@
         <v>269</v>
       </c>
       <c r="C38" t="s">
+        <v>295</v>
+      </c>
+      <c r="D38" t="s">
         <v>297</v>
-      </c>
-      <c r="D38" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3618,15 +3636,15 @@
         <v>269</v>
       </c>
       <c r="C39" t="s">
+        <v>296</v>
+      </c>
+      <c r="D39" t="s">
         <v>298</v>
-      </c>
-      <c r="D39" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B40" t="s">
         <v>270</v>
@@ -3640,142 +3658,142 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B41" t="s">
         <v>270</v>
       </c>
       <c r="C41" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D41" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B42" t="s">
         <v>270</v>
       </c>
       <c r="C42" t="s">
-        <v>275</v>
+        <v>698</v>
       </c>
       <c r="D42" t="s">
-        <v>276</v>
+        <v>699</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B43" t="s">
         <v>270</v>
       </c>
       <c r="C43" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D43" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B44" t="s">
         <v>268</v>
       </c>
       <c r="C44" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D44" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B45" t="s">
         <v>268</v>
       </c>
       <c r="C45" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D45" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B46" t="s">
         <v>268</v>
       </c>
       <c r="C46" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D46" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B47" t="s">
         <v>269</v>
       </c>
       <c r="C47" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D47" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B48" t="s">
         <v>269</v>
       </c>
       <c r="C48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D48" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B49" t="s">
         <v>269</v>
       </c>
       <c r="C49" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D49" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>306</v>
+      </c>
+      <c r="B50" t="s">
+        <v>307</v>
+      </c>
+      <c r="C50" t="s">
         <v>308</v>
       </c>
-      <c r="B50" t="s">
+      <c r="D50" t="s">
         <v>309</v>
-      </c>
-      <c r="C50" t="s">
-        <v>310</v>
-      </c>
-      <c r="D50" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3788,52 +3806,52 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>640</v>
+      </c>
+      <c r="C52" t="s">
+        <v>641</v>
+      </c>
+      <c r="D52" t="s">
         <v>642</v>
-      </c>
-      <c r="C52" t="s">
-        <v>643</v>
-      </c>
-      <c r="D52" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>658</v>
+      </c>
+      <c r="C53" t="s">
+        <v>659</v>
+      </c>
+      <c r="D53" t="s">
         <v>660</v>
-      </c>
-      <c r="C53" t="s">
-        <v>661</v>
-      </c>
-      <c r="D53" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>643</v>
+      </c>
+      <c r="B54" t="s">
+        <v>683</v>
+      </c>
+      <c r="C54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D54" t="s">
         <v>645</v>
-      </c>
-      <c r="B54" t="s">
-        <v>685</v>
-      </c>
-      <c r="C54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D54" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>646</v>
+      </c>
+      <c r="B55" t="s">
+        <v>683</v>
+      </c>
+      <c r="C55" t="s">
+        <v>647</v>
+      </c>
+      <c r="D55" t="s">
         <v>648</v>
-      </c>
-      <c r="B55" t="s">
-        <v>685</v>
-      </c>
-      <c r="C55" t="s">
-        <v>649</v>
-      </c>
-      <c r="D55" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3908,244 +3926,238 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>679</v>
-      </c>
-      <c r="B61" t="s">
-        <v>684</v>
+        <v>695</v>
       </c>
       <c r="C61" t="s">
-        <v>681</v>
+        <v>696</v>
       </c>
       <c r="D61" t="s">
-        <v>680</v>
+        <v>697</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>666</v>
-      </c>
-      <c r="B62" t="s">
-        <v>682</v>
+        <v>692</v>
       </c>
       <c r="C62" t="s">
-        <v>668</v>
+        <v>693</v>
       </c>
       <c r="D62" t="s">
-        <v>670</v>
+        <v>694</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="B63" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C63" t="s">
-        <v>669</v>
+        <v>679</v>
       </c>
       <c r="D63" t="s">
-        <v>671</v>
+        <v>678</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B64" t="s">
-        <v>251</v>
+        <v>680</v>
       </c>
       <c r="C64" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="D64" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>253</v>
+        <v>665</v>
       </c>
       <c r="B65" t="s">
+        <v>681</v>
+      </c>
+      <c r="C65" t="s">
+        <v>667</v>
+      </c>
+      <c r="D65" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>661</v>
+      </c>
+      <c r="B66" t="s">
         <v>251</v>
       </c>
-      <c r="C65" t="s">
-        <v>254</v>
-      </c>
-      <c r="D65" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
+      <c r="C66" t="s">
+        <v>662</v>
+      </c>
+      <c r="D66" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>51</v>
+        <v>253</v>
       </c>
       <c r="B67" t="s">
-        <v>45</v>
+        <v>251</v>
       </c>
       <c r="C67" t="s">
-        <v>52</v>
+        <v>254</v>
       </c>
       <c r="D67" t="s">
-        <v>52</v>
+        <v>255</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
+      <c r="A68" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B69" t="s">
         <v>45</v>
       </c>
       <c r="C69" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D69" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>91</v>
-      </c>
-      <c r="B70" t="s">
-        <v>92</v>
-      </c>
-      <c r="C70" t="s">
-        <v>100</v>
-      </c>
-      <c r="D70" t="s">
-        <v>101</v>
-      </c>
+      <c r="A70" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="B71" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="C71" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="D71" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C72" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D72" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="B73" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C73" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="D73" t="s">
-        <v>283</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B74" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C74" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D74" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
+      <c r="A75" t="s">
+        <v>116</v>
+      </c>
+      <c r="B75" t="s">
+        <v>92</v>
+      </c>
+      <c r="C75" t="s">
+        <v>117</v>
+      </c>
+      <c r="D75" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="B76" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="C76" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="D76" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>347</v>
-      </c>
-      <c r="B77" t="s">
-        <v>346</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="A77" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D77" t="s">
-        <v>353</v>
-      </c>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>348</v>
+        <v>55</v>
       </c>
       <c r="B78" t="s">
-        <v>346</v>
+        <v>45</v>
       </c>
       <c r="C78" t="s">
-        <v>353</v>
+        <v>56</v>
       </c>
       <c r="D78" t="s">
-        <v>353</v>
+        <v>57</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B79" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="C79" t="s">
         <v>350</v>
@@ -4156,1848 +4168,1876 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B80" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="C80" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D80" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>444</v>
+        <v>353</v>
+      </c>
+      <c r="B81" t="s">
+        <v>347</v>
       </c>
       <c r="C81" t="s">
-        <v>445</v>
+        <v>348</v>
       </c>
       <c r="D81" t="s">
-        <v>446</v>
+        <v>349</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>359</v>
+        <v>354</v>
+      </c>
+      <c r="B82" t="s">
+        <v>347</v>
       </c>
       <c r="C82" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D82" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="C83" t="s">
-        <v>362</v>
+        <v>443</v>
       </c>
       <c r="D83" t="s">
-        <v>363</v>
+        <v>444</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>438</v>
+        <v>357</v>
       </c>
       <c r="C84" t="s">
-        <v>442</v>
+        <v>359</v>
       </c>
       <c r="D84" t="s">
-        <v>443</v>
+        <v>358</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C85" t="s">
-        <v>441</v>
+        <v>360</v>
       </c>
       <c r="D85" t="s">
-        <v>440</v>
+        <v>361</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>364</v>
+        <v>436</v>
       </c>
       <c r="C86" t="s">
-        <v>366</v>
+        <v>440</v>
       </c>
       <c r="D86" t="s">
-        <v>365</v>
+        <v>441</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>380</v>
-      </c>
-      <c r="B87" t="s">
-        <v>381</v>
+        <v>437</v>
       </c>
       <c r="C87" t="s">
-        <v>382</v>
+        <v>439</v>
       </c>
       <c r="D87" t="s">
-        <v>383</v>
+        <v>438</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>431</v>
+        <v>362</v>
       </c>
       <c r="C88" t="s">
-        <v>433</v>
+        <v>364</v>
       </c>
       <c r="D88" t="s">
-        <v>435</v>
+        <v>363</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>432</v>
+        <v>378</v>
+      </c>
+      <c r="B89" t="s">
+        <v>379</v>
       </c>
       <c r="C89" t="s">
-        <v>434</v>
+        <v>380</v>
       </c>
       <c r="D89" t="s">
-        <v>436</v>
+        <v>381</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>384</v>
-      </c>
-      <c r="B90" t="s">
-        <v>385</v>
+        <v>429</v>
       </c>
       <c r="C90" t="s">
-        <v>386</v>
+        <v>431</v>
       </c>
       <c r="D90" t="s">
-        <v>387</v>
+        <v>433</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
       <c r="C91" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
       <c r="D91" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>450</v>
+        <v>382</v>
+      </c>
+      <c r="B92" t="s">
+        <v>383</v>
       </c>
       <c r="C92" t="s">
-        <v>451</v>
+        <v>384</v>
       </c>
       <c r="D92" t="s">
-        <v>452</v>
+        <v>385</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>367</v>
+        <v>447</v>
       </c>
       <c r="C93" t="s">
-        <v>396</v>
+        <v>421</v>
       </c>
       <c r="D93" t="s">
-        <v>368</v>
+        <v>422</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>388</v>
+        <v>448</v>
       </c>
       <c r="C94" t="s">
-        <v>389</v>
+        <v>449</v>
       </c>
       <c r="D94" t="s">
-        <v>389</v>
+        <v>450</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>390</v>
+        <v>365</v>
       </c>
       <c r="C95" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="D95" t="s">
-        <v>392</v>
+        <v>366</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="C96" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="D96" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="C97" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="D97" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="C98" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="D98" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="C99" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="D99" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>425</v>
+        <v>398</v>
       </c>
       <c r="C100" t="s">
-        <v>430</v>
+        <v>399</v>
       </c>
       <c r="D100" t="s">
-        <v>429</v>
+        <v>400</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="C101" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
       <c r="D101" t="s">
-        <v>447</v>
+        <v>403</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C102" t="s">
+        <v>428</v>
+      </c>
+      <c r="D102" t="s">
         <v>427</v>
-      </c>
-      <c r="D102" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C103" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="D103" t="s">
-        <v>414</v>
+        <v>445</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>411</v>
+        <v>424</v>
       </c>
       <c r="C104" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
       <c r="D104" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="C105" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="D105" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C106" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D106" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>535</v>
-      </c>
-      <c r="C107" s="11" t="s">
-        <v>536</v>
+        <v>418</v>
+      </c>
+      <c r="C107" t="s">
+        <v>419</v>
       </c>
       <c r="D107" t="s">
-        <v>537</v>
+        <v>420</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>453</v>
+        <v>410</v>
       </c>
       <c r="C108" t="s">
-        <v>454</v>
+        <v>416</v>
       </c>
       <c r="D108" t="s">
-        <v>455</v>
+        <v>417</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>456</v>
-      </c>
-      <c r="C109" t="s">
-        <v>511</v>
+        <v>533</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>534</v>
       </c>
       <c r="D109" t="s">
-        <v>509</v>
+        <v>535</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="C110" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="D110" t="s">
-        <v>510</v>
+        <v>453</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>541</v>
+        <v>454</v>
       </c>
       <c r="C111" t="s">
-        <v>462</v>
+        <v>509</v>
       </c>
       <c r="D111" t="s">
-        <v>463</v>
+        <v>507</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>559</v>
+        <v>456</v>
       </c>
       <c r="C112" t="s">
-        <v>557</v>
+        <v>455</v>
       </c>
       <c r="D112" t="s">
-        <v>558</v>
+        <v>508</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>464</v>
+        <v>539</v>
       </c>
       <c r="C113" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D113" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>503</v>
+        <v>557</v>
       </c>
       <c r="C114" t="s">
-        <v>505</v>
+        <v>555</v>
       </c>
       <c r="D114" t="s">
-        <v>507</v>
+        <v>556</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>504</v>
+        <v>462</v>
       </c>
       <c r="C115" t="s">
-        <v>506</v>
+        <v>463</v>
       </c>
       <c r="D115" t="s">
-        <v>508</v>
+        <v>464</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="C116" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="D116" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>545</v>
+        <v>502</v>
       </c>
       <c r="C117" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="D117" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="C118" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="D118" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>520</v>
+        <v>543</v>
       </c>
       <c r="C119" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
       <c r="D119" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="C120" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="D120" t="s">
-        <v>552</v>
+        <v>517</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>538</v>
-      </c>
-      <c r="C121" s="11" t="s">
-        <v>539</v>
+        <v>518</v>
+      </c>
+      <c r="C121" t="s">
+        <v>520</v>
       </c>
       <c r="D121" t="s">
-        <v>540</v>
+        <v>521</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>542</v>
-      </c>
-      <c r="C122" s="11" t="s">
-        <v>543</v>
+        <v>519</v>
+      </c>
+      <c r="C122" t="s">
+        <v>522</v>
       </c>
       <c r="D122" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="D123" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="D124" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>524</v>
+        <v>545</v>
       </c>
       <c r="D125" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="D126" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>568</v>
+        <v>522</v>
       </c>
       <c r="D127" t="s">
-        <v>569</v>
+        <v>550</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>570</v>
+        <v>554</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>574</v>
+        <v>551</v>
       </c>
       <c r="D128" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="D129" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>581</v>
+        <v>572</v>
       </c>
       <c r="D130" t="s">
-        <v>580</v>
+        <v>570</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="D131" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D132" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>574</v>
+      </c>
+      <c r="C133" s="11" t="s">
+        <v>576</v>
+      </c>
+      <c r="D133" t="s">
         <v>577</v>
-      </c>
-      <c r="C133" s="11" t="s">
-        <v>601</v>
-      </c>
-      <c r="D133" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="D134" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>588</v>
+        <v>599</v>
       </c>
       <c r="D135" t="s">
-        <v>590</v>
+        <v>600</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>597</v>
+        <v>583</v>
       </c>
       <c r="C136" s="11" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="D136" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>598</v>
+        <v>584</v>
       </c>
       <c r="C137" s="11" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
       <c r="D137" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>592</v>
-      </c>
-      <c r="D138" s="11" t="s">
+        <v>589</v>
+      </c>
+      <c r="D138" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="C139" s="11" t="s">
         <v>593</v>
       </c>
-      <c r="D139" s="11" t="s">
-        <v>593</v>
+      <c r="D139" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>604</v>
+        <v>590</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>605</v>
+        <v>590</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>610</v>
+        <v>598</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>613</v>
+        <v>591</v>
       </c>
       <c r="D141" s="11" t="s">
-        <v>614</v>
+        <v>591</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>601</v>
+      </c>
+      <c r="C142" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="D142" s="11" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>608</v>
+      </c>
+      <c r="C143" s="11" t="s">
         <v>611</v>
       </c>
-      <c r="C142" s="11" t="s">
+      <c r="D143" s="11" t="s">
         <v>612</v>
       </c>
-      <c r="D142" s="11" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B143" s="4"/>
-      <c r="C143" s="4"/>
-      <c r="D143" s="4"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>148</v>
-      </c>
-      <c r="B144" t="s">
-        <v>45</v>
-      </c>
-      <c r="C144" t="s">
-        <v>149</v>
-      </c>
-      <c r="D144" t="s">
-        <v>150</v>
+        <v>609</v>
+      </c>
+      <c r="C144" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="D144" s="11" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>154</v>
-      </c>
-      <c r="B145" t="s">
-        <v>151</v>
-      </c>
-      <c r="C145" t="s">
-        <v>152</v>
-      </c>
-      <c r="D145" t="s">
-        <v>153</v>
-      </c>
+      <c r="A145" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B145" s="4"/>
+      <c r="C145" s="4"/>
+      <c r="D145" s="4"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B146" t="s">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="C146" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="D146" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B147" t="s">
         <v>151</v>
       </c>
       <c r="C147" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D147" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B148" t="s">
         <v>158</v>
       </c>
       <c r="C148" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D148" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B149" t="s">
-        <v>162</v>
-      </c>
-      <c r="C149" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D149" s="9" t="s">
-        <v>164</v>
+        <v>151</v>
+      </c>
+      <c r="C149" t="s">
+        <v>155</v>
+      </c>
+      <c r="D149" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B150" t="s">
         <v>158</v>
       </c>
       <c r="C150" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D150" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B151" s="8"/>
-      <c r="C151" s="8"/>
-      <c r="D151" s="8"/>
+      <c r="A151" t="s">
+        <v>160</v>
+      </c>
+      <c r="B151" t="s">
+        <v>162</v>
+      </c>
+      <c r="C151" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D151" s="9" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>58</v>
+        <v>161</v>
       </c>
       <c r="B152" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="C152" t="s">
-        <v>59</v>
+        <v>163</v>
       </c>
       <c r="D152" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>106</v>
-      </c>
-      <c r="B153" t="s">
-        <v>8</v>
-      </c>
-      <c r="C153" t="s">
-        <v>107</v>
-      </c>
-      <c r="D153" t="s">
-        <v>108</v>
-      </c>
+      <c r="A153" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B153" s="8"/>
+      <c r="C153" s="8"/>
+      <c r="D153" s="8"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>619</v>
+        <v>58</v>
+      </c>
+      <c r="B154" t="s">
+        <v>8</v>
       </c>
       <c r="C154" t="s">
-        <v>620</v>
+        <v>59</v>
       </c>
       <c r="D154" t="s">
-        <v>621</v>
+        <v>60</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>622</v>
+        <v>106</v>
+      </c>
+      <c r="B155" t="s">
+        <v>8</v>
       </c>
       <c r="C155" t="s">
-        <v>623</v>
+        <v>107</v>
       </c>
       <c r="D155" t="s">
-        <v>624</v>
+        <v>108</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>654</v>
+        <v>617</v>
       </c>
       <c r="C156" t="s">
-        <v>656</v>
+        <v>618</v>
       </c>
       <c r="D156" t="s">
-        <v>657</v>
+        <v>619</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>655</v>
+        <v>620</v>
       </c>
       <c r="C157" t="s">
-        <v>659</v>
+        <v>621</v>
       </c>
       <c r="D157" t="s">
-        <v>658</v>
+        <v>622</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>61</v>
-      </c>
-      <c r="B158" t="s">
-        <v>8</v>
+        <v>652</v>
       </c>
       <c r="C158" t="s">
-        <v>62</v>
+        <v>654</v>
       </c>
       <c r="D158" t="s">
-        <v>63</v>
+        <v>655</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>64</v>
-      </c>
-      <c r="B159" t="s">
-        <v>8</v>
+        <v>653</v>
       </c>
       <c r="C159" t="s">
-        <v>65</v>
+        <v>657</v>
       </c>
       <c r="D159" t="s">
-        <v>241</v>
+        <v>656</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>236</v>
+        <v>61</v>
       </c>
       <c r="B160" t="s">
         <v>8</v>
       </c>
       <c r="C160" t="s">
-        <v>237</v>
+        <v>62</v>
       </c>
       <c r="D160" t="s">
-        <v>237</v>
+        <v>63</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>370</v>
+        <v>64</v>
       </c>
       <c r="B161" t="s">
         <v>8</v>
       </c>
       <c r="C161" t="s">
-        <v>636</v>
+        <v>65</v>
       </c>
       <c r="D161" t="s">
-        <v>638</v>
+        <v>241</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>637</v>
+        <v>236</v>
+      </c>
+      <c r="B162" t="s">
+        <v>8</v>
       </c>
       <c r="C162" t="s">
-        <v>635</v>
+        <v>237</v>
       </c>
       <c r="D162" t="s">
-        <v>639</v>
+        <v>237</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>174</v>
+        <v>368</v>
       </c>
       <c r="B163" t="s">
         <v>8</v>
       </c>
       <c r="C163" t="s">
-        <v>616</v>
+        <v>634</v>
       </c>
       <c r="D163" t="s">
-        <v>175</v>
+        <v>636</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>184</v>
-      </c>
-      <c r="B164" t="s">
-        <v>8</v>
+        <v>635</v>
       </c>
       <c r="C164" t="s">
-        <v>617</v>
+        <v>633</v>
       </c>
       <c r="D164" t="s">
-        <v>185</v>
+        <v>637</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B165" t="s">
         <v>8</v>
       </c>
       <c r="C165" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="D165" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>625</v>
+        <v>184</v>
       </c>
       <c r="B166" t="s">
         <v>8</v>
       </c>
       <c r="C166" t="s">
-        <v>626</v>
+        <v>615</v>
       </c>
       <c r="D166" t="s">
-        <v>627</v>
+        <v>185</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>632</v>
+        <v>192</v>
       </c>
       <c r="B167" t="s">
         <v>8</v>
       </c>
       <c r="C167" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="D167" t="s">
-        <v>628</v>
+        <v>193</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
       <c r="B168" t="s">
         <v>8</v>
       </c>
       <c r="C168" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="D168" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>173</v>
+        <v>630</v>
       </c>
       <c r="B169" t="s">
         <v>8</v>
       </c>
       <c r="C169" t="s">
-        <v>209</v>
+        <v>628</v>
       </c>
       <c r="D169" t="s">
-        <v>210</v>
+        <v>626</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>66</v>
+        <v>631</v>
       </c>
       <c r="B170" t="s">
         <v>8</v>
       </c>
       <c r="C170" t="s">
-        <v>67</v>
+        <v>629</v>
       </c>
       <c r="D170" t="s">
-        <v>68</v>
+        <v>627</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B171" t="s">
         <v>8</v>
       </c>
       <c r="C171" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="D171" t="s">
-        <v>16</v>
+        <v>210</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>186</v>
+        <v>66</v>
       </c>
       <c r="B172" t="s">
         <v>8</v>
       </c>
       <c r="C172" t="s">
-        <v>187</v>
+        <v>67</v>
       </c>
       <c r="D172" t="s">
-        <v>188</v>
+        <v>68</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>69</v>
+        <v>181</v>
       </c>
       <c r="B173" t="s">
         <v>8</v>
       </c>
       <c r="C173" t="s">
-        <v>70</v>
+        <v>176</v>
       </c>
       <c r="D173" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B174" t="s">
         <v>8</v>
       </c>
       <c r="C174" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D174" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>189</v>
+        <v>69</v>
       </c>
       <c r="B175" t="s">
         <v>8</v>
       </c>
       <c r="C175" t="s">
-        <v>190</v>
+        <v>70</v>
       </c>
       <c r="D175" t="s">
-        <v>191</v>
+        <v>71</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>72</v>
+        <v>180</v>
       </c>
       <c r="B176" t="s">
         <v>8</v>
       </c>
       <c r="C176" t="s">
-        <v>73</v>
+        <v>182</v>
       </c>
       <c r="D176" t="s">
-        <v>74</v>
+        <v>183</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="B177" t="s">
         <v>8</v>
       </c>
       <c r="C177" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D177" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>194</v>
+        <v>72</v>
       </c>
       <c r="B178" t="s">
         <v>8</v>
       </c>
       <c r="C178" t="s">
-        <v>195</v>
+        <v>73</v>
       </c>
       <c r="D178" t="s">
-        <v>196</v>
+        <v>74</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>213</v>
+        <v>179</v>
       </c>
       <c r="B179" t="s">
         <v>8</v>
       </c>
       <c r="C179" t="s">
-        <v>211</v>
+        <v>177</v>
       </c>
       <c r="D179" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="B180" t="s">
         <v>8</v>
       </c>
       <c r="C180" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="D180" t="s">
-        <v>118</v>
+        <v>196</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B181" t="s">
         <v>8</v>
       </c>
       <c r="C181" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D181" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>305</v>
+        <v>214</v>
+      </c>
+      <c r="B182" t="s">
+        <v>8</v>
       </c>
       <c r="C182" t="s">
-        <v>306</v>
+        <v>215</v>
       </c>
       <c r="D182" t="s">
-        <v>307</v>
+        <v>118</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>78</v>
+        <v>216</v>
       </c>
       <c r="B183" t="s">
         <v>8</v>
       </c>
       <c r="C183" t="s">
-        <v>79</v>
+        <v>217</v>
       </c>
       <c r="D183" t="s">
-        <v>80</v>
+        <v>218</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>7</v>
-      </c>
-      <c r="B184" t="s">
-        <v>8</v>
+        <v>303</v>
       </c>
       <c r="C184" t="s">
-        <v>9</v>
+        <v>304</v>
       </c>
       <c r="D184" t="s">
-        <v>10</v>
+        <v>305</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>459</v>
+        <v>78</v>
+      </c>
+      <c r="B185" t="s">
+        <v>8</v>
       </c>
       <c r="C185" t="s">
-        <v>460</v>
+        <v>79</v>
       </c>
       <c r="D185" t="s">
-        <v>461</v>
+        <v>80</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>219</v>
+        <v>7</v>
       </c>
       <c r="B186" t="s">
         <v>8</v>
       </c>
       <c r="C186" t="s">
-        <v>219</v>
+        <v>9</v>
       </c>
       <c r="D186" t="s">
-        <v>220</v>
+        <v>10</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>197</v>
-      </c>
-      <c r="B187" t="s">
-        <v>198</v>
+        <v>457</v>
       </c>
       <c r="C187" t="s">
-        <v>197</v>
+        <v>458</v>
       </c>
       <c r="D187" t="s">
-        <v>199</v>
+        <v>459</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B188" t="s">
         <v>8</v>
       </c>
       <c r="C188" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D188" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="B189" t="s">
         <v>198</v>
       </c>
       <c r="C189" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="D189" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>248</v>
+        <v>221</v>
       </c>
       <c r="B190" t="s">
         <v>8</v>
       </c>
       <c r="C190" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="D190" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="B191" t="s">
         <v>198</v>
       </c>
       <c r="C191" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="D191" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="B192" t="s">
         <v>8</v>
       </c>
       <c r="C192" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="D192" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="B193" t="s">
         <v>198</v>
       </c>
       <c r="C193" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="D193" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>119</v>
+        <v>230</v>
       </c>
       <c r="B194" t="s">
         <v>8</v>
       </c>
       <c r="C194" t="s">
-        <v>120</v>
+        <v>232</v>
       </c>
       <c r="D194" t="s">
-        <v>121</v>
+        <v>234</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B195" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="C195" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="D195" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="B196" t="s">
         <v>8</v>
       </c>
       <c r="C196" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="D196" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>406</v>
+        <v>227</v>
+      </c>
+      <c r="B197" t="s">
+        <v>8</v>
       </c>
       <c r="C197" t="s">
-        <v>407</v>
+        <v>228</v>
       </c>
       <c r="D197" t="s">
-        <v>408</v>
+        <v>229</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>525</v>
+        <v>14</v>
+      </c>
+      <c r="B198" t="s">
+        <v>8</v>
       </c>
       <c r="C198" t="s">
-        <v>526</v>
+        <v>15</v>
       </c>
       <c r="D198" t="s">
-        <v>527</v>
+        <v>16</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>448</v>
-      </c>
-      <c r="B199" t="s">
-        <v>337</v>
+        <v>404</v>
       </c>
       <c r="C199" t="s">
-        <v>338</v>
+        <v>405</v>
       </c>
       <c r="D199" t="s">
-        <v>339</v>
+        <v>406</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>467</v>
+        <v>523</v>
       </c>
       <c r="C200" t="s">
-        <v>479</v>
+        <v>524</v>
       </c>
       <c r="D200" t="s">
-        <v>491</v>
+        <v>525</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>468</v>
+        <v>446</v>
+      </c>
+      <c r="B201" t="s">
+        <v>335</v>
       </c>
       <c r="C201" t="s">
-        <v>480</v>
+        <v>336</v>
       </c>
       <c r="D201" t="s">
-        <v>492</v>
+        <v>337</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C202" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D202" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C203" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D203" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C204" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D204" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C205" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D205" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C206" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D206" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C207" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="D207" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C208" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D208" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C209" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D209" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C210" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D210" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C211" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="D211" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>530</v>
+        <v>475</v>
       </c>
       <c r="C212" t="s">
-        <v>529</v>
+        <v>487</v>
       </c>
       <c r="D212" t="s">
-        <v>528</v>
+        <v>499</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>606</v>
+        <v>476</v>
       </c>
       <c r="C213" t="s">
-        <v>2</v>
+        <v>488</v>
       </c>
       <c r="D213" t="s">
-        <v>607</v>
+        <v>500</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>608</v>
+        <v>528</v>
       </c>
       <c r="C214" t="s">
-        <v>609</v>
+        <v>527</v>
       </c>
       <c r="D214" t="s">
-        <v>3</v>
+        <v>526</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B215" s="2"/>
-      <c r="C215" s="2"/>
-      <c r="D215" s="2"/>
+      <c r="A215" t="s">
+        <v>604</v>
+      </c>
+      <c r="C215" t="s">
+        <v>2</v>
+      </c>
+      <c r="D215" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>123</v>
-      </c>
-      <c r="B216" t="s">
+        <v>606</v>
+      </c>
+      <c r="C216" t="s">
+        <v>607</v>
+      </c>
+      <c r="D216" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C216" t="s">
-        <v>142</v>
-      </c>
-      <c r="D216" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>140</v>
-      </c>
-      <c r="B217" t="s">
-        <v>122</v>
-      </c>
-      <c r="C217" t="s">
-        <v>143</v>
-      </c>
-      <c r="D217" t="s">
-        <v>146</v>
-      </c>
+      <c r="B217" s="2"/>
+      <c r="C217" s="2"/>
+      <c r="D217" s="2"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B218" t="s">
         <v>122</v>
       </c>
       <c r="C218" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="D218" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="B219" t="s">
         <v>122</v>
       </c>
       <c r="C219" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="D219" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B220" t="s">
         <v>122</v>
       </c>
       <c r="C220" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D220" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B221" t="s">
         <v>122</v>
       </c>
       <c r="C221" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="D221" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B222" t="s">
         <v>122</v>
       </c>
       <c r="C222" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="D222" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B223" t="s">
         <v>122</v>
       </c>
       <c r="C223" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D223" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B224" s="4"/>
-      <c r="C224" s="4"/>
-      <c r="D224" s="4"/>
+      <c r="A224" t="s">
+        <v>135</v>
+      </c>
+      <c r="B224" t="s">
+        <v>122</v>
+      </c>
+      <c r="C224" t="s">
+        <v>144</v>
+      </c>
+      <c r="D224" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="B225" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="C225" t="s">
-        <v>373</v>
+        <v>138</v>
       </c>
       <c r="D225" t="s">
-        <v>374</v>
+        <v>139</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
-        <v>371</v>
-      </c>
-      <c r="B226" t="s">
-        <v>82</v>
-      </c>
-      <c r="C226" t="s">
-        <v>369</v>
-      </c>
-      <c r="D226" t="s">
-        <v>372</v>
-      </c>
+      <c r="A226" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B226" s="4"/>
+      <c r="C226" s="4"/>
+      <c r="D226" s="4"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>172</v>
+        <v>81</v>
       </c>
       <c r="B227" t="s">
         <v>82</v>
       </c>
       <c r="C227" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D227" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="B228" t="s">
         <v>82</v>
       </c>
       <c r="C228" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="D228" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
       <c r="B229" t="s">
         <v>82</v>
       </c>
       <c r="C229" t="s">
-        <v>84</v>
+        <v>373</v>
       </c>
       <c r="D229" t="s">
-        <v>85</v>
+        <v>374</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>640</v>
+        <v>375</v>
+      </c>
+      <c r="B230" t="s">
+        <v>82</v>
       </c>
       <c r="C230" t="s">
-        <v>634</v>
+        <v>376</v>
       </c>
       <c r="D230" t="s">
-        <v>641</v>
+        <v>377</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
+        <v>83</v>
+      </c>
+      <c r="B231" t="s">
+        <v>82</v>
+      </c>
+      <c r="C231" t="s">
+        <v>84</v>
+      </c>
+      <c r="D231" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>638</v>
+      </c>
+      <c r="C232" t="s">
+        <v>632</v>
+      </c>
+      <c r="D232" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>649</v>
+      </c>
+      <c r="C233" t="s">
+        <v>650</v>
+      </c>
+      <c r="D233" t="s">
         <v>651</v>
-      </c>
-      <c r="C231" t="s">
-        <v>652</v>
-      </c>
-      <c r="D231" t="s">
-        <v>653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start converting map menus to page_sidebars
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F2FF23-B2FA-4EF2-B637-D40384150000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F759C1C4-4F55-4D1E-814B-FC7BF80FE923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1220,9 +1220,6 @@
     <t>Modifier paramètre secondaire</t>
   </si>
   <si>
-    <t>Add scondary parameter</t>
-  </si>
-  <si>
     <t>Edit secondary parameter</t>
   </si>
   <si>
@@ -2399,6 +2396,9 @@
   </si>
   <si>
     <t>maps_params</t>
+  </si>
+  <si>
+    <t>Add secondary parameter</t>
   </si>
 </sst>
 </file>
@@ -3345,8 +3345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3377,7 +3377,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -3391,18 +3391,18 @@
         <v>137</v>
       </c>
       <c r="B3" t="s">
+        <v>510</v>
+      </c>
+      <c r="C3" t="s">
+        <v>512</v>
+      </c>
+      <c r="D3" t="s">
         <v>511</v>
-      </c>
-      <c r="C3" t="s">
-        <v>513</v>
-      </c>
-      <c r="D3" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3413,7 +3413,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -3424,178 +3424,178 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B6" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C6" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D6" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B7" t="s">
+        <v>771</v>
+      </c>
+      <c r="C7" t="s">
         <v>772</v>
       </c>
-      <c r="C7" t="s">
-        <v>773</v>
-      </c>
       <c r="D7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B8" t="s">
+        <v>774</v>
+      </c>
+      <c r="C8" t="s">
         <v>775</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>776</v>
-      </c>
-      <c r="D8" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>714</v>
+      </c>
+      <c r="B9" t="s">
+        <v>752</v>
+      </c>
+      <c r="C9" t="s">
         <v>715</v>
       </c>
-      <c r="B9" t="s">
-        <v>753</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>716</v>
-      </c>
-      <c r="D9" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B10" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C10" t="s">
+        <v>720</v>
+      </c>
+      <c r="D10" t="s">
         <v>721</v>
-      </c>
-      <c r="D10" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>722</v>
+      </c>
+      <c r="B11" t="s">
+        <v>751</v>
+      </c>
+      <c r="C11" t="s">
         <v>723</v>
       </c>
-      <c r="B11" t="s">
-        <v>752</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>724</v>
-      </c>
-      <c r="D11" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>725</v>
+      </c>
+      <c r="B12" t="s">
+        <v>749</v>
+      </c>
+      <c r="C12" t="s">
         <v>726</v>
       </c>
-      <c r="B12" t="s">
-        <v>750</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>727</v>
-      </c>
-      <c r="D12" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>730</v>
+      </c>
+      <c r="B13" t="s">
+        <v>750</v>
+      </c>
+      <c r="C13" t="s">
         <v>731</v>
       </c>
-      <c r="B13" t="s">
-        <v>751</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>732</v>
-      </c>
-      <c r="D13" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B14" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C14" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D14" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B15" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C15" t="s">
+        <v>739</v>
+      </c>
+      <c r="D15" t="s">
         <v>740</v>
-      </c>
-      <c r="D15" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B16" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C16" t="s">
+        <v>741</v>
+      </c>
+      <c r="D16" t="s">
         <v>742</v>
-      </c>
-      <c r="D16" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B17" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C17" t="s">
+        <v>743</v>
+      </c>
+      <c r="D17" t="s">
         <v>744</v>
-      </c>
-      <c r="D17" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B18" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C18" t="s">
         <v>44</v>
@@ -3606,38 +3606,38 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B19" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C19" t="s">
+        <v>720</v>
+      </c>
+      <c r="D19" t="s">
         <v>721</v>
-      </c>
-      <c r="D19" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B20" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C20" t="s">
+        <v>723</v>
+      </c>
+      <c r="D20" t="s">
         <v>724</v>
-      </c>
-      <c r="D20" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B21" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C21" t="s">
         <v>46</v>
@@ -3648,52 +3648,52 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B22" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C22" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D22" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B23" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C23" t="s">
+        <v>762</v>
+      </c>
+      <c r="D23" t="s">
         <v>763</v>
-      </c>
-      <c r="D23" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>710</v>
+      </c>
+      <c r="B24" t="s">
+        <v>768</v>
+      </c>
+      <c r="C24" t="s">
         <v>711</v>
       </c>
-      <c r="B24" t="s">
-        <v>769</v>
-      </c>
-      <c r="C24" t="s">
-        <v>712</v>
-      </c>
       <c r="D24" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B25" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C25" t="s">
         <v>135</v>
@@ -3704,21 +3704,21 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B26" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C26" t="s">
+        <v>712</v>
+      </c>
+      <c r="D26" t="s">
         <v>713</v>
-      </c>
-      <c r="D26" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -3726,30 +3726,30 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>665</v>
+      </c>
+      <c r="B28" t="s">
         <v>666</v>
       </c>
-      <c r="B28" t="s">
-        <v>667</v>
-      </c>
       <c r="C28" t="s">
+        <v>668</v>
+      </c>
+      <c r="D28" t="s">
         <v>669</v>
-      </c>
-      <c r="D28" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B29" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C29" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3760,10 +3760,10 @@
         <v>18</v>
       </c>
       <c r="C30" t="s">
+        <v>538</v>
+      </c>
+      <c r="D30" t="s">
         <v>539</v>
-      </c>
-      <c r="D30" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3852,10 +3852,10 @@
         <v>293</v>
       </c>
       <c r="C37" t="s">
+        <v>540</v>
+      </c>
+      <c r="D37" t="s">
         <v>541</v>
-      </c>
-      <c r="D37" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3944,16 +3944,16 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B44" t="s">
         <v>309</v>
       </c>
       <c r="C44" t="s">
+        <v>543</v>
+      </c>
+      <c r="D44" t="s">
         <v>544</v>
-      </c>
-      <c r="D44" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4072,13 +4072,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>654</v>
+      </c>
+      <c r="C54" t="s">
         <v>655</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>656</v>
-      </c>
-      <c r="D54" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4139,7 +4139,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B59" t="s">
         <v>251</v>
@@ -4153,16 +4153,16 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B60" t="s">
         <v>251</v>
       </c>
       <c r="C60" t="s">
+        <v>652</v>
+      </c>
+      <c r="D60" t="s">
         <v>653</v>
-      </c>
-      <c r="D60" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4173,10 +4173,10 @@
         <v>251</v>
       </c>
       <c r="C61" t="s">
+        <v>678</v>
+      </c>
+      <c r="D61" t="s">
         <v>679</v>
-      </c>
-      <c r="D61" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4301,52 +4301,52 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>620</v>
+      </c>
+      <c r="C71" t="s">
         <v>621</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>622</v>
-      </c>
-      <c r="D71" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>638</v>
+      </c>
+      <c r="C72" t="s">
         <v>639</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>640</v>
-      </c>
-      <c r="D72" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>623</v>
+      </c>
+      <c r="B73" t="s">
+        <v>663</v>
+      </c>
+      <c r="C73" t="s">
         <v>624</v>
       </c>
-      <c r="B73" t="s">
-        <v>664</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>625</v>
-      </c>
-      <c r="D73" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>626</v>
+      </c>
+      <c r="B74" t="s">
+        <v>663</v>
+      </c>
+      <c r="C74" t="s">
         <v>627</v>
       </c>
-      <c r="B74" t="s">
-        <v>664</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>628</v>
-      </c>
-      <c r="D74" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -4421,91 +4421,91 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>703</v>
+      </c>
+      <c r="C80" t="s">
         <v>704</v>
       </c>
-      <c r="C80" t="s">
-        <v>705</v>
-      </c>
       <c r="D80" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>675</v>
+      </c>
+      <c r="C81" t="s">
         <v>676</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>677</v>
-      </c>
-      <c r="D81" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>672</v>
+      </c>
+      <c r="C82" t="s">
         <v>673</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>674</v>
-      </c>
-      <c r="D82" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>657</v>
+      </c>
+      <c r="B83" t="s">
+        <v>662</v>
+      </c>
+      <c r="C83" t="s">
+        <v>659</v>
+      </c>
+      <c r="D83" t="s">
         <v>658</v>
-      </c>
-      <c r="B83" t="s">
-        <v>663</v>
-      </c>
-      <c r="C83" t="s">
-        <v>660</v>
-      </c>
-      <c r="D83" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B84" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C84" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D84" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B85" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C85" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D85" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B86" t="s">
         <v>232</v>
       </c>
       <c r="C86" t="s">
+        <v>642</v>
+      </c>
+      <c r="D86" t="s">
         <v>643</v>
-      </c>
-      <c r="D86" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4666,13 +4666,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>422</v>
+      </c>
+      <c r="C99" t="s">
         <v>423</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>424</v>
-      </c>
-      <c r="D99" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4688,7 +4688,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C101" t="s">
         <v>341</v>
@@ -4699,24 +4699,24 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C102" t="s">
+        <v>420</v>
+      </c>
+      <c r="D102" t="s">
         <v>421</v>
-      </c>
-      <c r="D102" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>417</v>
+      </c>
+      <c r="C103" t="s">
+        <v>419</v>
+      </c>
+      <c r="D103" t="s">
         <v>418</v>
-      </c>
-      <c r="C103" t="s">
-        <v>420</v>
-      </c>
-      <c r="D103" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4746,24 +4746,24 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C106" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D106" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C107" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D107" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4782,24 +4782,24 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C109" t="s">
+        <v>401</v>
+      </c>
+      <c r="D109" t="s">
         <v>402</v>
-      </c>
-      <c r="D109" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>428</v>
+      </c>
+      <c r="C110" t="s">
         <v>429</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
         <v>430</v>
-      </c>
-      <c r="D110" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4881,13 +4881,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C118" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D118" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -4898,18 +4898,18 @@
         <v>392</v>
       </c>
       <c r="D119" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>404</v>
+      </c>
+      <c r="C120" t="s">
         <v>405</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D120" t="s">
         <v>406</v>
-      </c>
-      <c r="D120" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -4917,7 +4917,7 @@
         <v>389</v>
       </c>
       <c r="C121" t="s">
-        <v>395</v>
+        <v>780</v>
       </c>
       <c r="D121" t="s">
         <v>393</v>
@@ -4928,7 +4928,7 @@
         <v>390</v>
       </c>
       <c r="C122" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D122" t="s">
         <v>394</v>
@@ -4936,13 +4936,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>398</v>
+      </c>
+      <c r="C123" t="s">
         <v>399</v>
       </c>
-      <c r="C123" t="s">
+      <c r="D123" t="s">
         <v>400</v>
-      </c>
-      <c r="D123" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -4950,406 +4950,406 @@
         <v>391</v>
       </c>
       <c r="C124" t="s">
+        <v>396</v>
+      </c>
+      <c r="D124" t="s">
         <v>397</v>
-      </c>
-      <c r="D124" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>513</v>
+      </c>
+      <c r="C125" s="9" t="s">
         <v>514</v>
       </c>
-      <c r="C125" s="9" t="s">
+      <c r="D125" t="s">
         <v>515</v>
-      </c>
-      <c r="D125" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
+        <v>431</v>
+      </c>
+      <c r="C126" t="s">
         <v>432</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
         <v>433</v>
-      </c>
-      <c r="D126" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C127" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D127" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C128" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D128" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C129" t="s">
+        <v>440</v>
+      </c>
+      <c r="D129" t="s">
         <v>441</v>
-      </c>
-      <c r="D129" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C130" t="s">
+        <v>535</v>
+      </c>
+      <c r="D130" t="s">
         <v>536</v>
-      </c>
-      <c r="D130" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>442</v>
+      </c>
+      <c r="C131" t="s">
         <v>443</v>
       </c>
-      <c r="C131" t="s">
+      <c r="D131" t="s">
         <v>444</v>
-      </c>
-      <c r="D131" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C132" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D132" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C133" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D133" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>490</v>
+      </c>
+      <c r="C134" t="s">
         <v>491</v>
       </c>
-      <c r="C134" t="s">
+      <c r="D134" t="s">
         <v>492</v>
-      </c>
-      <c r="D134" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C135" t="s">
+        <v>493</v>
+      </c>
+      <c r="D135" t="s">
         <v>494</v>
-      </c>
-      <c r="D135" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>495</v>
+      </c>
+      <c r="C136" t="s">
         <v>496</v>
       </c>
-      <c r="C136" t="s">
+      <c r="D136" t="s">
         <v>497</v>
-      </c>
-      <c r="D136" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C137" t="s">
+        <v>500</v>
+      </c>
+      <c r="D137" t="s">
         <v>501</v>
-      </c>
-      <c r="D137" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C138" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D138" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>516</v>
+      </c>
+      <c r="C139" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="C139" s="9" t="s">
+      <c r="D139" t="s">
         <v>518</v>
-      </c>
-      <c r="D139" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
+        <v>520</v>
+      </c>
+      <c r="C140" s="9" t="s">
         <v>521</v>
       </c>
-      <c r="C140" s="9" t="s">
+      <c r="D140" t="s">
         <v>522</v>
-      </c>
-      <c r="D140" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>524</v>
+      </c>
+      <c r="C141" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="C141" s="9" t="s">
+      <c r="D141" t="s">
         <v>526</v>
-      </c>
-      <c r="D141" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>527</v>
+      </c>
+      <c r="C142" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="D142" t="s">
         <v>528</v>
-      </c>
-      <c r="C142" s="9" t="s">
-        <v>530</v>
-      </c>
-      <c r="D142" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D143" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C144" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="D144" t="s">
         <v>532</v>
-      </c>
-      <c r="D144" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>545</v>
+      </c>
+      <c r="C145" s="9" t="s">
         <v>546</v>
       </c>
-      <c r="C145" s="9" t="s">
+      <c r="D145" t="s">
         <v>547</v>
-      </c>
-      <c r="D145" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D146" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D147" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D148" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C149" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="D149" t="s">
         <v>557</v>
-      </c>
-      <c r="D149" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>560</v>
+      </c>
+      <c r="C150" s="9" t="s">
         <v>561</v>
       </c>
-      <c r="C150" s="9" t="s">
+      <c r="D150" t="s">
         <v>562</v>
-      </c>
-      <c r="D150" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C151" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="D151" t="s">
         <v>580</v>
-      </c>
-      <c r="D151" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D152" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D153" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D154" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C155" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="D155" t="s">
         <v>574</v>
-      </c>
-      <c r="D155" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D156" s="9" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D157" s="9" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>581</v>
+      </c>
+      <c r="C158" s="9" t="s">
         <v>582</v>
       </c>
-      <c r="C158" s="9" t="s">
+      <c r="D158" s="9" t="s">
         <v>583</v>
-      </c>
-      <c r="D158" s="9" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C159" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="D159" s="9" t="s">
         <v>592</v>
-      </c>
-      <c r="D159" s="9" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>589</v>
+      </c>
+      <c r="C160" s="9" t="s">
         <v>590</v>
       </c>
-      <c r="C160" s="9" t="s">
-        <v>591</v>
-      </c>
       <c r="D160" s="9" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -5362,46 +5362,46 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
+        <v>694</v>
+      </c>
+      <c r="C162" t="s">
         <v>695</v>
       </c>
-      <c r="C162" t="s">
+      <c r="D162" t="s">
         <v>696</v>
-      </c>
-      <c r="D162" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C163" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D163" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C164" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D164" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C165" s="7" t="s">
+        <v>691</v>
+      </c>
+      <c r="D165" s="7" t="s">
         <v>692</v>
-      </c>
-      <c r="D165" s="7" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -5440,10 +5440,10 @@
         <v>137</v>
       </c>
       <c r="C168" t="s">
+        <v>683</v>
+      </c>
+      <c r="D168" t="s">
         <v>684</v>
-      </c>
-      <c r="D168" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -5476,35 +5476,35 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C171" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D171" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C172" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D172" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>687</v>
+      </c>
+      <c r="C173" t="s">
         <v>688</v>
       </c>
-      <c r="C173" t="s">
+      <c r="D173" t="s">
         <v>689</v>
-      </c>
-      <c r="D173" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -5545,46 +5545,46 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>597</v>
+      </c>
+      <c r="C177" t="s">
         <v>598</v>
       </c>
-      <c r="C177" t="s">
+      <c r="D177" t="s">
         <v>599</v>
-      </c>
-      <c r="D177" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>600</v>
+      </c>
+      <c r="C178" t="s">
         <v>601</v>
       </c>
-      <c r="C178" t="s">
+      <c r="D178" t="s">
         <v>602</v>
-      </c>
-      <c r="D178" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C179" t="s">
+        <v>634</v>
+      </c>
+      <c r="D179" t="s">
         <v>635</v>
-      </c>
-      <c r="D179" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C180" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D180" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -5637,21 +5637,21 @@
         <v>8</v>
       </c>
       <c r="C184" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D184" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C185" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D185" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -5662,7 +5662,7 @@
         <v>8</v>
       </c>
       <c r="C186" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D186" t="s">
         <v>156</v>
@@ -5676,7 +5676,7 @@
         <v>8</v>
       </c>
       <c r="C187" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D187" t="s">
         <v>166</v>
@@ -5690,7 +5690,7 @@
         <v>8</v>
       </c>
       <c r="C188" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D188" t="s">
         <v>174</v>
@@ -5698,44 +5698,44 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B189" t="s">
         <v>8</v>
       </c>
       <c r="C189" t="s">
+        <v>604</v>
+      </c>
+      <c r="D189" t="s">
         <v>605</v>
-      </c>
-      <c r="D189" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B190" t="s">
         <v>8</v>
       </c>
       <c r="C190" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D190" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B191" t="s">
         <v>8</v>
       </c>
       <c r="C191" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D191" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -5961,13 +5961,13 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>437</v>
+      </c>
+      <c r="C208" t="s">
         <v>438</v>
       </c>
-      <c r="C208" t="s">
+      <c r="D208" t="s">
         <v>439</v>
-      </c>
-      <c r="D208" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -6137,18 +6137,18 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
+        <v>503</v>
+      </c>
+      <c r="C221" t="s">
         <v>504</v>
       </c>
-      <c r="C221" t="s">
+      <c r="D221" t="s">
         <v>505</v>
-      </c>
-      <c r="D221" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B222" t="s">
         <v>316</v>
@@ -6162,164 +6162,164 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C223" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D223" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C224" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D224" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C225" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D225" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C226" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D226" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C227" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D227" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C228" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D228" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C229" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D229" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C230" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D230" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C231" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D231" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C232" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D232" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C233" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D233" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C234" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D234" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C235" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D235" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C236" t="s">
         <v>2</v>
       </c>
       <c r="D236" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
+        <v>586</v>
+      </c>
+      <c r="C237" t="s">
         <v>587</v>
-      </c>
-      <c r="C237" t="s">
-        <v>588</v>
       </c>
       <c r="D237" t="s">
         <v>3</v>
@@ -6525,24 +6525,24 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
+        <v>618</v>
+      </c>
+      <c r="C253" t="s">
+        <v>612</v>
+      </c>
+      <c r="D253" t="s">
         <v>619</v>
-      </c>
-      <c r="C253" t="s">
-        <v>613</v>
-      </c>
-      <c r="D253" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
+        <v>629</v>
+      </c>
+      <c r="C254" t="s">
         <v>630</v>
       </c>
-      <c r="C254" t="s">
+      <c r="D254" t="s">
         <v>631</v>
-      </c>
-      <c r="D254" t="s">
-        <v>632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simplify discreteData module in preparation for continuousData module.
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16A3641-DDD0-4E02-A8EC-317B3A38B3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D387527E-260B-403F-89BF-CAC3FB372E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="794">
   <si>
     <t>id</t>
   </si>
@@ -2399,6 +2399,45 @@
   </si>
   <si>
     <t>Emplacements de surveillance</t>
+  </si>
+  <si>
+    <t>no_samps_locs</t>
+  </si>
+  <si>
+    <t>notification of automatic reset</t>
+  </si>
+  <si>
+    <t>This selection results in 0 corresponding measurements, location selector reset to its previous value.</t>
+  </si>
+  <si>
+    <t>Cette sélection ne correspond à aucune mesure, la sélection pour l'endroit a été réinitialisé à sa valeur précédente.</t>
+  </si>
+  <si>
+    <t>no_samps_sub_locs</t>
+  </si>
+  <si>
+    <t>This selection results in 0 corresponding measurements, sub-location selector reset to its previous value.</t>
+  </si>
+  <si>
+    <t>This selection results in 0 corresponding measurements, media type selector reset to its previous value.</t>
+  </si>
+  <si>
+    <t>Cette sélection ne correspond à aucune mesure, la sélection  de sous-endroit a été réinitialisé à sa valeur précédente.</t>
+  </si>
+  <si>
+    <t>Cette sélection ne correspond à aucune mesure, la sélection de type de média a été réinitialisé à sa valeur précédente.</t>
+  </si>
+  <si>
+    <t>no_samps_medias</t>
+  </si>
+  <si>
+    <t>no_samps_types</t>
+  </si>
+  <si>
+    <t>This selection results in 0 corresponding measurements, sample type selector reset to its previous value.</t>
+  </si>
+  <si>
+    <t>Cette sélection ne correspond à aucune mesure, la sélection de type d'échantillon a été réinitialisé à sa valeur précédente.</t>
   </si>
 </sst>
 </file>
@@ -3343,17 +3382,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D254"/>
+  <dimension ref="A1:D258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:XFD75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="3" max="3" width="79" customWidth="1"/>
     <col min="4" max="4" width="49.85546875" customWidth="1"/>
     <col min="5" max="5" width="54.42578125" customWidth="1"/>
   </cols>
@@ -4292,2264 +4331,2320 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
+      <c r="A70" t="s">
+        <v>781</v>
+      </c>
+      <c r="B70" t="s">
+        <v>782</v>
+      </c>
+      <c r="C70" t="s">
+        <v>783</v>
+      </c>
+      <c r="D70" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>620</v>
+        <v>785</v>
+      </c>
+      <c r="B71" t="s">
+        <v>782</v>
       </c>
       <c r="C71" t="s">
-        <v>621</v>
+        <v>786</v>
       </c>
       <c r="D71" t="s">
-        <v>622</v>
+        <v>788</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>638</v>
+        <v>790</v>
+      </c>
+      <c r="B72" t="s">
+        <v>782</v>
       </c>
       <c r="C72" t="s">
-        <v>639</v>
+        <v>787</v>
       </c>
       <c r="D72" t="s">
-        <v>640</v>
+        <v>789</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>623</v>
+        <v>791</v>
       </c>
       <c r="B73" t="s">
-        <v>663</v>
+        <v>782</v>
       </c>
       <c r="C73" t="s">
-        <v>624</v>
+        <v>792</v>
       </c>
       <c r="D73" t="s">
-        <v>625</v>
+        <v>793</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>626</v>
-      </c>
-      <c r="B74" t="s">
-        <v>663</v>
-      </c>
-      <c r="C74" t="s">
-        <v>627</v>
-      </c>
-      <c r="D74" t="s">
-        <v>628</v>
-      </c>
+      <c r="A74" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>183</v>
-      </c>
-      <c r="B75" t="s">
-        <v>184</v>
+        <v>620</v>
       </c>
       <c r="C75" t="s">
-        <v>78</v>
+        <v>621</v>
       </c>
       <c r="D75" t="s">
-        <v>79</v>
+        <v>622</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>64</v>
-      </c>
-      <c r="B76" t="s">
-        <v>186</v>
+        <v>638</v>
       </c>
       <c r="C76" t="s">
-        <v>65</v>
+        <v>639</v>
       </c>
       <c r="D76" t="s">
-        <v>66</v>
+        <v>640</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>181</v>
+        <v>623</v>
       </c>
       <c r="B77" t="s">
-        <v>187</v>
+        <v>663</v>
       </c>
       <c r="C77" t="s">
-        <v>188</v>
+        <v>624</v>
       </c>
       <c r="D77" t="s">
-        <v>189</v>
+        <v>625</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>219</v>
+        <v>626</v>
       </c>
       <c r="B78" t="s">
-        <v>220</v>
+        <v>663</v>
       </c>
       <c r="C78" t="s">
-        <v>223</v>
+        <v>627</v>
       </c>
       <c r="D78" t="s">
-        <v>224</v>
+        <v>628</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>221</v>
+        <v>183</v>
       </c>
       <c r="B79" t="s">
-        <v>220</v>
+        <v>184</v>
       </c>
       <c r="C79" t="s">
-        <v>237</v>
+        <v>78</v>
       </c>
       <c r="D79" t="s">
-        <v>237</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>703</v>
+        <v>64</v>
+      </c>
+      <c r="B80" t="s">
+        <v>186</v>
       </c>
       <c r="C80" t="s">
-        <v>704</v>
+        <v>65</v>
       </c>
       <c r="D80" t="s">
-        <v>702</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>675</v>
+        <v>181</v>
+      </c>
+      <c r="B81" t="s">
+        <v>187</v>
       </c>
       <c r="C81" t="s">
-        <v>676</v>
+        <v>188</v>
       </c>
       <c r="D81" t="s">
-        <v>677</v>
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>672</v>
+        <v>219</v>
+      </c>
+      <c r="B82" t="s">
+        <v>220</v>
       </c>
       <c r="C82" t="s">
-        <v>673</v>
+        <v>223</v>
       </c>
       <c r="D82" t="s">
-        <v>674</v>
+        <v>224</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>657</v>
+        <v>221</v>
       </c>
       <c r="B83" t="s">
-        <v>662</v>
+        <v>220</v>
       </c>
       <c r="C83" t="s">
-        <v>659</v>
+        <v>237</v>
       </c>
       <c r="D83" t="s">
-        <v>658</v>
+        <v>237</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>644</v>
-      </c>
-      <c r="B84" t="s">
-        <v>660</v>
+        <v>703</v>
       </c>
       <c r="C84" t="s">
-        <v>646</v>
+        <v>704</v>
       </c>
       <c r="D84" t="s">
-        <v>648</v>
+        <v>702</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>645</v>
-      </c>
-      <c r="B85" t="s">
-        <v>661</v>
+        <v>675</v>
       </c>
       <c r="C85" t="s">
-        <v>647</v>
+        <v>676</v>
       </c>
       <c r="D85" t="s">
-        <v>649</v>
+        <v>677</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>641</v>
-      </c>
-      <c r="B86" t="s">
-        <v>232</v>
+        <v>672</v>
       </c>
       <c r="C86" t="s">
-        <v>642</v>
+        <v>673</v>
       </c>
       <c r="D86" t="s">
-        <v>643</v>
+        <v>674</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>234</v>
+        <v>657</v>
       </c>
       <c r="B87" t="s">
-        <v>232</v>
+        <v>662</v>
       </c>
       <c r="C87" t="s">
-        <v>235</v>
+        <v>659</v>
       </c>
       <c r="D87" t="s">
-        <v>236</v>
+        <v>658</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
+      <c r="A88" t="s">
+        <v>644</v>
+      </c>
+      <c r="B88" t="s">
+        <v>660</v>
+      </c>
+      <c r="C88" t="s">
+        <v>646</v>
+      </c>
+      <c r="D88" t="s">
+        <v>648</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>80</v>
+        <v>645</v>
       </c>
       <c r="B89" t="s">
-        <v>81</v>
+        <v>661</v>
       </c>
       <c r="C89" t="s">
-        <v>89</v>
+        <v>647</v>
       </c>
       <c r="D89" t="s">
-        <v>90</v>
+        <v>649</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>82</v>
+        <v>641</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>232</v>
       </c>
       <c r="C90" t="s">
-        <v>85</v>
+        <v>642</v>
       </c>
       <c r="D90" t="s">
-        <v>87</v>
+        <v>643</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>84</v>
+        <v>234</v>
       </c>
       <c r="B91" t="s">
-        <v>83</v>
+        <v>232</v>
       </c>
       <c r="C91" t="s">
-        <v>86</v>
+        <v>235</v>
       </c>
       <c r="D91" t="s">
-        <v>88</v>
+        <v>236</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>103</v>
-      </c>
-      <c r="B92" t="s">
-        <v>81</v>
-      </c>
-      <c r="C92" t="s">
-        <v>104</v>
-      </c>
-      <c r="D92" t="s">
-        <v>262</v>
-      </c>
+      <c r="A92" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B93" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C93" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D93" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
+      <c r="A94" t="s">
+        <v>82</v>
+      </c>
+      <c r="B94" t="s">
+        <v>83</v>
+      </c>
+      <c r="C94" t="s">
+        <v>85</v>
+      </c>
+      <c r="D94" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>326</v>
+        <v>84</v>
       </c>
       <c r="B95" t="s">
-        <v>325</v>
+        <v>83</v>
       </c>
       <c r="C95" t="s">
-        <v>331</v>
+        <v>86</v>
       </c>
       <c r="D95" t="s">
-        <v>332</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>327</v>
+        <v>103</v>
       </c>
       <c r="B96" t="s">
-        <v>325</v>
+        <v>81</v>
       </c>
       <c r="C96" t="s">
-        <v>332</v>
+        <v>104</v>
       </c>
       <c r="D96" t="s">
-        <v>332</v>
+        <v>262</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>334</v>
+        <v>91</v>
       </c>
       <c r="B97" t="s">
-        <v>328</v>
+        <v>92</v>
       </c>
       <c r="C97" t="s">
-        <v>329</v>
+        <v>93</v>
       </c>
       <c r="D97" t="s">
-        <v>330</v>
+        <v>94</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>335</v>
-      </c>
-      <c r="B98" t="s">
-        <v>328</v>
-      </c>
-      <c r="C98" t="s">
-        <v>336</v>
-      </c>
-      <c r="D98" t="s">
-        <v>337</v>
-      </c>
+      <c r="A98" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>422</v>
+        <v>326</v>
+      </c>
+      <c r="B99" t="s">
+        <v>325</v>
       </c>
       <c r="C99" t="s">
-        <v>423</v>
+        <v>331</v>
       </c>
       <c r="D99" t="s">
-        <v>424</v>
+        <v>332</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>338</v>
+        <v>327</v>
+      </c>
+      <c r="B100" t="s">
+        <v>325</v>
       </c>
       <c r="C100" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D100" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>415</v>
+        <v>334</v>
+      </c>
+      <c r="B101" t="s">
+        <v>328</v>
       </c>
       <c r="C101" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="D101" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>416</v>
+        <v>335</v>
+      </c>
+      <c r="B102" t="s">
+        <v>328</v>
       </c>
       <c r="C102" t="s">
-        <v>420</v>
+        <v>336</v>
       </c>
       <c r="D102" t="s">
-        <v>421</v>
+        <v>337</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="C103" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D103" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C104" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D104" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>359</v>
-      </c>
-      <c r="B105" t="s">
-        <v>360</v>
+        <v>415</v>
       </c>
       <c r="C105" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="D105" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="C106" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="D106" t="s">
-        <v>413</v>
+        <v>421</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="C107" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="D107" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>363</v>
-      </c>
-      <c r="B108" t="s">
-        <v>364</v>
+        <v>343</v>
       </c>
       <c r="C108" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
       <c r="D108" t="s">
-        <v>366</v>
+        <v>344</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>427</v>
+        <v>359</v>
+      </c>
+      <c r="B109" t="s">
+        <v>360</v>
       </c>
       <c r="C109" t="s">
-        <v>401</v>
+        <v>361</v>
       </c>
       <c r="D109" t="s">
-        <v>402</v>
+        <v>362</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>428</v>
+        <v>409</v>
       </c>
       <c r="C110" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
       <c r="D110" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>346</v>
+        <v>410</v>
       </c>
       <c r="C111" t="s">
-        <v>375</v>
+        <v>412</v>
       </c>
       <c r="D111" t="s">
-        <v>347</v>
+        <v>414</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>367</v>
+        <v>363</v>
+      </c>
+      <c r="B112" t="s">
+        <v>364</v>
       </c>
       <c r="C112" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D112" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>369</v>
+        <v>427</v>
       </c>
       <c r="C113" t="s">
-        <v>370</v>
+        <v>401</v>
       </c>
       <c r="D113" t="s">
-        <v>371</v>
+        <v>402</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>372</v>
+        <v>428</v>
       </c>
       <c r="C114" t="s">
-        <v>373</v>
+        <v>429</v>
       </c>
       <c r="D114" t="s">
-        <v>374</v>
+        <v>430</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
       <c r="C115" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D115" t="s">
-        <v>378</v>
+        <v>347</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="C116" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="D116" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="C117" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="D117" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>403</v>
+        <v>372</v>
       </c>
       <c r="C118" t="s">
-        <v>408</v>
+        <v>373</v>
       </c>
       <c r="D118" t="s">
-        <v>407</v>
+        <v>374</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="C119" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="D119" t="s">
-        <v>425</v>
+        <v>378</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>404</v>
+        <v>379</v>
       </c>
       <c r="C120" t="s">
-        <v>405</v>
+        <v>380</v>
       </c>
       <c r="D120" t="s">
-        <v>406</v>
+        <v>381</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="C121" t="s">
-        <v>779</v>
+        <v>383</v>
       </c>
       <c r="D121" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="C122" t="s">
-        <v>395</v>
+        <v>408</v>
       </c>
       <c r="D122" t="s">
-        <v>394</v>
+        <v>407</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="C123" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="D123" t="s">
-        <v>400</v>
+        <v>425</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>391</v>
+        <v>404</v>
       </c>
       <c r="C124" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="D124" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>513</v>
-      </c>
-      <c r="C125" s="9" t="s">
-        <v>514</v>
+        <v>389</v>
+      </c>
+      <c r="C125" t="s">
+        <v>779</v>
       </c>
       <c r="D125" t="s">
-        <v>515</v>
+        <v>393</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>431</v>
+        <v>390</v>
       </c>
       <c r="C126" t="s">
-        <v>432</v>
+        <v>395</v>
       </c>
       <c r="D126" t="s">
-        <v>433</v>
+        <v>394</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>434</v>
+        <v>398</v>
       </c>
       <c r="C127" t="s">
-        <v>489</v>
+        <v>399</v>
       </c>
       <c r="D127" t="s">
-        <v>487</v>
+        <v>400</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>436</v>
+        <v>391</v>
       </c>
       <c r="C128" t="s">
-        <v>435</v>
+        <v>396</v>
       </c>
       <c r="D128" t="s">
-        <v>488</v>
+        <v>397</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>519</v>
-      </c>
-      <c r="C129" t="s">
-        <v>440</v>
+        <v>513</v>
+      </c>
+      <c r="C129" s="9" t="s">
+        <v>514</v>
       </c>
       <c r="D129" t="s">
-        <v>441</v>
+        <v>515</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>537</v>
+        <v>431</v>
       </c>
       <c r="C130" t="s">
-        <v>535</v>
+        <v>432</v>
       </c>
       <c r="D130" t="s">
-        <v>536</v>
+        <v>433</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="C131" t="s">
-        <v>443</v>
+        <v>489</v>
       </c>
       <c r="D131" t="s">
-        <v>444</v>
+        <v>487</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>481</v>
+        <v>436</v>
       </c>
       <c r="C132" t="s">
-        <v>483</v>
+        <v>435</v>
       </c>
       <c r="D132" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>482</v>
+        <v>519</v>
       </c>
       <c r="C133" t="s">
-        <v>484</v>
+        <v>440</v>
       </c>
       <c r="D133" t="s">
-        <v>486</v>
+        <v>441</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>490</v>
+        <v>537</v>
       </c>
       <c r="C134" t="s">
-        <v>491</v>
+        <v>535</v>
       </c>
       <c r="D134" t="s">
-        <v>492</v>
+        <v>536</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>523</v>
+        <v>442</v>
       </c>
       <c r="C135" t="s">
-        <v>493</v>
+        <v>443</v>
       </c>
       <c r="D135" t="s">
-        <v>494</v>
+        <v>444</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="C136" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
       <c r="D136" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>498</v>
+        <v>482</v>
       </c>
       <c r="C137" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="D137" t="s">
-        <v>501</v>
+        <v>486</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="C138" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="D138" t="s">
-        <v>530</v>
+        <v>492</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>516</v>
-      </c>
-      <c r="C139" s="9" t="s">
-        <v>517</v>
+        <v>523</v>
+      </c>
+      <c r="C139" t="s">
+        <v>493</v>
       </c>
       <c r="D139" t="s">
-        <v>518</v>
+        <v>494</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>520</v>
-      </c>
-      <c r="C140" s="9" t="s">
-        <v>521</v>
+        <v>495</v>
+      </c>
+      <c r="C140" t="s">
+        <v>496</v>
       </c>
       <c r="D140" t="s">
-        <v>522</v>
+        <v>497</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>524</v>
-      </c>
-      <c r="C141" s="9" t="s">
-        <v>525</v>
+        <v>498</v>
+      </c>
+      <c r="C141" t="s">
+        <v>500</v>
       </c>
       <c r="D141" t="s">
-        <v>526</v>
+        <v>501</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>527</v>
-      </c>
-      <c r="C142" s="9" t="s">
-        <v>529</v>
+        <v>499</v>
+      </c>
+      <c r="C142" t="s">
+        <v>502</v>
       </c>
       <c r="D142" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>533</v>
+        <v>516</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>502</v>
+        <v>517</v>
       </c>
       <c r="D143" t="s">
-        <v>530</v>
+        <v>518</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="D144" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>545</v>
+        <v>524</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>546</v>
+        <v>525</v>
       </c>
       <c r="D145" t="s">
-        <v>547</v>
+        <v>526</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>548</v>
+        <v>527</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>552</v>
+        <v>529</v>
       </c>
       <c r="D146" t="s">
-        <v>550</v>
+        <v>528</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>549</v>
+        <v>533</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>551</v>
+        <v>502</v>
       </c>
       <c r="D147" t="s">
-        <v>551</v>
+        <v>530</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>553</v>
+        <v>534</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>559</v>
+        <v>531</v>
       </c>
       <c r="D148" t="s">
-        <v>558</v>
+        <v>532</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="D149" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>560</v>
+        <v>548</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
       <c r="D150" t="s">
-        <v>562</v>
+        <v>550</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>579</v>
+        <v>551</v>
       </c>
       <c r="D151" t="s">
-        <v>580</v>
+        <v>551</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="D152" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="D153" t="s">
-        <v>568</v>
+        <v>557</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>575</v>
+        <v>560</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="D154" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>576</v>
+        <v>555</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="D155" t="s">
-        <v>574</v>
+        <v>580</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>577</v>
+        <v>563</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>570</v>
-      </c>
-      <c r="D156" s="9" t="s">
-        <v>570</v>
+        <v>565</v>
+      </c>
+      <c r="D156" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>571</v>
-      </c>
-      <c r="D157" s="9" t="s">
-        <v>571</v>
+        <v>566</v>
+      </c>
+      <c r="D157" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>582</v>
-      </c>
-      <c r="D158" s="9" t="s">
-        <v>583</v>
+        <v>569</v>
+      </c>
+      <c r="D158" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>591</v>
-      </c>
-      <c r="D159" s="9" t="s">
-        <v>592</v>
+        <v>573</v>
+      </c>
+      <c r="D159" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>590</v>
+        <v>570</v>
       </c>
       <c r="D160" s="9" t="s">
-        <v>593</v>
+        <v>570</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B161" s="3"/>
-      <c r="C161" s="3"/>
-      <c r="D161" s="3"/>
+      <c r="A161" t="s">
+        <v>578</v>
+      </c>
+      <c r="C161" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="D161" s="9" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>694</v>
-      </c>
-      <c r="C162" t="s">
-        <v>695</v>
-      </c>
-      <c r="D162" t="s">
-        <v>696</v>
+        <v>581</v>
+      </c>
+      <c r="C162" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="D162" s="9" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>690</v>
-      </c>
-      <c r="C163" t="s">
-        <v>697</v>
-      </c>
-      <c r="D163" t="s">
-        <v>699</v>
+        <v>588</v>
+      </c>
+      <c r="C163" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="D163" s="9" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>693</v>
-      </c>
-      <c r="C164" t="s">
-        <v>698</v>
-      </c>
-      <c r="D164" t="s">
-        <v>700</v>
+        <v>589</v>
+      </c>
+      <c r="C164" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="D164" s="9" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>701</v>
-      </c>
-      <c r="C165" s="7" t="s">
-        <v>691</v>
-      </c>
-      <c r="D165" s="7" t="s">
-        <v>692</v>
-      </c>
+      <c r="A165" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B165" s="3"/>
+      <c r="C165" s="3"/>
+      <c r="D165" s="3"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>140</v>
-      </c>
-      <c r="B166" t="s">
-        <v>137</v>
+        <v>694</v>
       </c>
       <c r="C166" t="s">
-        <v>138</v>
+        <v>695</v>
       </c>
       <c r="D166" t="s">
-        <v>139</v>
+        <v>696</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>141</v>
-      </c>
-      <c r="B167" t="s">
-        <v>142</v>
+        <v>690</v>
       </c>
       <c r="C167" t="s">
-        <v>150</v>
+        <v>697</v>
       </c>
       <c r="D167" t="s">
-        <v>151</v>
+        <v>699</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>147</v>
-      </c>
-      <c r="B168" t="s">
-        <v>137</v>
+        <v>693</v>
       </c>
       <c r="C168" t="s">
-        <v>683</v>
+        <v>698</v>
       </c>
       <c r="D168" t="s">
-        <v>684</v>
+        <v>700</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>143</v>
-      </c>
-      <c r="B169" t="s">
-        <v>142</v>
-      </c>
-      <c r="C169" t="s">
-        <v>149</v>
-      </c>
-      <c r="D169" t="s">
-        <v>148</v>
+        <v>701</v>
+      </c>
+      <c r="C169" s="7" t="s">
+        <v>691</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B170" t="s">
-        <v>145</v>
-      </c>
-      <c r="C170" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D170" s="7" t="s">
-        <v>146</v>
+        <v>137</v>
+      </c>
+      <c r="C170" t="s">
+        <v>138</v>
+      </c>
+      <c r="D170" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>681</v>
+        <v>141</v>
+      </c>
+      <c r="B171" t="s">
+        <v>142</v>
       </c>
       <c r="C171" t="s">
-        <v>680</v>
+        <v>150</v>
       </c>
       <c r="D171" t="s">
-        <v>680</v>
+        <v>151</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>682</v>
+        <v>147</v>
+      </c>
+      <c r="B172" t="s">
+        <v>137</v>
       </c>
       <c r="C172" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="D172" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>687</v>
+        <v>143</v>
+      </c>
+      <c r="B173" t="s">
+        <v>142</v>
       </c>
       <c r="C173" t="s">
-        <v>688</v>
+        <v>149</v>
       </c>
       <c r="D173" t="s">
-        <v>689</v>
+        <v>148</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B174" s="6"/>
-      <c r="C174" s="6"/>
-      <c r="D174" s="6"/>
+      <c r="A174" t="s">
+        <v>144</v>
+      </c>
+      <c r="B174" t="s">
+        <v>145</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D174" s="7" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>47</v>
-      </c>
-      <c r="B175" t="s">
-        <v>8</v>
+        <v>681</v>
       </c>
       <c r="C175" t="s">
-        <v>48</v>
+        <v>680</v>
       </c>
       <c r="D175" t="s">
-        <v>49</v>
+        <v>680</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>95</v>
-      </c>
-      <c r="B176" t="s">
-        <v>8</v>
+        <v>682</v>
       </c>
       <c r="C176" t="s">
-        <v>96</v>
+        <v>686</v>
       </c>
       <c r="D176" t="s">
-        <v>97</v>
+        <v>685</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>597</v>
+        <v>687</v>
       </c>
       <c r="C177" t="s">
-        <v>598</v>
+        <v>688</v>
       </c>
       <c r="D177" t="s">
-        <v>599</v>
+        <v>689</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>600</v>
-      </c>
-      <c r="C178" t="s">
-        <v>601</v>
-      </c>
-      <c r="D178" t="s">
-        <v>602</v>
-      </c>
+      <c r="A178" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B178" s="6"/>
+      <c r="C178" s="6"/>
+      <c r="D178" s="6"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>632</v>
+        <v>47</v>
+      </c>
+      <c r="B179" t="s">
+        <v>8</v>
       </c>
       <c r="C179" t="s">
-        <v>634</v>
+        <v>48</v>
       </c>
       <c r="D179" t="s">
-        <v>635</v>
+        <v>49</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>633</v>
+        <v>95</v>
+      </c>
+      <c r="B180" t="s">
+        <v>8</v>
       </c>
       <c r="C180" t="s">
-        <v>637</v>
+        <v>96</v>
       </c>
       <c r="D180" t="s">
-        <v>636</v>
+        <v>97</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>50</v>
-      </c>
-      <c r="B181" t="s">
-        <v>8</v>
+        <v>597</v>
       </c>
       <c r="C181" t="s">
-        <v>51</v>
+        <v>598</v>
       </c>
       <c r="D181" t="s">
-        <v>52</v>
+        <v>599</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>53</v>
-      </c>
-      <c r="B182" t="s">
-        <v>8</v>
+        <v>600</v>
       </c>
       <c r="C182" t="s">
-        <v>54</v>
+        <v>601</v>
       </c>
       <c r="D182" t="s">
-        <v>222</v>
+        <v>602</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>217</v>
-      </c>
-      <c r="B183" t="s">
-        <v>8</v>
+        <v>632</v>
       </c>
       <c r="C183" t="s">
-        <v>218</v>
+        <v>634</v>
       </c>
       <c r="D183" t="s">
-        <v>218</v>
+        <v>635</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>349</v>
-      </c>
-      <c r="B184" t="s">
-        <v>8</v>
+        <v>633</v>
       </c>
       <c r="C184" t="s">
-        <v>614</v>
+        <v>637</v>
       </c>
       <c r="D184" t="s">
-        <v>616</v>
+        <v>636</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>615</v>
+        <v>50</v>
+      </c>
+      <c r="B185" t="s">
+        <v>8</v>
       </c>
       <c r="C185" t="s">
-        <v>613</v>
+        <v>51</v>
       </c>
       <c r="D185" t="s">
-        <v>617</v>
+        <v>52</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
       <c r="B186" t="s">
         <v>8</v>
       </c>
       <c r="C186" t="s">
-        <v>594</v>
+        <v>54</v>
       </c>
       <c r="D186" t="s">
-        <v>156</v>
+        <v>222</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>165</v>
+        <v>217</v>
       </c>
       <c r="B187" t="s">
         <v>8</v>
       </c>
       <c r="C187" t="s">
-        <v>595</v>
+        <v>218</v>
       </c>
       <c r="D187" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>173</v>
+        <v>349</v>
       </c>
       <c r="B188" t="s">
         <v>8</v>
       </c>
       <c r="C188" t="s">
-        <v>596</v>
+        <v>614</v>
       </c>
       <c r="D188" t="s">
-        <v>174</v>
+        <v>616</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>603</v>
-      </c>
-      <c r="B189" t="s">
-        <v>8</v>
+        <v>615</v>
       </c>
       <c r="C189" t="s">
-        <v>604</v>
+        <v>613</v>
       </c>
       <c r="D189" t="s">
-        <v>605</v>
+        <v>617</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>610</v>
+        <v>155</v>
       </c>
       <c r="B190" t="s">
         <v>8</v>
       </c>
       <c r="C190" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
       <c r="D190" t="s">
-        <v>606</v>
+        <v>156</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>611</v>
+        <v>165</v>
       </c>
       <c r="B191" t="s">
         <v>8</v>
       </c>
       <c r="C191" t="s">
-        <v>609</v>
+        <v>595</v>
       </c>
       <c r="D191" t="s">
-        <v>607</v>
+        <v>166</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="B192" t="s">
         <v>8</v>
       </c>
       <c r="C192" t="s">
-        <v>190</v>
+        <v>596</v>
       </c>
       <c r="D192" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>55</v>
+        <v>603</v>
       </c>
       <c r="B193" t="s">
         <v>8</v>
       </c>
       <c r="C193" t="s">
-        <v>56</v>
+        <v>604</v>
       </c>
       <c r="D193" t="s">
-        <v>57</v>
+        <v>605</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>162</v>
+        <v>610</v>
       </c>
       <c r="B194" t="s">
         <v>8</v>
       </c>
       <c r="C194" t="s">
-        <v>157</v>
+        <v>608</v>
       </c>
       <c r="D194" t="s">
-        <v>16</v>
+        <v>606</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>167</v>
+        <v>611</v>
       </c>
       <c r="B195" t="s">
         <v>8</v>
       </c>
       <c r="C195" t="s">
-        <v>168</v>
+        <v>609</v>
       </c>
       <c r="D195" t="s">
-        <v>169</v>
+        <v>607</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="B196" t="s">
         <v>8</v>
       </c>
       <c r="C196" t="s">
-        <v>59</v>
+        <v>190</v>
       </c>
       <c r="D196" t="s">
-        <v>60</v>
+        <v>191</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>161</v>
+        <v>55</v>
       </c>
       <c r="B197" t="s">
         <v>8</v>
       </c>
       <c r="C197" t="s">
-        <v>163</v>
+        <v>56</v>
       </c>
       <c r="D197" t="s">
-        <v>164</v>
+        <v>57</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B198" t="s">
         <v>8</v>
       </c>
       <c r="C198" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="D198" t="s">
-        <v>172</v>
+        <v>16</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>61</v>
+        <v>167</v>
       </c>
       <c r="B199" t="s">
         <v>8</v>
       </c>
       <c r="C199" t="s">
-        <v>62</v>
+        <v>168</v>
       </c>
       <c r="D199" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>160</v>
+        <v>58</v>
       </c>
       <c r="B200" t="s">
         <v>8</v>
       </c>
       <c r="C200" t="s">
-        <v>158</v>
+        <v>59</v>
       </c>
       <c r="D200" t="s">
-        <v>159</v>
+        <v>60</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B201" t="s">
         <v>8</v>
       </c>
       <c r="C201" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D201" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="B202" t="s">
         <v>8</v>
       </c>
       <c r="C202" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="D202" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>195</v>
+        <v>61</v>
       </c>
       <c r="B203" t="s">
         <v>8</v>
       </c>
       <c r="C203" t="s">
-        <v>196</v>
+        <v>62</v>
       </c>
       <c r="D203" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>197</v>
+        <v>160</v>
       </c>
       <c r="B204" t="s">
         <v>8</v>
       </c>
       <c r="C204" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="D204" t="s">
-        <v>199</v>
+        <v>159</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>284</v>
+        <v>175</v>
+      </c>
+      <c r="B205" t="s">
+        <v>8</v>
       </c>
       <c r="C205" t="s">
-        <v>285</v>
+        <v>176</v>
       </c>
       <c r="D205" t="s">
-        <v>286</v>
+        <v>177</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>67</v>
+        <v>194</v>
       </c>
       <c r="B206" t="s">
         <v>8</v>
       </c>
       <c r="C206" t="s">
-        <v>68</v>
+        <v>192</v>
       </c>
       <c r="D206" t="s">
-        <v>69</v>
+        <v>193</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="B207" t="s">
         <v>8</v>
       </c>
       <c r="C207" t="s">
-        <v>9</v>
+        <v>196</v>
       </c>
       <c r="D207" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>437</v>
+        <v>197</v>
+      </c>
+      <c r="B208" t="s">
+        <v>8</v>
       </c>
       <c r="C208" t="s">
-        <v>438</v>
+        <v>198</v>
       </c>
       <c r="D208" t="s">
-        <v>439</v>
+        <v>199</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>200</v>
-      </c>
-      <c r="B209" t="s">
-        <v>8</v>
+        <v>284</v>
       </c>
       <c r="C209" t="s">
-        <v>200</v>
+        <v>285</v>
       </c>
       <c r="D209" t="s">
-        <v>201</v>
+        <v>286</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="B210" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C210" t="s">
-        <v>178</v>
+        <v>68</v>
       </c>
       <c r="D210" t="s">
-        <v>180</v>
+        <v>69</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>202</v>
+        <v>7</v>
       </c>
       <c r="B211" t="s">
         <v>8</v>
       </c>
       <c r="C211" t="s">
-        <v>204</v>
+        <v>9</v>
       </c>
       <c r="D211" t="s">
-        <v>205</v>
+        <v>10</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>203</v>
-      </c>
-      <c r="B212" t="s">
-        <v>179</v>
+        <v>437</v>
       </c>
       <c r="C212" t="s">
-        <v>206</v>
+        <v>438</v>
       </c>
       <c r="D212" t="s">
-        <v>207</v>
+        <v>439</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="B213" t="s">
         <v>8</v>
       </c>
       <c r="C213" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="D213" t="s">
-        <v>227</v>
+        <v>201</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>230</v>
+        <v>178</v>
       </c>
       <c r="B214" t="s">
         <v>179</v>
       </c>
       <c r="C214" t="s">
-        <v>226</v>
+        <v>178</v>
       </c>
       <c r="D214" t="s">
-        <v>228</v>
+        <v>180</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B215" t="s">
         <v>8</v>
       </c>
       <c r="C215" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D215" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B216" t="s">
         <v>179</v>
       </c>
       <c r="C216" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D216" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>106</v>
+        <v>229</v>
       </c>
       <c r="B217" t="s">
         <v>8</v>
       </c>
       <c r="C217" t="s">
-        <v>107</v>
+        <v>225</v>
       </c>
       <c r="D217" t="s">
-        <v>108</v>
+        <v>227</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="B218" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="C218" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="D218" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
       <c r="B219" t="s">
         <v>8</v>
       </c>
       <c r="C219" t="s">
-        <v>15</v>
+        <v>213</v>
       </c>
       <c r="D219" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>385</v>
+        <v>212</v>
+      </c>
+      <c r="B220" t="s">
+        <v>179</v>
       </c>
       <c r="C220" t="s">
-        <v>386</v>
+        <v>214</v>
       </c>
       <c r="D220" t="s">
-        <v>387</v>
+        <v>216</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>503</v>
+        <v>106</v>
+      </c>
+      <c r="B221" t="s">
+        <v>8</v>
       </c>
       <c r="C221" t="s">
-        <v>504</v>
+        <v>107</v>
       </c>
       <c r="D221" t="s">
-        <v>505</v>
+        <v>108</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>426</v>
+        <v>208</v>
       </c>
       <c r="B222" t="s">
-        <v>316</v>
+        <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>317</v>
+        <v>209</v>
       </c>
       <c r="D222" t="s">
-        <v>318</v>
+        <v>210</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>445</v>
+        <v>14</v>
+      </c>
+      <c r="B223" t="s">
+        <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>457</v>
+        <v>15</v>
       </c>
       <c r="D223" t="s">
-        <v>469</v>
+        <v>16</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>446</v>
+        <v>385</v>
       </c>
       <c r="C224" t="s">
-        <v>458</v>
+        <v>386</v>
       </c>
       <c r="D224" t="s">
-        <v>470</v>
+        <v>387</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>447</v>
+        <v>503</v>
       </c>
       <c r="C225" t="s">
-        <v>459</v>
+        <v>504</v>
       </c>
       <c r="D225" t="s">
-        <v>471</v>
+        <v>505</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>448</v>
+        <v>426</v>
+      </c>
+      <c r="B226" t="s">
+        <v>316</v>
       </c>
       <c r="C226" t="s">
-        <v>460</v>
+        <v>317</v>
       </c>
       <c r="D226" t="s">
-        <v>472</v>
+        <v>318</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C227" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D227" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C228" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="D228" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C229" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="D229" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C230" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D230" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C231" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D231" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C232" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D232" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C233" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D233" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C234" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D234" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>508</v>
+        <v>453</v>
       </c>
       <c r="C235" t="s">
-        <v>507</v>
+        <v>465</v>
       </c>
       <c r="D235" t="s">
-        <v>506</v>
+        <v>477</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>584</v>
+        <v>454</v>
       </c>
       <c r="C236" t="s">
-        <v>2</v>
+        <v>466</v>
       </c>
       <c r="D236" t="s">
-        <v>585</v>
+        <v>478</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>586</v>
+        <v>455</v>
       </c>
       <c r="C237" t="s">
-        <v>587</v>
+        <v>467</v>
       </c>
       <c r="D237" t="s">
-        <v>3</v>
+        <v>479</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B238" s="2"/>
-      <c r="C238" s="2"/>
-      <c r="D238" s="2"/>
+      <c r="A238" t="s">
+        <v>456</v>
+      </c>
+      <c r="C238" t="s">
+        <v>468</v>
+      </c>
+      <c r="D238" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>110</v>
-      </c>
-      <c r="B239" t="s">
-        <v>109</v>
+        <v>508</v>
       </c>
       <c r="C239" t="s">
-        <v>129</v>
+        <v>507</v>
       </c>
       <c r="D239" t="s">
-        <v>128</v>
+        <v>506</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>127</v>
-      </c>
-      <c r="B240" t="s">
-        <v>109</v>
+        <v>584</v>
       </c>
       <c r="C240" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="D240" t="s">
-        <v>133</v>
+        <v>585</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>111</v>
-      </c>
-      <c r="B241" t="s">
+        <v>586</v>
+      </c>
+      <c r="C241" t="s">
+        <v>587</v>
+      </c>
+      <c r="D241" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C241" t="s">
-        <v>112</v>
-      </c>
-      <c r="D241" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>116</v>
-      </c>
-      <c r="B242" t="s">
-        <v>109</v>
-      </c>
-      <c r="C242" t="s">
-        <v>117</v>
-      </c>
-      <c r="D242" t="s">
-        <v>118</v>
-      </c>
+      <c r="B242" s="2"/>
+      <c r="C242" s="2"/>
+      <c r="D242" s="2"/>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B243" t="s">
         <v>109</v>
       </c>
       <c r="C243" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="D243" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B244" t="s">
         <v>109</v>
       </c>
       <c r="C244" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D244" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B245" t="s">
         <v>109</v>
       </c>
       <c r="C245" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="D245" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B246" t="s">
         <v>109</v>
       </c>
       <c r="C246" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D246" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A247" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B247" s="3"/>
-      <c r="C247" s="3"/>
-      <c r="D247" s="3"/>
+      <c r="A247" t="s">
+        <v>113</v>
+      </c>
+      <c r="B247" t="s">
+        <v>109</v>
+      </c>
+      <c r="C247" t="s">
+        <v>114</v>
+      </c>
+      <c r="D247" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="B248" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="C248" t="s">
-        <v>352</v>
+        <v>132</v>
       </c>
       <c r="D248" t="s">
-        <v>353</v>
+        <v>121</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>350</v>
+        <v>122</v>
       </c>
       <c r="B249" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="C249" t="s">
-        <v>348</v>
+        <v>131</v>
       </c>
       <c r="D249" t="s">
-        <v>351</v>
+        <v>123</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="B250" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="C250" t="s">
-        <v>354</v>
+        <v>125</v>
       </c>
       <c r="D250" t="s">
-        <v>355</v>
+        <v>126</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>356</v>
-      </c>
-      <c r="B251" t="s">
-        <v>71</v>
-      </c>
-      <c r="C251" t="s">
-        <v>357</v>
-      </c>
-      <c r="D251" t="s">
-        <v>358</v>
-      </c>
+      <c r="A251" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B251" s="3"/>
+      <c r="C251" s="3"/>
+      <c r="D251" s="3"/>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B252" t="s">
         <v>71</v>
       </c>
       <c r="C252" t="s">
-        <v>73</v>
+        <v>352</v>
       </c>
       <c r="D252" t="s">
-        <v>74</v>
+        <v>353</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>618</v>
+        <v>350</v>
+      </c>
+      <c r="B253" t="s">
+        <v>71</v>
       </c>
       <c r="C253" t="s">
-        <v>612</v>
+        <v>348</v>
       </c>
       <c r="D253" t="s">
-        <v>619</v>
+        <v>351</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
+        <v>153</v>
+      </c>
+      <c r="B254" t="s">
+        <v>71</v>
+      </c>
+      <c r="C254" t="s">
+        <v>354</v>
+      </c>
+      <c r="D254" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>356</v>
+      </c>
+      <c r="B255" t="s">
+        <v>71</v>
+      </c>
+      <c r="C255" t="s">
+        <v>357</v>
+      </c>
+      <c r="D255" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>72</v>
+      </c>
+      <c r="B256" t="s">
+        <v>71</v>
+      </c>
+      <c r="C256" t="s">
+        <v>73</v>
+      </c>
+      <c r="D256" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>618</v>
+      </c>
+      <c r="C257" t="s">
+        <v>612</v>
+      </c>
+      <c r="D257" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
         <v>629</v>
       </c>
-      <c r="C254" t="s">
+      <c r="C258" t="s">
         <v>630</v>
       </c>
-      <c r="D254" t="s">
+      <c r="D258" t="s">
         <v>631</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C165" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
-    <hyperlink ref="D165" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
+    <hyperlink ref="C169" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
+    <hyperlink ref="D169" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
further normalization of db to have column for aggregation_type, required rejigs.
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D387527E-260B-403F-89BF-CAC3FB372E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FE3602-4416-4A6B-90EB-3381C6F3B261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="797">
   <si>
     <t>id</t>
   </si>
@@ -2438,6 +2438,15 @@
   </si>
   <si>
     <t>Cette sélection ne correspond à aucune mesure, la sélection de type d'échantillon a été réinitialisé à sa valeur précédente.</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>Depth/height (meters)</t>
+  </si>
+  <si>
+    <t>Profondeur/hauteur (mètres)</t>
   </si>
 </sst>
 </file>
@@ -3382,10 +3391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D258"/>
+  <dimension ref="A1:D259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:XFD75"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5684,959 +5693,970 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>50</v>
-      </c>
-      <c r="B185" t="s">
-        <v>8</v>
+        <v>794</v>
       </c>
       <c r="C185" t="s">
-        <v>51</v>
+        <v>795</v>
       </c>
       <c r="D185" t="s">
-        <v>52</v>
+        <v>796</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B186" t="s">
         <v>8</v>
       </c>
       <c r="C186" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D186" t="s">
-        <v>222</v>
+        <v>52</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>217</v>
+        <v>53</v>
       </c>
       <c r="B187" t="s">
         <v>8</v>
       </c>
       <c r="C187" t="s">
-        <v>218</v>
+        <v>54</v>
       </c>
       <c r="D187" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>349</v>
+        <v>217</v>
       </c>
       <c r="B188" t="s">
         <v>8</v>
       </c>
       <c r="C188" t="s">
-        <v>614</v>
+        <v>218</v>
       </c>
       <c r="D188" t="s">
-        <v>616</v>
+        <v>218</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>615</v>
+        <v>349</v>
+      </c>
+      <c r="B189" t="s">
+        <v>8</v>
       </c>
       <c r="C189" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D189" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>155</v>
-      </c>
-      <c r="B190" t="s">
-        <v>8</v>
+        <v>615</v>
       </c>
       <c r="C190" t="s">
-        <v>594</v>
+        <v>613</v>
       </c>
       <c r="D190" t="s">
-        <v>156</v>
+        <v>617</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B191" t="s">
         <v>8</v>
       </c>
       <c r="C191" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D191" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B192" t="s">
         <v>8</v>
       </c>
       <c r="C192" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D192" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>603</v>
+        <v>173</v>
       </c>
       <c r="B193" t="s">
         <v>8</v>
       </c>
       <c r="C193" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="D193" t="s">
-        <v>605</v>
+        <v>174</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
       <c r="B194" t="s">
         <v>8</v>
       </c>
       <c r="C194" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="D194" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B195" t="s">
         <v>8</v>
       </c>
       <c r="C195" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D195" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>154</v>
+        <v>611</v>
       </c>
       <c r="B196" t="s">
         <v>8</v>
       </c>
       <c r="C196" t="s">
-        <v>190</v>
+        <v>609</v>
       </c>
       <c r="D196" t="s">
-        <v>191</v>
+        <v>607</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>55</v>
+        <v>154</v>
       </c>
       <c r="B197" t="s">
         <v>8</v>
       </c>
       <c r="C197" t="s">
-        <v>56</v>
+        <v>190</v>
       </c>
       <c r="D197" t="s">
-        <v>57</v>
+        <v>191</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>162</v>
+        <v>55</v>
       </c>
       <c r="B198" t="s">
         <v>8</v>
       </c>
       <c r="C198" t="s">
-        <v>157</v>
+        <v>56</v>
       </c>
       <c r="D198" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B199" t="s">
         <v>8</v>
       </c>
       <c r="C199" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D199" t="s">
-        <v>169</v>
+        <v>16</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>58</v>
+        <v>167</v>
       </c>
       <c r="B200" t="s">
         <v>8</v>
       </c>
       <c r="C200" t="s">
-        <v>59</v>
+        <v>168</v>
       </c>
       <c r="D200" t="s">
-        <v>60</v>
+        <v>169</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>161</v>
+        <v>58</v>
       </c>
       <c r="B201" t="s">
         <v>8</v>
       </c>
       <c r="C201" t="s">
-        <v>163</v>
+        <v>59</v>
       </c>
       <c r="D201" t="s">
-        <v>164</v>
+        <v>60</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B202" t="s">
         <v>8</v>
       </c>
       <c r="C202" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D202" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>61</v>
+        <v>170</v>
       </c>
       <c r="B203" t="s">
         <v>8</v>
       </c>
       <c r="C203" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
       <c r="D203" t="s">
-        <v>63</v>
+        <v>172</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>160</v>
+        <v>61</v>
       </c>
       <c r="B204" t="s">
         <v>8</v>
       </c>
       <c r="C204" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
       <c r="D204" t="s">
-        <v>159</v>
+        <v>63</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B205" t="s">
         <v>8</v>
       </c>
       <c r="C205" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="D205" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="B206" t="s">
         <v>8</v>
       </c>
       <c r="C206" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="D206" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B207" t="s">
         <v>8</v>
       </c>
       <c r="C207" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D207" t="s">
-        <v>105</v>
+        <v>193</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B208" t="s">
         <v>8</v>
       </c>
       <c r="C208" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D208" t="s">
-        <v>199</v>
+        <v>105</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>284</v>
+        <v>197</v>
+      </c>
+      <c r="B209" t="s">
+        <v>8</v>
       </c>
       <c r="C209" t="s">
-        <v>285</v>
+        <v>198</v>
       </c>
       <c r="D209" t="s">
-        <v>286</v>
+        <v>199</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>67</v>
-      </c>
-      <c r="B210" t="s">
-        <v>8</v>
+        <v>284</v>
       </c>
       <c r="C210" t="s">
-        <v>68</v>
+        <v>285</v>
       </c>
       <c r="D210" t="s">
-        <v>69</v>
+        <v>286</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="B211" t="s">
         <v>8</v>
       </c>
       <c r="C211" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="D211" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>437</v>
+        <v>7</v>
+      </c>
+      <c r="B212" t="s">
+        <v>8</v>
       </c>
       <c r="C212" t="s">
-        <v>438</v>
+        <v>9</v>
       </c>
       <c r="D212" t="s">
-        <v>439</v>
+        <v>10</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>200</v>
-      </c>
-      <c r="B213" t="s">
-        <v>8</v>
+        <v>437</v>
       </c>
       <c r="C213" t="s">
-        <v>200</v>
+        <v>438</v>
       </c>
       <c r="D213" t="s">
-        <v>201</v>
+        <v>439</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="B214" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C214" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="D214" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="B215" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="C215" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="D215" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B216" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C216" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D216" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="B217" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="C217" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="D217" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B218" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C218" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D218" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="B219" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="C219" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="D219" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B220" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C220" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D220" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>106</v>
+        <v>212</v>
       </c>
       <c r="B221" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="C221" t="s">
-        <v>107</v>
+        <v>214</v>
       </c>
       <c r="D221" t="s">
-        <v>108</v>
+        <v>216</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>208</v>
+        <v>106</v>
       </c>
       <c r="B222" t="s">
         <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>209</v>
+        <v>107</v>
       </c>
       <c r="D222" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>14</v>
+        <v>208</v>
       </c>
       <c r="B223" t="s">
         <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
       <c r="D223" t="s">
-        <v>16</v>
+        <v>210</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>385</v>
+        <v>14</v>
+      </c>
+      <c r="B224" t="s">
+        <v>8</v>
       </c>
       <c r="C224" t="s">
-        <v>386</v>
+        <v>15</v>
       </c>
       <c r="D224" t="s">
-        <v>387</v>
+        <v>16</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>503</v>
+        <v>385</v>
       </c>
       <c r="C225" t="s">
-        <v>504</v>
+        <v>386</v>
       </c>
       <c r="D225" t="s">
-        <v>505</v>
+        <v>387</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>426</v>
-      </c>
-      <c r="B226" t="s">
-        <v>316</v>
+        <v>503</v>
       </c>
       <c r="C226" t="s">
-        <v>317</v>
+        <v>504</v>
       </c>
       <c r="D226" t="s">
-        <v>318</v>
+        <v>505</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>445</v>
+        <v>426</v>
+      </c>
+      <c r="B227" t="s">
+        <v>316</v>
       </c>
       <c r="C227" t="s">
-        <v>457</v>
+        <v>317</v>
       </c>
       <c r="D227" t="s">
-        <v>469</v>
+        <v>318</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C228" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D228" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C229" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D229" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C230" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D230" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C231" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D231" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C232" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D232" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C233" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D233" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C234" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D234" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C235" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D235" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C236" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D236" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C237" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D237" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C238" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D238" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>508</v>
+        <v>456</v>
       </c>
       <c r="C239" t="s">
-        <v>507</v>
+        <v>468</v>
       </c>
       <c r="D239" t="s">
-        <v>506</v>
+        <v>480</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>584</v>
+        <v>508</v>
       </c>
       <c r="C240" t="s">
-        <v>2</v>
+        <v>507</v>
       </c>
       <c r="D240" t="s">
-        <v>585</v>
+        <v>506</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
+        <v>584</v>
+      </c>
+      <c r="C241" t="s">
+        <v>2</v>
+      </c>
+      <c r="D241" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
         <v>586</v>
       </c>
-      <c r="C241" t="s">
+      <c r="C242" t="s">
         <v>587</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D242" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="2" t="s">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B242" s="2"/>
-      <c r="C242" s="2"/>
-      <c r="D242" s="2"/>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>110</v>
-      </c>
-      <c r="B243" t="s">
-        <v>109</v>
-      </c>
-      <c r="C243" t="s">
-        <v>129</v>
-      </c>
-      <c r="D243" t="s">
-        <v>128</v>
-      </c>
+      <c r="B243" s="2"/>
+      <c r="C243" s="2"/>
+      <c r="D243" s="2"/>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B244" t="s">
         <v>109</v>
       </c>
       <c r="C244" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D244" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B245" t="s">
         <v>109</v>
       </c>
       <c r="C245" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="D245" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B246" t="s">
         <v>109</v>
       </c>
       <c r="C246" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D246" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B247" t="s">
         <v>109</v>
       </c>
       <c r="C247" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D247" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B248" t="s">
         <v>109</v>
       </c>
       <c r="C248" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="D248" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B249" t="s">
         <v>109</v>
       </c>
       <c r="C249" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D249" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B250" t="s">
         <v>109</v>
       </c>
       <c r="C250" t="s">
+        <v>131</v>
+      </c>
+      <c r="D250" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>124</v>
+      </c>
+      <c r="B251" t="s">
+        <v>109</v>
+      </c>
+      <c r="C251" t="s">
         <v>125</v>
       </c>
-      <c r="D250" t="s">
+      <c r="D251" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" s="3" t="s">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B251" s="3"/>
-      <c r="C251" s="3"/>
-      <c r="D251" s="3"/>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>70</v>
-      </c>
-      <c r="B252" t="s">
-        <v>71</v>
-      </c>
-      <c r="C252" t="s">
-        <v>352</v>
-      </c>
-      <c r="D252" t="s">
-        <v>353</v>
-      </c>
+      <c r="B252" s="3"/>
+      <c r="C252" s="3"/>
+      <c r="D252" s="3"/>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>350</v>
+        <v>70</v>
       </c>
       <c r="B253" t="s">
         <v>71</v>
       </c>
       <c r="C253" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="D253" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>153</v>
+        <v>350</v>
       </c>
       <c r="B254" t="s">
         <v>71</v>
       </c>
       <c r="C254" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D254" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>356</v>
+        <v>153</v>
       </c>
       <c r="B255" t="s">
         <v>71</v>
       </c>
       <c r="C255" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D255" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>72</v>
+        <v>356</v>
       </c>
       <c r="B256" t="s">
         <v>71</v>
       </c>
       <c r="C256" t="s">
-        <v>73</v>
+        <v>357</v>
       </c>
       <c r="D256" t="s">
-        <v>74</v>
+        <v>358</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>618</v>
+        <v>72</v>
+      </c>
+      <c r="B257" t="s">
+        <v>71</v>
       </c>
       <c r="C257" t="s">
-        <v>612</v>
+        <v>73</v>
       </c>
       <c r="D257" t="s">
-        <v>619</v>
+        <v>74</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
+        <v>618</v>
+      </c>
+      <c r="C258" t="s">
+        <v>612</v>
+      </c>
+      <c r="D258" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
         <v>629</v>
       </c>
-      <c r="C258" t="s">
+      <c r="C259" t="s">
         <v>630</v>
       </c>
-      <c r="D258" t="s">
+      <c r="D259" t="s">
         <v>631</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit for codex review
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E51C94-6FAE-49D1-9A1D-2F70704F980A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79929A7B-C20F-47FA-A38B-63E962ADE613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="846">
   <si>
     <t>id</t>
   </si>
@@ -2483,6 +2483,117 @@
   </si>
   <si>
     <t>dl_data_continuous</t>
+  </si>
+  <si>
+    <t>view_timeseries</t>
+  </si>
+  <si>
+    <t>Show timeseries</t>
+  </si>
+  <si>
+    <t>Voir les séries temporelles</t>
+  </si>
+  <si>
+    <t>aggregation_type(s)</t>
+  </si>
+  <si>
+    <t>Aggregation type(s)</t>
+  </si>
+  <si>
+    <t>Type d'agrégation des mesures</t>
+  </si>
+  <si>
+    <t>aggregation_type_col</t>
+  </si>
+  <si>
+    <t>aggregation_type</t>
+  </si>
+  <si>
+    <t>aggregation_type_fr</t>
+  </si>
+  <si>
+    <t>Nominal recording rate</t>
+  </si>
+  <si>
+    <t>Rythme d'enregistrement nominal</t>
+  </si>
+  <si>
+    <t>nominal_rate</t>
+  </si>
+  <si>
+    <t>date_start</t>
+  </si>
+  <si>
+    <t>date_end</t>
+  </si>
+  <si>
+    <t>continuous data selector</t>
+  </si>
+  <si>
+    <t>With data starting after</t>
+  </si>
+  <si>
+    <t>With data ending before</t>
+  </si>
+  <si>
+    <t>Avec des données à partir de</t>
+  </si>
+  <si>
+    <t>Avec des données avant</t>
+  </si>
+  <si>
+    <t>This selection results in 0 corresponding timeseries, depth/height selector reset to its previous value</t>
+  </si>
+  <si>
+    <t>no_ts_z</t>
+  </si>
+  <si>
+    <t>no_ts_locs</t>
+  </si>
+  <si>
+    <t>no_ts_sub_locs</t>
+  </si>
+  <si>
+    <t>no_ts_medias</t>
+  </si>
+  <si>
+    <t>This selection results in 0 corresponding timeseries, location selector reset to its previous value.</t>
+  </si>
+  <si>
+    <t>Cette sélection ne correspond à aucune série temporelle, la sélection pour l'endroit a été réinitialisé à sa valeur précédente.</t>
+  </si>
+  <si>
+    <t>Cette sélection ne correspond à aucune série temporelle, la sélection  de sous-endroit a été réinitialisé à sa valeur précédente.</t>
+  </si>
+  <si>
+    <t>Cette sélection ne correspond à aucune série temporelle, la sélection de la profondeur/hauteur a été réinitialisé à sa valeur précédente.</t>
+  </si>
+  <si>
+    <t>Cette sélection ne correspond à aucune série temporelle, la sélection de type de média a été réinitialisé à sa valeur précédente.</t>
+  </si>
+  <si>
+    <t>This selection results in 0 corresponding timeseries, sub-location selector reset to its previous value.</t>
+  </si>
+  <si>
+    <t>This selection results in 0 corresponding timeseries, media type selector reset to its previous value.</t>
+  </si>
+  <si>
+    <t>no_ts_agg</t>
+  </si>
+  <si>
+    <t>This selection results in 0 corresponding timeseries, aggregation type selector reset to its previous value.</t>
+  </si>
+  <si>
+    <t>Cette sélection ne correspond à aucune série temporelle, la sélection de type d'aggrégation a été réinitialisé à sa valeur précédente.</t>
+  </si>
+  <si>
+    <t>no_ts_rate</t>
+  </si>
+  <si>
+    <t>This selection results in 0 corresponding timeseries, recording rate selector reset to its previous value.</t>
+  </si>
+  <si>
+    <t>Cette sélection ne correspond à aucune série temporelle, la sélection du rythme d'enregistrement a été réinitialisé à sa valeur précédente.</t>
   </si>
 </sst>
 </file>
@@ -3427,10 +3538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D263"/>
+  <dimension ref="A1:D275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4293,2458 +4404,2614 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>263</v>
+        <v>821</v>
       </c>
       <c r="B64" t="s">
-        <v>249</v>
+        <v>823</v>
       </c>
       <c r="C64" t="s">
-        <v>264</v>
+        <v>824</v>
       </c>
       <c r="D64" t="s">
-        <v>265</v>
+        <v>826</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>281</v>
+        <v>822</v>
       </c>
       <c r="B65" t="s">
-        <v>249</v>
+        <v>823</v>
       </c>
       <c r="C65" t="s">
-        <v>282</v>
+        <v>825</v>
       </c>
       <c r="D65" t="s">
-        <v>283</v>
+        <v>827</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B66" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C66" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D66" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="B67" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C67" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="D67" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B68" t="s">
         <v>250</v>
       </c>
       <c r="C68" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D68" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="B69" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="C69" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="D69" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>781</v>
+        <v>272</v>
       </c>
       <c r="B70" t="s">
-        <v>782</v>
+        <v>250</v>
       </c>
       <c r="C70" t="s">
-        <v>783</v>
+        <v>273</v>
       </c>
       <c r="D70" t="s">
-        <v>784</v>
+        <v>274</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>785</v>
+        <v>287</v>
       </c>
       <c r="B71" t="s">
-        <v>782</v>
+        <v>288</v>
       </c>
       <c r="C71" t="s">
-        <v>786</v>
+        <v>289</v>
       </c>
       <c r="D71" t="s">
-        <v>788</v>
+        <v>290</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>790</v>
+        <v>781</v>
       </c>
       <c r="B72" t="s">
         <v>782</v>
       </c>
       <c r="C72" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="D72" t="s">
-        <v>789</v>
+        <v>784</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="B73" t="s">
         <v>782</v>
       </c>
       <c r="C73" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="D73" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
+      <c r="A74" t="s">
+        <v>790</v>
+      </c>
+      <c r="B74" t="s">
+        <v>782</v>
+      </c>
+      <c r="C74" t="s">
+        <v>787</v>
+      </c>
+      <c r="D74" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>620</v>
+        <v>791</v>
+      </c>
+      <c r="B75" t="s">
+        <v>782</v>
       </c>
       <c r="C75" t="s">
-        <v>621</v>
+        <v>792</v>
       </c>
       <c r="D75" t="s">
-        <v>622</v>
+        <v>793</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>638</v>
+        <v>830</v>
+      </c>
+      <c r="B76" t="s">
+        <v>782</v>
       </c>
       <c r="C76" t="s">
-        <v>639</v>
+        <v>833</v>
       </c>
       <c r="D76" t="s">
-        <v>640</v>
+        <v>834</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>623</v>
+        <v>831</v>
       </c>
       <c r="B77" t="s">
-        <v>663</v>
+        <v>782</v>
       </c>
       <c r="C77" t="s">
-        <v>624</v>
+        <v>838</v>
       </c>
       <c r="D77" t="s">
-        <v>625</v>
+        <v>835</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>626</v>
+        <v>829</v>
       </c>
       <c r="B78" t="s">
-        <v>663</v>
+        <v>782</v>
       </c>
       <c r="C78" t="s">
-        <v>627</v>
+        <v>828</v>
       </c>
       <c r="D78" t="s">
-        <v>628</v>
+        <v>836</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>183</v>
+        <v>832</v>
       </c>
       <c r="B79" t="s">
-        <v>184</v>
+        <v>782</v>
       </c>
       <c r="C79" t="s">
-        <v>78</v>
+        <v>839</v>
       </c>
       <c r="D79" t="s">
-        <v>79</v>
+        <v>837</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>64</v>
+        <v>840</v>
       </c>
       <c r="B80" t="s">
-        <v>186</v>
+        <v>782</v>
       </c>
       <c r="C80" t="s">
-        <v>65</v>
+        <v>841</v>
       </c>
       <c r="D80" t="s">
-        <v>66</v>
+        <v>842</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>181</v>
+        <v>843</v>
       </c>
       <c r="B81" t="s">
-        <v>187</v>
+        <v>782</v>
       </c>
       <c r="C81" t="s">
-        <v>188</v>
+        <v>844</v>
       </c>
       <c r="D81" t="s">
-        <v>189</v>
+        <v>845</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>219</v>
-      </c>
-      <c r="B82" t="s">
-        <v>220</v>
-      </c>
-      <c r="C82" t="s">
-        <v>223</v>
-      </c>
-      <c r="D82" t="s">
-        <v>224</v>
-      </c>
+      <c r="A82" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>221</v>
-      </c>
-      <c r="B83" t="s">
-        <v>220</v>
+        <v>620</v>
       </c>
       <c r="C83" t="s">
-        <v>237</v>
+        <v>621</v>
       </c>
       <c r="D83" t="s">
-        <v>237</v>
+        <v>622</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>703</v>
+        <v>638</v>
       </c>
       <c r="C84" t="s">
-        <v>704</v>
+        <v>639</v>
       </c>
       <c r="D84" t="s">
-        <v>702</v>
+        <v>640</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>675</v>
+        <v>623</v>
+      </c>
+      <c r="B85" t="s">
+        <v>663</v>
       </c>
       <c r="C85" t="s">
-        <v>676</v>
+        <v>624</v>
       </c>
       <c r="D85" t="s">
-        <v>677</v>
+        <v>625</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>672</v>
+        <v>626</v>
+      </c>
+      <c r="B86" t="s">
+        <v>663</v>
       </c>
       <c r="C86" t="s">
-        <v>673</v>
+        <v>627</v>
       </c>
       <c r="D86" t="s">
-        <v>674</v>
+        <v>628</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>657</v>
+        <v>183</v>
       </c>
       <c r="B87" t="s">
-        <v>662</v>
+        <v>184</v>
       </c>
       <c r="C87" t="s">
-        <v>659</v>
+        <v>78</v>
       </c>
       <c r="D87" t="s">
-        <v>658</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>799</v>
+        <v>64</v>
+      </c>
+      <c r="B88" t="s">
+        <v>186</v>
       </c>
       <c r="C88" t="s">
-        <v>800</v>
+        <v>65</v>
       </c>
       <c r="D88" t="s">
-        <v>801</v>
+        <v>66</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>808</v>
+        <v>181</v>
+      </c>
+      <c r="B89" t="s">
+        <v>187</v>
       </c>
       <c r="C89" t="s">
-        <v>803</v>
+        <v>188</v>
       </c>
       <c r="D89" t="s">
-        <v>802</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>644</v>
+        <v>219</v>
       </c>
       <c r="B90" t="s">
-        <v>660</v>
+        <v>220</v>
       </c>
       <c r="C90" t="s">
-        <v>646</v>
+        <v>223</v>
       </c>
       <c r="D90" t="s">
-        <v>648</v>
+        <v>224</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>645</v>
+        <v>221</v>
       </c>
       <c r="B91" t="s">
-        <v>661</v>
+        <v>220</v>
       </c>
       <c r="C91" t="s">
-        <v>647</v>
+        <v>237</v>
       </c>
       <c r="D91" t="s">
-        <v>649</v>
+        <v>237</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>641</v>
-      </c>
-      <c r="B92" t="s">
-        <v>232</v>
+        <v>703</v>
       </c>
       <c r="C92" t="s">
-        <v>642</v>
+        <v>704</v>
       </c>
       <c r="D92" t="s">
-        <v>643</v>
+        <v>702</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>234</v>
-      </c>
-      <c r="B93" t="s">
-        <v>232</v>
+        <v>675</v>
       </c>
       <c r="C93" t="s">
-        <v>235</v>
+        <v>676</v>
       </c>
       <c r="D93" t="s">
-        <v>236</v>
+        <v>677</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>797</v>
+        <v>672</v>
       </c>
       <c r="C94" t="s">
-        <v>804</v>
+        <v>673</v>
       </c>
       <c r="D94" t="s">
-        <v>806</v>
+        <v>674</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>798</v>
+        <v>809</v>
       </c>
       <c r="C95" t="s">
-        <v>805</v>
+        <v>810</v>
       </c>
       <c r="D95" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="4"/>
+      <c r="A96" t="s">
+        <v>657</v>
+      </c>
+      <c r="B96" t="s">
+        <v>662</v>
+      </c>
+      <c r="C96" t="s">
+        <v>659</v>
+      </c>
+      <c r="D96" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>80</v>
-      </c>
-      <c r="B97" t="s">
-        <v>81</v>
+        <v>799</v>
       </c>
       <c r="C97" t="s">
-        <v>89</v>
+        <v>800</v>
       </c>
       <c r="D97" t="s">
-        <v>90</v>
+        <v>801</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>82</v>
-      </c>
-      <c r="B98" t="s">
-        <v>83</v>
+        <v>808</v>
       </c>
       <c r="C98" t="s">
-        <v>85</v>
+        <v>803</v>
       </c>
       <c r="D98" t="s">
-        <v>87</v>
+        <v>802</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>84</v>
+        <v>644</v>
       </c>
       <c r="B99" t="s">
-        <v>83</v>
+        <v>660</v>
       </c>
       <c r="C99" t="s">
-        <v>86</v>
+        <v>646</v>
       </c>
       <c r="D99" t="s">
-        <v>88</v>
+        <v>648</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>103</v>
+        <v>645</v>
       </c>
       <c r="B100" t="s">
-        <v>81</v>
+        <v>661</v>
       </c>
       <c r="C100" t="s">
-        <v>104</v>
+        <v>647</v>
       </c>
       <c r="D100" t="s">
-        <v>262</v>
+        <v>649</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>91</v>
+        <v>641</v>
       </c>
       <c r="B101" t="s">
-        <v>92</v>
+        <v>232</v>
       </c>
       <c r="C101" t="s">
-        <v>93</v>
+        <v>642</v>
       </c>
       <c r="D101" t="s">
-        <v>94</v>
+        <v>643</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="B102" s="5"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
+      <c r="A102" t="s">
+        <v>234</v>
+      </c>
+      <c r="B102" t="s">
+        <v>232</v>
+      </c>
+      <c r="C102" t="s">
+        <v>235</v>
+      </c>
+      <c r="D102" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>326</v>
-      </c>
-      <c r="B103" t="s">
-        <v>325</v>
+        <v>797</v>
       </c>
       <c r="C103" t="s">
-        <v>331</v>
+        <v>804</v>
       </c>
       <c r="D103" t="s">
-        <v>332</v>
+        <v>806</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>327</v>
-      </c>
-      <c r="B104" t="s">
-        <v>325</v>
+        <v>798</v>
       </c>
       <c r="C104" t="s">
-        <v>332</v>
+        <v>805</v>
       </c>
       <c r="D104" t="s">
-        <v>332</v>
+        <v>807</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>334</v>
-      </c>
-      <c r="B105" t="s">
-        <v>328</v>
+        <v>820</v>
       </c>
       <c r="C105" t="s">
-        <v>329</v>
+        <v>818</v>
       </c>
       <c r="D105" t="s">
-        <v>330</v>
+        <v>819</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>335</v>
-      </c>
-      <c r="B106" t="s">
-        <v>328</v>
-      </c>
-      <c r="C106" t="s">
-        <v>336</v>
-      </c>
-      <c r="D106" t="s">
-        <v>337</v>
-      </c>
+      <c r="A106" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>422</v>
+        <v>80</v>
+      </c>
+      <c r="B107" t="s">
+        <v>81</v>
       </c>
       <c r="C107" t="s">
-        <v>423</v>
+        <v>89</v>
       </c>
       <c r="D107" t="s">
-        <v>424</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>338</v>
+        <v>82</v>
+      </c>
+      <c r="B108" t="s">
+        <v>83</v>
       </c>
       <c r="C108" t="s">
-        <v>340</v>
+        <v>85</v>
       </c>
       <c r="D108" t="s">
-        <v>339</v>
+        <v>87</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>415</v>
+        <v>84</v>
+      </c>
+      <c r="B109" t="s">
+        <v>83</v>
       </c>
       <c r="C109" t="s">
-        <v>341</v>
+        <v>86</v>
       </c>
       <c r="D109" t="s">
-        <v>342</v>
+        <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>416</v>
+        <v>103</v>
+      </c>
+      <c r="B110" t="s">
+        <v>81</v>
       </c>
       <c r="C110" t="s">
-        <v>420</v>
+        <v>104</v>
       </c>
       <c r="D110" t="s">
-        <v>421</v>
+        <v>262</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>417</v>
+        <v>91</v>
+      </c>
+      <c r="B111" t="s">
+        <v>92</v>
       </c>
       <c r="C111" t="s">
-        <v>419</v>
+        <v>93</v>
       </c>
       <c r="D111" t="s">
-        <v>418</v>
+        <v>94</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>343</v>
-      </c>
-      <c r="C112" t="s">
-        <v>345</v>
-      </c>
-      <c r="D112" t="s">
-        <v>344</v>
-      </c>
+      <c r="A112" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>359</v>
+        <v>326</v>
       </c>
       <c r="B113" t="s">
-        <v>360</v>
+        <v>325</v>
       </c>
       <c r="C113" t="s">
-        <v>361</v>
+        <v>331</v>
       </c>
       <c r="D113" t="s">
-        <v>362</v>
+        <v>332</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>409</v>
+        <v>327</v>
+      </c>
+      <c r="B114" t="s">
+        <v>325</v>
       </c>
       <c r="C114" t="s">
-        <v>411</v>
+        <v>332</v>
       </c>
       <c r="D114" t="s">
-        <v>413</v>
+        <v>332</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>410</v>
+        <v>334</v>
+      </c>
+      <c r="B115" t="s">
+        <v>328</v>
       </c>
       <c r="C115" t="s">
-        <v>412</v>
+        <v>329</v>
       </c>
       <c r="D115" t="s">
-        <v>414</v>
+        <v>330</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>363</v>
+        <v>335</v>
       </c>
       <c r="B116" t="s">
-        <v>364</v>
+        <v>328</v>
       </c>
       <c r="C116" t="s">
-        <v>365</v>
+        <v>336</v>
       </c>
       <c r="D116" t="s">
-        <v>366</v>
+        <v>337</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="C117" t="s">
-        <v>401</v>
+        <v>423</v>
       </c>
       <c r="D117" t="s">
-        <v>402</v>
+        <v>424</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>428</v>
+        <v>338</v>
       </c>
       <c r="C118" t="s">
-        <v>429</v>
+        <v>340</v>
       </c>
       <c r="D118" t="s">
-        <v>430</v>
+        <v>339</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>346</v>
+        <v>415</v>
       </c>
       <c r="C119" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="D119" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>367</v>
+        <v>416</v>
       </c>
       <c r="C120" t="s">
-        <v>368</v>
+        <v>420</v>
       </c>
       <c r="D120" t="s">
-        <v>368</v>
+        <v>421</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>369</v>
+        <v>417</v>
       </c>
       <c r="C121" t="s">
-        <v>370</v>
+        <v>419</v>
       </c>
       <c r="D121" t="s">
-        <v>371</v>
+        <v>418</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>372</v>
+        <v>343</v>
       </c>
       <c r="C122" t="s">
-        <v>373</v>
+        <v>345</v>
       </c>
       <c r="D122" t="s">
-        <v>374</v>
+        <v>344</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>376</v>
+        <v>359</v>
+      </c>
+      <c r="B123" t="s">
+        <v>360</v>
       </c>
       <c r="C123" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="D123" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>379</v>
+        <v>409</v>
       </c>
       <c r="C124" t="s">
-        <v>380</v>
+        <v>411</v>
       </c>
       <c r="D124" t="s">
-        <v>381</v>
+        <v>413</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>382</v>
+        <v>410</v>
       </c>
       <c r="C125" t="s">
-        <v>383</v>
+        <v>412</v>
       </c>
       <c r="D125" t="s">
-        <v>384</v>
+        <v>414</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>403</v>
+        <v>363</v>
+      </c>
+      <c r="B126" t="s">
+        <v>364</v>
       </c>
       <c r="C126" t="s">
-        <v>408</v>
+        <v>365</v>
       </c>
       <c r="D126" t="s">
-        <v>407</v>
+        <v>366</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>388</v>
+        <v>427</v>
       </c>
       <c r="C127" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="D127" t="s">
-        <v>425</v>
+        <v>402</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>404</v>
+        <v>428</v>
       </c>
       <c r="C128" t="s">
-        <v>405</v>
+        <v>429</v>
       </c>
       <c r="D128" t="s">
-        <v>406</v>
+        <v>430</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="C129" t="s">
-        <v>779</v>
+        <v>375</v>
       </c>
       <c r="D129" t="s">
-        <v>393</v>
+        <v>347</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
       <c r="C130" t="s">
-        <v>395</v>
+        <v>368</v>
       </c>
       <c r="D130" t="s">
-        <v>394</v>
+        <v>368</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>398</v>
+        <v>369</v>
       </c>
       <c r="C131" t="s">
-        <v>399</v>
+        <v>370</v>
       </c>
       <c r="D131" t="s">
-        <v>400</v>
+        <v>371</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="C132" t="s">
-        <v>396</v>
+        <v>373</v>
       </c>
       <c r="D132" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>513</v>
-      </c>
-      <c r="C133" s="9" t="s">
-        <v>514</v>
+        <v>376</v>
+      </c>
+      <c r="C133" t="s">
+        <v>377</v>
       </c>
       <c r="D133" t="s">
-        <v>515</v>
+        <v>378</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>431</v>
+        <v>379</v>
       </c>
       <c r="C134" t="s">
-        <v>432</v>
+        <v>380</v>
       </c>
       <c r="D134" t="s">
-        <v>433</v>
+        <v>381</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>434</v>
+        <v>382</v>
       </c>
       <c r="C135" t="s">
-        <v>489</v>
+        <v>383</v>
       </c>
       <c r="D135" t="s">
-        <v>487</v>
+        <v>384</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>436</v>
+        <v>403</v>
       </c>
       <c r="C136" t="s">
-        <v>435</v>
+        <v>408</v>
       </c>
       <c r="D136" t="s">
-        <v>488</v>
+        <v>407</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>519</v>
+        <v>388</v>
       </c>
       <c r="C137" t="s">
-        <v>440</v>
+        <v>392</v>
       </c>
       <c r="D137" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>537</v>
+        <v>404</v>
       </c>
       <c r="C138" t="s">
-        <v>535</v>
+        <v>405</v>
       </c>
       <c r="D138" t="s">
-        <v>536</v>
+        <v>406</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>442</v>
+        <v>389</v>
       </c>
       <c r="C139" t="s">
-        <v>443</v>
+        <v>779</v>
       </c>
       <c r="D139" t="s">
-        <v>444</v>
+        <v>393</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>481</v>
+        <v>390</v>
       </c>
       <c r="C140" t="s">
-        <v>483</v>
+        <v>395</v>
       </c>
       <c r="D140" t="s">
-        <v>485</v>
+        <v>394</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>482</v>
+        <v>398</v>
       </c>
       <c r="C141" t="s">
-        <v>484</v>
+        <v>399</v>
       </c>
       <c r="D141" t="s">
-        <v>486</v>
+        <v>400</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>490</v>
+        <v>391</v>
       </c>
       <c r="C142" t="s">
-        <v>491</v>
+        <v>396</v>
       </c>
       <c r="D142" t="s">
-        <v>492</v>
+        <v>397</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>523</v>
-      </c>
-      <c r="C143" t="s">
-        <v>493</v>
+        <v>513</v>
+      </c>
+      <c r="C143" s="9" t="s">
+        <v>514</v>
       </c>
       <c r="D143" t="s">
-        <v>494</v>
+        <v>515</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>495</v>
+        <v>431</v>
       </c>
       <c r="C144" t="s">
-        <v>496</v>
+        <v>432</v>
       </c>
       <c r="D144" t="s">
-        <v>497</v>
+        <v>433</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>498</v>
+        <v>434</v>
       </c>
       <c r="C145" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="D145" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>499</v>
+        <v>436</v>
       </c>
       <c r="C146" t="s">
-        <v>502</v>
+        <v>435</v>
       </c>
       <c r="D146" t="s">
-        <v>530</v>
+        <v>488</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>516</v>
-      </c>
-      <c r="C147" s="9" t="s">
-        <v>517</v>
+        <v>519</v>
+      </c>
+      <c r="C147" t="s">
+        <v>440</v>
       </c>
       <c r="D147" t="s">
-        <v>518</v>
+        <v>441</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>520</v>
-      </c>
-      <c r="C148" s="9" t="s">
-        <v>521</v>
+        <v>537</v>
+      </c>
+      <c r="C148" t="s">
+        <v>535</v>
       </c>
       <c r="D148" t="s">
-        <v>522</v>
+        <v>536</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>524</v>
-      </c>
-      <c r="C149" s="9" t="s">
-        <v>525</v>
+        <v>442</v>
+      </c>
+      <c r="C149" t="s">
+        <v>443</v>
       </c>
       <c r="D149" t="s">
-        <v>526</v>
+        <v>444</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>527</v>
-      </c>
-      <c r="C150" s="9" t="s">
-        <v>529</v>
+        <v>481</v>
+      </c>
+      <c r="C150" t="s">
+        <v>483</v>
       </c>
       <c r="D150" t="s">
-        <v>528</v>
+        <v>485</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>533</v>
-      </c>
-      <c r="C151" s="9" t="s">
-        <v>502</v>
+        <v>482</v>
+      </c>
+      <c r="C151" t="s">
+        <v>484</v>
       </c>
       <c r="D151" t="s">
-        <v>530</v>
+        <v>486</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>534</v>
-      </c>
-      <c r="C152" s="9" t="s">
-        <v>531</v>
+        <v>490</v>
+      </c>
+      <c r="C152" t="s">
+        <v>491</v>
       </c>
       <c r="D152" t="s">
-        <v>532</v>
+        <v>492</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>545</v>
-      </c>
-      <c r="C153" s="9" t="s">
-        <v>546</v>
+        <v>523</v>
+      </c>
+      <c r="C153" t="s">
+        <v>493</v>
       </c>
       <c r="D153" t="s">
-        <v>547</v>
+        <v>494</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>548</v>
-      </c>
-      <c r="C154" s="9" t="s">
-        <v>552</v>
+        <v>495</v>
+      </c>
+      <c r="C154" t="s">
+        <v>496</v>
       </c>
       <c r="D154" t="s">
-        <v>550</v>
+        <v>497</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>549</v>
-      </c>
-      <c r="C155" s="9" t="s">
-        <v>551</v>
+        <v>498</v>
+      </c>
+      <c r="C155" t="s">
+        <v>500</v>
       </c>
       <c r="D155" t="s">
-        <v>551</v>
+        <v>501</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>553</v>
-      </c>
-      <c r="C156" s="9" t="s">
-        <v>559</v>
+        <v>499</v>
+      </c>
+      <c r="C156" t="s">
+        <v>502</v>
       </c>
       <c r="D156" t="s">
-        <v>558</v>
+        <v>530</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>554</v>
+        <v>516</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>556</v>
+        <v>517</v>
       </c>
       <c r="D157" t="s">
-        <v>557</v>
+        <v>518</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>560</v>
+        <v>520</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>561</v>
+        <v>521</v>
       </c>
       <c r="D158" t="s">
-        <v>562</v>
+        <v>522</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>555</v>
+        <v>524</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>579</v>
+        <v>525</v>
       </c>
       <c r="D159" t="s">
-        <v>580</v>
+        <v>526</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>563</v>
+        <v>527</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>565</v>
+        <v>529</v>
       </c>
       <c r="D160" t="s">
-        <v>567</v>
+        <v>528</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>564</v>
+        <v>533</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>566</v>
+        <v>502</v>
       </c>
       <c r="D161" t="s">
-        <v>568</v>
+        <v>530</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>575</v>
+        <v>534</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>569</v>
+        <v>531</v>
       </c>
       <c r="D162" t="s">
-        <v>572</v>
+        <v>532</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>576</v>
+        <v>545</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>573</v>
+        <v>546</v>
       </c>
       <c r="D163" t="s">
-        <v>574</v>
+        <v>547</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>577</v>
+        <v>548</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>570</v>
-      </c>
-      <c r="D164" s="9" t="s">
-        <v>570</v>
+        <v>552</v>
+      </c>
+      <c r="D164" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>578</v>
+        <v>549</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>571</v>
-      </c>
-      <c r="D165" s="9" t="s">
-        <v>571</v>
+        <v>551</v>
+      </c>
+      <c r="D165" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>581</v>
+        <v>553</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>582</v>
-      </c>
-      <c r="D166" s="9" t="s">
-        <v>583</v>
+        <v>559</v>
+      </c>
+      <c r="D166" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>588</v>
+        <v>554</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>591</v>
-      </c>
-      <c r="D167" s="9" t="s">
-        <v>592</v>
+        <v>556</v>
+      </c>
+      <c r="D167" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>589</v>
+        <v>560</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>590</v>
-      </c>
-      <c r="D168" s="9" t="s">
-        <v>593</v>
+        <v>561</v>
+      </c>
+      <c r="D168" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B169" s="3"/>
-      <c r="C169" s="3"/>
-      <c r="D169" s="3"/>
+      <c r="A169" t="s">
+        <v>555</v>
+      </c>
+      <c r="C169" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="D169" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>694</v>
-      </c>
-      <c r="C170" t="s">
-        <v>695</v>
+        <v>563</v>
+      </c>
+      <c r="C170" s="9" t="s">
+        <v>565</v>
       </c>
       <c r="D170" t="s">
-        <v>696</v>
+        <v>567</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>690</v>
-      </c>
-      <c r="C171" t="s">
-        <v>697</v>
+        <v>564</v>
+      </c>
+      <c r="C171" s="9" t="s">
+        <v>566</v>
       </c>
       <c r="D171" t="s">
-        <v>699</v>
+        <v>568</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>693</v>
-      </c>
-      <c r="C172" t="s">
-        <v>698</v>
+        <v>575</v>
+      </c>
+      <c r="C172" s="9" t="s">
+        <v>569</v>
       </c>
       <c r="D172" t="s">
-        <v>700</v>
+        <v>572</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>701</v>
-      </c>
-      <c r="C173" s="7" t="s">
-        <v>691</v>
-      </c>
-      <c r="D173" s="7" t="s">
-        <v>692</v>
+        <v>576</v>
+      </c>
+      <c r="C173" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="D173" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>140</v>
-      </c>
-      <c r="B174" t="s">
-        <v>137</v>
-      </c>
-      <c r="C174" t="s">
-        <v>138</v>
-      </c>
-      <c r="D174" t="s">
-        <v>139</v>
+        <v>577</v>
+      </c>
+      <c r="C174" s="9" t="s">
+        <v>570</v>
+      </c>
+      <c r="D174" s="9" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>141</v>
-      </c>
-      <c r="B175" t="s">
-        <v>142</v>
-      </c>
-      <c r="C175" t="s">
-        <v>150</v>
-      </c>
-      <c r="D175" t="s">
-        <v>151</v>
+        <v>578</v>
+      </c>
+      <c r="C175" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="D175" s="9" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>147</v>
-      </c>
-      <c r="B176" t="s">
-        <v>137</v>
-      </c>
-      <c r="C176" t="s">
-        <v>683</v>
-      </c>
-      <c r="D176" t="s">
-        <v>684</v>
+        <v>581</v>
+      </c>
+      <c r="C176" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="D176" s="9" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>143</v>
-      </c>
-      <c r="B177" t="s">
-        <v>142</v>
-      </c>
-      <c r="C177" t="s">
-        <v>149</v>
-      </c>
-      <c r="D177" t="s">
-        <v>148</v>
+        <v>588</v>
+      </c>
+      <c r="C177" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="D177" s="9" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>144</v>
-      </c>
-      <c r="B178" t="s">
-        <v>145</v>
-      </c>
-      <c r="C178" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D178" s="7" t="s">
-        <v>146</v>
+        <v>589</v>
+      </c>
+      <c r="C178" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="D178" s="9" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>681</v>
-      </c>
-      <c r="C179" t="s">
-        <v>680</v>
-      </c>
-      <c r="D179" t="s">
-        <v>680</v>
-      </c>
+      <c r="A179" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B179" s="3"/>
+      <c r="C179" s="3"/>
+      <c r="D179" s="3"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>682</v>
+        <v>694</v>
       </c>
       <c r="C180" t="s">
-        <v>686</v>
+        <v>695</v>
       </c>
       <c r="D180" t="s">
-        <v>685</v>
+        <v>696</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="C181" t="s">
-        <v>688</v>
+        <v>697</v>
       </c>
       <c r="D181" t="s">
-        <v>689</v>
+        <v>699</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B182" s="6"/>
-      <c r="C182" s="6"/>
-      <c r="D182" s="6"/>
+      <c r="A182" t="s">
+        <v>693</v>
+      </c>
+      <c r="C182" t="s">
+        <v>698</v>
+      </c>
+      <c r="D182" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>47</v>
-      </c>
-      <c r="B183" t="s">
-        <v>8</v>
-      </c>
-      <c r="C183" t="s">
-        <v>48</v>
-      </c>
-      <c r="D183" t="s">
-        <v>49</v>
+        <v>701</v>
+      </c>
+      <c r="C183" s="7" t="s">
+        <v>691</v>
+      </c>
+      <c r="D183" s="7" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="B184" t="s">
-        <v>8</v>
+        <v>137</v>
       </c>
       <c r="C184" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="D184" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>597</v>
+        <v>141</v>
+      </c>
+      <c r="B185" t="s">
+        <v>142</v>
       </c>
       <c r="C185" t="s">
-        <v>598</v>
+        <v>150</v>
       </c>
       <c r="D185" t="s">
-        <v>599</v>
+        <v>151</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>600</v>
+        <v>147</v>
+      </c>
+      <c r="B186" t="s">
+        <v>137</v>
       </c>
       <c r="C186" t="s">
-        <v>601</v>
+        <v>683</v>
       </c>
       <c r="D186" t="s">
-        <v>602</v>
+        <v>684</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>632</v>
+        <v>143</v>
+      </c>
+      <c r="B187" t="s">
+        <v>142</v>
       </c>
       <c r="C187" t="s">
-        <v>634</v>
+        <v>149</v>
       </c>
       <c r="D187" t="s">
-        <v>635</v>
+        <v>148</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>633</v>
-      </c>
-      <c r="C188" t="s">
-        <v>637</v>
-      </c>
-      <c r="D188" t="s">
-        <v>636</v>
+        <v>144</v>
+      </c>
+      <c r="B188" t="s">
+        <v>145</v>
+      </c>
+      <c r="C188" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D188" s="7" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>794</v>
+        <v>681</v>
       </c>
       <c r="C189" t="s">
-        <v>795</v>
+        <v>680</v>
       </c>
       <c r="D189" t="s">
-        <v>796</v>
+        <v>680</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>50</v>
-      </c>
-      <c r="B190" t="s">
-        <v>8</v>
+        <v>682</v>
       </c>
       <c r="C190" t="s">
-        <v>51</v>
+        <v>686</v>
       </c>
       <c r="D190" t="s">
-        <v>52</v>
+        <v>685</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>53</v>
-      </c>
-      <c r="B191" t="s">
-        <v>8</v>
+        <v>687</v>
       </c>
       <c r="C191" t="s">
-        <v>54</v>
+        <v>688</v>
       </c>
       <c r="D191" t="s">
-        <v>222</v>
+        <v>689</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>217</v>
-      </c>
-      <c r="B192" t="s">
-        <v>8</v>
-      </c>
-      <c r="C192" t="s">
-        <v>218</v>
-      </c>
-      <c r="D192" t="s">
-        <v>218</v>
-      </c>
+      <c r="A192" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B192" s="6"/>
+      <c r="C192" s="6"/>
+      <c r="D192" s="6"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>349</v>
+        <v>47</v>
       </c>
       <c r="B193" t="s">
         <v>8</v>
       </c>
       <c r="C193" t="s">
-        <v>614</v>
+        <v>48</v>
       </c>
       <c r="D193" t="s">
-        <v>616</v>
+        <v>49</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>615</v>
+        <v>95</v>
+      </c>
+      <c r="B194" t="s">
+        <v>8</v>
       </c>
       <c r="C194" t="s">
-        <v>613</v>
+        <v>96</v>
       </c>
       <c r="D194" t="s">
-        <v>617</v>
+        <v>97</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>155</v>
-      </c>
-      <c r="B195" t="s">
-        <v>8</v>
+        <v>597</v>
       </c>
       <c r="C195" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="D195" t="s">
-        <v>156</v>
+        <v>599</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>165</v>
-      </c>
-      <c r="B196" t="s">
-        <v>8</v>
+        <v>600</v>
       </c>
       <c r="C196" t="s">
-        <v>595</v>
+        <v>601</v>
       </c>
       <c r="D196" t="s">
-        <v>166</v>
+        <v>602</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>173</v>
-      </c>
-      <c r="B197" t="s">
-        <v>8</v>
+        <v>632</v>
       </c>
       <c r="C197" t="s">
-        <v>596</v>
+        <v>634</v>
       </c>
       <c r="D197" t="s">
-        <v>174</v>
+        <v>635</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>603</v>
-      </c>
-      <c r="B198" t="s">
-        <v>8</v>
+        <v>633</v>
       </c>
       <c r="C198" t="s">
-        <v>604</v>
+        <v>637</v>
       </c>
       <c r="D198" t="s">
-        <v>605</v>
+        <v>636</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>610</v>
-      </c>
-      <c r="B199" t="s">
-        <v>8</v>
+        <v>794</v>
       </c>
       <c r="C199" t="s">
-        <v>608</v>
+        <v>795</v>
       </c>
       <c r="D199" t="s">
-        <v>606</v>
+        <v>796</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>611</v>
+        <v>50</v>
       </c>
       <c r="B200" t="s">
         <v>8</v>
       </c>
       <c r="C200" t="s">
-        <v>609</v>
+        <v>51</v>
       </c>
       <c r="D200" t="s">
-        <v>607</v>
+        <v>52</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>154</v>
+        <v>53</v>
       </c>
       <c r="B201" t="s">
         <v>8</v>
       </c>
       <c r="C201" t="s">
-        <v>190</v>
+        <v>54</v>
       </c>
       <c r="D201" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>55</v>
+        <v>217</v>
       </c>
       <c r="B202" t="s">
         <v>8</v>
       </c>
       <c r="C202" t="s">
-        <v>56</v>
+        <v>218</v>
       </c>
       <c r="D202" t="s">
-        <v>57</v>
+        <v>218</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>162</v>
+        <v>349</v>
       </c>
       <c r="B203" t="s">
         <v>8</v>
       </c>
       <c r="C203" t="s">
-        <v>157</v>
+        <v>614</v>
       </c>
       <c r="D203" t="s">
-        <v>16</v>
+        <v>616</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>167</v>
-      </c>
-      <c r="B204" t="s">
-        <v>8</v>
+        <v>615</v>
       </c>
       <c r="C204" t="s">
-        <v>168</v>
+        <v>613</v>
       </c>
       <c r="D204" t="s">
-        <v>169</v>
+        <v>617</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>58</v>
-      </c>
-      <c r="B205" t="s">
-        <v>8</v>
+        <v>812</v>
       </c>
       <c r="C205" t="s">
-        <v>59</v>
+        <v>813</v>
       </c>
       <c r="D205" t="s">
-        <v>60</v>
+        <v>814</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B206" t="s">
         <v>8</v>
       </c>
       <c r="C206" t="s">
-        <v>163</v>
+        <v>594</v>
       </c>
       <c r="D206" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B207" t="s">
         <v>8</v>
       </c>
       <c r="C207" t="s">
-        <v>171</v>
+        <v>595</v>
       </c>
       <c r="D207" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>61</v>
+        <v>173</v>
       </c>
       <c r="B208" t="s">
         <v>8</v>
       </c>
       <c r="C208" t="s">
-        <v>62</v>
+        <v>596</v>
       </c>
       <c r="D208" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>160</v>
+        <v>603</v>
       </c>
       <c r="B209" t="s">
         <v>8</v>
       </c>
       <c r="C209" t="s">
-        <v>158</v>
+        <v>604</v>
       </c>
       <c r="D209" t="s">
-        <v>159</v>
+        <v>605</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>175</v>
+        <v>610</v>
       </c>
       <c r="B210" t="s">
         <v>8</v>
       </c>
       <c r="C210" t="s">
-        <v>176</v>
+        <v>608</v>
       </c>
       <c r="D210" t="s">
-        <v>177</v>
+        <v>606</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>194</v>
+        <v>611</v>
       </c>
       <c r="B211" t="s">
         <v>8</v>
       </c>
       <c r="C211" t="s">
-        <v>192</v>
+        <v>609</v>
       </c>
       <c r="D211" t="s">
-        <v>193</v>
+        <v>607</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>195</v>
+        <v>154</v>
       </c>
       <c r="B212" t="s">
         <v>8</v>
       </c>
       <c r="C212" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D212" t="s">
-        <v>105</v>
+        <v>191</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>197</v>
+        <v>55</v>
       </c>
       <c r="B213" t="s">
         <v>8</v>
       </c>
       <c r="C213" t="s">
-        <v>198</v>
+        <v>56</v>
       </c>
       <c r="D213" t="s">
-        <v>199</v>
+        <v>57</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>284</v>
+        <v>162</v>
+      </c>
+      <c r="B214" t="s">
+        <v>8</v>
       </c>
       <c r="C214" t="s">
-        <v>285</v>
+        <v>157</v>
       </c>
       <c r="D214" t="s">
-        <v>286</v>
+        <v>16</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>67</v>
+        <v>167</v>
       </c>
       <c r="B215" t="s">
         <v>8</v>
       </c>
       <c r="C215" t="s">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="D215" t="s">
-        <v>69</v>
+        <v>169</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B216" t="s">
         <v>8</v>
       </c>
       <c r="C216" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="D216" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>437</v>
+        <v>161</v>
+      </c>
+      <c r="B217" t="s">
+        <v>8</v>
       </c>
       <c r="C217" t="s">
-        <v>438</v>
+        <v>163</v>
       </c>
       <c r="D217" t="s">
-        <v>439</v>
+        <v>164</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="B218" t="s">
         <v>8</v>
       </c>
       <c r="C218" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="D218" t="s">
-        <v>201</v>
+        <v>172</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>178</v>
+        <v>61</v>
       </c>
       <c r="B219" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C219" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="D219" t="s">
-        <v>180</v>
+        <v>63</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>202</v>
+        <v>160</v>
       </c>
       <c r="B220" t="s">
         <v>8</v>
       </c>
       <c r="C220" t="s">
-        <v>204</v>
+        <v>158</v>
       </c>
       <c r="D220" t="s">
-        <v>205</v>
+        <v>159</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="B221" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C221" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="D221" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>229</v>
+        <v>194</v>
       </c>
       <c r="B222" t="s">
         <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>225</v>
+        <v>192</v>
       </c>
       <c r="D222" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
       <c r="B223" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
       <c r="D223" t="s">
-        <v>228</v>
+        <v>105</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="B224" t="s">
         <v>8</v>
       </c>
       <c r="C224" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D224" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>212</v>
-      </c>
-      <c r="B225" t="s">
-        <v>179</v>
+        <v>284</v>
       </c>
       <c r="C225" t="s">
-        <v>214</v>
+        <v>285</v>
       </c>
       <c r="D225" t="s">
-        <v>216</v>
+        <v>286</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="B226" t="s">
         <v>8</v>
       </c>
       <c r="C226" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
       <c r="D226" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>208</v>
+        <v>7</v>
       </c>
       <c r="B227" t="s">
         <v>8</v>
       </c>
       <c r="C227" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="D227" t="s">
-        <v>210</v>
+        <v>10</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>14</v>
-      </c>
-      <c r="B228" t="s">
-        <v>8</v>
+        <v>437</v>
       </c>
       <c r="C228" t="s">
-        <v>15</v>
+        <v>438</v>
       </c>
       <c r="D228" t="s">
-        <v>16</v>
+        <v>439</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>385</v>
+        <v>200</v>
+      </c>
+      <c r="B229" t="s">
+        <v>8</v>
       </c>
       <c r="C229" t="s">
-        <v>386</v>
+        <v>200</v>
       </c>
       <c r="D229" t="s">
-        <v>387</v>
+        <v>201</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>503</v>
+        <v>178</v>
+      </c>
+      <c r="B230" t="s">
+        <v>179</v>
       </c>
       <c r="C230" t="s">
-        <v>504</v>
+        <v>178</v>
       </c>
       <c r="D230" t="s">
-        <v>505</v>
+        <v>180</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>426</v>
+        <v>202</v>
       </c>
       <c r="B231" t="s">
-        <v>316</v>
+        <v>8</v>
       </c>
       <c r="C231" t="s">
-        <v>317</v>
+        <v>204</v>
       </c>
       <c r="D231" t="s">
-        <v>318</v>
+        <v>205</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>445</v>
+        <v>203</v>
+      </c>
+      <c r="B232" t="s">
+        <v>179</v>
       </c>
       <c r="C232" t="s">
-        <v>457</v>
+        <v>206</v>
       </c>
       <c r="D232" t="s">
-        <v>469</v>
+        <v>207</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>446</v>
+        <v>229</v>
+      </c>
+      <c r="B233" t="s">
+        <v>8</v>
       </c>
       <c r="C233" t="s">
-        <v>458</v>
+        <v>225</v>
       </c>
       <c r="D233" t="s">
-        <v>470</v>
+        <v>227</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>447</v>
+        <v>230</v>
+      </c>
+      <c r="B234" t="s">
+        <v>179</v>
       </c>
       <c r="C234" t="s">
-        <v>459</v>
+        <v>226</v>
       </c>
       <c r="D234" t="s">
-        <v>471</v>
+        <v>228</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>448</v>
+        <v>211</v>
+      </c>
+      <c r="B235" t="s">
+        <v>8</v>
       </c>
       <c r="C235" t="s">
-        <v>460</v>
+        <v>213</v>
       </c>
       <c r="D235" t="s">
-        <v>472</v>
+        <v>215</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>449</v>
+        <v>212</v>
+      </c>
+      <c r="B236" t="s">
+        <v>179</v>
       </c>
       <c r="C236" t="s">
-        <v>461</v>
+        <v>214</v>
       </c>
       <c r="D236" t="s">
-        <v>474</v>
+        <v>216</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>450</v>
+        <v>106</v>
+      </c>
+      <c r="B237" t="s">
+        <v>8</v>
       </c>
       <c r="C237" t="s">
-        <v>462</v>
+        <v>107</v>
       </c>
       <c r="D237" t="s">
-        <v>473</v>
+        <v>108</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>451</v>
+        <v>208</v>
+      </c>
+      <c r="B238" t="s">
+        <v>8</v>
       </c>
       <c r="C238" t="s">
-        <v>463</v>
+        <v>209</v>
       </c>
       <c r="D238" t="s">
-        <v>475</v>
+        <v>210</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>452</v>
+        <v>14</v>
+      </c>
+      <c r="B239" t="s">
+        <v>8</v>
       </c>
       <c r="C239" t="s">
-        <v>464</v>
+        <v>15</v>
       </c>
       <c r="D239" t="s">
-        <v>476</v>
+        <v>16</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>453</v>
+        <v>385</v>
       </c>
       <c r="C240" t="s">
-        <v>465</v>
+        <v>386</v>
       </c>
       <c r="D240" t="s">
-        <v>477</v>
+        <v>387</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>454</v>
+        <v>503</v>
       </c>
       <c r="C241" t="s">
-        <v>466</v>
+        <v>504</v>
       </c>
       <c r="D241" t="s">
-        <v>478</v>
+        <v>505</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>455</v>
+        <v>426</v>
+      </c>
+      <c r="B242" t="s">
+        <v>316</v>
       </c>
       <c r="C242" t="s">
-        <v>467</v>
+        <v>317</v>
       </c>
       <c r="D242" t="s">
-        <v>479</v>
+        <v>318</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
       <c r="C243" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="D243" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>508</v>
+        <v>446</v>
       </c>
       <c r="C244" t="s">
-        <v>507</v>
+        <v>458</v>
       </c>
       <c r="D244" t="s">
-        <v>506</v>
+        <v>470</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>584</v>
+        <v>447</v>
       </c>
       <c r="C245" t="s">
-        <v>2</v>
+        <v>459</v>
       </c>
       <c r="D245" t="s">
-        <v>585</v>
+        <v>471</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>586</v>
+        <v>448</v>
       </c>
       <c r="C246" t="s">
-        <v>587</v>
+        <v>460</v>
       </c>
       <c r="D246" t="s">
-        <v>3</v>
+        <v>472</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A247" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B247" s="2"/>
-      <c r="C247" s="2"/>
-      <c r="D247" s="2"/>
+      <c r="A247" t="s">
+        <v>449</v>
+      </c>
+      <c r="C247" t="s">
+        <v>461</v>
+      </c>
+      <c r="D247" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>110</v>
-      </c>
-      <c r="B248" t="s">
-        <v>109</v>
+        <v>450</v>
       </c>
       <c r="C248" t="s">
-        <v>129</v>
+        <v>462</v>
       </c>
       <c r="D248" t="s">
-        <v>128</v>
+        <v>473</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>127</v>
-      </c>
-      <c r="B249" t="s">
-        <v>109</v>
+        <v>451</v>
       </c>
       <c r="C249" t="s">
-        <v>130</v>
+        <v>463</v>
       </c>
       <c r="D249" t="s">
-        <v>133</v>
+        <v>475</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>111</v>
-      </c>
-      <c r="B250" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
       <c r="C250" t="s">
-        <v>112</v>
+        <v>464</v>
       </c>
       <c r="D250" t="s">
-        <v>119</v>
+        <v>476</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>116</v>
-      </c>
-      <c r="B251" t="s">
-        <v>109</v>
+        <v>453</v>
       </c>
       <c r="C251" t="s">
-        <v>117</v>
+        <v>465</v>
       </c>
       <c r="D251" t="s">
-        <v>118</v>
+        <v>477</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>113</v>
-      </c>
-      <c r="B252" t="s">
-        <v>109</v>
+        <v>454</v>
       </c>
       <c r="C252" t="s">
-        <v>114</v>
+        <v>466</v>
       </c>
       <c r="D252" t="s">
-        <v>115</v>
+        <v>478</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>120</v>
-      </c>
-      <c r="B253" t="s">
-        <v>109</v>
+        <v>455</v>
       </c>
       <c r="C253" t="s">
-        <v>132</v>
+        <v>467</v>
       </c>
       <c r="D253" t="s">
-        <v>121</v>
+        <v>479</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>122</v>
-      </c>
-      <c r="B254" t="s">
-        <v>109</v>
+        <v>456</v>
       </c>
       <c r="C254" t="s">
-        <v>131</v>
+        <v>468</v>
       </c>
       <c r="D254" t="s">
-        <v>123</v>
+        <v>480</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>124</v>
-      </c>
-      <c r="B255" t="s">
-        <v>109</v>
+        <v>508</v>
       </c>
       <c r="C255" t="s">
-        <v>125</v>
+        <v>507</v>
       </c>
       <c r="D255" t="s">
-        <v>126</v>
+        <v>506</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B256" s="3"/>
-      <c r="C256" s="3"/>
-      <c r="D256" s="3"/>
+      <c r="A256" t="s">
+        <v>584</v>
+      </c>
+      <c r="C256" t="s">
+        <v>2</v>
+      </c>
+      <c r="D256" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>70</v>
-      </c>
-      <c r="B257" t="s">
-        <v>71</v>
+        <v>586</v>
       </c>
       <c r="C257" t="s">
-        <v>352</v>
+        <v>587</v>
       </c>
       <c r="D257" t="s">
-        <v>353</v>
+        <v>3</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
-        <v>350</v>
-      </c>
-      <c r="B258" t="s">
-        <v>71</v>
-      </c>
-      <c r="C258" t="s">
-        <v>348</v>
-      </c>
-      <c r="D258" t="s">
-        <v>351</v>
-      </c>
+      <c r="A258" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B258" s="2"/>
+      <c r="C258" s="2"/>
+      <c r="D258" s="2"/>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="B259" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="C259" t="s">
-        <v>354</v>
+        <v>129</v>
       </c>
       <c r="D259" t="s">
-        <v>355</v>
+        <v>128</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>356</v>
+        <v>127</v>
       </c>
       <c r="B260" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="C260" t="s">
-        <v>357</v>
+        <v>130</v>
       </c>
       <c r="D260" t="s">
-        <v>358</v>
+        <v>133</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="B261" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="C261" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="D261" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>618</v>
+        <v>116</v>
+      </c>
+      <c r="B262" t="s">
+        <v>109</v>
       </c>
       <c r="C262" t="s">
-        <v>612</v>
+        <v>117</v>
       </c>
       <c r="D262" t="s">
-        <v>619</v>
+        <v>118</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
+        <v>113</v>
+      </c>
+      <c r="B263" t="s">
+        <v>109</v>
+      </c>
+      <c r="C263" t="s">
+        <v>114</v>
+      </c>
+      <c r="D263" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>120</v>
+      </c>
+      <c r="B264" t="s">
+        <v>109</v>
+      </c>
+      <c r="C264" t="s">
+        <v>132</v>
+      </c>
+      <c r="D264" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>122</v>
+      </c>
+      <c r="B265" t="s">
+        <v>109</v>
+      </c>
+      <c r="C265" t="s">
+        <v>131</v>
+      </c>
+      <c r="D265" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>124</v>
+      </c>
+      <c r="B266" t="s">
+        <v>109</v>
+      </c>
+      <c r="C266" t="s">
+        <v>125</v>
+      </c>
+      <c r="D266" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B267" s="3"/>
+      <c r="C267" s="3"/>
+      <c r="D267" s="3"/>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>70</v>
+      </c>
+      <c r="B268" t="s">
+        <v>71</v>
+      </c>
+      <c r="C268" t="s">
+        <v>352</v>
+      </c>
+      <c r="D268" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>350</v>
+      </c>
+      <c r="B269" t="s">
+        <v>71</v>
+      </c>
+      <c r="C269" t="s">
+        <v>348</v>
+      </c>
+      <c r="D269" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>153</v>
+      </c>
+      <c r="B270" t="s">
+        <v>71</v>
+      </c>
+      <c r="C270" t="s">
+        <v>354</v>
+      </c>
+      <c r="D270" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>356</v>
+      </c>
+      <c r="B271" t="s">
+        <v>71</v>
+      </c>
+      <c r="C271" t="s">
+        <v>357</v>
+      </c>
+      <c r="D271" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>72</v>
+      </c>
+      <c r="B272" t="s">
+        <v>71</v>
+      </c>
+      <c r="C272" t="s">
+        <v>73</v>
+      </c>
+      <c r="D272" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>618</v>
+      </c>
+      <c r="C273" t="s">
+        <v>612</v>
+      </c>
+      <c r="D273" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
         <v>629</v>
       </c>
-      <c r="C263" t="s">
+      <c r="C274" t="s">
         <v>630</v>
       </c>
-      <c r="D263" t="s">
+      <c r="D274" t="s">
         <v>631</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>815</v>
+      </c>
+      <c r="C275" t="s">
+        <v>816</v>
+      </c>
+      <c r="D275" t="s">
+        <v>817</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C173" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
-    <hyperlink ref="D173" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
+    <hyperlink ref="C183" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
+    <hyperlink ref="D183" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
continuous data download is close!
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79929A7B-C20F-47FA-A38B-63E962ADE613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3DA642-3008-4BFC-9F98-B1317A4111CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="853">
   <si>
     <t>id</t>
   </si>
@@ -758,9 +758,6 @@
     <t>dl_num_rows</t>
   </si>
   <si>
-    <t>Number of rows that will be returned:</t>
-  </si>
-  <si>
     <t>Nombre de rangées à télécharger:</t>
   </si>
   <si>
@@ -791,9 +788,6 @@
     <t>modal message</t>
   </si>
   <si>
-    <t>Subset of data (3 rows per timeseries)</t>
-  </si>
-  <si>
     <t>Journalière (avec statistiques)</t>
   </si>
   <si>
@@ -803,15 +797,6 @@
     <t>Sous-ensemble de données (3 lignes par série temporelle)</t>
   </si>
   <si>
-    <t>extra_tbl_msg</t>
-  </si>
-  <si>
-    <t>Tables for grades and approvals will also be included as part of your download.</t>
-  </si>
-  <si>
-    <t>Des tableaux pour les notes de qualité et les approbations seront également inclus dans votre téléchargement.</t>
-  </si>
-  <si>
     <t>date_range_select</t>
   </si>
   <si>
@@ -863,18 +848,6 @@
     <t>loc_meta_msg</t>
   </si>
   <si>
-    <t>Hourly + daily</t>
-  </si>
-  <si>
-    <t>Max + daily</t>
-  </si>
-  <si>
-    <t>Horaire + journalière</t>
-  </si>
-  <si>
-    <t>Maximum + journalière</t>
-  </si>
-  <si>
     <t>Résolution:</t>
   </si>
   <si>
@@ -1970,18 +1943,12 @@
     <t>view_data1</t>
   </si>
   <si>
-    <t>view_data2</t>
-  </si>
-  <si>
     <t>View</t>
   </si>
   <si>
     <t>sample results</t>
   </si>
   <si>
-    <t>Voir les résultats de</t>
-  </si>
-  <si>
     <t>échantillons</t>
   </si>
   <si>
@@ -1998,9 +1965,6 @@
   </si>
   <si>
     <t>dl_num_results</t>
-  </si>
-  <si>
-    <t>Number of results that will be returned:</t>
   </si>
   <si>
     <t>Nombre de résultats à télécharger:</t>
@@ -2092,12 +2056,6 @@
     <t>Réinitialiser les filtres</t>
   </si>
   <si>
-    <t>Subset of location metadata (up to first three rows)</t>
-  </si>
-  <si>
-    <t>Sous-ensemble des métadonnées des sites (jusqu'aux trois premières lignes)</t>
-  </si>
-  <si>
     <t>Application version</t>
   </si>
   <si>
@@ -2594,6 +2552,69 @@
   </si>
   <si>
     <t>Cette sélection ne correspond à aucune série temporelle, la sélection du rythme d'enregistrement a été réinitialisé à sa valeur précédente.</t>
+  </si>
+  <si>
+    <t>dl_additional_data</t>
+  </si>
+  <si>
+    <t>Tables for grades, approvals, and qualifiers will also be included as part of your download.</t>
+  </si>
+  <si>
+    <t>Des tableaux pour les qualificatifs, cotes, et niveaux d'approbations feront parti de votre téléchargement.</t>
+  </si>
+  <si>
+    <t>continuous_subset_msg</t>
+  </si>
+  <si>
+    <t>Subset of daily mean data (first and last result per timeseries)</t>
+  </si>
+  <si>
+    <t>Sous-ensemble des moyennes journalières (premier et dernier résultat par série temporelle)</t>
+  </si>
+  <si>
+    <t>Subset of location metadata (up to first three locations)</t>
+  </si>
+  <si>
+    <t>Sous-ensemble des métadonnées des sites (jusqu'aux trois premiers endroits)</t>
+  </si>
+  <si>
+    <t>Hourly + daily (with stats)</t>
+  </si>
+  <si>
+    <t>Max + daily (with stats)</t>
+  </si>
+  <si>
+    <t>Maximum + journalière (avec stats)</t>
+  </si>
+  <si>
+    <t>Horaire + journalière (avec stats)</t>
+  </si>
+  <si>
+    <t>Number of rows which will be returned:</t>
+  </si>
+  <si>
+    <t>Number of results which will be returned:</t>
+  </si>
+  <si>
+    <t>Subset of data (first and last measurement per timeseries)</t>
+  </si>
+  <si>
+    <t>view_data2_continuous</t>
+  </si>
+  <si>
+    <t>text, part2</t>
+  </si>
+  <si>
+    <t>timeseries details</t>
+  </si>
+  <si>
+    <t>view_data2_discrete</t>
+  </si>
+  <si>
+    <t>Voir les détails de</t>
+  </si>
+  <si>
+    <t>séries temporelles</t>
   </si>
 </sst>
 </file>
@@ -3538,10 +3559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D275"/>
+  <dimension ref="A1:D277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3572,7 +3593,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -3586,18 +3607,18 @@
         <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="C3" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="D3" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>705</v>
+        <v>691</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3608,7 +3629,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>753</v>
+        <v>739</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -3619,178 +3640,178 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>773</v>
+        <v>759</v>
       </c>
       <c r="B6" t="s">
-        <v>770</v>
+        <v>756</v>
       </c>
       <c r="C6" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="D6" t="s">
-        <v>708</v>
+        <v>694</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>777</v>
+        <v>763</v>
       </c>
       <c r="B7" t="s">
-        <v>771</v>
+        <v>757</v>
       </c>
       <c r="C7" t="s">
-        <v>772</v>
+        <v>758</v>
       </c>
       <c r="D7" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>778</v>
+        <v>764</v>
       </c>
       <c r="B8" t="s">
-        <v>774</v>
+        <v>760</v>
       </c>
       <c r="C8" t="s">
-        <v>775</v>
+        <v>761</v>
       </c>
       <c r="D8" t="s">
-        <v>776</v>
+        <v>762</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>714</v>
+        <v>700</v>
       </c>
       <c r="B9" t="s">
-        <v>752</v>
+        <v>738</v>
       </c>
       <c r="C9" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="D9" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>717</v>
+        <v>703</v>
       </c>
       <c r="B10" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
       <c r="C10" t="s">
-        <v>720</v>
+        <v>706</v>
       </c>
       <c r="D10" t="s">
-        <v>721</v>
+        <v>707</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>722</v>
+        <v>708</v>
       </c>
       <c r="B11" t="s">
-        <v>751</v>
+        <v>737</v>
       </c>
       <c r="C11" t="s">
-        <v>723</v>
+        <v>709</v>
       </c>
       <c r="D11" t="s">
-        <v>724</v>
+        <v>710</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>725</v>
+        <v>711</v>
       </c>
       <c r="B12" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="C12" t="s">
-        <v>726</v>
+        <v>712</v>
       </c>
       <c r="D12" t="s">
-        <v>727</v>
+        <v>713</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>730</v>
+        <v>716</v>
       </c>
       <c r="B13" t="s">
-        <v>750</v>
+        <v>736</v>
       </c>
       <c r="C13" t="s">
-        <v>731</v>
+        <v>717</v>
       </c>
       <c r="D13" t="s">
-        <v>732</v>
+        <v>718</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>733</v>
+        <v>719</v>
       </c>
       <c r="B14" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="C14" t="s">
-        <v>738</v>
+        <v>724</v>
       </c>
       <c r="D14" t="s">
-        <v>737</v>
+        <v>723</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>734</v>
+        <v>720</v>
       </c>
       <c r="B15" t="s">
-        <v>747</v>
+        <v>733</v>
       </c>
       <c r="C15" t="s">
-        <v>739</v>
+        <v>725</v>
       </c>
       <c r="D15" t="s">
-        <v>740</v>
+        <v>726</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>735</v>
+        <v>721</v>
       </c>
       <c r="B16" t="s">
-        <v>746</v>
+        <v>732</v>
       </c>
       <c r="C16" t="s">
-        <v>741</v>
+        <v>727</v>
       </c>
       <c r="D16" t="s">
-        <v>742</v>
+        <v>728</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>736</v>
+        <v>722</v>
       </c>
       <c r="B17" t="s">
-        <v>745</v>
+        <v>731</v>
       </c>
       <c r="C17" t="s">
-        <v>743</v>
+        <v>729</v>
       </c>
       <c r="D17" t="s">
-        <v>744</v>
+        <v>730</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>706</v>
+        <v>692</v>
       </c>
       <c r="B18" t="s">
-        <v>754</v>
+        <v>740</v>
       </c>
       <c r="C18" t="s">
         <v>44</v>
@@ -3801,38 +3822,38 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>728</v>
+        <v>714</v>
       </c>
       <c r="B19" t="s">
-        <v>756</v>
+        <v>742</v>
       </c>
       <c r="C19" t="s">
-        <v>720</v>
+        <v>706</v>
       </c>
       <c r="D19" t="s">
-        <v>721</v>
+        <v>707</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>729</v>
+        <v>715</v>
       </c>
       <c r="B20" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="C20" t="s">
-        <v>723</v>
+        <v>709</v>
       </c>
       <c r="D20" t="s">
-        <v>724</v>
+        <v>710</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>707</v>
+        <v>693</v>
       </c>
       <c r="B21" t="s">
-        <v>758</v>
+        <v>744</v>
       </c>
       <c r="C21" t="s">
         <v>46</v>
@@ -3843,52 +3864,52 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>759</v>
+        <v>745</v>
       </c>
       <c r="B22" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C22" t="s">
-        <v>761</v>
+        <v>747</v>
       </c>
       <c r="D22" t="s">
-        <v>764</v>
+        <v>750</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>760</v>
+        <v>746</v>
       </c>
       <c r="B23" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="C23" t="s">
-        <v>762</v>
+        <v>748</v>
       </c>
       <c r="D23" t="s">
-        <v>763</v>
+        <v>749</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>710</v>
+        <v>696</v>
       </c>
       <c r="B24" t="s">
-        <v>768</v>
+        <v>754</v>
       </c>
       <c r="C24" t="s">
-        <v>711</v>
+        <v>697</v>
       </c>
       <c r="D24" t="s">
-        <v>711</v>
+        <v>697</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>718</v>
+        <v>704</v>
       </c>
       <c r="B25" t="s">
-        <v>767</v>
+        <v>753</v>
       </c>
       <c r="C25" t="s">
         <v>135</v>
@@ -3899,21 +3920,21 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>719</v>
+        <v>705</v>
       </c>
       <c r="B26" t="s">
-        <v>769</v>
+        <v>755</v>
       </c>
       <c r="C26" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="D26" t="s">
-        <v>713</v>
+        <v>699</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>664</v>
+        <v>652</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -3921,30 +3942,30 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>665</v>
+        <v>653</v>
       </c>
       <c r="B28" t="s">
-        <v>666</v>
+        <v>654</v>
       </c>
       <c r="C28" t="s">
-        <v>668</v>
+        <v>656</v>
       </c>
       <c r="D28" t="s">
-        <v>669</v>
+        <v>657</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>667</v>
+        <v>655</v>
       </c>
       <c r="B29" t="s">
-        <v>666</v>
+        <v>654</v>
       </c>
       <c r="C29" t="s">
-        <v>671</v>
+        <v>659</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>670</v>
+        <v>658</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3955,10 +3976,10 @@
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
       <c r="D30" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4033,7 +4054,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -4041,142 +4062,142 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B37" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C37" t="s">
-        <v>540</v>
+        <v>531</v>
       </c>
       <c r="D37" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B38" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="C38" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D38" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B39" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C39" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D39" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>293</v>
+      </c>
+      <c r="B40" t="s">
+        <v>299</v>
+      </c>
+      <c r="C40" t="s">
         <v>302</v>
       </c>
-      <c r="B40" t="s">
-        <v>308</v>
-      </c>
-      <c r="C40" t="s">
-        <v>311</v>
-      </c>
       <c r="D40" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B41" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C41" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="D41" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="B42" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="C42" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="D42" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="B43" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C43" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D43" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
       <c r="B44" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C44" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
       <c r="D44" t="s">
-        <v>544</v>
+        <v>535</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B45" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C45" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="D45" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="B46" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="C46" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="D46" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4256,220 +4277,220 @@
         <v>240</v>
       </c>
       <c r="B53" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C53" t="s">
+        <v>844</v>
+      </c>
+      <c r="D53" t="s">
         <v>241</v>
-      </c>
-      <c r="D53" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>654</v>
+        <v>643</v>
       </c>
       <c r="C54" t="s">
-        <v>655</v>
+        <v>845</v>
       </c>
       <c r="D54" t="s">
-        <v>656</v>
+        <v>644</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>246</v>
+      </c>
+      <c r="B55" t="s">
+        <v>248</v>
+      </c>
+      <c r="C55" t="s">
         <v>247</v>
       </c>
-      <c r="B55" t="s">
-        <v>249</v>
-      </c>
-      <c r="C55" t="s">
-        <v>248</v>
-      </c>
       <c r="D55" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B56" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C56" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D56" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B57" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C57" t="s">
-        <v>276</v>
+        <v>840</v>
       </c>
       <c r="D57" t="s">
-        <v>278</v>
+        <v>843</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B58" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C58" t="s">
-        <v>277</v>
+        <v>841</v>
       </c>
       <c r="D58" t="s">
-        <v>279</v>
+        <v>842</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>650</v>
+        <v>639</v>
       </c>
       <c r="B59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C59" t="s">
-        <v>252</v>
+        <v>846</v>
       </c>
       <c r="D59" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>651</v>
+        <v>640</v>
       </c>
       <c r="B60" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C60" t="s">
-        <v>652</v>
+        <v>641</v>
       </c>
       <c r="D60" t="s">
-        <v>653</v>
+        <v>642</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B61" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C61" t="s">
-        <v>678</v>
+        <v>838</v>
       </c>
       <c r="D61" t="s">
-        <v>679</v>
+        <v>839</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>254</v>
+      </c>
+      <c r="B62" t="s">
+        <v>248</v>
+      </c>
+      <c r="C62" t="s">
+        <v>255</v>
+      </c>
+      <c r="D62" t="s">
         <v>256</v>
-      </c>
-      <c r="B62" t="s">
-        <v>251</v>
-      </c>
-      <c r="C62" t="s">
-        <v>257</v>
-      </c>
-      <c r="D62" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>259</v>
+        <v>807</v>
       </c>
       <c r="B63" t="s">
-        <v>249</v>
+        <v>809</v>
       </c>
       <c r="C63" t="s">
-        <v>260</v>
+        <v>810</v>
       </c>
       <c r="D63" t="s">
-        <v>261</v>
+        <v>812</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>821</v>
+        <v>808</v>
       </c>
       <c r="B64" t="s">
-        <v>823</v>
+        <v>809</v>
       </c>
       <c r="C64" t="s">
-        <v>824</v>
+        <v>811</v>
       </c>
       <c r="D64" t="s">
-        <v>826</v>
+        <v>813</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>822</v>
+        <v>258</v>
       </c>
       <c r="B65" t="s">
-        <v>823</v>
+        <v>248</v>
       </c>
       <c r="C65" t="s">
-        <v>825</v>
+        <v>259</v>
       </c>
       <c r="D65" t="s">
-        <v>827</v>
+        <v>260</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="B66" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C66" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="D66" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="B67" t="s">
         <v>249</v>
       </c>
       <c r="C67" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="D67" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>262</v>
+      </c>
+      <c r="B68" t="s">
+        <v>249</v>
+      </c>
+      <c r="C68" t="s">
+        <v>265</v>
+      </c>
+      <c r="D68" t="s">
         <v>266</v>
-      </c>
-      <c r="B68" t="s">
-        <v>250</v>
-      </c>
-      <c r="C68" t="s">
-        <v>268</v>
-      </c>
-      <c r="D68" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4477,2541 +4498,2563 @@
         <v>267</v>
       </c>
       <c r="B69" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C69" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D69" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B70" t="s">
-        <v>250</v>
+        <v>279</v>
       </c>
       <c r="C70" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="D70" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>287</v>
+        <v>767</v>
       </c>
       <c r="B71" t="s">
-        <v>288</v>
+        <v>768</v>
       </c>
       <c r="C71" t="s">
-        <v>289</v>
+        <v>769</v>
       </c>
       <c r="D71" t="s">
-        <v>290</v>
+        <v>770</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>781</v>
+        <v>771</v>
       </c>
       <c r="B72" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="C72" t="s">
-        <v>783</v>
+        <v>772</v>
       </c>
       <c r="D72" t="s">
-        <v>784</v>
+        <v>774</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>785</v>
+        <v>776</v>
       </c>
       <c r="B73" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="C73" t="s">
-        <v>786</v>
+        <v>773</v>
       </c>
       <c r="D73" t="s">
-        <v>788</v>
+        <v>775</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>790</v>
+        <v>777</v>
       </c>
       <c r="B74" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="C74" t="s">
-        <v>787</v>
+        <v>778</v>
       </c>
       <c r="D74" t="s">
-        <v>789</v>
+        <v>779</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>791</v>
+        <v>816</v>
       </c>
       <c r="B75" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="C75" t="s">
-        <v>792</v>
+        <v>819</v>
       </c>
       <c r="D75" t="s">
-        <v>793</v>
+        <v>820</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>830</v>
+        <v>817</v>
       </c>
       <c r="B76" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="C76" t="s">
-        <v>833</v>
+        <v>824</v>
       </c>
       <c r="D76" t="s">
-        <v>834</v>
+        <v>821</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>831</v>
+        <v>815</v>
       </c>
       <c r="B77" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="C77" t="s">
-        <v>838</v>
+        <v>814</v>
       </c>
       <c r="D77" t="s">
-        <v>835</v>
+        <v>822</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>829</v>
+        <v>818</v>
       </c>
       <c r="B78" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="C78" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="D78" t="s">
-        <v>836</v>
+        <v>823</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="B79" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="C79" t="s">
-        <v>839</v>
+        <v>827</v>
       </c>
       <c r="D79" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>840</v>
+        <v>829</v>
       </c>
       <c r="B80" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="C80" t="s">
-        <v>841</v>
+        <v>830</v>
       </c>
       <c r="D80" t="s">
-        <v>842</v>
+        <v>831</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>843</v>
-      </c>
-      <c r="B81" t="s">
-        <v>782</v>
+        <v>835</v>
       </c>
       <c r="C81" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="D81" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
+      <c r="A82" t="s">
+        <v>832</v>
+      </c>
+      <c r="C82" t="s">
+        <v>833</v>
+      </c>
+      <c r="D82" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>620</v>
-      </c>
-      <c r="C83" t="s">
-        <v>621</v>
-      </c>
-      <c r="D83" t="s">
-        <v>622</v>
-      </c>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>638</v>
+        <v>611</v>
       </c>
       <c r="C84" t="s">
-        <v>639</v>
+        <v>612</v>
       </c>
       <c r="D84" t="s">
-        <v>640</v>
+        <v>613</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>623</v>
-      </c>
-      <c r="B85" t="s">
-        <v>663</v>
+        <v>629</v>
       </c>
       <c r="C85" t="s">
-        <v>624</v>
+        <v>630</v>
       </c>
       <c r="D85" t="s">
-        <v>625</v>
+        <v>631</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>626</v>
+        <v>614</v>
       </c>
       <c r="B86" t="s">
-        <v>663</v>
+        <v>651</v>
       </c>
       <c r="C86" t="s">
-        <v>627</v>
+        <v>615</v>
       </c>
       <c r="D86" t="s">
-        <v>628</v>
+        <v>616</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>183</v>
+        <v>617</v>
       </c>
       <c r="B87" t="s">
-        <v>184</v>
+        <v>651</v>
       </c>
       <c r="C87" t="s">
-        <v>78</v>
+        <v>618</v>
       </c>
       <c r="D87" t="s">
-        <v>79</v>
+        <v>619</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="B88" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C88" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="D88" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>181</v>
+        <v>64</v>
       </c>
       <c r="B89" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C89" t="s">
-        <v>188</v>
+        <v>65</v>
       </c>
       <c r="D89" t="s">
-        <v>189</v>
+        <v>66</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>219</v>
+        <v>181</v>
       </c>
       <c r="B90" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="C90" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="D90" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B91" t="s">
         <v>220</v>
       </c>
       <c r="C91" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="D91" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>703</v>
+        <v>221</v>
+      </c>
+      <c r="B92" t="s">
+        <v>220</v>
       </c>
       <c r="C92" t="s">
-        <v>704</v>
+        <v>237</v>
       </c>
       <c r="D92" t="s">
-        <v>702</v>
+        <v>237</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>675</v>
+        <v>689</v>
       </c>
       <c r="C93" t="s">
-        <v>676</v>
+        <v>690</v>
       </c>
       <c r="D93" t="s">
-        <v>677</v>
+        <v>688</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>672</v>
+        <v>663</v>
       </c>
       <c r="C94" t="s">
-        <v>673</v>
+        <v>664</v>
       </c>
       <c r="D94" t="s">
-        <v>674</v>
+        <v>665</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>809</v>
+        <v>660</v>
       </c>
       <c r="C95" t="s">
-        <v>810</v>
+        <v>661</v>
       </c>
       <c r="D95" t="s">
-        <v>811</v>
+        <v>662</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>657</v>
-      </c>
-      <c r="B96" t="s">
-        <v>662</v>
+        <v>795</v>
       </c>
       <c r="C96" t="s">
-        <v>659</v>
+        <v>796</v>
       </c>
       <c r="D96" t="s">
-        <v>658</v>
+        <v>797</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>799</v>
+        <v>645</v>
+      </c>
+      <c r="B97" t="s">
+        <v>650</v>
       </c>
       <c r="C97" t="s">
-        <v>800</v>
+        <v>647</v>
       </c>
       <c r="D97" t="s">
-        <v>801</v>
+        <v>646</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>808</v>
+        <v>785</v>
       </c>
       <c r="C98" t="s">
-        <v>803</v>
+        <v>786</v>
       </c>
       <c r="D98" t="s">
-        <v>802</v>
+        <v>787</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>644</v>
-      </c>
-      <c r="B99" t="s">
-        <v>660</v>
+        <v>794</v>
       </c>
       <c r="C99" t="s">
-        <v>646</v>
+        <v>789</v>
       </c>
       <c r="D99" t="s">
-        <v>648</v>
+        <v>788</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="B100" t="s">
-        <v>661</v>
+        <v>648</v>
       </c>
       <c r="C100" t="s">
-        <v>647</v>
+        <v>636</v>
       </c>
       <c r="D100" t="s">
-        <v>649</v>
+        <v>851</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>641</v>
+        <v>850</v>
       </c>
       <c r="B101" t="s">
-        <v>232</v>
+        <v>649</v>
       </c>
       <c r="C101" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="D101" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>234</v>
+        <v>847</v>
       </c>
       <c r="B102" t="s">
-        <v>232</v>
+        <v>848</v>
       </c>
       <c r="C102" t="s">
-        <v>235</v>
+        <v>849</v>
       </c>
       <c r="D102" t="s">
-        <v>236</v>
+        <v>852</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>797</v>
+        <v>632</v>
+      </c>
+      <c r="B103" t="s">
+        <v>232</v>
       </c>
       <c r="C103" t="s">
-        <v>804</v>
+        <v>633</v>
       </c>
       <c r="D103" t="s">
-        <v>806</v>
+        <v>634</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>798</v>
+        <v>234</v>
+      </c>
+      <c r="B104" t="s">
+        <v>232</v>
       </c>
       <c r="C104" t="s">
-        <v>805</v>
+        <v>235</v>
       </c>
       <c r="D104" t="s">
-        <v>807</v>
+        <v>236</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>820</v>
+        <v>783</v>
       </c>
       <c r="C105" t="s">
-        <v>818</v>
+        <v>790</v>
       </c>
       <c r="D105" t="s">
-        <v>819</v>
+        <v>792</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B106" s="4"/>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
+      <c r="A106" t="s">
+        <v>784</v>
+      </c>
+      <c r="C106" t="s">
+        <v>791</v>
+      </c>
+      <c r="D106" t="s">
+        <v>793</v>
+      </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>80</v>
-      </c>
-      <c r="B107" t="s">
-        <v>81</v>
+        <v>806</v>
       </c>
       <c r="C107" t="s">
-        <v>89</v>
+        <v>804</v>
       </c>
       <c r="D107" t="s">
-        <v>90</v>
+        <v>805</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>82</v>
-      </c>
-      <c r="B108" t="s">
-        <v>83</v>
-      </c>
-      <c r="C108" t="s">
-        <v>85</v>
-      </c>
-      <c r="D108" t="s">
-        <v>87</v>
-      </c>
+      <c r="A108" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B109" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C109" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D109" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="B110" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C110" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="D110" t="s">
-        <v>262</v>
+        <v>87</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B111" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C111" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D111" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="B112" s="5"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
+      <c r="A112" t="s">
+        <v>103</v>
+      </c>
+      <c r="B112" t="s">
+        <v>81</v>
+      </c>
+      <c r="C112" t="s">
+        <v>104</v>
+      </c>
+      <c r="D112" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>326</v>
+        <v>91</v>
       </c>
       <c r="B113" t="s">
-        <v>325</v>
+        <v>92</v>
       </c>
       <c r="C113" t="s">
-        <v>331</v>
+        <v>93</v>
       </c>
       <c r="D113" t="s">
-        <v>332</v>
+        <v>94</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>327</v>
-      </c>
-      <c r="B114" t="s">
-        <v>325</v>
-      </c>
-      <c r="C114" t="s">
-        <v>332</v>
-      </c>
-      <c r="D114" t="s">
-        <v>332</v>
-      </c>
+      <c r="A114" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="B115" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="C115" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D115" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="B116" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="C116" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="D116" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>422</v>
+        <v>325</v>
+      </c>
+      <c r="B117" t="s">
+        <v>319</v>
       </c>
       <c r="C117" t="s">
-        <v>423</v>
+        <v>320</v>
       </c>
       <c r="D117" t="s">
-        <v>424</v>
+        <v>321</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>338</v>
+        <v>326</v>
+      </c>
+      <c r="B118" t="s">
+        <v>319</v>
       </c>
       <c r="C118" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="D118" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>413</v>
+      </c>
+      <c r="C119" t="s">
+        <v>414</v>
+      </c>
+      <c r="D119" t="s">
         <v>415</v>
-      </c>
-      <c r="C119" t="s">
-        <v>341</v>
-      </c>
-      <c r="D119" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>416</v>
+        <v>329</v>
       </c>
       <c r="C120" t="s">
-        <v>420</v>
+        <v>331</v>
       </c>
       <c r="D120" t="s">
-        <v>421</v>
+        <v>330</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="C121" t="s">
-        <v>419</v>
+        <v>332</v>
       </c>
       <c r="D121" t="s">
-        <v>418</v>
+        <v>333</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>343</v>
+        <v>407</v>
       </c>
       <c r="C122" t="s">
-        <v>345</v>
+        <v>411</v>
       </c>
       <c r="D122" t="s">
-        <v>344</v>
+        <v>412</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>359</v>
-      </c>
-      <c r="B123" t="s">
-        <v>360</v>
+        <v>408</v>
       </c>
       <c r="C123" t="s">
-        <v>361</v>
+        <v>410</v>
       </c>
       <c r="D123" t="s">
-        <v>362</v>
+        <v>409</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>409</v>
+        <v>334</v>
       </c>
       <c r="C124" t="s">
-        <v>411</v>
+        <v>336</v>
       </c>
       <c r="D124" t="s">
-        <v>413</v>
+        <v>335</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>410</v>
+        <v>350</v>
+      </c>
+      <c r="B125" t="s">
+        <v>351</v>
       </c>
       <c r="C125" t="s">
-        <v>412</v>
+        <v>352</v>
       </c>
       <c r="D125" t="s">
-        <v>414</v>
+        <v>353</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>363</v>
-      </c>
-      <c r="B126" t="s">
-        <v>364</v>
+        <v>400</v>
       </c>
       <c r="C126" t="s">
-        <v>365</v>
+        <v>402</v>
       </c>
       <c r="D126" t="s">
-        <v>366</v>
+        <v>404</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>427</v>
+        <v>401</v>
       </c>
       <c r="C127" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="D127" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>428</v>
+        <v>354</v>
+      </c>
+      <c r="B128" t="s">
+        <v>355</v>
       </c>
       <c r="C128" t="s">
-        <v>429</v>
+        <v>356</v>
       </c>
       <c r="D128" t="s">
-        <v>430</v>
+        <v>357</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>346</v>
+        <v>418</v>
       </c>
       <c r="C129" t="s">
-        <v>375</v>
+        <v>392</v>
       </c>
       <c r="D129" t="s">
-        <v>347</v>
+        <v>393</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>367</v>
+        <v>419</v>
       </c>
       <c r="C130" t="s">
-        <v>368</v>
+        <v>420</v>
       </c>
       <c r="D130" t="s">
-        <v>368</v>
+        <v>421</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>369</v>
+        <v>337</v>
       </c>
       <c r="C131" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D131" t="s">
-        <v>371</v>
+        <v>338</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="C132" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="D132" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="C133" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="D133" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="C134" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="D134" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="C135" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="D135" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>403</v>
+        <v>370</v>
       </c>
       <c r="C136" t="s">
-        <v>408</v>
+        <v>371</v>
       </c>
       <c r="D136" t="s">
-        <v>407</v>
+        <v>372</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="C137" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
       <c r="D137" t="s">
-        <v>425</v>
+        <v>375</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C138" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D138" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="C139" t="s">
-        <v>779</v>
+        <v>383</v>
       </c>
       <c r="D139" t="s">
-        <v>393</v>
+        <v>416</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="C140" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D140" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="C141" t="s">
-        <v>399</v>
+        <v>765</v>
       </c>
       <c r="D141" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="C142" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="D142" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>513</v>
-      </c>
-      <c r="C143" s="9" t="s">
-        <v>514</v>
+        <v>389</v>
+      </c>
+      <c r="C143" t="s">
+        <v>390</v>
       </c>
       <c r="D143" t="s">
-        <v>515</v>
+        <v>391</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>431</v>
+        <v>382</v>
       </c>
       <c r="C144" t="s">
-        <v>432</v>
+        <v>387</v>
       </c>
       <c r="D144" t="s">
-        <v>433</v>
+        <v>388</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>434</v>
-      </c>
-      <c r="C145" t="s">
-        <v>489</v>
+        <v>504</v>
+      </c>
+      <c r="C145" s="9" t="s">
+        <v>505</v>
       </c>
       <c r="D145" t="s">
-        <v>487</v>
+        <v>506</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="C146" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="D146" t="s">
-        <v>488</v>
+        <v>424</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>519</v>
+        <v>425</v>
       </c>
       <c r="C147" t="s">
-        <v>440</v>
+        <v>480</v>
       </c>
       <c r="D147" t="s">
-        <v>441</v>
+        <v>478</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>537</v>
+        <v>427</v>
       </c>
       <c r="C148" t="s">
-        <v>535</v>
+        <v>426</v>
       </c>
       <c r="D148" t="s">
-        <v>536</v>
+        <v>479</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>442</v>
+        <v>510</v>
       </c>
       <c r="C149" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="D149" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>481</v>
+        <v>528</v>
       </c>
       <c r="C150" t="s">
-        <v>483</v>
+        <v>526</v>
       </c>
       <c r="D150" t="s">
-        <v>485</v>
+        <v>527</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>482</v>
+        <v>433</v>
       </c>
       <c r="C151" t="s">
-        <v>484</v>
+        <v>434</v>
       </c>
       <c r="D151" t="s">
-        <v>486</v>
+        <v>435</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>490</v>
+        <v>472</v>
       </c>
       <c r="C152" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="D152" t="s">
-        <v>492</v>
+        <v>476</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>523</v>
+        <v>473</v>
       </c>
       <c r="C153" t="s">
-        <v>493</v>
+        <v>475</v>
       </c>
       <c r="D153" t="s">
-        <v>494</v>
+        <v>477</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="C154" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="D154" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>498</v>
+        <v>514</v>
       </c>
       <c r="C155" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="D155" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
       <c r="C156" t="s">
-        <v>502</v>
+        <v>487</v>
       </c>
       <c r="D156" t="s">
-        <v>530</v>
+        <v>488</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>516</v>
-      </c>
-      <c r="C157" s="9" t="s">
-        <v>517</v>
+        <v>489</v>
+      </c>
+      <c r="C157" t="s">
+        <v>491</v>
       </c>
       <c r="D157" t="s">
-        <v>518</v>
+        <v>492</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>520</v>
-      </c>
-      <c r="C158" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="C158" t="s">
+        <v>493</v>
+      </c>
+      <c r="D158" t="s">
         <v>521</v>
-      </c>
-      <c r="D158" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>524</v>
+        <v>507</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>525</v>
+        <v>508</v>
       </c>
       <c r="D159" t="s">
-        <v>526</v>
+        <v>509</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>527</v>
+        <v>511</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>529</v>
+        <v>512</v>
       </c>
       <c r="D160" t="s">
-        <v>528</v>
+        <v>513</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>533</v>
+        <v>515</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>502</v>
+        <v>516</v>
       </c>
       <c r="D161" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>531</v>
+        <v>520</v>
       </c>
       <c r="D162" t="s">
-        <v>532</v>
+        <v>519</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>545</v>
+        <v>524</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>546</v>
+        <v>493</v>
       </c>
       <c r="D163" t="s">
-        <v>547</v>
+        <v>521</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>548</v>
+        <v>525</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>552</v>
+        <v>522</v>
       </c>
       <c r="D164" t="s">
-        <v>550</v>
+        <v>523</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
       <c r="D165" t="s">
-        <v>551</v>
+        <v>538</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>553</v>
+        <v>539</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="D166" t="s">
-        <v>558</v>
+        <v>541</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="D167" t="s">
-        <v>557</v>
+        <v>542</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>560</v>
+        <v>544</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>561</v>
+        <v>550</v>
       </c>
       <c r="D168" t="s">
-        <v>562</v>
+        <v>549</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>579</v>
+        <v>547</v>
       </c>
       <c r="D169" t="s">
-        <v>580</v>
+        <v>548</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>563</v>
+        <v>551</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>565</v>
+        <v>552</v>
       </c>
       <c r="D170" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>564</v>
+        <v>546</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="D171" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>575</v>
+        <v>554</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>569</v>
+        <v>556</v>
       </c>
       <c r="D172" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>576</v>
+        <v>555</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="D173" t="s">
-        <v>574</v>
+        <v>559</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>577</v>
+        <v>566</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>570</v>
-      </c>
-      <c r="D174" s="9" t="s">
-        <v>570</v>
+        <v>560</v>
+      </c>
+      <c r="D174" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>571</v>
-      </c>
-      <c r="D175" s="9" t="s">
-        <v>571</v>
+        <v>564</v>
+      </c>
+      <c r="D175" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>581</v>
+        <v>568</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>582</v>
+        <v>561</v>
       </c>
       <c r="D176" s="9" t="s">
-        <v>583</v>
+        <v>561</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>588</v>
+        <v>569</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>591</v>
+        <v>562</v>
       </c>
       <c r="D177" s="9" t="s">
-        <v>592</v>
+        <v>562</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>589</v>
+        <v>572</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>590</v>
+        <v>573</v>
       </c>
       <c r="D178" s="9" t="s">
-        <v>593</v>
+        <v>574</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B179" s="3"/>
-      <c r="C179" s="3"/>
-      <c r="D179" s="3"/>
+      <c r="A179" t="s">
+        <v>579</v>
+      </c>
+      <c r="C179" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="D179" s="9" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>694</v>
-      </c>
-      <c r="C180" t="s">
-        <v>695</v>
-      </c>
-      <c r="D180" t="s">
-        <v>696</v>
+        <v>580</v>
+      </c>
+      <c r="C180" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="D180" s="9" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>690</v>
-      </c>
-      <c r="C181" t="s">
-        <v>697</v>
-      </c>
-      <c r="D181" t="s">
-        <v>699</v>
-      </c>
+      <c r="A181" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B181" s="3"/>
+      <c r="C181" s="3"/>
+      <c r="D181" s="3"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>693</v>
+        <v>680</v>
       </c>
       <c r="C182" t="s">
-        <v>698</v>
+        <v>681</v>
       </c>
       <c r="D182" t="s">
-        <v>700</v>
+        <v>682</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>701</v>
-      </c>
-      <c r="C183" s="7" t="s">
-        <v>691</v>
-      </c>
-      <c r="D183" s="7" t="s">
-        <v>692</v>
+        <v>676</v>
+      </c>
+      <c r="C183" t="s">
+        <v>683</v>
+      </c>
+      <c r="D183" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>140</v>
-      </c>
-      <c r="B184" t="s">
-        <v>137</v>
+        <v>679</v>
       </c>
       <c r="C184" t="s">
-        <v>138</v>
+        <v>684</v>
       </c>
       <c r="D184" t="s">
-        <v>139</v>
+        <v>686</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>141</v>
-      </c>
-      <c r="B185" t="s">
-        <v>142</v>
-      </c>
-      <c r="C185" t="s">
-        <v>150</v>
-      </c>
-      <c r="D185" t="s">
-        <v>151</v>
+        <v>687</v>
+      </c>
+      <c r="C185" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="D185" s="7" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B186" t="s">
         <v>137</v>
       </c>
       <c r="C186" t="s">
-        <v>683</v>
+        <v>138</v>
       </c>
       <c r="D186" t="s">
-        <v>684</v>
+        <v>139</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B187" t="s">
         <v>142</v>
       </c>
       <c r="C187" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D187" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B188" t="s">
-        <v>145</v>
-      </c>
-      <c r="C188" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D188" s="7" t="s">
-        <v>146</v>
+        <v>137</v>
+      </c>
+      <c r="C188" t="s">
+        <v>669</v>
+      </c>
+      <c r="D188" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>681</v>
+        <v>143</v>
+      </c>
+      <c r="B189" t="s">
+        <v>142</v>
       </c>
       <c r="C189" t="s">
-        <v>680</v>
+        <v>149</v>
       </c>
       <c r="D189" t="s">
-        <v>680</v>
+        <v>148</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>682</v>
-      </c>
-      <c r="C190" t="s">
-        <v>686</v>
-      </c>
-      <c r="D190" t="s">
-        <v>685</v>
+        <v>144</v>
+      </c>
+      <c r="B190" t="s">
+        <v>145</v>
+      </c>
+      <c r="C190" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D190" s="7" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>687</v>
+        <v>667</v>
       </c>
       <c r="C191" t="s">
-        <v>688</v>
+        <v>666</v>
       </c>
       <c r="D191" t="s">
-        <v>689</v>
+        <v>666</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B192" s="6"/>
-      <c r="C192" s="6"/>
-      <c r="D192" s="6"/>
+      <c r="A192" t="s">
+        <v>668</v>
+      </c>
+      <c r="C192" t="s">
+        <v>672</v>
+      </c>
+      <c r="D192" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>47</v>
-      </c>
-      <c r="B193" t="s">
-        <v>8</v>
+        <v>673</v>
       </c>
       <c r="C193" t="s">
-        <v>48</v>
+        <v>674</v>
       </c>
       <c r="D193" t="s">
-        <v>49</v>
+        <v>675</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>95</v>
-      </c>
-      <c r="B194" t="s">
-        <v>8</v>
-      </c>
-      <c r="C194" t="s">
-        <v>96</v>
-      </c>
-      <c r="D194" t="s">
-        <v>97</v>
-      </c>
+      <c r="A194" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B194" s="6"/>
+      <c r="C194" s="6"/>
+      <c r="D194" s="6"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>597</v>
+        <v>47</v>
+      </c>
+      <c r="B195" t="s">
+        <v>8</v>
       </c>
       <c r="C195" t="s">
-        <v>598</v>
+        <v>48</v>
       </c>
       <c r="D195" t="s">
-        <v>599</v>
+        <v>49</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>600</v>
+        <v>95</v>
+      </c>
+      <c r="B196" t="s">
+        <v>8</v>
       </c>
       <c r="C196" t="s">
-        <v>601</v>
+        <v>96</v>
       </c>
       <c r="D196" t="s">
-        <v>602</v>
+        <v>97</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>632</v>
+        <v>588</v>
       </c>
       <c r="C197" t="s">
-        <v>634</v>
+        <v>589</v>
       </c>
       <c r="D197" t="s">
-        <v>635</v>
+        <v>590</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>633</v>
+        <v>591</v>
       </c>
       <c r="C198" t="s">
-        <v>637</v>
+        <v>592</v>
       </c>
       <c r="D198" t="s">
-        <v>636</v>
+        <v>593</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>794</v>
+        <v>623</v>
       </c>
       <c r="C199" t="s">
-        <v>795</v>
+        <v>625</v>
       </c>
       <c r="D199" t="s">
-        <v>796</v>
+        <v>626</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>50</v>
-      </c>
-      <c r="B200" t="s">
-        <v>8</v>
+        <v>624</v>
       </c>
       <c r="C200" t="s">
-        <v>51</v>
+        <v>628</v>
       </c>
       <c r="D200" t="s">
-        <v>52</v>
+        <v>627</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>53</v>
-      </c>
-      <c r="B201" t="s">
-        <v>8</v>
+        <v>780</v>
       </c>
       <c r="C201" t="s">
-        <v>54</v>
+        <v>781</v>
       </c>
       <c r="D201" t="s">
-        <v>222</v>
+        <v>782</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>217</v>
+        <v>50</v>
       </c>
       <c r="B202" t="s">
         <v>8</v>
       </c>
       <c r="C202" t="s">
-        <v>218</v>
+        <v>51</v>
       </c>
       <c r="D202" t="s">
-        <v>218</v>
+        <v>52</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>349</v>
+        <v>53</v>
       </c>
       <c r="B203" t="s">
         <v>8</v>
       </c>
       <c r="C203" t="s">
-        <v>614</v>
+        <v>54</v>
       </c>
       <c r="D203" t="s">
-        <v>616</v>
+        <v>222</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>615</v>
+        <v>217</v>
+      </c>
+      <c r="B204" t="s">
+        <v>8</v>
       </c>
       <c r="C204" t="s">
-        <v>613</v>
+        <v>218</v>
       </c>
       <c r="D204" t="s">
-        <v>617</v>
+        <v>218</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>812</v>
+        <v>340</v>
+      </c>
+      <c r="B205" t="s">
+        <v>8</v>
       </c>
       <c r="C205" t="s">
-        <v>813</v>
+        <v>605</v>
       </c>
       <c r="D205" t="s">
-        <v>814</v>
+        <v>607</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>155</v>
-      </c>
-      <c r="B206" t="s">
-        <v>8</v>
+        <v>606</v>
       </c>
       <c r="C206" t="s">
-        <v>594</v>
+        <v>604</v>
       </c>
       <c r="D206" t="s">
-        <v>156</v>
+        <v>608</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>165</v>
-      </c>
-      <c r="B207" t="s">
-        <v>8</v>
+        <v>798</v>
       </c>
       <c r="C207" t="s">
-        <v>595</v>
+        <v>799</v>
       </c>
       <c r="D207" t="s">
-        <v>166</v>
+        <v>800</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="B208" t="s">
         <v>8</v>
       </c>
       <c r="C208" t="s">
-        <v>596</v>
+        <v>585</v>
       </c>
       <c r="D208" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>603</v>
+        <v>165</v>
       </c>
       <c r="B209" t="s">
         <v>8</v>
       </c>
       <c r="C209" t="s">
-        <v>604</v>
+        <v>586</v>
       </c>
       <c r="D209" t="s">
-        <v>605</v>
+        <v>166</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>610</v>
+        <v>173</v>
       </c>
       <c r="B210" t="s">
         <v>8</v>
       </c>
       <c r="C210" t="s">
-        <v>608</v>
+        <v>587</v>
       </c>
       <c r="D210" t="s">
-        <v>606</v>
+        <v>174</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>611</v>
+        <v>594</v>
       </c>
       <c r="B211" t="s">
         <v>8</v>
       </c>
       <c r="C211" t="s">
-        <v>609</v>
+        <v>595</v>
       </c>
       <c r="D211" t="s">
-        <v>607</v>
+        <v>596</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>154</v>
+        <v>601</v>
       </c>
       <c r="B212" t="s">
         <v>8</v>
       </c>
       <c r="C212" t="s">
-        <v>190</v>
+        <v>599</v>
       </c>
       <c r="D212" t="s">
-        <v>191</v>
+        <v>597</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>55</v>
+        <v>602</v>
       </c>
       <c r="B213" t="s">
         <v>8</v>
       </c>
       <c r="C213" t="s">
-        <v>56</v>
+        <v>600</v>
       </c>
       <c r="D213" t="s">
-        <v>57</v>
+        <v>598</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B214" t="s">
         <v>8</v>
       </c>
       <c r="C214" t="s">
-        <v>157</v>
+        <v>190</v>
       </c>
       <c r="D214" t="s">
-        <v>16</v>
+        <v>191</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>167</v>
+        <v>55</v>
       </c>
       <c r="B215" t="s">
         <v>8</v>
       </c>
       <c r="C215" t="s">
-        <v>168</v>
+        <v>56</v>
       </c>
       <c r="D215" t="s">
-        <v>169</v>
+        <v>57</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>58</v>
+        <v>162</v>
       </c>
       <c r="B216" t="s">
         <v>8</v>
       </c>
       <c r="C216" t="s">
-        <v>59</v>
+        <v>157</v>
       </c>
       <c r="D216" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B217" t="s">
         <v>8</v>
       </c>
       <c r="C217" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D217" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>170</v>
+        <v>58</v>
       </c>
       <c r="B218" t="s">
         <v>8</v>
       </c>
       <c r="C218" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="D218" t="s">
-        <v>172</v>
+        <v>60</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>61</v>
+        <v>161</v>
       </c>
       <c r="B219" t="s">
         <v>8</v>
       </c>
       <c r="C219" t="s">
-        <v>62</v>
+        <v>163</v>
       </c>
       <c r="D219" t="s">
-        <v>63</v>
+        <v>164</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B220" t="s">
         <v>8</v>
       </c>
       <c r="C220" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="D220" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>175</v>
+        <v>61</v>
       </c>
       <c r="B221" t="s">
         <v>8</v>
       </c>
       <c r="C221" t="s">
-        <v>176</v>
+        <v>62</v>
       </c>
       <c r="D221" t="s">
-        <v>177</v>
+        <v>63</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
       <c r="B222" t="s">
         <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
       <c r="D222" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="B223" t="s">
         <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="D223" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B224" t="s">
         <v>8</v>
       </c>
       <c r="C224" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D224" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>284</v>
+        <v>195</v>
+      </c>
+      <c r="B225" t="s">
+        <v>8</v>
       </c>
       <c r="C225" t="s">
-        <v>285</v>
+        <v>196</v>
       </c>
       <c r="D225" t="s">
-        <v>286</v>
+        <v>105</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>67</v>
+        <v>197</v>
       </c>
       <c r="B226" t="s">
         <v>8</v>
       </c>
       <c r="C226" t="s">
-        <v>68</v>
+        <v>198</v>
       </c>
       <c r="D226" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>7</v>
-      </c>
-      <c r="B227" t="s">
-        <v>8</v>
+        <v>275</v>
       </c>
       <c r="C227" t="s">
-        <v>9</v>
+        <v>276</v>
       </c>
       <c r="D227" t="s">
-        <v>10</v>
+        <v>277</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>437</v>
+        <v>67</v>
+      </c>
+      <c r="B228" t="s">
+        <v>8</v>
       </c>
       <c r="C228" t="s">
-        <v>438</v>
+        <v>68</v>
       </c>
       <c r="D228" t="s">
-        <v>439</v>
+        <v>69</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="B229" t="s">
         <v>8</v>
       </c>
       <c r="C229" t="s">
-        <v>200</v>
+        <v>9</v>
       </c>
       <c r="D229" t="s">
-        <v>201</v>
+        <v>10</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>178</v>
-      </c>
-      <c r="B230" t="s">
-        <v>179</v>
+        <v>428</v>
       </c>
       <c r="C230" t="s">
-        <v>178</v>
+        <v>429</v>
       </c>
       <c r="D230" t="s">
-        <v>180</v>
+        <v>430</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B231" t="s">
         <v>8</v>
       </c>
       <c r="C231" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D231" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="B232" t="s">
         <v>179</v>
       </c>
       <c r="C232" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
       <c r="D232" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>229</v>
+        <v>202</v>
       </c>
       <c r="B233" t="s">
         <v>8</v>
       </c>
       <c r="C233" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="D233" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="B234" t="s">
         <v>179</v>
       </c>
       <c r="C234" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="D234" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="B235" t="s">
         <v>8</v>
       </c>
       <c r="C235" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="D235" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="B236" t="s">
         <v>179</v>
       </c>
       <c r="C236" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="D236" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>106</v>
+        <v>211</v>
       </c>
       <c r="B237" t="s">
         <v>8</v>
       </c>
       <c r="C237" t="s">
-        <v>107</v>
+        <v>213</v>
       </c>
       <c r="D237" t="s">
-        <v>108</v>
+        <v>215</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B238" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="C238" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="D238" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="B239" t="s">
         <v>8</v>
       </c>
       <c r="C239" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="D239" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>385</v>
+        <v>208</v>
+      </c>
+      <c r="B240" t="s">
+        <v>8</v>
       </c>
       <c r="C240" t="s">
-        <v>386</v>
+        <v>209</v>
       </c>
       <c r="D240" t="s">
-        <v>387</v>
+        <v>210</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>503</v>
+        <v>14</v>
+      </c>
+      <c r="B241" t="s">
+        <v>8</v>
       </c>
       <c r="C241" t="s">
-        <v>504</v>
+        <v>15</v>
       </c>
       <c r="D241" t="s">
-        <v>505</v>
+        <v>16</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>426</v>
-      </c>
-      <c r="B242" t="s">
-        <v>316</v>
+        <v>376</v>
       </c>
       <c r="C242" t="s">
-        <v>317</v>
+        <v>377</v>
       </c>
       <c r="D242" t="s">
-        <v>318</v>
+        <v>378</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>445</v>
+        <v>494</v>
       </c>
       <c r="C243" t="s">
-        <v>457</v>
+        <v>495</v>
       </c>
       <c r="D243" t="s">
-        <v>469</v>
+        <v>496</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>446</v>
+        <v>417</v>
+      </c>
+      <c r="B244" t="s">
+        <v>307</v>
       </c>
       <c r="C244" t="s">
-        <v>458</v>
+        <v>308</v>
       </c>
       <c r="D244" t="s">
-        <v>470</v>
+        <v>309</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
       <c r="C245" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="D245" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="C246" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="D246" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C247" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
       <c r="D247" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="C248" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="D248" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="C249" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="D249" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="C250" t="s">
+        <v>453</v>
+      </c>
+      <c r="D250" t="s">
         <v>464</v>
-      </c>
-      <c r="D250" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="C251" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="D251" t="s">
-        <v>477</v>
+        <v>466</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="C252" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
       <c r="D252" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
       <c r="C253" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="D253" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
       <c r="C254" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="D254" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>508</v>
+        <v>446</v>
       </c>
       <c r="C255" t="s">
-        <v>507</v>
+        <v>458</v>
       </c>
       <c r="D255" t="s">
-        <v>506</v>
+        <v>470</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>584</v>
+        <v>447</v>
       </c>
       <c r="C256" t="s">
-        <v>2</v>
+        <v>459</v>
       </c>
       <c r="D256" t="s">
-        <v>585</v>
+        <v>471</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>586</v>
+        <v>499</v>
       </c>
       <c r="C257" t="s">
-        <v>587</v>
+        <v>498</v>
       </c>
       <c r="D257" t="s">
-        <v>3</v>
+        <v>497</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A258" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B258" s="2"/>
-      <c r="C258" s="2"/>
-      <c r="D258" s="2"/>
+      <c r="A258" t="s">
+        <v>575</v>
+      </c>
+      <c r="C258" t="s">
+        <v>2</v>
+      </c>
+      <c r="D258" t="s">
+        <v>576</v>
+      </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>110</v>
-      </c>
-      <c r="B259" t="s">
+        <v>577</v>
+      </c>
+      <c r="C259" t="s">
+        <v>578</v>
+      </c>
+      <c r="D259" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C259" t="s">
-        <v>129</v>
-      </c>
-      <c r="D259" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A260" t="s">
-        <v>127</v>
-      </c>
-      <c r="B260" t="s">
-        <v>109</v>
-      </c>
-      <c r="C260" t="s">
-        <v>130</v>
-      </c>
-      <c r="D260" t="s">
-        <v>133</v>
-      </c>
+      <c r="B260" s="2"/>
+      <c r="C260" s="2"/>
+      <c r="D260" s="2"/>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B261" t="s">
         <v>109</v>
       </c>
       <c r="C261" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="D261" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B262" t="s">
         <v>109</v>
       </c>
       <c r="C262" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D262" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B263" t="s">
         <v>109</v>
       </c>
       <c r="C263" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D263" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B264" t="s">
         <v>109</v>
       </c>
       <c r="C264" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="D264" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B265" t="s">
         <v>109</v>
       </c>
       <c r="C265" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="D265" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B266" t="s">
         <v>109</v>
       </c>
       <c r="C266" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D266" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A267" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B267" s="3"/>
-      <c r="C267" s="3"/>
-      <c r="D267" s="3"/>
+      <c r="A267" t="s">
+        <v>122</v>
+      </c>
+      <c r="B267" t="s">
+        <v>109</v>
+      </c>
+      <c r="C267" t="s">
+        <v>131</v>
+      </c>
+      <c r="D267" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="B268" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="C268" t="s">
-        <v>352</v>
+        <v>125</v>
       </c>
       <c r="D268" t="s">
-        <v>353</v>
+        <v>126</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A269" t="s">
-        <v>350</v>
-      </c>
-      <c r="B269" t="s">
-        <v>71</v>
-      </c>
-      <c r="C269" t="s">
-        <v>348</v>
-      </c>
-      <c r="D269" t="s">
-        <v>351</v>
-      </c>
+      <c r="A269" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B269" s="3"/>
+      <c r="C269" s="3"/>
+      <c r="D269" s="3"/>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>153</v>
+        <v>70</v>
       </c>
       <c r="B270" t="s">
         <v>71</v>
       </c>
       <c r="C270" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="D270" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="B271" t="s">
         <v>71</v>
       </c>
       <c r="C271" t="s">
-        <v>357</v>
+        <v>339</v>
       </c>
       <c r="D271" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>72</v>
+        <v>153</v>
       </c>
       <c r="B272" t="s">
         <v>71</v>
       </c>
       <c r="C272" t="s">
-        <v>73</v>
+        <v>345</v>
       </c>
       <c r="D272" t="s">
-        <v>74</v>
+        <v>346</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>618</v>
+        <v>347</v>
+      </c>
+      <c r="B273" t="s">
+        <v>71</v>
       </c>
       <c r="C273" t="s">
-        <v>612</v>
+        <v>348</v>
       </c>
       <c r="D273" t="s">
-        <v>619</v>
+        <v>349</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>629</v>
+        <v>72</v>
+      </c>
+      <c r="B274" t="s">
+        <v>71</v>
       </c>
       <c r="C274" t="s">
-        <v>630</v>
+        <v>73</v>
       </c>
       <c r="D274" t="s">
-        <v>631</v>
+        <v>74</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>815</v>
+        <v>609</v>
       </c>
       <c r="C275" t="s">
-        <v>816</v>
+        <v>603</v>
       </c>
       <c r="D275" t="s">
-        <v>817</v>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>620</v>
+      </c>
+      <c r="C276" t="s">
+        <v>621</v>
+      </c>
+      <c r="D276" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>801</v>
+      </c>
+      <c r="C277" t="s">
+        <v>802</v>
+      </c>
+      <c r="D277" t="s">
+        <v>803</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C183" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
-    <hyperlink ref="D183" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
+    <hyperlink ref="C185" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
+    <hyperlink ref="D185" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Only translations to home page text remaining
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3DA642-3008-4BFC-9F98-B1317A4111CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A602E42E-9B10-4221-BA65-109F4BBF82D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="856">
   <si>
     <t>id</t>
   </si>
@@ -2615,6 +2615,15 @@
   </si>
   <si>
     <t>séries temporelles</t>
+  </si>
+  <si>
+    <t>homeText_saved</t>
+  </si>
+  <si>
+    <t>Plongez dans le monde de l'hydrologie, de la météorologie et de la chimie de l'eau avec le département de l'environment du gouvernement du Yukon. Notre mission? Mettre les données à portée de main, en alignement avec l'initiative de Gouvernement Ouvert pour la transparence, l'engagement des citoyens et l'incitation à la recherche créative. 📊 📈 Explorez les données en temps réel comme jamais auparavant, disponibles sous entente de nos limitations de responsabilité.</t>
+  </si>
+  <si>
+    <t>Dive into the world of hydrology, meteorology, and water chemistry with the Yukon Department of Environment's Water Resources Branch. Our mission? To bring data to your fingertips, aligning with the Open Government initiative for transparency, citizen empowerment, and sparking research creativity. 📊 📈 Explore real-time data like never before, made available under the terms of our limitations of liability.</t>
   </si>
 </sst>
 </file>
@@ -3559,10 +3568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D277"/>
+  <dimension ref="A1:D278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3984,7 +3993,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>853</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
@@ -3998,1111 +4007,1111 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>855</v>
       </c>
       <c r="D32" t="s">
-        <v>26</v>
+        <v>854</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
         <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B35" t="s">
         <v>31</v>
       </c>
       <c r="C35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" t="s">
         <v>35</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>282</v>
-      </c>
-      <c r="B37" t="s">
-        <v>284</v>
-      </c>
-      <c r="C37" t="s">
-        <v>531</v>
-      </c>
-      <c r="D37" t="s">
-        <v>532</v>
-      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B38" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C38" t="s">
-        <v>288</v>
+        <v>531</v>
       </c>
       <c r="D38" t="s">
-        <v>289</v>
+        <v>532</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B39" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C39" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D39" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B40" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="C40" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="D40" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B41" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C41" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="D41" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B42" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C42" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="D42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C43" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="D43" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>533</v>
+        <v>298</v>
       </c>
       <c r="B44" t="s">
         <v>300</v>
       </c>
       <c r="C44" t="s">
-        <v>534</v>
+        <v>296</v>
       </c>
       <c r="D44" t="s">
-        <v>535</v>
+        <v>301</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>310</v>
+        <v>533</v>
       </c>
       <c r="B45" t="s">
         <v>300</v>
       </c>
       <c r="C45" t="s">
-        <v>311</v>
+        <v>534</v>
       </c>
       <c r="D45" t="s">
-        <v>312</v>
+        <v>535</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>310</v>
+      </c>
+      <c r="B46" t="s">
+        <v>300</v>
+      </c>
+      <c r="C46" t="s">
+        <v>311</v>
+      </c>
+      <c r="D46" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>313</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>307</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>314</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>37</v>
-      </c>
-      <c r="B48" t="s">
-        <v>38</v>
-      </c>
-      <c r="C48" t="s">
-        <v>152</v>
-      </c>
-      <c r="D48" t="s">
-        <v>39</v>
-      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>40</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>41</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>42</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>233</v>
-      </c>
-      <c r="B51" t="s">
-        <v>231</v>
-      </c>
-      <c r="C51" t="s">
-        <v>238</v>
-      </c>
-      <c r="D51" t="s">
-        <v>239</v>
-      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>233</v>
       </c>
       <c r="B52" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>238</v>
       </c>
       <c r="D52" t="s">
-        <v>77</v>
+        <v>239</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>240</v>
+        <v>75</v>
       </c>
       <c r="B53" t="s">
-        <v>242</v>
+        <v>185</v>
       </c>
       <c r="C53" t="s">
-        <v>844</v>
+        <v>76</v>
       </c>
       <c r="D53" t="s">
-        <v>241</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>643</v>
+        <v>240</v>
+      </c>
+      <c r="B54" t="s">
+        <v>242</v>
       </c>
       <c r="C54" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D54" t="s">
-        <v>644</v>
+        <v>241</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>246</v>
-      </c>
-      <c r="B55" t="s">
-        <v>248</v>
+        <v>643</v>
       </c>
       <c r="C55" t="s">
-        <v>247</v>
+        <v>845</v>
       </c>
       <c r="D55" t="s">
-        <v>271</v>
+        <v>644</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B56" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C56" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D56" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B57" t="s">
         <v>249</v>
       </c>
       <c r="C57" t="s">
-        <v>840</v>
+        <v>252</v>
       </c>
       <c r="D57" t="s">
-        <v>843</v>
+        <v>251</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B58" t="s">
         <v>249</v>
       </c>
       <c r="C58" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D58" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>639</v>
+        <v>245</v>
       </c>
       <c r="B59" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C59" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
       <c r="D59" t="s">
-        <v>253</v>
+        <v>842</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B60" t="s">
         <v>250</v>
       </c>
       <c r="C60" t="s">
-        <v>641</v>
+        <v>846</v>
       </c>
       <c r="D60" t="s">
-        <v>642</v>
+        <v>253</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>270</v>
+        <v>640</v>
       </c>
       <c r="B61" t="s">
         <v>250</v>
       </c>
       <c r="C61" t="s">
-        <v>838</v>
+        <v>641</v>
       </c>
       <c r="D61" t="s">
-        <v>839</v>
+        <v>642</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="B62" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C62" t="s">
-        <v>255</v>
+        <v>838</v>
       </c>
       <c r="D62" t="s">
-        <v>256</v>
+        <v>839</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>807</v>
+        <v>254</v>
       </c>
       <c r="B63" t="s">
-        <v>809</v>
+        <v>248</v>
       </c>
       <c r="C63" t="s">
-        <v>810</v>
+        <v>255</v>
       </c>
       <c r="D63" t="s">
-        <v>812</v>
+        <v>256</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B64" t="s">
         <v>809</v>
       </c>
       <c r="C64" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D64" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>258</v>
+        <v>808</v>
       </c>
       <c r="B65" t="s">
-        <v>248</v>
+        <v>809</v>
       </c>
       <c r="C65" t="s">
-        <v>259</v>
+        <v>811</v>
       </c>
       <c r="D65" t="s">
-        <v>260</v>
+        <v>813</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="B66" t="s">
         <v>248</v>
       </c>
       <c r="C66" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="D66" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="B67" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C67" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="D67" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B68" t="s">
         <v>249</v>
       </c>
       <c r="C68" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D68" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B69" t="s">
         <v>249</v>
       </c>
       <c r="C69" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D69" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="B70" t="s">
-        <v>279</v>
+        <v>249</v>
       </c>
       <c r="C70" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="D70" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>767</v>
+        <v>278</v>
       </c>
       <c r="B71" t="s">
-        <v>768</v>
+        <v>279</v>
       </c>
       <c r="C71" t="s">
-        <v>769</v>
+        <v>280</v>
       </c>
       <c r="D71" t="s">
-        <v>770</v>
+        <v>281</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="B72" t="s">
         <v>768</v>
       </c>
       <c r="C72" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D72" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="B73" t="s">
         <v>768</v>
       </c>
       <c r="C73" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D73" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B74" t="s">
         <v>768</v>
       </c>
       <c r="C74" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="D74" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>816</v>
+        <v>777</v>
       </c>
       <c r="B75" t="s">
         <v>768</v>
       </c>
       <c r="C75" t="s">
-        <v>819</v>
+        <v>778</v>
       </c>
       <c r="D75" t="s">
-        <v>820</v>
+        <v>779</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B76" t="s">
         <v>768</v>
       </c>
       <c r="C76" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="D76" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="B77" t="s">
         <v>768</v>
       </c>
       <c r="C77" t="s">
-        <v>814</v>
+        <v>824</v>
       </c>
       <c r="D77" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="B78" t="s">
         <v>768</v>
       </c>
       <c r="C78" t="s">
-        <v>825</v>
+        <v>814</v>
       </c>
       <c r="D78" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="B79" t="s">
         <v>768</v>
       </c>
       <c r="C79" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D79" t="s">
-        <v>828</v>
+        <v>823</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="B80" t="s">
         <v>768</v>
       </c>
       <c r="C80" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="D80" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>835</v>
+        <v>829</v>
+      </c>
+      <c r="B81" t="s">
+        <v>768</v>
       </c>
       <c r="C81" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="D81" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>835</v>
+      </c>
+      <c r="C82" t="s">
+        <v>836</v>
+      </c>
+      <c r="D82" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>832</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>833</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D83" t="s">
         <v>834</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>611</v>
-      </c>
-      <c r="C84" t="s">
-        <v>612</v>
-      </c>
-      <c r="D84" t="s">
-        <v>613</v>
-      </c>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>629</v>
+        <v>611</v>
       </c>
       <c r="C85" t="s">
-        <v>630</v>
+        <v>612</v>
       </c>
       <c r="D85" t="s">
-        <v>631</v>
+        <v>613</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>614</v>
-      </c>
-      <c r="B86" t="s">
-        <v>651</v>
+        <v>629</v>
       </c>
       <c r="C86" t="s">
-        <v>615</v>
+        <v>630</v>
       </c>
       <c r="D86" t="s">
-        <v>616</v>
+        <v>631</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="B87" t="s">
         <v>651</v>
       </c>
       <c r="C87" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="D87" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>183</v>
+        <v>617</v>
       </c>
       <c r="B88" t="s">
-        <v>184</v>
+        <v>651</v>
       </c>
       <c r="C88" t="s">
-        <v>78</v>
+        <v>618</v>
       </c>
       <c r="D88" t="s">
-        <v>79</v>
+        <v>619</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="B89" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C89" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="D89" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>181</v>
+        <v>64</v>
       </c>
       <c r="B90" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C90" t="s">
-        <v>188</v>
+        <v>65</v>
       </c>
       <c r="D90" t="s">
-        <v>189</v>
+        <v>66</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>219</v>
+        <v>181</v>
       </c>
       <c r="B91" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="C91" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="D91" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B92" t="s">
         <v>220</v>
       </c>
       <c r="C92" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="D92" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>689</v>
+        <v>221</v>
+      </c>
+      <c r="B93" t="s">
+        <v>220</v>
       </c>
       <c r="C93" t="s">
-        <v>690</v>
+        <v>237</v>
       </c>
       <c r="D93" t="s">
-        <v>688</v>
+        <v>237</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>663</v>
+        <v>689</v>
       </c>
       <c r="C94" t="s">
-        <v>664</v>
+        <v>690</v>
       </c>
       <c r="D94" t="s">
-        <v>665</v>
+        <v>688</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="C95" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="D95" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>795</v>
+        <v>660</v>
       </c>
       <c r="C96" t="s">
-        <v>796</v>
+        <v>661</v>
       </c>
       <c r="D96" t="s">
-        <v>797</v>
+        <v>662</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>645</v>
-      </c>
-      <c r="B97" t="s">
-        <v>650</v>
+        <v>795</v>
       </c>
       <c r="C97" t="s">
-        <v>647</v>
+        <v>796</v>
       </c>
       <c r="D97" t="s">
-        <v>646</v>
+        <v>797</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>785</v>
+        <v>645</v>
+      </c>
+      <c r="B98" t="s">
+        <v>650</v>
       </c>
       <c r="C98" t="s">
-        <v>786</v>
+        <v>647</v>
       </c>
       <c r="D98" t="s">
-        <v>787</v>
+        <v>646</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>794</v>
+        <v>785</v>
       </c>
       <c r="C99" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="D99" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>635</v>
-      </c>
-      <c r="B100" t="s">
-        <v>648</v>
+        <v>794</v>
       </c>
       <c r="C100" t="s">
-        <v>636</v>
+        <v>789</v>
       </c>
       <c r="D100" t="s">
-        <v>851</v>
+        <v>788</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>850</v>
+        <v>635</v>
       </c>
       <c r="B101" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C101" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D101" t="s">
-        <v>638</v>
+        <v>851</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c r="B102" t="s">
-        <v>848</v>
+        <v>649</v>
       </c>
       <c r="C102" t="s">
-        <v>849</v>
+        <v>637</v>
       </c>
       <c r="D102" t="s">
-        <v>852</v>
+        <v>638</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>632</v>
+        <v>847</v>
       </c>
       <c r="B103" t="s">
-        <v>232</v>
+        <v>848</v>
       </c>
       <c r="C103" t="s">
-        <v>633</v>
+        <v>849</v>
       </c>
       <c r="D103" t="s">
-        <v>634</v>
+        <v>852</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>234</v>
+        <v>632</v>
       </c>
       <c r="B104" t="s">
         <v>232</v>
       </c>
       <c r="C104" t="s">
-        <v>235</v>
+        <v>633</v>
       </c>
       <c r="D104" t="s">
-        <v>236</v>
+        <v>634</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>783</v>
+        <v>234</v>
+      </c>
+      <c r="B105" t="s">
+        <v>232</v>
       </c>
       <c r="C105" t="s">
-        <v>790</v>
+        <v>235</v>
       </c>
       <c r="D105" t="s">
-        <v>792</v>
+        <v>236</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C106" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D106" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>784</v>
+      </c>
+      <c r="C107" t="s">
+        <v>791</v>
+      </c>
+      <c r="D107" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>806</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C108" t="s">
         <v>804</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D108" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>80</v>
-      </c>
-      <c r="B109" t="s">
-        <v>81</v>
-      </c>
-      <c r="C109" t="s">
-        <v>89</v>
-      </c>
-      <c r="D109" t="s">
-        <v>90</v>
-      </c>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B110" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C110" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D110" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B111" t="s">
         <v>83</v>
       </c>
       <c r="C111" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D111" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B112" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C112" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D112" t="s">
-        <v>257</v>
+        <v>88</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>103</v>
+      </c>
+      <c r="B113" t="s">
+        <v>81</v>
+      </c>
+      <c r="C113" t="s">
+        <v>104</v>
+      </c>
+      <c r="D113" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>91</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>92</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" t="s">
         <v>93</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D114" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>317</v>
-      </c>
-      <c r="B115" t="s">
-        <v>316</v>
-      </c>
-      <c r="C115" t="s">
-        <v>322</v>
-      </c>
-      <c r="D115" t="s">
-        <v>323</v>
-      </c>
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B116" t="s">
         <v>316</v>
       </c>
       <c r="C116" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D116" t="s">
         <v>323</v>
@@ -5110,1951 +5119,1965 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="B117" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C117" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D117" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B118" t="s">
         <v>319</v>
       </c>
       <c r="C118" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D118" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>413</v>
+        <v>326</v>
+      </c>
+      <c r="B119" t="s">
+        <v>319</v>
       </c>
       <c r="C119" t="s">
-        <v>414</v>
+        <v>327</v>
       </c>
       <c r="D119" t="s">
-        <v>415</v>
+        <v>328</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>329</v>
+        <v>413</v>
       </c>
       <c r="C120" t="s">
-        <v>331</v>
+        <v>414</v>
       </c>
       <c r="D120" t="s">
-        <v>330</v>
+        <v>415</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>406</v>
+        <v>329</v>
       </c>
       <c r="C121" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D121" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C122" t="s">
-        <v>411</v>
+        <v>332</v>
       </c>
       <c r="D122" t="s">
-        <v>412</v>
+        <v>333</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C123" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D123" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>334</v>
+        <v>408</v>
       </c>
       <c r="C124" t="s">
-        <v>336</v>
+        <v>410</v>
       </c>
       <c r="D124" t="s">
-        <v>335</v>
+        <v>409</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>350</v>
-      </c>
-      <c r="B125" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="C125" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="D125" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>400</v>
+        <v>350</v>
+      </c>
+      <c r="B126" t="s">
+        <v>351</v>
       </c>
       <c r="C126" t="s">
-        <v>402</v>
+        <v>352</v>
       </c>
       <c r="D126" t="s">
-        <v>404</v>
+        <v>353</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C127" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D127" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>354</v>
-      </c>
-      <c r="B128" t="s">
-        <v>355</v>
+        <v>401</v>
       </c>
       <c r="C128" t="s">
-        <v>356</v>
+        <v>403</v>
       </c>
       <c r="D128" t="s">
-        <v>357</v>
+        <v>405</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>418</v>
+        <v>354</v>
+      </c>
+      <c r="B129" t="s">
+        <v>355</v>
       </c>
       <c r="C129" t="s">
-        <v>392</v>
+        <v>356</v>
       </c>
       <c r="D129" t="s">
-        <v>393</v>
+        <v>357</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C130" t="s">
-        <v>420</v>
+        <v>392</v>
       </c>
       <c r="D130" t="s">
-        <v>421</v>
+        <v>393</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>337</v>
+        <v>419</v>
       </c>
       <c r="C131" t="s">
-        <v>366</v>
+        <v>420</v>
       </c>
       <c r="D131" t="s">
-        <v>338</v>
+        <v>421</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
       <c r="C132" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="D132" t="s">
-        <v>359</v>
+        <v>338</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C133" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D133" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C134" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D134" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C135" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D135" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C136" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D136" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C137" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D137" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>394</v>
+        <v>373</v>
       </c>
       <c r="C138" t="s">
-        <v>399</v>
+        <v>374</v>
       </c>
       <c r="D138" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>379</v>
+        <v>394</v>
       </c>
       <c r="C139" t="s">
-        <v>383</v>
+        <v>399</v>
       </c>
       <c r="D139" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="C140" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="D140" t="s">
-        <v>397</v>
+        <v>416</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>380</v>
+        <v>395</v>
       </c>
       <c r="C141" t="s">
-        <v>765</v>
+        <v>396</v>
       </c>
       <c r="D141" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C142" t="s">
-        <v>386</v>
+        <v>765</v>
       </c>
       <c r="D142" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="C143" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D143" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="C144" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="D144" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>504</v>
-      </c>
-      <c r="C145" s="9" t="s">
-        <v>505</v>
+        <v>382</v>
+      </c>
+      <c r="C145" t="s">
+        <v>387</v>
       </c>
       <c r="D145" t="s">
-        <v>506</v>
+        <v>388</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>422</v>
-      </c>
-      <c r="C146" t="s">
-        <v>423</v>
+        <v>504</v>
+      </c>
+      <c r="C146" s="9" t="s">
+        <v>505</v>
       </c>
       <c r="D146" t="s">
-        <v>424</v>
+        <v>506</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C147" t="s">
-        <v>480</v>
+        <v>423</v>
       </c>
       <c r="D147" t="s">
-        <v>478</v>
+        <v>424</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C148" t="s">
-        <v>426</v>
+        <v>480</v>
       </c>
       <c r="D148" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>510</v>
+        <v>427</v>
       </c>
       <c r="C149" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D149" t="s">
-        <v>432</v>
+        <v>479</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>528</v>
+        <v>510</v>
       </c>
       <c r="C150" t="s">
-        <v>526</v>
+        <v>431</v>
       </c>
       <c r="D150" t="s">
-        <v>527</v>
+        <v>432</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>433</v>
+        <v>528</v>
       </c>
       <c r="C151" t="s">
-        <v>434</v>
+        <v>526</v>
       </c>
       <c r="D151" t="s">
-        <v>435</v>
+        <v>527</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>472</v>
+        <v>433</v>
       </c>
       <c r="C152" t="s">
-        <v>474</v>
+        <v>434</v>
       </c>
       <c r="D152" t="s">
-        <v>476</v>
+        <v>435</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C153" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D153" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="C154" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="D154" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>514</v>
+        <v>481</v>
       </c>
       <c r="C155" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D155" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>486</v>
+        <v>514</v>
       </c>
       <c r="C156" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D156" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C157" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="D157" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C158" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D158" t="s">
-        <v>521</v>
+        <v>492</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>507</v>
-      </c>
-      <c r="C159" s="9" t="s">
-        <v>508</v>
+        <v>490</v>
+      </c>
+      <c r="C159" t="s">
+        <v>493</v>
       </c>
       <c r="D159" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D160" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D161" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D162" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>493</v>
+        <v>520</v>
       </c>
       <c r="D163" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>522</v>
+        <v>493</v>
       </c>
       <c r="D164" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>537</v>
+        <v>522</v>
       </c>
       <c r="D165" t="s">
-        <v>538</v>
+        <v>523</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="D166" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D167" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="D168" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="D169" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="D170" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>570</v>
+        <v>552</v>
       </c>
       <c r="D171" t="s">
-        <v>571</v>
+        <v>553</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>556</v>
+        <v>570</v>
       </c>
       <c r="D172" t="s">
-        <v>558</v>
+        <v>571</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D173" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>566</v>
+        <v>555</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="D174" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D175" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>561</v>
-      </c>
-      <c r="D176" s="9" t="s">
-        <v>561</v>
+        <v>564</v>
+      </c>
+      <c r="D176" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D177" s="9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
       <c r="D178" s="9" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="D179" s="9" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>579</v>
+      </c>
+      <c r="C180" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="D180" s="9" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>580</v>
       </c>
-      <c r="C180" s="9" t="s">
+      <c r="C181" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="D180" s="9" t="s">
+      <c r="D181" s="9" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="3" t="s">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B181" s="3"/>
-      <c r="C181" s="3"/>
-      <c r="D181" s="3"/>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>680</v>
-      </c>
-      <c r="C182" t="s">
-        <v>681</v>
-      </c>
-      <c r="D182" t="s">
-        <v>682</v>
-      </c>
+      <c r="B182" s="3"/>
+      <c r="C182" s="3"/>
+      <c r="D182" s="3"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="C183" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D183" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="C184" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D184" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>687</v>
-      </c>
-      <c r="C185" s="7" t="s">
-        <v>677</v>
-      </c>
-      <c r="D185" s="7" t="s">
-        <v>678</v>
+        <v>679</v>
+      </c>
+      <c r="C185" t="s">
+        <v>684</v>
+      </c>
+      <c r="D185" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>140</v>
-      </c>
-      <c r="B186" t="s">
-        <v>137</v>
-      </c>
-      <c r="C186" t="s">
-        <v>138</v>
-      </c>
-      <c r="D186" t="s">
-        <v>139</v>
+        <v>687</v>
+      </c>
+      <c r="C186" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="D186" s="7" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B187" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C187" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="D187" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B188" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C188" t="s">
-        <v>669</v>
+        <v>150</v>
       </c>
       <c r="D188" t="s">
-        <v>670</v>
+        <v>151</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B189" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C189" t="s">
-        <v>149</v>
+        <v>669</v>
       </c>
       <c r="D189" t="s">
-        <v>148</v>
+        <v>670</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B190" t="s">
-        <v>145</v>
-      </c>
-      <c r="C190" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D190" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
+      </c>
+      <c r="C190" t="s">
+        <v>149</v>
+      </c>
+      <c r="D190" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>667</v>
-      </c>
-      <c r="C191" t="s">
-        <v>666</v>
-      </c>
-      <c r="D191" t="s">
-        <v>666</v>
+        <v>144</v>
+      </c>
+      <c r="B191" t="s">
+        <v>145</v>
+      </c>
+      <c r="C191" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D191" s="7" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C192" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="D192" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>668</v>
+      </c>
+      <c r="C193" t="s">
+        <v>672</v>
+      </c>
+      <c r="D193" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>673</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C194" t="s">
         <v>674</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D194" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="6" t="s">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B194" s="6"/>
-      <c r="C194" s="6"/>
-      <c r="D194" s="6"/>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>47</v>
-      </c>
-      <c r="B195" t="s">
-        <v>8</v>
-      </c>
-      <c r="C195" t="s">
-        <v>48</v>
-      </c>
-      <c r="D195" t="s">
-        <v>49</v>
-      </c>
+      <c r="B195" s="6"/>
+      <c r="C195" s="6"/>
+      <c r="D195" s="6"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="B196" t="s">
         <v>8</v>
       </c>
       <c r="C196" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="D196" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>588</v>
+        <v>95</v>
+      </c>
+      <c r="B197" t="s">
+        <v>8</v>
       </c>
       <c r="C197" t="s">
-        <v>589</v>
+        <v>96</v>
       </c>
       <c r="D197" t="s">
-        <v>590</v>
+        <v>97</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C198" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D198" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>623</v>
+        <v>591</v>
       </c>
       <c r="C199" t="s">
-        <v>625</v>
+        <v>592</v>
       </c>
       <c r="D199" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C200" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D200" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>780</v>
+        <v>624</v>
       </c>
       <c r="C201" t="s">
-        <v>781</v>
+        <v>628</v>
       </c>
       <c r="D201" t="s">
-        <v>782</v>
+        <v>627</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>50</v>
-      </c>
-      <c r="B202" t="s">
-        <v>8</v>
+        <v>780</v>
       </c>
       <c r="C202" t="s">
-        <v>51</v>
+        <v>781</v>
       </c>
       <c r="D202" t="s">
-        <v>52</v>
+        <v>782</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B203" t="s">
         <v>8</v>
       </c>
       <c r="C203" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D203" t="s">
-        <v>222</v>
+        <v>52</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>217</v>
+        <v>53</v>
       </c>
       <c r="B204" t="s">
         <v>8</v>
       </c>
       <c r="C204" t="s">
-        <v>218</v>
+        <v>54</v>
       </c>
       <c r="D204" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>340</v>
+        <v>217</v>
       </c>
       <c r="B205" t="s">
         <v>8</v>
       </c>
       <c r="C205" t="s">
-        <v>605</v>
+        <v>218</v>
       </c>
       <c r="D205" t="s">
-        <v>607</v>
+        <v>218</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>606</v>
+        <v>340</v>
+      </c>
+      <c r="B206" t="s">
+        <v>8</v>
       </c>
       <c r="C206" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D206" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>798</v>
+        <v>606</v>
       </c>
       <c r="C207" t="s">
-        <v>799</v>
+        <v>604</v>
       </c>
       <c r="D207" t="s">
-        <v>800</v>
+        <v>608</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>155</v>
-      </c>
-      <c r="B208" t="s">
-        <v>8</v>
+        <v>798</v>
       </c>
       <c r="C208" t="s">
-        <v>585</v>
+        <v>799</v>
       </c>
       <c r="D208" t="s">
-        <v>156</v>
+        <v>800</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B209" t="s">
         <v>8</v>
       </c>
       <c r="C209" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D209" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B210" t="s">
         <v>8</v>
       </c>
       <c r="C210" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D210" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>594</v>
+        <v>173</v>
       </c>
       <c r="B211" t="s">
         <v>8</v>
       </c>
       <c r="C211" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="D211" t="s">
-        <v>596</v>
+        <v>174</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="B212" t="s">
         <v>8</v>
       </c>
       <c r="C212" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D212" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B213" t="s">
         <v>8</v>
       </c>
       <c r="C213" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D213" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>154</v>
+        <v>602</v>
       </c>
       <c r="B214" t="s">
         <v>8</v>
       </c>
       <c r="C214" t="s">
-        <v>190</v>
+        <v>600</v>
       </c>
       <c r="D214" t="s">
-        <v>191</v>
+        <v>598</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>55</v>
+        <v>154</v>
       </c>
       <c r="B215" t="s">
         <v>8</v>
       </c>
       <c r="C215" t="s">
-        <v>56</v>
+        <v>190</v>
       </c>
       <c r="D215" t="s">
-        <v>57</v>
+        <v>191</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>162</v>
+        <v>55</v>
       </c>
       <c r="B216" t="s">
         <v>8</v>
       </c>
       <c r="C216" t="s">
-        <v>157</v>
+        <v>56</v>
       </c>
       <c r="D216" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B217" t="s">
         <v>8</v>
       </c>
       <c r="C217" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D217" t="s">
-        <v>169</v>
+        <v>16</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>58</v>
+        <v>167</v>
       </c>
       <c r="B218" t="s">
         <v>8</v>
       </c>
       <c r="C218" t="s">
-        <v>59</v>
+        <v>168</v>
       </c>
       <c r="D218" t="s">
-        <v>60</v>
+        <v>169</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>161</v>
+        <v>58</v>
       </c>
       <c r="B219" t="s">
         <v>8</v>
       </c>
       <c r="C219" t="s">
-        <v>163</v>
+        <v>59</v>
       </c>
       <c r="D219" t="s">
-        <v>164</v>
+        <v>60</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B220" t="s">
         <v>8</v>
       </c>
       <c r="C220" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D220" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>61</v>
+        <v>170</v>
       </c>
       <c r="B221" t="s">
         <v>8</v>
       </c>
       <c r="C221" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
       <c r="D221" t="s">
-        <v>63</v>
+        <v>172</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>160</v>
+        <v>61</v>
       </c>
       <c r="B222" t="s">
         <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
       <c r="D222" t="s">
-        <v>159</v>
+        <v>63</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B223" t="s">
         <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="D223" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="B224" t="s">
         <v>8</v>
       </c>
       <c r="C224" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="D224" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B225" t="s">
         <v>8</v>
       </c>
       <c r="C225" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D225" t="s">
-        <v>105</v>
+        <v>193</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B226" t="s">
         <v>8</v>
       </c>
       <c r="C226" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D226" t="s">
-        <v>199</v>
+        <v>105</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>275</v>
+        <v>197</v>
+      </c>
+      <c r="B227" t="s">
+        <v>8</v>
       </c>
       <c r="C227" t="s">
-        <v>276</v>
+        <v>198</v>
       </c>
       <c r="D227" t="s">
-        <v>277</v>
+        <v>199</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>67</v>
-      </c>
-      <c r="B228" t="s">
-        <v>8</v>
+        <v>275</v>
       </c>
       <c r="C228" t="s">
-        <v>68</v>
+        <v>276</v>
       </c>
       <c r="D228" t="s">
-        <v>69</v>
+        <v>277</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="B229" t="s">
         <v>8</v>
       </c>
       <c r="C229" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="D229" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>428</v>
+        <v>7</v>
+      </c>
+      <c r="B230" t="s">
+        <v>8</v>
       </c>
       <c r="C230" t="s">
-        <v>429</v>
+        <v>9</v>
       </c>
       <c r="D230" t="s">
-        <v>430</v>
+        <v>10</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>200</v>
-      </c>
-      <c r="B231" t="s">
-        <v>8</v>
+        <v>428</v>
       </c>
       <c r="C231" t="s">
-        <v>200</v>
+        <v>429</v>
       </c>
       <c r="D231" t="s">
-        <v>201</v>
+        <v>430</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="B232" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C232" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="D232" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="B233" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="C233" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="D233" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B234" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C234" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D234" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="B235" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="C235" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="D235" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B236" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C236" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D236" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="B237" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="C237" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="D237" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B238" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C238" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D238" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>106</v>
+        <v>212</v>
       </c>
       <c r="B239" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="C239" t="s">
-        <v>107</v>
+        <v>214</v>
       </c>
       <c r="D239" t="s">
-        <v>108</v>
+        <v>216</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>208</v>
+        <v>106</v>
       </c>
       <c r="B240" t="s">
         <v>8</v>
       </c>
       <c r="C240" t="s">
-        <v>209</v>
+        <v>107</v>
       </c>
       <c r="D240" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>14</v>
+        <v>208</v>
       </c>
       <c r="B241" t="s">
         <v>8</v>
       </c>
       <c r="C241" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
       <c r="D241" t="s">
-        <v>16</v>
+        <v>210</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>376</v>
+        <v>14</v>
+      </c>
+      <c r="B242" t="s">
+        <v>8</v>
       </c>
       <c r="C242" t="s">
-        <v>377</v>
+        <v>15</v>
       </c>
       <c r="D242" t="s">
-        <v>378</v>
+        <v>16</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>494</v>
+        <v>376</v>
       </c>
       <c r="C243" t="s">
-        <v>495</v>
+        <v>377</v>
       </c>
       <c r="D243" t="s">
-        <v>496</v>
+        <v>378</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>417</v>
-      </c>
-      <c r="B244" t="s">
-        <v>307</v>
+        <v>494</v>
       </c>
       <c r="C244" t="s">
-        <v>308</v>
+        <v>495</v>
       </c>
       <c r="D244" t="s">
-        <v>309</v>
+        <v>496</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>436</v>
+        <v>417</v>
+      </c>
+      <c r="B245" t="s">
+        <v>307</v>
       </c>
       <c r="C245" t="s">
-        <v>448</v>
+        <v>308</v>
       </c>
       <c r="D245" t="s">
-        <v>460</v>
+        <v>309</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C246" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D246" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C247" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D247" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C248" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D248" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C249" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D249" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C250" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D250" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C251" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D251" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C252" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D252" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C253" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D253" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C254" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D254" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C255" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D255" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C256" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D256" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>499</v>
+        <v>447</v>
       </c>
       <c r="C257" t="s">
-        <v>498</v>
+        <v>459</v>
       </c>
       <c r="D257" t="s">
-        <v>497</v>
+        <v>471</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>575</v>
+        <v>499</v>
       </c>
       <c r="C258" t="s">
-        <v>2</v>
+        <v>498</v>
       </c>
       <c r="D258" t="s">
-        <v>576</v>
+        <v>497</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
+        <v>575</v>
+      </c>
+      <c r="C259" t="s">
+        <v>2</v>
+      </c>
+      <c r="D259" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
         <v>577</v>
       </c>
-      <c r="C259" t="s">
+      <c r="C260" t="s">
         <v>578</v>
       </c>
-      <c r="D259" t="s">
+      <c r="D260" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A260" s="2" t="s">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B260" s="2"/>
-      <c r="C260" s="2"/>
-      <c r="D260" s="2"/>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A261" t="s">
-        <v>110</v>
-      </c>
-      <c r="B261" t="s">
-        <v>109</v>
-      </c>
-      <c r="C261" t="s">
-        <v>129</v>
-      </c>
-      <c r="D261" t="s">
-        <v>128</v>
-      </c>
+      <c r="B261" s="2"/>
+      <c r="C261" s="2"/>
+      <c r="D261" s="2"/>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B262" t="s">
         <v>109</v>
       </c>
       <c r="C262" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D262" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B263" t="s">
         <v>109</v>
       </c>
       <c r="C263" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="D263" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B264" t="s">
         <v>109</v>
       </c>
       <c r="C264" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D264" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B265" t="s">
         <v>109</v>
       </c>
       <c r="C265" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D265" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B266" t="s">
         <v>109</v>
       </c>
       <c r="C266" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="D266" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B267" t="s">
         <v>109</v>
       </c>
       <c r="C267" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D267" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B268" t="s">
         <v>109</v>
       </c>
       <c r="C268" t="s">
+        <v>131</v>
+      </c>
+      <c r="D268" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>124</v>
+      </c>
+      <c r="B269" t="s">
+        <v>109</v>
+      </c>
+      <c r="C269" t="s">
         <v>125</v>
       </c>
-      <c r="D268" t="s">
+      <c r="D269" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A269" s="3" t="s">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B269" s="3"/>
-      <c r="C269" s="3"/>
-      <c r="D269" s="3"/>
-    </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A270" t="s">
-        <v>70</v>
-      </c>
-      <c r="B270" t="s">
-        <v>71</v>
-      </c>
-      <c r="C270" t="s">
-        <v>343</v>
-      </c>
-      <c r="D270" t="s">
-        <v>344</v>
-      </c>
+      <c r="B270" s="3"/>
+      <c r="C270" s="3"/>
+      <c r="D270" s="3"/>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>341</v>
+        <v>70</v>
       </c>
       <c r="B271" t="s">
         <v>71</v>
       </c>
       <c r="C271" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="D271" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>153</v>
+        <v>341</v>
       </c>
       <c r="B272" t="s">
         <v>71</v>
       </c>
       <c r="C272" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D272" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>347</v>
+        <v>153</v>
       </c>
       <c r="B273" t="s">
         <v>71</v>
       </c>
       <c r="C273" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D273" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>72</v>
+        <v>347</v>
       </c>
       <c r="B274" t="s">
         <v>71</v>
       </c>
       <c r="C274" t="s">
-        <v>73</v>
+        <v>348</v>
       </c>
       <c r="D274" t="s">
-        <v>74</v>
+        <v>349</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>609</v>
+        <v>72</v>
+      </c>
+      <c r="B275" t="s">
+        <v>71</v>
       </c>
       <c r="C275" t="s">
-        <v>603</v>
+        <v>73</v>
       </c>
       <c r="D275" t="s">
-        <v>610</v>
+        <v>74</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
       <c r="C276" t="s">
-        <v>621</v>
+        <v>603</v>
       </c>
       <c r="D276" t="s">
-        <v>622</v>
+        <v>610</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
+        <v>620</v>
+      </c>
+      <c r="C277" t="s">
+        <v>621</v>
+      </c>
+      <c r="D277" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
         <v>801</v>
       </c>
-      <c r="C277" t="s">
+      <c r="C278" t="s">
         <v>802</v>
       </c>
-      <c r="D277" t="s">
+      <c r="D278" t="s">
         <v>803</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C185" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
-    <hyperlink ref="D185" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
+    <hyperlink ref="C186" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
+    <hyperlink ref="D186" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
UI cleanup and translations
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD0BAB3-E671-4BD5-80FC-A2E9B76A4FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFB5893-4B53-4BD9-8B49-469281867907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="880">
   <si>
     <t>id</t>
   </si>
@@ -98,12 +98,6 @@
     <t>Home page welcome message</t>
   </si>
   <si>
-    <t>Dive into the world of hydrology, meteorology, and water chemistry with the Yukon Water Resources Branch's latest insights. Our mission? To bring data to your fingertips, aligning with the Open Government initiative for transparency, citizen empowerment, and sparking research creativity.&lt;br&gt;&lt;br&gt;📊 📈 Explore real-time data like never before, made available under the terms of our limitations of liability. Let's innovate together!</t>
-  </si>
-  <si>
-    <t>Plongez dans le monde de l'hydrologie, de la météorologie et de la chimie de l'eau avec les dernières perspectives de la Branche des ressources en eau du Yukon. Notre mission? Mettre les données à portée de main, en alignement avec l'initiative de Gouvernement Ouvert pour la transparence, l'engagement des citoyens et l'incitation à la recherche créative.&lt;br&gt;&lt;br&gt;📊 📈 Explorez les données en temps réel comme jamais auparavant, disponibles sous entente de nos limitations de responsabilité. Innovons ensemble !</t>
-  </si>
-  <si>
     <t>disclaimer_title</t>
   </si>
   <si>
@@ -2588,9 +2582,6 @@
     <t>séries temporelles</t>
   </si>
   <si>
-    <t>homeText_saved</t>
-  </si>
-  <si>
     <t>Plongez dans le monde de l'hydrologie, de la météorologie et de la chimie de l'eau avec le département de l'environment du gouvernement du Yukon. Notre mission? Mettre les données à portée de main, en alignement avec l'initiative de Gouvernement Ouvert pour la transparence, l'engagement des citoyens et l'incitation à la recherche créative. 📊 📈 Explorez les données en temps réel comme jamais auparavant, disponibles sous entente de nos limitations de responsabilité.</t>
   </si>
   <si>
@@ -2631,6 +2622,57 @@
   </si>
   <si>
     <t>Heads up: the most recent measurements will be compared against historical daily means values. Keep this in mind when viewing parameters that fluctuate throughout a day, such as temperature.</t>
+  </si>
+  <si>
+    <t>home_discrete_continuous</t>
+  </si>
+  <si>
+    <t>home_discrete_continuous_title</t>
+  </si>
+  <si>
+    <t>A note about how our data is organized:</t>
+  </si>
+  <si>
+    <t>Explainer for discrete vs continuous</t>
+  </si>
+  <si>
+    <t>We classify our data as either &lt;b&gt;discrete (snapshot)&lt;/b&gt; or &lt;b&gt;continuous&lt;/b&gt; based on measurement frequency, method of collection, and relevant metadata.&lt;div style="margin-top:0.25em;"&gt;&lt;/div&gt;&lt;li&gt;&lt;b&gt;Discrete data&lt;/b&gt; are snapshot observations collected manually (e.g. snow surveys results) or by laboratory analysis and require descriptions of how the sample was acquired, the analysis method, etc.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Continuous data&lt;/b&gt; come from automated instruments that record at regular intervals (e.g. hourly) and may include metadata on instrument type and recording interval.&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>Nous classons nos données en deux catégories : &lt;b&gt;discrètes&lt;/b&gt; ou &lt;b&gt;continues&lt;/b&gt; en fonction de la fréquence des mesures, de la méthode de collecte et des métadonnées pertinentes.&lt;div style="margin-top:0.25em;"&gt;&lt;/div&gt;&lt;li&gt;&lt;b&gt;Données discrètes&lt;/b&gt; : observations ponctuelles recueillies manuellement (p. ex. résultats des relevés de neige) ou par analyse en laboratoire, nécessitant une description du prélèvement, de la méthode d’analyse, etc.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Données continues&lt;/b&gt; : issues d’instruments automatisés enregistrant à intervalles réguliers (p. ex. toutes les heures) et pouvant inclure des métadonnées sur le type d’instrument et l’intervalle d’enregistrement.&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>Note au sujet de l'organization de nos données:</t>
+  </si>
+  <si>
+    <t>home_map_locs_btn</t>
+  </si>
+  <si>
+    <t>See a map of monitoring locations</t>
+  </si>
+  <si>
+    <t>Voire une carte avec les sites de surveillance</t>
+  </si>
+  <si>
+    <t>home_plot_cont_btn</t>
+  </si>
+  <si>
+    <t>home_plot_disc_btn</t>
+  </si>
+  <si>
+    <t>home_dl_cont_btn</t>
+  </si>
+  <si>
+    <t>home_dl_disc_btn</t>
+  </si>
+  <si>
+    <t>Voire une carte des conditions actuelles ou historiques</t>
+  </si>
+  <si>
+    <t>home_map_params_btn</t>
+  </si>
+  <si>
+    <t>See a map of  current or past conditions</t>
   </si>
 </sst>
 </file>
@@ -3567,10 +3609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D281"/>
+  <dimension ref="A1:D288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3601,7 +3643,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -3612,21 +3654,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
+        <v>499</v>
+      </c>
+      <c r="C3" t="s">
         <v>501</v>
       </c>
-      <c r="C3" t="s">
-        <v>503</v>
-      </c>
       <c r="D3" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3637,7 +3679,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -3648,301 +3690,301 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B6" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C6" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D6" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B7" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C7" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D7" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B8" t="s">
+        <v>756</v>
+      </c>
+      <c r="C8" t="s">
+        <v>757</v>
+      </c>
+      <c r="D8" t="s">
         <v>758</v>
-      </c>
-      <c r="C8" t="s">
-        <v>759</v>
-      </c>
-      <c r="D8" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>696</v>
+      </c>
+      <c r="B9" t="s">
+        <v>734</v>
+      </c>
+      <c r="C9" t="s">
+        <v>697</v>
+      </c>
+      <c r="D9" t="s">
         <v>698</v>
-      </c>
-      <c r="B9" t="s">
-        <v>736</v>
-      </c>
-      <c r="C9" t="s">
-        <v>699</v>
-      </c>
-      <c r="D9" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B10" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C10" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>704</v>
+      </c>
+      <c r="B11" t="s">
+        <v>733</v>
+      </c>
+      <c r="C11" t="s">
+        <v>705</v>
+      </c>
+      <c r="D11" t="s">
         <v>706</v>
-      </c>
-      <c r="B11" t="s">
-        <v>735</v>
-      </c>
-      <c r="C11" t="s">
-        <v>707</v>
-      </c>
-      <c r="D11" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>707</v>
+      </c>
+      <c r="B12" t="s">
+        <v>731</v>
+      </c>
+      <c r="C12" t="s">
+        <v>708</v>
+      </c>
+      <c r="D12" t="s">
         <v>709</v>
-      </c>
-      <c r="B12" t="s">
-        <v>733</v>
-      </c>
-      <c r="C12" t="s">
-        <v>710</v>
-      </c>
-      <c r="D12" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>712</v>
+      </c>
+      <c r="B13" t="s">
+        <v>732</v>
+      </c>
+      <c r="C13" t="s">
+        <v>713</v>
+      </c>
+      <c r="D13" t="s">
         <v>714</v>
-      </c>
-      <c r="B13" t="s">
-        <v>734</v>
-      </c>
-      <c r="C13" t="s">
-        <v>715</v>
-      </c>
-      <c r="D13" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B14" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C14" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D14" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B15" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C15" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="D15" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B16" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C16" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D16" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B17" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="C17" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D17" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B18" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B19" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C19" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D19" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B20" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C20" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D20" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B21" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>741</v>
+      </c>
+      <c r="B22" t="s">
+        <v>747</v>
+      </c>
+      <c r="C22" t="s">
         <v>743</v>
       </c>
-      <c r="B22" t="s">
-        <v>749</v>
-      </c>
-      <c r="C22" t="s">
-        <v>745</v>
-      </c>
       <c r="D22" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>742</v>
+      </c>
+      <c r="B23" t="s">
+        <v>748</v>
+      </c>
+      <c r="C23" t="s">
         <v>744</v>
       </c>
-      <c r="B23" t="s">
-        <v>750</v>
-      </c>
-      <c r="C23" t="s">
-        <v>746</v>
-      </c>
       <c r="D23" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B24" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C24" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D24" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B25" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B26" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C26" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="D26" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -3950,30 +3992,30 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B28" t="s">
+        <v>652</v>
+      </c>
+      <c r="C28" t="s">
         <v>654</v>
       </c>
-      <c r="C28" t="s">
-        <v>656</v>
-      </c>
       <c r="D28" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B29" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C29" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3984,1003 +4026,1009 @@
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D30" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>851</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>850</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>849</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>864</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>866</v>
       </c>
       <c r="C32" t="s">
-        <v>853</v>
+        <v>865</v>
       </c>
       <c r="D32" t="s">
-        <v>852</v>
+        <v>869</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>863</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>866</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>867</v>
       </c>
       <c r="D33" t="s">
-        <v>26</v>
+        <v>868</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>870</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>230</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>871</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>872</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>878</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>230</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>879</v>
       </c>
       <c r="D35" t="s">
-        <v>33</v>
+        <v>877</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>873</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>230</v>
       </c>
       <c r="C36" t="s">
-        <v>35</v>
+        <v>787</v>
       </c>
       <c r="D36" t="s">
-        <v>36</v>
+        <v>788</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+      <c r="A37" t="s">
+        <v>874</v>
+      </c>
+      <c r="B37" t="s">
+        <v>230</v>
+      </c>
+      <c r="C37" t="s">
+        <v>786</v>
+      </c>
+      <c r="D37" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>282</v>
+        <v>875</v>
       </c>
       <c r="B38" t="s">
-        <v>284</v>
+        <v>230</v>
       </c>
       <c r="C38" t="s">
-        <v>531</v>
+        <v>785</v>
       </c>
       <c r="D38" t="s">
-        <v>532</v>
+        <v>783</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>285</v>
+        <v>876</v>
       </c>
       <c r="B39" t="s">
-        <v>287</v>
+        <v>230</v>
       </c>
       <c r="C39" t="s">
-        <v>288</v>
+        <v>782</v>
       </c>
       <c r="D39" t="s">
-        <v>289</v>
+        <v>784</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>286</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>292</v>
+        <v>22</v>
       </c>
       <c r="C40" t="s">
-        <v>291</v>
+        <v>23</v>
       </c>
       <c r="D40" t="s">
-        <v>290</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>293</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>299</v>
+        <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>302</v>
+        <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>303</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>297</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>300</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>294</v>
+        <v>30</v>
       </c>
       <c r="D42" t="s">
-        <v>304</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>295</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>299</v>
+        <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>306</v>
+        <v>33</v>
       </c>
       <c r="D43" t="s">
-        <v>305</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>298</v>
-      </c>
-      <c r="B44" t="s">
-        <v>300</v>
-      </c>
-      <c r="C44" t="s">
-        <v>296</v>
-      </c>
-      <c r="D44" t="s">
-        <v>301</v>
-      </c>
+      <c r="A44" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>533</v>
+        <v>280</v>
       </c>
       <c r="B45" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="C45" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="D45" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>310</v>
+        <v>283</v>
       </c>
       <c r="B46" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="C46" t="s">
-        <v>311</v>
+        <v>286</v>
       </c>
       <c r="D46" t="s">
-        <v>312</v>
+        <v>287</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
       <c r="B47" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="C47" t="s">
-        <v>314</v>
+        <v>289</v>
       </c>
       <c r="D47" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+      <c r="A48" t="s">
+        <v>291</v>
+      </c>
+      <c r="B48" t="s">
+        <v>297</v>
+      </c>
+      <c r="C48" t="s">
+        <v>300</v>
+      </c>
+      <c r="D48" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>37</v>
+        <v>295</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>298</v>
       </c>
       <c r="C49" t="s">
-        <v>152</v>
+        <v>292</v>
       </c>
       <c r="D49" t="s">
-        <v>39</v>
+        <v>302</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>40</v>
+        <v>293</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>297</v>
       </c>
       <c r="C50" t="s">
-        <v>42</v>
+        <v>304</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>303</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="A51" t="s">
+        <v>296</v>
+      </c>
+      <c r="B51" t="s">
+        <v>298</v>
+      </c>
+      <c r="C51" t="s">
+        <v>294</v>
+      </c>
+      <c r="D51" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>233</v>
+        <v>531</v>
       </c>
       <c r="B52" t="s">
-        <v>231</v>
+        <v>298</v>
       </c>
       <c r="C52" t="s">
-        <v>238</v>
+        <v>532</v>
       </c>
       <c r="D52" t="s">
-        <v>239</v>
+        <v>533</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>75</v>
+        <v>308</v>
       </c>
       <c r="B53" t="s">
-        <v>185</v>
+        <v>298</v>
       </c>
       <c r="C53" t="s">
-        <v>76</v>
+        <v>309</v>
       </c>
       <c r="D53" t="s">
-        <v>77</v>
+        <v>310</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>240</v>
+        <v>311</v>
       </c>
       <c r="B54" t="s">
-        <v>242</v>
+        <v>305</v>
       </c>
       <c r="C54" t="s">
-        <v>842</v>
+        <v>312</v>
       </c>
       <c r="D54" t="s">
-        <v>241</v>
+        <v>313</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>643</v>
-      </c>
-      <c r="C55" t="s">
-        <v>843</v>
-      </c>
-      <c r="D55" t="s">
-        <v>644</v>
-      </c>
+      <c r="A55" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>246</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>248</v>
+        <v>36</v>
       </c>
       <c r="C56" t="s">
-        <v>247</v>
+        <v>150</v>
       </c>
       <c r="D56" t="s">
-        <v>271</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>243</v>
+        <v>38</v>
       </c>
       <c r="B57" t="s">
-        <v>249</v>
+        <v>39</v>
       </c>
       <c r="C57" t="s">
-        <v>252</v>
+        <v>40</v>
       </c>
       <c r="D57" t="s">
-        <v>251</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>244</v>
-      </c>
-      <c r="B58" t="s">
-        <v>249</v>
-      </c>
-      <c r="C58" t="s">
-        <v>838</v>
-      </c>
-      <c r="D58" t="s">
-        <v>841</v>
-      </c>
+      <c r="A58" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="B59" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="C59" t="s">
-        <v>839</v>
+        <v>236</v>
       </c>
       <c r="D59" t="s">
-        <v>840</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>639</v>
+        <v>73</v>
       </c>
       <c r="B60" t="s">
-        <v>250</v>
+        <v>183</v>
       </c>
       <c r="C60" t="s">
-        <v>844</v>
+        <v>74</v>
       </c>
       <c r="D60" t="s">
-        <v>253</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>640</v>
+        <v>238</v>
       </c>
       <c r="B61" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C61" t="s">
-        <v>641</v>
+        <v>840</v>
       </c>
       <c r="D61" t="s">
-        <v>642</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>270</v>
-      </c>
-      <c r="B62" t="s">
-        <v>250</v>
+        <v>641</v>
       </c>
       <c r="C62" t="s">
-        <v>836</v>
+        <v>841</v>
       </c>
       <c r="D62" t="s">
-        <v>837</v>
+        <v>642</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="B63" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C63" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="D63" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>805</v>
+        <v>241</v>
       </c>
       <c r="B64" t="s">
-        <v>807</v>
+        <v>247</v>
       </c>
       <c r="C64" t="s">
-        <v>808</v>
+        <v>250</v>
       </c>
       <c r="D64" t="s">
-        <v>810</v>
+        <v>249</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>806</v>
+        <v>242</v>
       </c>
       <c r="B65" t="s">
-        <v>807</v>
+        <v>247</v>
       </c>
       <c r="C65" t="s">
-        <v>809</v>
+        <v>836</v>
       </c>
       <c r="D65" t="s">
-        <v>811</v>
+        <v>839</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B66" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C66" t="s">
-        <v>259</v>
+        <v>837</v>
       </c>
       <c r="D66" t="s">
-        <v>260</v>
+        <v>838</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>272</v>
+        <v>637</v>
       </c>
       <c r="B67" t="s">
         <v>248</v>
       </c>
       <c r="C67" t="s">
-        <v>273</v>
+        <v>842</v>
       </c>
       <c r="D67" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>261</v>
+        <v>638</v>
       </c>
       <c r="B68" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C68" t="s">
-        <v>263</v>
+        <v>639</v>
       </c>
       <c r="D68" t="s">
-        <v>264</v>
+        <v>640</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B69" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C69" t="s">
-        <v>265</v>
+        <v>834</v>
       </c>
       <c r="D69" t="s">
-        <v>266</v>
+        <v>835</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="B70" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C70" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="D70" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>278</v>
+        <v>803</v>
       </c>
       <c r="B71" t="s">
-        <v>279</v>
+        <v>805</v>
       </c>
       <c r="C71" t="s">
-        <v>280</v>
+        <v>806</v>
       </c>
       <c r="D71" t="s">
-        <v>281</v>
+        <v>808</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>765</v>
+        <v>804</v>
       </c>
       <c r="B72" t="s">
-        <v>766</v>
+        <v>805</v>
       </c>
       <c r="C72" t="s">
-        <v>767</v>
+        <v>807</v>
       </c>
       <c r="D72" t="s">
-        <v>768</v>
+        <v>809</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>769</v>
+        <v>256</v>
       </c>
       <c r="B73" t="s">
-        <v>766</v>
+        <v>246</v>
       </c>
       <c r="C73" t="s">
-        <v>770</v>
+        <v>257</v>
       </c>
       <c r="D73" t="s">
-        <v>772</v>
+        <v>258</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>774</v>
+        <v>270</v>
       </c>
       <c r="B74" t="s">
-        <v>766</v>
+        <v>246</v>
       </c>
       <c r="C74" t="s">
-        <v>771</v>
+        <v>271</v>
       </c>
       <c r="D74" t="s">
-        <v>773</v>
+        <v>272</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>775</v>
+        <v>259</v>
       </c>
       <c r="B75" t="s">
-        <v>766</v>
+        <v>247</v>
       </c>
       <c r="C75" t="s">
-        <v>776</v>
+        <v>261</v>
       </c>
       <c r="D75" t="s">
-        <v>777</v>
+        <v>262</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>814</v>
+        <v>260</v>
       </c>
       <c r="B76" t="s">
-        <v>766</v>
+        <v>247</v>
       </c>
       <c r="C76" t="s">
-        <v>817</v>
+        <v>263</v>
       </c>
       <c r="D76" t="s">
-        <v>818</v>
+        <v>264</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>815</v>
+        <v>265</v>
       </c>
       <c r="B77" t="s">
-        <v>766</v>
+        <v>247</v>
       </c>
       <c r="C77" t="s">
-        <v>822</v>
+        <v>266</v>
       </c>
       <c r="D77" t="s">
-        <v>819</v>
+        <v>267</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>813</v>
+        <v>276</v>
       </c>
       <c r="B78" t="s">
-        <v>766</v>
+        <v>277</v>
       </c>
       <c r="C78" t="s">
-        <v>812</v>
+        <v>278</v>
       </c>
       <c r="D78" t="s">
-        <v>820</v>
+        <v>279</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>816</v>
+        <v>763</v>
       </c>
       <c r="B79" t="s">
+        <v>764</v>
+      </c>
+      <c r="C79" t="s">
+        <v>765</v>
+      </c>
+      <c r="D79" t="s">
         <v>766</v>
-      </c>
-      <c r="C79" t="s">
-        <v>823</v>
-      </c>
-      <c r="D79" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>824</v>
+        <v>767</v>
       </c>
       <c r="B80" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C80" t="s">
-        <v>825</v>
+        <v>768</v>
       </c>
       <c r="D80" t="s">
-        <v>826</v>
+        <v>770</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>827</v>
+        <v>772</v>
       </c>
       <c r="B81" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C81" t="s">
-        <v>828</v>
+        <v>769</v>
       </c>
       <c r="D81" t="s">
-        <v>829</v>
+        <v>771</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>833</v>
+        <v>773</v>
+      </c>
+      <c r="B82" t="s">
+        <v>764</v>
       </c>
       <c r="C82" t="s">
-        <v>834</v>
+        <v>774</v>
       </c>
       <c r="D82" t="s">
-        <v>835</v>
+        <v>775</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>830</v>
+        <v>812</v>
+      </c>
+      <c r="B83" t="s">
+        <v>764</v>
       </c>
       <c r="C83" t="s">
-        <v>831</v>
+        <v>815</v>
       </c>
       <c r="D83" t="s">
-        <v>832</v>
+        <v>816</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
+      <c r="A84" t="s">
+        <v>813</v>
+      </c>
+      <c r="B84" t="s">
+        <v>764</v>
+      </c>
+      <c r="C84" t="s">
+        <v>820</v>
+      </c>
+      <c r="D84" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>611</v>
+        <v>811</v>
+      </c>
+      <c r="B85" t="s">
+        <v>764</v>
       </c>
       <c r="C85" t="s">
-        <v>612</v>
+        <v>810</v>
       </c>
       <c r="D85" t="s">
-        <v>613</v>
+        <v>818</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>629</v>
+        <v>814</v>
+      </c>
+      <c r="B86" t="s">
+        <v>764</v>
       </c>
       <c r="C86" t="s">
-        <v>630</v>
+        <v>821</v>
       </c>
       <c r="D86" t="s">
-        <v>631</v>
+        <v>819</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>614</v>
+        <v>822</v>
       </c>
       <c r="B87" t="s">
-        <v>651</v>
+        <v>764</v>
       </c>
       <c r="C87" t="s">
-        <v>615</v>
+        <v>823</v>
       </c>
       <c r="D87" t="s">
-        <v>616</v>
+        <v>824</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>617</v>
+        <v>825</v>
       </c>
       <c r="B88" t="s">
-        <v>651</v>
+        <v>764</v>
       </c>
       <c r="C88" t="s">
-        <v>618</v>
+        <v>826</v>
       </c>
       <c r="D88" t="s">
-        <v>619</v>
+        <v>827</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>183</v>
-      </c>
-      <c r="B89" t="s">
-        <v>184</v>
+        <v>831</v>
       </c>
       <c r="C89" t="s">
-        <v>78</v>
+        <v>832</v>
       </c>
       <c r="D89" t="s">
-        <v>79</v>
+        <v>833</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>64</v>
-      </c>
-      <c r="B90" t="s">
-        <v>186</v>
+        <v>828</v>
       </c>
       <c r="C90" t="s">
-        <v>65</v>
+        <v>829</v>
       </c>
       <c r="D90" t="s">
-        <v>66</v>
+        <v>830</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>181</v>
-      </c>
-      <c r="B91" t="s">
-        <v>187</v>
-      </c>
-      <c r="C91" t="s">
-        <v>188</v>
-      </c>
-      <c r="D91" t="s">
-        <v>189</v>
-      </c>
+      <c r="A91" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>219</v>
-      </c>
-      <c r="B92" t="s">
-        <v>220</v>
+        <v>609</v>
       </c>
       <c r="C92" t="s">
-        <v>223</v>
+        <v>610</v>
       </c>
       <c r="D92" t="s">
-        <v>224</v>
+        <v>611</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>221</v>
-      </c>
-      <c r="B93" t="s">
-        <v>220</v>
+        <v>627</v>
       </c>
       <c r="C93" t="s">
-        <v>237</v>
+        <v>628</v>
       </c>
       <c r="D93" t="s">
-        <v>237</v>
+        <v>629</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>687</v>
+        <v>612</v>
+      </c>
+      <c r="B94" t="s">
+        <v>649</v>
       </c>
       <c r="C94" t="s">
-        <v>688</v>
+        <v>613</v>
       </c>
       <c r="D94" t="s">
-        <v>686</v>
+        <v>614</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>661</v>
+        <v>615</v>
+      </c>
+      <c r="B95" t="s">
+        <v>649</v>
       </c>
       <c r="C95" t="s">
-        <v>662</v>
+        <v>616</v>
       </c>
       <c r="D95" t="s">
-        <v>663</v>
+        <v>617</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>658</v>
+        <v>181</v>
+      </c>
+      <c r="B96" t="s">
+        <v>182</v>
       </c>
       <c r="C96" t="s">
-        <v>659</v>
+        <v>76</v>
       </c>
       <c r="D96" t="s">
-        <v>660</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>793</v>
+        <v>62</v>
+      </c>
+      <c r="B97" t="s">
+        <v>184</v>
       </c>
       <c r="C97" t="s">
-        <v>794</v>
+        <v>63</v>
       </c>
       <c r="D97" t="s">
-        <v>795</v>
+        <v>64</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>645</v>
+        <v>179</v>
       </c>
       <c r="B98" t="s">
-        <v>650</v>
+        <v>185</v>
       </c>
       <c r="C98" t="s">
-        <v>647</v>
+        <v>186</v>
       </c>
       <c r="D98" t="s">
-        <v>646</v>
+        <v>187</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>783</v>
+        <v>217</v>
+      </c>
+      <c r="B99" t="s">
+        <v>218</v>
       </c>
       <c r="C99" t="s">
-        <v>784</v>
+        <v>221</v>
       </c>
       <c r="D99" t="s">
-        <v>785</v>
+        <v>222</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>792</v>
+        <v>219</v>
+      </c>
+      <c r="B100" t="s">
+        <v>218</v>
       </c>
       <c r="C100" t="s">
-        <v>787</v>
+        <v>235</v>
       </c>
       <c r="D100" t="s">
-        <v>786</v>
+        <v>235</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>635</v>
-      </c>
-      <c r="B101" t="s">
-        <v>648</v>
+        <v>685</v>
       </c>
       <c r="C101" t="s">
-        <v>636</v>
+        <v>686</v>
       </c>
       <c r="D101" t="s">
-        <v>849</v>
+        <v>684</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>848</v>
-      </c>
-      <c r="B102" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
       <c r="C102" t="s">
-        <v>637</v>
+        <v>660</v>
       </c>
       <c r="D102" t="s">
-        <v>638</v>
+        <v>661</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>845</v>
-      </c>
-      <c r="B103" t="s">
-        <v>846</v>
+        <v>656</v>
       </c>
       <c r="C103" t="s">
-        <v>847</v>
+        <v>657</v>
       </c>
       <c r="D103" t="s">
-        <v>850</v>
+        <v>658</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>632</v>
-      </c>
-      <c r="B104" t="s">
-        <v>232</v>
+        <v>791</v>
       </c>
       <c r="C104" t="s">
-        <v>633</v>
+        <v>792</v>
       </c>
       <c r="D104" t="s">
-        <v>634</v>
+        <v>793</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>234</v>
+        <v>643</v>
       </c>
       <c r="B105" t="s">
-        <v>232</v>
+        <v>648</v>
       </c>
       <c r="C105" t="s">
-        <v>235</v>
+        <v>645</v>
       </c>
       <c r="D105" t="s">
-        <v>236</v>
+        <v>644</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4988,2131 +5036,2223 @@
         <v>781</v>
       </c>
       <c r="C106" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="D106" t="s">
-        <v>790</v>
+        <v>783</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>782</v>
+        <v>790</v>
       </c>
       <c r="C107" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D107" t="s">
-        <v>791</v>
+        <v>784</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>804</v>
+        <v>633</v>
+      </c>
+      <c r="B108" t="s">
+        <v>646</v>
       </c>
       <c r="C108" t="s">
-        <v>802</v>
+        <v>634</v>
       </c>
       <c r="D108" t="s">
-        <v>803</v>
+        <v>847</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4"/>
+      <c r="A109" t="s">
+        <v>846</v>
+      </c>
+      <c r="B109" t="s">
+        <v>647</v>
+      </c>
+      <c r="C109" t="s">
+        <v>635</v>
+      </c>
+      <c r="D109" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>80</v>
+        <v>843</v>
       </c>
       <c r="B110" t="s">
-        <v>81</v>
+        <v>844</v>
       </c>
       <c r="C110" t="s">
-        <v>89</v>
+        <v>845</v>
       </c>
       <c r="D110" t="s">
-        <v>90</v>
+        <v>848</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>82</v>
+        <v>630</v>
       </c>
       <c r="B111" t="s">
-        <v>83</v>
+        <v>230</v>
       </c>
       <c r="C111" t="s">
-        <v>85</v>
+        <v>631</v>
       </c>
       <c r="D111" t="s">
-        <v>87</v>
+        <v>632</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>84</v>
+        <v>232</v>
       </c>
       <c r="B112" t="s">
-        <v>83</v>
+        <v>230</v>
       </c>
       <c r="C112" t="s">
-        <v>86</v>
+        <v>233</v>
       </c>
       <c r="D112" t="s">
-        <v>88</v>
+        <v>234</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>103</v>
-      </c>
-      <c r="B113" t="s">
-        <v>81</v>
+        <v>779</v>
       </c>
       <c r="C113" t="s">
-        <v>104</v>
+        <v>786</v>
       </c>
       <c r="D113" t="s">
-        <v>257</v>
+        <v>788</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>91</v>
-      </c>
-      <c r="B114" t="s">
-        <v>92</v>
+        <v>780</v>
       </c>
       <c r="C114" t="s">
-        <v>93</v>
+        <v>787</v>
       </c>
       <c r="D114" t="s">
-        <v>94</v>
+        <v>789</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="B115" s="5"/>
-      <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
+      <c r="A115" t="s">
+        <v>802</v>
+      </c>
+      <c r="C115" t="s">
+        <v>800</v>
+      </c>
+      <c r="D115" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>317</v>
-      </c>
-      <c r="B116" t="s">
-        <v>316</v>
-      </c>
-      <c r="C116" t="s">
-        <v>322</v>
-      </c>
-      <c r="D116" t="s">
-        <v>323</v>
-      </c>
+      <c r="A116" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>318</v>
+        <v>78</v>
       </c>
       <c r="B117" t="s">
-        <v>316</v>
+        <v>79</v>
       </c>
       <c r="C117" t="s">
-        <v>323</v>
+        <v>87</v>
       </c>
       <c r="D117" t="s">
-        <v>323</v>
+        <v>88</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>325</v>
+        <v>80</v>
       </c>
       <c r="B118" t="s">
-        <v>319</v>
+        <v>81</v>
       </c>
       <c r="C118" t="s">
-        <v>320</v>
+        <v>83</v>
       </c>
       <c r="D118" t="s">
-        <v>321</v>
+        <v>85</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>326</v>
+        <v>82</v>
       </c>
       <c r="B119" t="s">
-        <v>319</v>
+        <v>81</v>
       </c>
       <c r="C119" t="s">
-        <v>327</v>
+        <v>84</v>
       </c>
       <c r="D119" t="s">
-        <v>328</v>
+        <v>86</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>413</v>
+        <v>101</v>
+      </c>
+      <c r="B120" t="s">
+        <v>79</v>
       </c>
       <c r="C120" t="s">
-        <v>414</v>
+        <v>102</v>
       </c>
       <c r="D120" t="s">
-        <v>415</v>
+        <v>255</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>329</v>
+        <v>89</v>
+      </c>
+      <c r="B121" t="s">
+        <v>90</v>
       </c>
       <c r="C121" t="s">
-        <v>331</v>
+        <v>91</v>
       </c>
       <c r="D121" t="s">
-        <v>330</v>
+        <v>92</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>406</v>
-      </c>
-      <c r="C122" t="s">
-        <v>332</v>
-      </c>
-      <c r="D122" t="s">
-        <v>333</v>
-      </c>
+      <c r="A122" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>407</v>
+        <v>315</v>
+      </c>
+      <c r="B123" t="s">
+        <v>314</v>
       </c>
       <c r="C123" t="s">
-        <v>411</v>
+        <v>320</v>
       </c>
       <c r="D123" t="s">
-        <v>412</v>
+        <v>321</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>408</v>
+        <v>316</v>
+      </c>
+      <c r="B124" t="s">
+        <v>314</v>
       </c>
       <c r="C124" t="s">
-        <v>410</v>
+        <v>321</v>
       </c>
       <c r="D124" t="s">
-        <v>409</v>
+        <v>321</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>334</v>
+        <v>323</v>
+      </c>
+      <c r="B125" t="s">
+        <v>317</v>
       </c>
       <c r="C125" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="D125" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
       <c r="B126" t="s">
-        <v>351</v>
+        <v>317</v>
       </c>
       <c r="C126" t="s">
-        <v>352</v>
+        <v>325</v>
       </c>
       <c r="D126" t="s">
-        <v>353</v>
+        <v>326</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="C127" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="D127" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>401</v>
+        <v>327</v>
       </c>
       <c r="C128" t="s">
-        <v>403</v>
+        <v>329</v>
       </c>
       <c r="D128" t="s">
-        <v>405</v>
+        <v>328</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>354</v>
-      </c>
-      <c r="B129" t="s">
-        <v>355</v>
+        <v>404</v>
       </c>
       <c r="C129" t="s">
-        <v>356</v>
+        <v>330</v>
       </c>
       <c r="D129" t="s">
-        <v>357</v>
+        <v>331</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="C130" t="s">
-        <v>392</v>
+        <v>409</v>
       </c>
       <c r="D130" t="s">
-        <v>393</v>
+        <v>410</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="C131" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="D131" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C132" t="s">
-        <v>366</v>
+        <v>334</v>
       </c>
       <c r="D132" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>358</v>
+        <v>348</v>
+      </c>
+      <c r="B133" t="s">
+        <v>349</v>
       </c>
       <c r="C133" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D133" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>360</v>
+        <v>398</v>
       </c>
       <c r="C134" t="s">
-        <v>361</v>
+        <v>400</v>
       </c>
       <c r="D134" t="s">
-        <v>362</v>
+        <v>402</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>363</v>
+        <v>399</v>
       </c>
       <c r="C135" t="s">
-        <v>364</v>
+        <v>401</v>
       </c>
       <c r="D135" t="s">
-        <v>365</v>
+        <v>403</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>367</v>
+        <v>352</v>
+      </c>
+      <c r="B136" t="s">
+        <v>353</v>
       </c>
       <c r="C136" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="D136" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>370</v>
+        <v>416</v>
       </c>
       <c r="C137" t="s">
-        <v>371</v>
+        <v>390</v>
       </c>
       <c r="D137" t="s">
-        <v>372</v>
+        <v>391</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>373</v>
+        <v>417</v>
       </c>
       <c r="C138" t="s">
-        <v>374</v>
+        <v>418</v>
       </c>
       <c r="D138" t="s">
-        <v>375</v>
+        <v>419</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>863</v>
+        <v>335</v>
       </c>
       <c r="C139" t="s">
-        <v>865</v>
+        <v>364</v>
       </c>
       <c r="D139" t="s">
-        <v>864</v>
+        <v>336</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>394</v>
+        <v>356</v>
       </c>
       <c r="C140" t="s">
-        <v>399</v>
+        <v>357</v>
       </c>
       <c r="D140" t="s">
-        <v>398</v>
+        <v>357</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>860</v>
-      </c>
-      <c r="B141" t="s">
-        <v>856</v>
+        <v>358</v>
       </c>
       <c r="C141" t="s">
-        <v>857</v>
+        <v>359</v>
       </c>
       <c r="D141" t="s">
-        <v>858</v>
+        <v>360</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="C142" t="s">
-        <v>383</v>
+        <v>362</v>
       </c>
       <c r="D142" t="s">
-        <v>416</v>
+        <v>363</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>862</v>
+        <v>365</v>
       </c>
       <c r="C143" t="s">
-        <v>861</v>
+        <v>366</v>
       </c>
       <c r="D143" t="s">
-        <v>859</v>
+        <v>367</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>395</v>
+        <v>368</v>
       </c>
       <c r="C144" t="s">
-        <v>396</v>
+        <v>369</v>
       </c>
       <c r="D144" t="s">
-        <v>397</v>
+        <v>370</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="C145" t="s">
-        <v>763</v>
+        <v>372</v>
       </c>
       <c r="D145" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>381</v>
+        <v>860</v>
       </c>
       <c r="C146" t="s">
-        <v>386</v>
+        <v>862</v>
       </c>
       <c r="D146" t="s">
-        <v>385</v>
+        <v>861</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C147" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="D147" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>382</v>
+        <v>857</v>
+      </c>
+      <c r="B148" t="s">
+        <v>853</v>
       </c>
       <c r="C148" t="s">
-        <v>387</v>
+        <v>854</v>
       </c>
       <c r="D148" t="s">
-        <v>388</v>
+        <v>855</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>504</v>
-      </c>
-      <c r="C149" s="9" t="s">
-        <v>505</v>
+        <v>377</v>
+      </c>
+      <c r="C149" t="s">
+        <v>381</v>
       </c>
       <c r="D149" t="s">
-        <v>506</v>
+        <v>414</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>422</v>
+        <v>859</v>
       </c>
       <c r="C150" t="s">
-        <v>423</v>
+        <v>858</v>
       </c>
       <c r="D150" t="s">
-        <v>424</v>
+        <v>856</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>425</v>
+        <v>393</v>
       </c>
       <c r="C151" t="s">
-        <v>480</v>
+        <v>394</v>
       </c>
       <c r="D151" t="s">
-        <v>478</v>
+        <v>395</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>427</v>
+        <v>378</v>
       </c>
       <c r="C152" t="s">
-        <v>426</v>
+        <v>761</v>
       </c>
       <c r="D152" t="s">
-        <v>479</v>
+        <v>382</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>510</v>
+        <v>379</v>
       </c>
       <c r="C153" t="s">
-        <v>431</v>
+        <v>384</v>
       </c>
       <c r="D153" t="s">
-        <v>432</v>
+        <v>383</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>528</v>
+        <v>387</v>
       </c>
       <c r="C154" t="s">
-        <v>526</v>
+        <v>388</v>
       </c>
       <c r="D154" t="s">
-        <v>527</v>
+        <v>389</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>433</v>
+        <v>380</v>
       </c>
       <c r="C155" t="s">
-        <v>434</v>
+        <v>385</v>
       </c>
       <c r="D155" t="s">
-        <v>435</v>
+        <v>386</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>472</v>
-      </c>
-      <c r="C156" t="s">
-        <v>474</v>
+        <v>502</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>503</v>
       </c>
       <c r="D156" t="s">
-        <v>476</v>
+        <v>504</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>473</v>
+        <v>420</v>
       </c>
       <c r="C157" t="s">
-        <v>475</v>
+        <v>421</v>
       </c>
       <c r="D157" t="s">
-        <v>477</v>
+        <v>422</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>481</v>
+        <v>423</v>
       </c>
       <c r="C158" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D158" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>514</v>
+        <v>425</v>
       </c>
       <c r="C159" t="s">
-        <v>484</v>
+        <v>424</v>
       </c>
       <c r="D159" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>486</v>
+        <v>508</v>
       </c>
       <c r="C160" t="s">
-        <v>487</v>
+        <v>429</v>
       </c>
       <c r="D160" t="s">
-        <v>488</v>
+        <v>430</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>489</v>
+        <v>526</v>
       </c>
       <c r="C161" t="s">
-        <v>491</v>
+        <v>524</v>
       </c>
       <c r="D161" t="s">
-        <v>492</v>
+        <v>525</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>490</v>
+        <v>431</v>
       </c>
       <c r="C162" t="s">
-        <v>493</v>
+        <v>432</v>
       </c>
       <c r="D162" t="s">
-        <v>521</v>
+        <v>433</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>507</v>
-      </c>
-      <c r="C163" s="9" t="s">
-        <v>508</v>
+        <v>470</v>
+      </c>
+      <c r="C163" t="s">
+        <v>472</v>
       </c>
       <c r="D163" t="s">
-        <v>509</v>
+        <v>474</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>511</v>
-      </c>
-      <c r="C164" s="9" t="s">
-        <v>512</v>
+        <v>471</v>
+      </c>
+      <c r="C164" t="s">
+        <v>473</v>
       </c>
       <c r="D164" t="s">
-        <v>513</v>
+        <v>475</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>515</v>
-      </c>
-      <c r="C165" s="9" t="s">
-        <v>516</v>
+        <v>479</v>
+      </c>
+      <c r="C165" t="s">
+        <v>480</v>
       </c>
       <c r="D165" t="s">
-        <v>517</v>
+        <v>481</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>518</v>
-      </c>
-      <c r="C166" s="9" t="s">
-        <v>520</v>
+        <v>512</v>
+      </c>
+      <c r="C166" t="s">
+        <v>482</v>
       </c>
       <c r="D166" t="s">
-        <v>519</v>
+        <v>483</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>524</v>
-      </c>
-      <c r="C167" s="9" t="s">
-        <v>493</v>
+        <v>484</v>
+      </c>
+      <c r="C167" t="s">
+        <v>485</v>
       </c>
       <c r="D167" t="s">
-        <v>521</v>
+        <v>486</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>525</v>
-      </c>
-      <c r="C168" s="9" t="s">
-        <v>522</v>
+        <v>487</v>
+      </c>
+      <c r="C168" t="s">
+        <v>489</v>
       </c>
       <c r="D168" t="s">
-        <v>523</v>
+        <v>490</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>536</v>
-      </c>
-      <c r="C169" s="9" t="s">
-        <v>537</v>
+        <v>488</v>
+      </c>
+      <c r="C169" t="s">
+        <v>491</v>
       </c>
       <c r="D169" t="s">
-        <v>538</v>
+        <v>519</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>539</v>
+        <v>505</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>543</v>
+        <v>506</v>
       </c>
       <c r="D170" t="s">
-        <v>541</v>
+        <v>507</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>540</v>
+        <v>509</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>542</v>
+        <v>510</v>
       </c>
       <c r="D171" t="s">
-        <v>542</v>
+        <v>511</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>544</v>
+        <v>513</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>550</v>
+        <v>514</v>
       </c>
       <c r="D172" t="s">
-        <v>549</v>
+        <v>515</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>545</v>
+        <v>516</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>547</v>
+        <v>518</v>
       </c>
       <c r="D173" t="s">
-        <v>548</v>
+        <v>517</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>551</v>
+        <v>522</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>552</v>
+        <v>491</v>
       </c>
       <c r="D174" t="s">
-        <v>553</v>
+        <v>519</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>546</v>
+        <v>523</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>570</v>
+        <v>520</v>
       </c>
       <c r="D175" t="s">
-        <v>571</v>
+        <v>521</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>554</v>
+        <v>534</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>556</v>
+        <v>535</v>
       </c>
       <c r="D176" t="s">
-        <v>558</v>
+        <v>536</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>555</v>
+        <v>537</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="D177" t="s">
-        <v>559</v>
+        <v>539</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>566</v>
+        <v>538</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>560</v>
+        <v>540</v>
       </c>
       <c r="D178" t="s">
-        <v>563</v>
+        <v>540</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>567</v>
+        <v>542</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>564</v>
+        <v>548</v>
       </c>
       <c r="D179" t="s">
-        <v>565</v>
+        <v>547</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>568</v>
+        <v>543</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>561</v>
-      </c>
-      <c r="D180" s="9" t="s">
-        <v>561</v>
+        <v>545</v>
+      </c>
+      <c r="D180" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>569</v>
+        <v>549</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>562</v>
-      </c>
-      <c r="D181" s="9" t="s">
-        <v>562</v>
+        <v>550</v>
+      </c>
+      <c r="D181" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>572</v>
+        <v>544</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>573</v>
-      </c>
-      <c r="D182" s="9" t="s">
-        <v>574</v>
+        <v>568</v>
+      </c>
+      <c r="D182" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>579</v>
+        <v>552</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>582</v>
-      </c>
-      <c r="D183" s="9" t="s">
-        <v>583</v>
+        <v>554</v>
+      </c>
+      <c r="D183" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>580</v>
+        <v>553</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>581</v>
-      </c>
-      <c r="D184" s="9" t="s">
-        <v>584</v>
+        <v>555</v>
+      </c>
+      <c r="D184" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B185" s="3"/>
-      <c r="C185" s="3"/>
-      <c r="D185" s="3"/>
+      <c r="A185" t="s">
+        <v>564</v>
+      </c>
+      <c r="C185" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="D185" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>678</v>
-      </c>
-      <c r="C186" t="s">
-        <v>679</v>
+        <v>565</v>
+      </c>
+      <c r="C186" s="9" t="s">
+        <v>562</v>
       </c>
       <c r="D186" t="s">
-        <v>680</v>
+        <v>563</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>674</v>
-      </c>
-      <c r="C187" t="s">
-        <v>681</v>
-      </c>
-      <c r="D187" t="s">
-        <v>683</v>
+        <v>566</v>
+      </c>
+      <c r="C187" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="D187" s="9" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>677</v>
-      </c>
-      <c r="C188" t="s">
-        <v>682</v>
-      </c>
-      <c r="D188" t="s">
-        <v>684</v>
+        <v>567</v>
+      </c>
+      <c r="C188" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="D188" s="9" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>685</v>
-      </c>
-      <c r="C189" s="7" t="s">
-        <v>675</v>
-      </c>
-      <c r="D189" s="7" t="s">
-        <v>676</v>
+        <v>570</v>
+      </c>
+      <c r="C189" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="D189" s="9" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>140</v>
-      </c>
-      <c r="B190" t="s">
-        <v>137</v>
-      </c>
-      <c r="C190" t="s">
-        <v>138</v>
-      </c>
-      <c r="D190" t="s">
-        <v>139</v>
+        <v>577</v>
+      </c>
+      <c r="C190" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="D190" s="9" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>141</v>
-      </c>
-      <c r="B191" t="s">
-        <v>142</v>
-      </c>
-      <c r="C191" t="s">
-        <v>150</v>
-      </c>
-      <c r="D191" t="s">
-        <v>151</v>
+        <v>578</v>
+      </c>
+      <c r="C191" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="D191" s="9" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>147</v>
-      </c>
-      <c r="B192" t="s">
-        <v>137</v>
-      </c>
-      <c r="C192" t="s">
-        <v>667</v>
-      </c>
-      <c r="D192" t="s">
-        <v>668</v>
-      </c>
+      <c r="A192" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B192" s="3"/>
+      <c r="C192" s="3"/>
+      <c r="D192" s="3"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>143</v>
-      </c>
-      <c r="B193" t="s">
-        <v>142</v>
+        <v>676</v>
       </c>
       <c r="C193" t="s">
-        <v>149</v>
+        <v>677</v>
       </c>
       <c r="D193" t="s">
-        <v>148</v>
+        <v>678</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>144</v>
-      </c>
-      <c r="B194" t="s">
-        <v>145</v>
-      </c>
-      <c r="C194" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D194" s="7" t="s">
-        <v>146</v>
+        <v>672</v>
+      </c>
+      <c r="C194" t="s">
+        <v>679</v>
+      </c>
+      <c r="D194" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="C195" t="s">
-        <v>664</v>
+        <v>680</v>
       </c>
       <c r="D195" t="s">
-        <v>664</v>
+        <v>682</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>666</v>
-      </c>
-      <c r="C196" t="s">
-        <v>670</v>
-      </c>
-      <c r="D196" t="s">
-        <v>669</v>
+        <v>683</v>
+      </c>
+      <c r="C196" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="D196" s="7" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>671</v>
+        <v>138</v>
+      </c>
+      <c r="B197" t="s">
+        <v>135</v>
       </c>
       <c r="C197" t="s">
-        <v>672</v>
+        <v>136</v>
       </c>
       <c r="D197" t="s">
-        <v>673</v>
+        <v>137</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B198" s="6"/>
-      <c r="C198" s="6"/>
-      <c r="D198" s="6"/>
+      <c r="A198" t="s">
+        <v>139</v>
+      </c>
+      <c r="B198" t="s">
+        <v>140</v>
+      </c>
+      <c r="C198" t="s">
+        <v>148</v>
+      </c>
+      <c r="D198" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>47</v>
+        <v>145</v>
       </c>
       <c r="B199" t="s">
-        <v>8</v>
+        <v>135</v>
       </c>
       <c r="C199" t="s">
-        <v>48</v>
+        <v>665</v>
       </c>
       <c r="D199" t="s">
-        <v>49</v>
+        <v>666</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="B200" t="s">
-        <v>8</v>
+        <v>140</v>
       </c>
       <c r="C200" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="D200" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>588</v>
-      </c>
-      <c r="C201" t="s">
-        <v>589</v>
-      </c>
-      <c r="D201" t="s">
-        <v>590</v>
+        <v>142</v>
+      </c>
+      <c r="B201" t="s">
+        <v>143</v>
+      </c>
+      <c r="C201" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D201" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>591</v>
+        <v>663</v>
       </c>
       <c r="C202" t="s">
-        <v>592</v>
+        <v>662</v>
       </c>
       <c r="D202" t="s">
-        <v>593</v>
+        <v>662</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>623</v>
+        <v>664</v>
       </c>
       <c r="C203" t="s">
-        <v>625</v>
+        <v>668</v>
       </c>
       <c r="D203" t="s">
-        <v>626</v>
+        <v>667</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>624</v>
+        <v>669</v>
       </c>
       <c r="C204" t="s">
-        <v>628</v>
+        <v>670</v>
       </c>
       <c r="D204" t="s">
-        <v>627</v>
+        <v>671</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>778</v>
-      </c>
-      <c r="C205" t="s">
-        <v>779</v>
-      </c>
-      <c r="D205" t="s">
-        <v>780</v>
-      </c>
+      <c r="A205" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B205" s="6"/>
+      <c r="C205" s="6"/>
+      <c r="D205" s="6"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B206" t="s">
         <v>8</v>
       </c>
       <c r="C206" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D206" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="B207" t="s">
         <v>8</v>
       </c>
       <c r="C207" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="D207" t="s">
-        <v>222</v>
+        <v>95</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>217</v>
-      </c>
-      <c r="B208" t="s">
-        <v>8</v>
+        <v>586</v>
       </c>
       <c r="C208" t="s">
-        <v>218</v>
+        <v>587</v>
       </c>
       <c r="D208" t="s">
-        <v>218</v>
+        <v>588</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>340</v>
-      </c>
-      <c r="B209" t="s">
-        <v>8</v>
+        <v>589</v>
       </c>
       <c r="C209" t="s">
-        <v>605</v>
+        <v>590</v>
       </c>
       <c r="D209" t="s">
-        <v>607</v>
+        <v>591</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>606</v>
+        <v>621</v>
       </c>
       <c r="C210" t="s">
-        <v>604</v>
+        <v>623</v>
       </c>
       <c r="D210" t="s">
-        <v>608</v>
+        <v>624</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>796</v>
+        <v>622</v>
       </c>
       <c r="C211" t="s">
-        <v>797</v>
+        <v>626</v>
       </c>
       <c r="D211" t="s">
-        <v>798</v>
+        <v>625</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>155</v>
-      </c>
-      <c r="B212" t="s">
-        <v>8</v>
+        <v>776</v>
       </c>
       <c r="C212" t="s">
-        <v>585</v>
+        <v>777</v>
       </c>
       <c r="D212" t="s">
-        <v>156</v>
+        <v>778</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>165</v>
+        <v>48</v>
       </c>
       <c r="B213" t="s">
         <v>8</v>
       </c>
       <c r="C213" t="s">
-        <v>586</v>
+        <v>49</v>
       </c>
       <c r="D213" t="s">
-        <v>166</v>
+        <v>50</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>173</v>
+        <v>51</v>
       </c>
       <c r="B214" t="s">
         <v>8</v>
       </c>
       <c r="C214" t="s">
-        <v>587</v>
+        <v>52</v>
       </c>
       <c r="D214" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>594</v>
+        <v>215</v>
       </c>
       <c r="B215" t="s">
         <v>8</v>
       </c>
       <c r="C215" t="s">
-        <v>595</v>
+        <v>216</v>
       </c>
       <c r="D215" t="s">
-        <v>596</v>
+        <v>216</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>601</v>
+        <v>338</v>
       </c>
       <c r="B216" t="s">
         <v>8</v>
       </c>
       <c r="C216" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="D216" t="s">
-        <v>597</v>
+        <v>605</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
+        <v>604</v>
+      </c>
+      <c r="C217" t="s">
         <v>602</v>
       </c>
-      <c r="B217" t="s">
-        <v>8</v>
-      </c>
-      <c r="C217" t="s">
-        <v>600</v>
-      </c>
       <c r="D217" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>154</v>
-      </c>
-      <c r="B218" t="s">
-        <v>8</v>
+        <v>794</v>
       </c>
       <c r="C218" t="s">
-        <v>190</v>
+        <v>795</v>
       </c>
       <c r="D218" t="s">
-        <v>191</v>
+        <v>796</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="B219" t="s">
         <v>8</v>
       </c>
       <c r="C219" t="s">
-        <v>56</v>
+        <v>583</v>
       </c>
       <c r="D219" t="s">
-        <v>57</v>
+        <v>154</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B220" t="s">
         <v>8</v>
       </c>
       <c r="C220" t="s">
-        <v>157</v>
+        <v>584</v>
       </c>
       <c r="D220" t="s">
-        <v>16</v>
+        <v>164</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B221" t="s">
         <v>8</v>
       </c>
       <c r="C221" t="s">
-        <v>168</v>
+        <v>585</v>
       </c>
       <c r="D221" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>58</v>
+        <v>592</v>
       </c>
       <c r="B222" t="s">
         <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>59</v>
+        <v>593</v>
       </c>
       <c r="D222" t="s">
-        <v>60</v>
+        <v>594</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>161</v>
+        <v>599</v>
       </c>
       <c r="B223" t="s">
         <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>163</v>
+        <v>597</v>
       </c>
       <c r="D223" t="s">
-        <v>164</v>
+        <v>595</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>170</v>
+        <v>600</v>
       </c>
       <c r="B224" t="s">
         <v>8</v>
       </c>
       <c r="C224" t="s">
-        <v>171</v>
+        <v>598</v>
       </c>
       <c r="D224" t="s">
-        <v>172</v>
+        <v>596</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>61</v>
+        <v>152</v>
       </c>
       <c r="B225" t="s">
         <v>8</v>
       </c>
       <c r="C225" t="s">
-        <v>62</v>
+        <v>188</v>
       </c>
       <c r="D225" t="s">
-        <v>63</v>
+        <v>189</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>160</v>
+        <v>53</v>
       </c>
       <c r="B226" t="s">
         <v>8</v>
       </c>
       <c r="C226" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
       <c r="D226" t="s">
-        <v>159</v>
+        <v>55</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B227" t="s">
         <v>8</v>
       </c>
       <c r="C227" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="D227" t="s">
-        <v>177</v>
+        <v>16</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
       <c r="B228" t="s">
         <v>8</v>
       </c>
       <c r="C228" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="D228" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>195</v>
+        <v>56</v>
       </c>
       <c r="B229" t="s">
         <v>8</v>
       </c>
       <c r="C229" t="s">
-        <v>196</v>
+        <v>57</v>
       </c>
       <c r="D229" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="B230" t="s">
         <v>8</v>
       </c>
       <c r="C230" t="s">
-        <v>198</v>
+        <v>161</v>
       </c>
       <c r="D230" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>275</v>
+        <v>168</v>
+      </c>
+      <c r="B231" t="s">
+        <v>8</v>
       </c>
       <c r="C231" t="s">
-        <v>276</v>
+        <v>169</v>
       </c>
       <c r="D231" t="s">
-        <v>277</v>
+        <v>170</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B232" t="s">
         <v>8</v>
       </c>
       <c r="C232" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D232" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="B233" t="s">
         <v>8</v>
       </c>
       <c r="C233" t="s">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="D233" t="s">
-        <v>10</v>
+        <v>157</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>428</v>
+        <v>173</v>
+      </c>
+      <c r="B234" t="s">
+        <v>8</v>
       </c>
       <c r="C234" t="s">
-        <v>429</v>
+        <v>174</v>
       </c>
       <c r="D234" t="s">
-        <v>430</v>
+        <v>175</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B235" t="s">
         <v>8</v>
       </c>
       <c r="C235" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D235" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="B236" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C236" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="D236" t="s">
-        <v>180</v>
+        <v>103</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B237" t="s">
         <v>8</v>
       </c>
       <c r="C237" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D237" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>203</v>
-      </c>
-      <c r="B238" t="s">
-        <v>179</v>
+        <v>273</v>
       </c>
       <c r="C238" t="s">
-        <v>206</v>
+        <v>274</v>
       </c>
       <c r="D238" t="s">
-        <v>207</v>
+        <v>275</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>229</v>
+        <v>65</v>
       </c>
       <c r="B239" t="s">
         <v>8</v>
       </c>
       <c r="C239" t="s">
-        <v>225</v>
+        <v>66</v>
       </c>
       <c r="D239" t="s">
-        <v>227</v>
+        <v>67</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>230</v>
+        <v>7</v>
       </c>
       <c r="B240" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C240" t="s">
-        <v>226</v>
+        <v>9</v>
       </c>
       <c r="D240" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>211</v>
-      </c>
-      <c r="B241" t="s">
-        <v>8</v>
+        <v>426</v>
       </c>
       <c r="C241" t="s">
-        <v>213</v>
+        <v>427</v>
       </c>
       <c r="D241" t="s">
-        <v>215</v>
+        <v>428</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B242" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C242" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="D242" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>106</v>
+        <v>176</v>
       </c>
       <c r="B243" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="C243" t="s">
-        <v>107</v>
+        <v>176</v>
       </c>
       <c r="D243" t="s">
-        <v>108</v>
+        <v>178</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B244" t="s">
         <v>8</v>
       </c>
       <c r="C244" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D244" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>14</v>
+        <v>201</v>
       </c>
       <c r="B245" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="C245" t="s">
-        <v>15</v>
+        <v>204</v>
       </c>
       <c r="D245" t="s">
-        <v>16</v>
+        <v>205</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>376</v>
+        <v>227</v>
+      </c>
+      <c r="B246" t="s">
+        <v>8</v>
       </c>
       <c r="C246" t="s">
-        <v>377</v>
+        <v>223</v>
       </c>
       <c r="D246" t="s">
-        <v>378</v>
+        <v>225</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>494</v>
+        <v>228</v>
+      </c>
+      <c r="B247" t="s">
+        <v>177</v>
       </c>
       <c r="C247" t="s">
-        <v>495</v>
+        <v>224</v>
       </c>
       <c r="D247" t="s">
-        <v>496</v>
+        <v>226</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>417</v>
+        <v>209</v>
       </c>
       <c r="B248" t="s">
-        <v>307</v>
+        <v>8</v>
       </c>
       <c r="C248" t="s">
-        <v>308</v>
+        <v>211</v>
       </c>
       <c r="D248" t="s">
-        <v>309</v>
+        <v>213</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>436</v>
+        <v>210</v>
+      </c>
+      <c r="B249" t="s">
+        <v>177</v>
       </c>
       <c r="C249" t="s">
-        <v>448</v>
+        <v>212</v>
       </c>
       <c r="D249" t="s">
-        <v>460</v>
+        <v>214</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>437</v>
+        <v>104</v>
+      </c>
+      <c r="B250" t="s">
+        <v>8</v>
       </c>
       <c r="C250" t="s">
-        <v>449</v>
+        <v>105</v>
       </c>
       <c r="D250" t="s">
-        <v>461</v>
+        <v>106</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>438</v>
+        <v>206</v>
+      </c>
+      <c r="B251" t="s">
+        <v>8</v>
       </c>
       <c r="C251" t="s">
-        <v>450</v>
+        <v>207</v>
       </c>
       <c r="D251" t="s">
-        <v>462</v>
+        <v>208</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>439</v>
+        <v>14</v>
+      </c>
+      <c r="B252" t="s">
+        <v>8</v>
       </c>
       <c r="C252" t="s">
-        <v>451</v>
+        <v>15</v>
       </c>
       <c r="D252" t="s">
-        <v>463</v>
+        <v>16</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>440</v>
+        <v>374</v>
       </c>
       <c r="C253" t="s">
-        <v>452</v>
+        <v>375</v>
       </c>
       <c r="D253" t="s">
-        <v>465</v>
+        <v>376</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>441</v>
+        <v>492</v>
       </c>
       <c r="C254" t="s">
-        <v>453</v>
+        <v>493</v>
       </c>
       <c r="D254" t="s">
-        <v>464</v>
+        <v>494</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>442</v>
+        <v>415</v>
+      </c>
+      <c r="B255" t="s">
+        <v>305</v>
       </c>
       <c r="C255" t="s">
-        <v>454</v>
+        <v>306</v>
       </c>
       <c r="D255" t="s">
-        <v>466</v>
+        <v>307</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="C256" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="D256" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="C257" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="D257" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="C258" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="D258" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="C259" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="D259" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="C260" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="D260" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>499</v>
+        <v>439</v>
       </c>
       <c r="C261" t="s">
-        <v>498</v>
+        <v>451</v>
       </c>
       <c r="D261" t="s">
-        <v>497</v>
+        <v>462</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>575</v>
+        <v>440</v>
       </c>
       <c r="C262" t="s">
-        <v>2</v>
+        <v>452</v>
       </c>
       <c r="D262" t="s">
-        <v>576</v>
+        <v>464</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>577</v>
+        <v>441</v>
       </c>
       <c r="C263" t="s">
-        <v>578</v>
+        <v>453</v>
       </c>
       <c r="D263" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A264" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B264" s="2"/>
-      <c r="C264" s="2"/>
-      <c r="D264" s="2"/>
+      <c r="A264" t="s">
+        <v>442</v>
+      </c>
+      <c r="C264" t="s">
+        <v>454</v>
+      </c>
+      <c r="D264" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>110</v>
-      </c>
-      <c r="B265" t="s">
-        <v>109</v>
+        <v>443</v>
       </c>
       <c r="C265" t="s">
-        <v>129</v>
+        <v>455</v>
       </c>
       <c r="D265" t="s">
-        <v>128</v>
+        <v>467</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>127</v>
-      </c>
-      <c r="B266" t="s">
-        <v>109</v>
+        <v>444</v>
       </c>
       <c r="C266" t="s">
-        <v>130</v>
+        <v>456</v>
       </c>
       <c r="D266" t="s">
-        <v>133</v>
+        <v>468</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>111</v>
-      </c>
-      <c r="B267" t="s">
-        <v>109</v>
+        <v>445</v>
       </c>
       <c r="C267" t="s">
-        <v>112</v>
+        <v>457</v>
       </c>
       <c r="D267" t="s">
-        <v>119</v>
+        <v>469</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>116</v>
-      </c>
-      <c r="B268" t="s">
-        <v>109</v>
+        <v>497</v>
       </c>
       <c r="C268" t="s">
-        <v>117</v>
+        <v>496</v>
       </c>
       <c r="D268" t="s">
-        <v>118</v>
+        <v>495</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>113</v>
-      </c>
-      <c r="B269" t="s">
-        <v>109</v>
+        <v>573</v>
       </c>
       <c r="C269" t="s">
-        <v>114</v>
+        <v>2</v>
       </c>
       <c r="D269" t="s">
-        <v>115</v>
+        <v>574</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>120</v>
-      </c>
-      <c r="B270" t="s">
-        <v>109</v>
+        <v>575</v>
       </c>
       <c r="C270" t="s">
-        <v>132</v>
+        <v>576</v>
       </c>
       <c r="D270" t="s">
-        <v>121</v>
+        <v>3</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A271" t="s">
-        <v>122</v>
-      </c>
-      <c r="B271" t="s">
-        <v>109</v>
-      </c>
-      <c r="C271" t="s">
-        <v>131</v>
-      </c>
-      <c r="D271" t="s">
-        <v>123</v>
-      </c>
+      <c r="A271" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B271" s="2"/>
+      <c r="C271" s="2"/>
+      <c r="D271" s="2"/>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B272" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C272" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D272" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A273" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B273" s="3"/>
-      <c r="C273" s="3"/>
-      <c r="D273" s="3"/>
+      <c r="A273" t="s">
+        <v>125</v>
+      </c>
+      <c r="B273" t="s">
+        <v>107</v>
+      </c>
+      <c r="C273" t="s">
+        <v>128</v>
+      </c>
+      <c r="D273" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="B274" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="C274" t="s">
-        <v>343</v>
+        <v>110</v>
       </c>
       <c r="D274" t="s">
-        <v>344</v>
+        <v>117</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>341</v>
+        <v>114</v>
       </c>
       <c r="B275" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="C275" t="s">
-        <v>339</v>
+        <v>115</v>
       </c>
       <c r="D275" t="s">
-        <v>342</v>
+        <v>116</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="B276" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="C276" t="s">
-        <v>345</v>
+        <v>112</v>
       </c>
       <c r="D276" t="s">
-        <v>346</v>
+        <v>113</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>347</v>
+        <v>118</v>
       </c>
       <c r="B277" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="C277" t="s">
-        <v>348</v>
+        <v>130</v>
       </c>
       <c r="D277" t="s">
-        <v>349</v>
+        <v>119</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="B278" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="C278" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="D278" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>609</v>
+        <v>122</v>
+      </c>
+      <c r="B279" t="s">
+        <v>107</v>
       </c>
       <c r="C279" t="s">
-        <v>603</v>
+        <v>123</v>
       </c>
       <c r="D279" t="s">
-        <v>610</v>
+        <v>124</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>620</v>
-      </c>
-      <c r="C280" t="s">
-        <v>621</v>
-      </c>
-      <c r="D280" t="s">
-        <v>622</v>
-      </c>
+      <c r="A280" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B280" s="3"/>
+      <c r="C280" s="3"/>
+      <c r="D280" s="3"/>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
+        <v>68</v>
+      </c>
+      <c r="B281" t="s">
+        <v>69</v>
+      </c>
+      <c r="C281" t="s">
+        <v>341</v>
+      </c>
+      <c r="D281" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>339</v>
+      </c>
+      <c r="B282" t="s">
+        <v>69</v>
+      </c>
+      <c r="C282" t="s">
+        <v>337</v>
+      </c>
+      <c r="D282" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>151</v>
+      </c>
+      <c r="B283" t="s">
+        <v>69</v>
+      </c>
+      <c r="C283" t="s">
+        <v>343</v>
+      </c>
+      <c r="D283" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>345</v>
+      </c>
+      <c r="B284" t="s">
+        <v>69</v>
+      </c>
+      <c r="C284" t="s">
+        <v>346</v>
+      </c>
+      <c r="D284" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>70</v>
+      </c>
+      <c r="B285" t="s">
+        <v>69</v>
+      </c>
+      <c r="C285" t="s">
+        <v>71</v>
+      </c>
+      <c r="D285" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>607</v>
+      </c>
+      <c r="C286" t="s">
+        <v>601</v>
+      </c>
+      <c r="D286" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>618</v>
+      </c>
+      <c r="C287" t="s">
+        <v>619</v>
+      </c>
+      <c r="D287" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>797</v>
+      </c>
+      <c r="C288" t="s">
+        <v>798</v>
+      </c>
+      <c r="D288" t="s">
         <v>799</v>
-      </c>
-      <c r="C281" t="s">
-        <v>800</v>
-      </c>
-      <c r="D281" t="s">
-        <v>801</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C189" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
-    <hyperlink ref="D189" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
+    <hyperlink ref="C196" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
+    <hyperlink ref="D196" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
more widespread application level caching.
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFB5893-4B53-4BD9-8B49-469281867907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1801D2-82AD-46CC-9444-FE3E76B1390E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -284,18 +284,6 @@
     <t>img_type_man</t>
   </si>
   <si>
-    <t>auto (series)</t>
-  </si>
-  <si>
-    <t>manual (one-off)</t>
-  </si>
-  <si>
-    <t>automatique (série)</t>
-  </si>
-  <si>
-    <t>manuelle (non-série)</t>
-  </si>
-  <si>
     <t>Image Type</t>
   </si>
   <si>
@@ -2673,6 +2661,18 @@
   </si>
   <si>
     <t>See a map of  current or past conditions</t>
+  </si>
+  <si>
+    <t>Automatic (series)</t>
+  </si>
+  <si>
+    <t>Automatique (série)</t>
+  </si>
+  <si>
+    <t>Manual (one-off)</t>
+  </si>
+  <si>
+    <t>Manuelle (non-série)</t>
   </si>
 </sst>
 </file>
@@ -3611,8 +3611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="A207" sqref="A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3643,7 +3643,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -3654,21 +3654,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C3" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D3" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3679,7 +3679,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -3690,178 +3690,178 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="B6" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="C6" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="D6" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B7" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="C7" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D7" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="B8" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="C8" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="D8" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="B9" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="C9" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="D9" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>695</v>
+      </c>
+      <c r="B10" t="s">
+        <v>733</v>
+      </c>
+      <c r="C10" t="s">
+        <v>698</v>
+      </c>
+      <c r="D10" t="s">
         <v>699</v>
-      </c>
-      <c r="B10" t="s">
-        <v>737</v>
-      </c>
-      <c r="C10" t="s">
-        <v>702</v>
-      </c>
-      <c r="D10" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="B11" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C11" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="D11" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="B12" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="C12" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="D12" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="B13" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="C13" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="D13" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>711</v>
+      </c>
+      <c r="B14" t="s">
+        <v>726</v>
+      </c>
+      <c r="C14" t="s">
+        <v>716</v>
+      </c>
+      <c r="D14" t="s">
         <v>715</v>
-      </c>
-      <c r="B14" t="s">
-        <v>730</v>
-      </c>
-      <c r="C14" t="s">
-        <v>720</v>
-      </c>
-      <c r="D14" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B15" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="C15" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="D15" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B16" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="C16" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="D16" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="B17" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="C17" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="D17" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="B18" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="C18" t="s">
         <v>42</v>
@@ -3872,38 +3872,38 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="B19" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C19" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="D19" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="B20" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="C20" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="D20" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B21" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
@@ -3914,77 +3914,77 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B22" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="C22" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D22" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="B23" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="C23" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="D23" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="B24" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C24" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="D24" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="B25" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D25" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="B26" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="C26" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="D26" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -3992,30 +3992,30 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>647</v>
+      </c>
+      <c r="B28" t="s">
+        <v>648</v>
+      </c>
+      <c r="C28" t="s">
+        <v>650</v>
+      </c>
+      <c r="D28" t="s">
         <v>651</v>
-      </c>
-      <c r="B28" t="s">
-        <v>652</v>
-      </c>
-      <c r="C28" t="s">
-        <v>654</v>
-      </c>
-      <c r="D28" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B29" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="C29" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4026,10 +4026,10 @@
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D30" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4040,122 +4040,122 @@
         <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="D31" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="B32" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="C32" t="s">
+        <v>861</v>
+      </c>
+      <c r="D32" t="s">
         <v>865</v>
-      </c>
-      <c r="D32" t="s">
-        <v>869</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>859</v>
+      </c>
+      <c r="B33" t="s">
+        <v>862</v>
+      </c>
+      <c r="C33" t="s">
         <v>863</v>
       </c>
-      <c r="B33" t="s">
-        <v>866</v>
-      </c>
-      <c r="C33" t="s">
-        <v>867</v>
-      </c>
       <c r="D33" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B34" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C34" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="D34" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="B35" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C35" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="D35" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="B36" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C36" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="D36" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="B37" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C37" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="D37" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="B38" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C38" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="D38" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="B39" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C39" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="D39" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4216,7 +4216,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -4224,147 +4224,147 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B45" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C45" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D45" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>279</v>
+      </c>
+      <c r="B46" t="s">
+        <v>281</v>
+      </c>
+      <c r="C46" t="s">
+        <v>282</v>
+      </c>
+      <c r="D46" t="s">
         <v>283</v>
-      </c>
-      <c r="B46" t="s">
-        <v>285</v>
-      </c>
-      <c r="C46" t="s">
-        <v>286</v>
-      </c>
-      <c r="D46" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>280</v>
+      </c>
+      <c r="B47" t="s">
+        <v>286</v>
+      </c>
+      <c r="C47" t="s">
+        <v>285</v>
+      </c>
+      <c r="D47" t="s">
         <v>284</v>
-      </c>
-      <c r="B47" t="s">
-        <v>290</v>
-      </c>
-      <c r="C47" t="s">
-        <v>289</v>
-      </c>
-      <c r="D47" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B48" t="s">
+        <v>293</v>
+      </c>
+      <c r="C48" t="s">
+        <v>296</v>
+      </c>
+      <c r="D48" t="s">
         <v>297</v>
-      </c>
-      <c r="C48" t="s">
-        <v>300</v>
-      </c>
-      <c r="D48" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B49" t="s">
+        <v>294</v>
+      </c>
+      <c r="C49" t="s">
+        <v>288</v>
+      </c>
+      <c r="D49" t="s">
         <v>298</v>
-      </c>
-      <c r="C49" t="s">
-        <v>292</v>
-      </c>
-      <c r="D49" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>289</v>
+      </c>
+      <c r="B50" t="s">
         <v>293</v>
       </c>
-      <c r="B50" t="s">
-        <v>297</v>
-      </c>
       <c r="C50" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D50" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B51" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C51" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D51" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="B52" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C52" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D52" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B53" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C53" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D53" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B54" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C54" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D54" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -4378,7 +4378,7 @@
         <v>36</v>
       </c>
       <c r="C56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D56" t="s">
         <v>37</v>
@@ -4400,7 +4400,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -4408,16 +4408,16 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B59" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C59" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D59" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4425,7 +4425,7 @@
         <v>73</v>
       </c>
       <c r="B60" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C60" t="s">
         <v>74</v>
@@ -4436,418 +4436,418 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B61" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C61" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="D61" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="C62" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="D62" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B63" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C63" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D63" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B64" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C64" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D64" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B65" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C65" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="D65" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>239</v>
+      </c>
+      <c r="B66" t="s">
         <v>243</v>
       </c>
-      <c r="B66" t="s">
-        <v>247</v>
-      </c>
       <c r="C66" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="D66" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B67" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C67" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="D67" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B68" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C68" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D68" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B69" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C69" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="D69" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B70" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C70" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D70" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B71" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="C71" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="D71" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="B72" t="s">
+        <v>801</v>
+      </c>
+      <c r="C72" t="s">
+        <v>803</v>
+      </c>
+      <c r="D72" t="s">
         <v>805</v>
-      </c>
-      <c r="C72" t="s">
-        <v>807</v>
-      </c>
-      <c r="D72" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B73" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C73" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D73" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B74" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C74" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D74" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B75" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C75" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D75" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>256</v>
+      </c>
+      <c r="B76" t="s">
+        <v>243</v>
+      </c>
+      <c r="C76" t="s">
+        <v>259</v>
+      </c>
+      <c r="D76" t="s">
         <v>260</v>
-      </c>
-      <c r="B76" t="s">
-        <v>247</v>
-      </c>
-      <c r="C76" t="s">
-        <v>263</v>
-      </c>
-      <c r="D76" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B77" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C77" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D77" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B78" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C78" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D78" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B79" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C79" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="D79" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="B80" t="s">
+        <v>760</v>
+      </c>
+      <c r="C80" t="s">
         <v>764</v>
       </c>
-      <c r="C80" t="s">
-        <v>768</v>
-      </c>
       <c r="D80" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="B81" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C81" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="D81" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="B82" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C82" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="D82" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>808</v>
+      </c>
+      <c r="B83" t="s">
+        <v>760</v>
+      </c>
+      <c r="C83" t="s">
+        <v>811</v>
+      </c>
+      <c r="D83" t="s">
         <v>812</v>
-      </c>
-      <c r="B83" t="s">
-        <v>764</v>
-      </c>
-      <c r="C83" t="s">
-        <v>815</v>
-      </c>
-      <c r="D83" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>809</v>
+      </c>
+      <c r="B84" t="s">
+        <v>760</v>
+      </c>
+      <c r="C84" t="s">
+        <v>816</v>
+      </c>
+      <c r="D84" t="s">
         <v>813</v>
-      </c>
-      <c r="B84" t="s">
-        <v>764</v>
-      </c>
-      <c r="C84" t="s">
-        <v>820</v>
-      </c>
-      <c r="D84" t="s">
-        <v>817</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="B85" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C85" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="D85" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B86" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C86" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="D86" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B87" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C87" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="D87" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="B88" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C88" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="D88" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="C89" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="D89" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="C90" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="D90" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
@@ -4855,60 +4855,60 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="C92" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D92" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C93" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="D93" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B94" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C94" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D94" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B95" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C95" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="D95" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B96" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C96" t="s">
         <v>76</v>
@@ -4922,7 +4922,7 @@
         <v>62</v>
       </c>
       <c r="B97" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C97" t="s">
         <v>63</v>
@@ -4933,232 +4933,232 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B98" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C98" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D98" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>213</v>
+      </c>
+      <c r="B99" t="s">
+        <v>214</v>
+      </c>
+      <c r="C99" t="s">
         <v>217</v>
       </c>
-      <c r="B99" t="s">
+      <c r="D99" t="s">
         <v>218</v>
-      </c>
-      <c r="C99" t="s">
-        <v>221</v>
-      </c>
-      <c r="D99" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B100" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C100" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D100" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="C101" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="D101" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C102" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D102" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C103" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="D103" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C104" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="D104" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="B105" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="C105" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="D105" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="C106" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="D106" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="C107" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="D107" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B108" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C108" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="D108" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="B109" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C109" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D109" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="B110" t="s">
+        <v>840</v>
+      </c>
+      <c r="C110" t="s">
+        <v>841</v>
+      </c>
+      <c r="D110" t="s">
         <v>844</v>
-      </c>
-      <c r="C110" t="s">
-        <v>845</v>
-      </c>
-      <c r="D110" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="B111" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C111" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="D111" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B112" t="s">
+        <v>226</v>
+      </c>
+      <c r="C112" t="s">
+        <v>229</v>
+      </c>
+      <c r="D112" t="s">
         <v>230</v>
-      </c>
-      <c r="C112" t="s">
-        <v>233</v>
-      </c>
-      <c r="D112" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C113" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="D113" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C114" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="D114" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="C115" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="D115" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
@@ -5172,10 +5172,10 @@
         <v>79</v>
       </c>
       <c r="C117" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D117" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -5186,10 +5186,10 @@
         <v>81</v>
       </c>
       <c r="C118" t="s">
-        <v>83</v>
+        <v>876</v>
       </c>
       <c r="D118" t="s">
-        <v>85</v>
+        <v>877</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -5200,43 +5200,43 @@
         <v>81</v>
       </c>
       <c r="C119" t="s">
-        <v>84</v>
+        <v>878</v>
       </c>
       <c r="D119" t="s">
-        <v>86</v>
+        <v>879</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B120" t="s">
         <v>79</v>
       </c>
       <c r="C120" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D120" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B121" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C121" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D121" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
@@ -5244,787 +5244,787 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B123" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C123" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D123" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B124" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C124" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D124" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B125" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C125" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D125" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B126" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C126" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D126" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C127" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D127" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C128" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D128" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C129" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D129" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>401</v>
+      </c>
+      <c r="C130" t="s">
         <v>405</v>
       </c>
-      <c r="C130" t="s">
-        <v>409</v>
-      </c>
       <c r="D130" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C131" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D131" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C132" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D132" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B133" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C133" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D133" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>394</v>
+      </c>
+      <c r="C134" t="s">
+        <v>396</v>
+      </c>
+      <c r="D134" t="s">
         <v>398</v>
-      </c>
-      <c r="C134" t="s">
-        <v>400</v>
-      </c>
-      <c r="D134" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
+        <v>395</v>
+      </c>
+      <c r="C135" t="s">
+        <v>397</v>
+      </c>
+      <c r="D135" t="s">
         <v>399</v>
-      </c>
-      <c r="C135" t="s">
-        <v>401</v>
-      </c>
-      <c r="D135" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B136" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C136" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D136" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C137" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D137" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C138" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D138" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C139" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D139" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C140" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D140" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C141" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D141" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C142" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D142" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C143" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D143" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C144" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D144" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C145" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D145" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="C146" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="D146" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>388</v>
+      </c>
+      <c r="C147" t="s">
+        <v>393</v>
+      </c>
+      <c r="D147" t="s">
         <v>392</v>
-      </c>
-      <c r="C147" t="s">
-        <v>397</v>
-      </c>
-      <c r="D147" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="B148" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="C148" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="D148" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>373</v>
+      </c>
+      <c r="C149" t="s">
         <v>377</v>
       </c>
-      <c r="C149" t="s">
-        <v>381</v>
-      </c>
       <c r="D149" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="C150" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="D150" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C151" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D151" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>374</v>
+      </c>
+      <c r="C152" t="s">
+        <v>757</v>
+      </c>
+      <c r="D152" t="s">
         <v>378</v>
-      </c>
-      <c r="C152" t="s">
-        <v>761</v>
-      </c>
-      <c r="D152" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>375</v>
+      </c>
+      <c r="C153" t="s">
+        <v>380</v>
+      </c>
+      <c r="D153" t="s">
         <v>379</v>
-      </c>
-      <c r="C153" t="s">
-        <v>384</v>
-      </c>
-      <c r="D153" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C154" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D154" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C155" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D155" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D156" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C157" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D157" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C158" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="D158" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C159" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D159" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C160" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D160" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C161" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D161" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C162" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D162" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>466</v>
+      </c>
+      <c r="C163" t="s">
+        <v>468</v>
+      </c>
+      <c r="D163" t="s">
         <v>470</v>
-      </c>
-      <c r="C163" t="s">
-        <v>472</v>
-      </c>
-      <c r="D163" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>467</v>
+      </c>
+      <c r="C164" t="s">
+        <v>469</v>
+      </c>
+      <c r="D164" t="s">
         <v>471</v>
-      </c>
-      <c r="C164" t="s">
-        <v>473</v>
-      </c>
-      <c r="D164" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C165" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D165" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C166" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D166" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C167" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D167" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C168" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D168" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C169" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="D169" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="D170" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D171" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D172" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D173" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="D174" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D175" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D176" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>533</v>
+      </c>
+      <c r="C177" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="C177" s="9" t="s">
-        <v>541</v>
-      </c>
       <c r="D177" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="D178" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="D179" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="D180" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="D181" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="D182" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
+        <v>548</v>
+      </c>
+      <c r="C183" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D183" t="s">
         <v>552</v>
-      </c>
-      <c r="C183" s="9" t="s">
-        <v>554</v>
-      </c>
-      <c r="D183" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>549</v>
+      </c>
+      <c r="C184" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="D184" t="s">
         <v>553</v>
-      </c>
-      <c r="C184" s="9" t="s">
-        <v>555</v>
-      </c>
-      <c r="D184" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D185" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D186" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D187" s="9" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C188" s="9" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="D188" s="9" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C189" s="9" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>573</v>
+      </c>
+      <c r="C190" s="9" t="s">
+        <v>576</v>
+      </c>
+      <c r="D190" s="9" t="s">
         <v>577</v>
-      </c>
-      <c r="C190" s="9" t="s">
-        <v>580</v>
-      </c>
-      <c r="D190" s="9" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>574</v>
+      </c>
+      <c r="C191" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="D191" s="9" t="s">
         <v>578</v>
-      </c>
-      <c r="C191" s="9" t="s">
-        <v>579</v>
-      </c>
-      <c r="D191" s="9" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
@@ -6032,154 +6032,154 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="C193" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D193" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="C194" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D194" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C195" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D195" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="C196" s="7" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="D196" s="7" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B197" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C197" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D197" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B198" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C198" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D198" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B199" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C199" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="D199" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B200" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C200" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D200" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B201" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C201" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D201" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C202" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="D202" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>660</v>
+      </c>
+      <c r="C203" t="s">
         <v>664</v>
       </c>
-      <c r="C203" t="s">
-        <v>668</v>
-      </c>
       <c r="D203" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C204" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D204" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B205" s="6"/>
       <c r="C205" s="6"/>
@@ -6201,71 +6201,71 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B207" t="s">
         <v>8</v>
       </c>
       <c r="C207" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D207" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C208" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D208" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C209" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D209" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="C210" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="D210" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
+        <v>618</v>
+      </c>
+      <c r="C211" t="s">
         <v>622</v>
       </c>
-      <c r="C211" t="s">
-        <v>626</v>
-      </c>
       <c r="D211" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C212" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D212" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -6293,155 +6293,155 @@
         <v>52</v>
       </c>
       <c r="D214" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B215" t="s">
         <v>8</v>
       </c>
       <c r="C215" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D215" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B216" t="s">
         <v>8</v>
       </c>
       <c r="C216" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="D216" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C217" t="s">
+        <v>598</v>
+      </c>
+      <c r="D217" t="s">
         <v>602</v>
-      </c>
-      <c r="D217" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="C218" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="D218" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B219" t="s">
         <v>8</v>
       </c>
       <c r="C219" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D219" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B220" t="s">
         <v>8</v>
       </c>
       <c r="C220" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="D220" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B221" t="s">
         <v>8</v>
       </c>
       <c r="C221" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D221" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B222" t="s">
         <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D222" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="B223" t="s">
         <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="D223" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B224" t="s">
         <v>8</v>
       </c>
       <c r="C224" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D224" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B225" t="s">
         <v>8</v>
       </c>
       <c r="C225" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D225" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -6460,13 +6460,13 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B227" t="s">
         <v>8</v>
       </c>
       <c r="C227" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D227" t="s">
         <v>16</v>
@@ -6474,16 +6474,16 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B228" t="s">
         <v>8</v>
       </c>
       <c r="C228" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D228" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -6502,30 +6502,30 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B230" t="s">
         <v>8</v>
       </c>
       <c r="C230" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D230" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B231" t="s">
         <v>8</v>
       </c>
       <c r="C231" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D231" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -6544,83 +6544,83 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B233" t="s">
         <v>8</v>
       </c>
       <c r="C233" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D233" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B234" t="s">
         <v>8</v>
       </c>
       <c r="C234" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D234" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B235" t="s">
         <v>8</v>
       </c>
       <c r="C235" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D235" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B236" t="s">
         <v>8</v>
       </c>
       <c r="C236" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D236" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B237" t="s">
         <v>8</v>
       </c>
       <c r="C237" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D237" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C238" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D238" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -6653,153 +6653,153 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C241" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D241" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B242" t="s">
         <v>8</v>
       </c>
       <c r="C242" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D242" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B243" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C243" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D243" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B244" t="s">
         <v>8</v>
       </c>
       <c r="C244" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D244" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
+        <v>197</v>
+      </c>
+      <c r="B245" t="s">
+        <v>173</v>
+      </c>
+      <c r="C245" t="s">
+        <v>200</v>
+      </c>
+      <c r="D245" t="s">
         <v>201</v>
-      </c>
-      <c r="B245" t="s">
-        <v>177</v>
-      </c>
-      <c r="C245" t="s">
-        <v>204</v>
-      </c>
-      <c r="D245" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B246" t="s">
         <v>8</v>
       </c>
       <c r="C246" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D246" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B247" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C247" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D247" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B248" t="s">
         <v>8</v>
       </c>
       <c r="C248" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D248" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
+        <v>206</v>
+      </c>
+      <c r="B249" t="s">
+        <v>173</v>
+      </c>
+      <c r="C249" t="s">
+        <v>208</v>
+      </c>
+      <c r="D249" t="s">
         <v>210</v>
-      </c>
-      <c r="B249" t="s">
-        <v>177</v>
-      </c>
-      <c r="C249" t="s">
-        <v>212</v>
-      </c>
-      <c r="D249" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B250" t="s">
         <v>8</v>
       </c>
       <c r="C250" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D250" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B251" t="s">
         <v>8</v>
       </c>
       <c r="C251" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D251" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -6818,200 +6818,200 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C253" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D253" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C254" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D254" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B255" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C255" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D255" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C256" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D256" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C257" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="D257" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C258" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D258" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C259" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D259" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C260" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D260" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C261" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D261" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C262" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D262" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C263" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D263" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C264" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="D264" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C265" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="D265" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C266" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D266" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C267" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D267" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C268" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D268" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C269" t="s">
         <v>2</v>
       </c>
       <c r="D269" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C270" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="D270" t="s">
         <v>3</v>
@@ -7019,7 +7019,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B271" s="2"/>
       <c r="C271" s="2"/>
@@ -7027,119 +7027,119 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B272" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C272" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D272" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B273" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C273" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D273" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B274" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C274" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D274" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B275" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C275" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D275" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B276" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C276" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D276" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B277" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C277" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D277" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B278" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C278" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D278" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B279" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C279" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D279" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B280" s="3"/>
       <c r="C280" s="3"/>
@@ -7153,52 +7153,52 @@
         <v>69</v>
       </c>
       <c r="C281" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D281" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B282" t="s">
         <v>69</v>
       </c>
       <c r="C282" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D282" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B283" t="s">
         <v>69</v>
       </c>
       <c r="C283" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D283" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B284" t="s">
         <v>69</v>
       </c>
       <c r="C284" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D284" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
@@ -7217,35 +7217,35 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="C286" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="D286" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="C287" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="D287" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="C288" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="D288" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progress save on update to continous plot function
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1801D2-82AD-46CC-9444-FE3E76B1390E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AC095E-81C8-4F24-8DE9-338264134B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="886">
   <si>
     <t>id</t>
   </si>
@@ -2673,6 +2673,24 @@
   </si>
   <si>
     <t>Manuelle (non-série)</t>
+  </si>
+  <si>
+    <t>Aggregation type</t>
+  </si>
+  <si>
+    <t>Sample media</t>
+  </si>
+  <si>
+    <t>Média d'échantillonage</t>
+  </si>
+  <si>
+    <t>date_range_select_doy</t>
+  </si>
+  <si>
+    <t>Start/end days (year is ignored)</t>
+  </si>
+  <si>
+    <t>Dates de début/fin (l'année est ignorée)</t>
   </si>
 </sst>
 </file>
@@ -3609,10 +3627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D288"/>
+  <dimension ref="A1:D291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="A207" sqref="A207"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4573,698 +4591,695 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>799</v>
-      </c>
-      <c r="B71" t="s">
-        <v>801</v>
+        <v>883</v>
       </c>
       <c r="C71" t="s">
-        <v>802</v>
+        <v>884</v>
       </c>
       <c r="D71" t="s">
-        <v>804</v>
+        <v>885</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B72" t="s">
         <v>801</v>
       </c>
       <c r="C72" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D72" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>252</v>
+        <v>800</v>
       </c>
       <c r="B73" t="s">
-        <v>242</v>
+        <v>801</v>
       </c>
       <c r="C73" t="s">
-        <v>253</v>
+        <v>803</v>
       </c>
       <c r="D73" t="s">
-        <v>254</v>
+        <v>805</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="B74" t="s">
         <v>242</v>
       </c>
       <c r="C74" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="D74" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="B75" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C75" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="D75" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B76" t="s">
         <v>243</v>
       </c>
       <c r="C76" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D76" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B77" t="s">
         <v>243</v>
       </c>
       <c r="C77" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D77" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B78" t="s">
-        <v>273</v>
+        <v>243</v>
       </c>
       <c r="C78" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="D78" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>759</v>
+        <v>272</v>
       </c>
       <c r="B79" t="s">
-        <v>760</v>
+        <v>273</v>
       </c>
       <c r="C79" t="s">
-        <v>761</v>
+        <v>274</v>
       </c>
       <c r="D79" t="s">
-        <v>762</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B80" t="s">
         <v>760</v>
       </c>
       <c r="C80" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D80" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="B81" t="s">
         <v>760</v>
       </c>
       <c r="C81" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D81" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B82" t="s">
         <v>760</v>
       </c>
       <c r="C82" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="D82" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>808</v>
+        <v>769</v>
       </c>
       <c r="B83" t="s">
         <v>760</v>
       </c>
       <c r="C83" t="s">
-        <v>811</v>
+        <v>770</v>
       </c>
       <c r="D83" t="s">
-        <v>812</v>
+        <v>771</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B84" t="s">
         <v>760</v>
       </c>
       <c r="C84" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
       <c r="D84" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="B85" t="s">
         <v>760</v>
       </c>
       <c r="C85" t="s">
-        <v>806</v>
+        <v>816</v>
       </c>
       <c r="D85" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="B86" t="s">
         <v>760</v>
       </c>
       <c r="C86" t="s">
-        <v>817</v>
+        <v>806</v>
       </c>
       <c r="D86" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="B87" t="s">
         <v>760</v>
       </c>
       <c r="C87" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="D87" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="B88" t="s">
         <v>760</v>
       </c>
       <c r="C88" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="D88" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>827</v>
+        <v>821</v>
+      </c>
+      <c r="B89" t="s">
+        <v>760</v>
       </c>
       <c r="C89" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="D89" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>827</v>
+      </c>
+      <c r="C90" t="s">
+        <v>828</v>
+      </c>
+      <c r="D90" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>824</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>825</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D91" t="s">
         <v>826</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="8" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>605</v>
-      </c>
-      <c r="C92" t="s">
-        <v>606</v>
-      </c>
-      <c r="D92" t="s">
-        <v>607</v>
-      </c>
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>623</v>
+        <v>605</v>
       </c>
       <c r="C93" t="s">
-        <v>624</v>
+        <v>606</v>
       </c>
       <c r="D93" t="s">
-        <v>625</v>
+        <v>607</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>608</v>
-      </c>
-      <c r="B94" t="s">
-        <v>645</v>
+        <v>623</v>
       </c>
       <c r="C94" t="s">
-        <v>609</v>
+        <v>624</v>
       </c>
       <c r="D94" t="s">
-        <v>610</v>
+        <v>625</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B95" t="s">
         <v>645</v>
       </c>
       <c r="C95" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D95" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>177</v>
+        <v>611</v>
       </c>
       <c r="B96" t="s">
-        <v>178</v>
+        <v>645</v>
       </c>
       <c r="C96" t="s">
-        <v>76</v>
+        <v>612</v>
       </c>
       <c r="D96" t="s">
-        <v>77</v>
+        <v>613</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="B97" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C97" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="D97" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>175</v>
+        <v>62</v>
       </c>
       <c r="B98" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C98" t="s">
-        <v>182</v>
+        <v>63</v>
       </c>
       <c r="D98" t="s">
-        <v>183</v>
+        <v>64</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>213</v>
+        <v>175</v>
       </c>
       <c r="B99" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="C99" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
       <c r="D99" t="s">
-        <v>218</v>
+        <v>183</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B100" t="s">
         <v>214</v>
       </c>
       <c r="C100" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="D100" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>681</v>
+        <v>215</v>
+      </c>
+      <c r="B101" t="s">
+        <v>214</v>
       </c>
       <c r="C101" t="s">
-        <v>682</v>
+        <v>231</v>
       </c>
       <c r="D101" t="s">
-        <v>680</v>
+        <v>231</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>655</v>
+        <v>681</v>
       </c>
       <c r="C102" t="s">
-        <v>656</v>
+        <v>682</v>
       </c>
       <c r="D102" t="s">
-        <v>657</v>
+        <v>680</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="C103" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="D103" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>787</v>
+        <v>652</v>
       </c>
       <c r="C104" t="s">
-        <v>788</v>
+        <v>653</v>
       </c>
       <c r="D104" t="s">
-        <v>789</v>
+        <v>654</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>639</v>
-      </c>
-      <c r="B105" t="s">
-        <v>644</v>
+        <v>787</v>
       </c>
       <c r="C105" t="s">
-        <v>641</v>
+        <v>788</v>
       </c>
       <c r="D105" t="s">
-        <v>640</v>
+        <v>789</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>777</v>
+        <v>639</v>
+      </c>
+      <c r="B106" t="s">
+        <v>644</v>
       </c>
       <c r="C106" t="s">
-        <v>778</v>
+        <v>641</v>
       </c>
       <c r="D106" t="s">
-        <v>779</v>
+        <v>640</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>786</v>
+        <v>777</v>
       </c>
       <c r="C107" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="D107" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>629</v>
-      </c>
-      <c r="B108" t="s">
-        <v>642</v>
+        <v>786</v>
       </c>
       <c r="C108" t="s">
-        <v>630</v>
+        <v>781</v>
       </c>
       <c r="D108" t="s">
-        <v>843</v>
+        <v>780</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>842</v>
+        <v>629</v>
       </c>
       <c r="B109" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C109" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D109" t="s">
-        <v>632</v>
+        <v>843</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="B110" t="s">
-        <v>840</v>
+        <v>643</v>
       </c>
       <c r="C110" t="s">
-        <v>841</v>
+        <v>631</v>
       </c>
       <c r="D110" t="s">
-        <v>844</v>
+        <v>632</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>626</v>
+        <v>839</v>
       </c>
       <c r="B111" t="s">
-        <v>226</v>
+        <v>840</v>
       </c>
       <c r="C111" t="s">
-        <v>627</v>
+        <v>841</v>
       </c>
       <c r="D111" t="s">
-        <v>628</v>
+        <v>844</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>228</v>
+        <v>626</v>
       </c>
       <c r="B112" t="s">
         <v>226</v>
       </c>
       <c r="C112" t="s">
-        <v>229</v>
+        <v>627</v>
       </c>
       <c r="D112" t="s">
-        <v>230</v>
+        <v>628</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>775</v>
+        <v>228</v>
+      </c>
+      <c r="B113" t="s">
+        <v>226</v>
       </c>
       <c r="C113" t="s">
-        <v>782</v>
+        <v>229</v>
       </c>
       <c r="D113" t="s">
-        <v>784</v>
+        <v>230</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C114" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D114" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>776</v>
+      </c>
+      <c r="C115" t="s">
+        <v>783</v>
+      </c>
+      <c r="D115" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>798</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C116" t="s">
         <v>796</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D116" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B116" s="4"/>
-      <c r="C116" s="4"/>
-      <c r="D116" s="4"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>78</v>
-      </c>
-      <c r="B117" t="s">
-        <v>79</v>
-      </c>
-      <c r="C117" t="s">
-        <v>83</v>
-      </c>
-      <c r="D117" t="s">
-        <v>84</v>
-      </c>
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B118" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C118" t="s">
-        <v>876</v>
+        <v>83</v>
       </c>
       <c r="D118" t="s">
-        <v>877</v>
+        <v>84</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B119" t="s">
         <v>81</v>
       </c>
       <c r="C119" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="D119" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B120" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C120" t="s">
-        <v>98</v>
+        <v>878</v>
       </c>
       <c r="D120" t="s">
-        <v>251</v>
+        <v>879</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>97</v>
+      </c>
+      <c r="B121" t="s">
+        <v>79</v>
+      </c>
+      <c r="C121" t="s">
+        <v>98</v>
+      </c>
+      <c r="D121" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>85</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B122" t="s">
         <v>86</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C122" t="s">
         <v>87</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D122" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="5" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="B122" s="5"/>
-      <c r="C122" s="5"/>
-      <c r="D122" s="5"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>311</v>
-      </c>
-      <c r="B123" t="s">
-        <v>310</v>
-      </c>
-      <c r="C123" t="s">
-        <v>316</v>
-      </c>
-      <c r="D123" t="s">
-        <v>317</v>
-      </c>
+      <c r="B123" s="5"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B124" t="s">
         <v>310</v>
       </c>
       <c r="C124" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D124" t="s">
         <v>317</v>
@@ -5272,1987 +5287,2023 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B125" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C125" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D125" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B126" t="s">
         <v>313</v>
       </c>
       <c r="C126" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D126" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>407</v>
+        <v>320</v>
+      </c>
+      <c r="B127" t="s">
+        <v>313</v>
       </c>
       <c r="C127" t="s">
-        <v>408</v>
+        <v>321</v>
       </c>
       <c r="D127" t="s">
-        <v>409</v>
+        <v>322</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>323</v>
+        <v>407</v>
       </c>
       <c r="C128" t="s">
-        <v>325</v>
+        <v>408</v>
       </c>
       <c r="D128" t="s">
-        <v>324</v>
+        <v>409</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>400</v>
+        <v>323</v>
       </c>
       <c r="C129" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D129" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C130" t="s">
-        <v>405</v>
+        <v>326</v>
       </c>
       <c r="D130" t="s">
-        <v>406</v>
+        <v>327</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C131" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D131" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>328</v>
+        <v>402</v>
       </c>
       <c r="C132" t="s">
-        <v>330</v>
+        <v>404</v>
       </c>
       <c r="D132" t="s">
-        <v>329</v>
+        <v>403</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>344</v>
-      </c>
-      <c r="B133" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
       <c r="C133" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="D133" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>394</v>
+        <v>344</v>
+      </c>
+      <c r="B134" t="s">
+        <v>345</v>
       </c>
       <c r="C134" t="s">
-        <v>396</v>
+        <v>346</v>
       </c>
       <c r="D134" t="s">
-        <v>398</v>
+        <v>347</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C135" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D135" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>348</v>
-      </c>
-      <c r="B136" t="s">
-        <v>349</v>
+        <v>395</v>
       </c>
       <c r="C136" t="s">
-        <v>350</v>
+        <v>397</v>
       </c>
       <c r="D136" t="s">
-        <v>351</v>
+        <v>399</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>412</v>
+        <v>348</v>
+      </c>
+      <c r="B137" t="s">
+        <v>349</v>
       </c>
       <c r="C137" t="s">
-        <v>386</v>
+        <v>350</v>
       </c>
       <c r="D137" t="s">
-        <v>387</v>
+        <v>351</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C138" t="s">
-        <v>414</v>
+        <v>386</v>
       </c>
       <c r="D138" t="s">
-        <v>415</v>
+        <v>387</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>331</v>
+        <v>413</v>
       </c>
       <c r="C139" t="s">
-        <v>360</v>
+        <v>414</v>
       </c>
       <c r="D139" t="s">
-        <v>332</v>
+        <v>415</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
       <c r="C140" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="D140" t="s">
-        <v>353</v>
+        <v>332</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C141" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D141" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C142" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D142" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C143" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D143" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C144" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D144" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C145" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D145" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>856</v>
+        <v>367</v>
       </c>
       <c r="C146" t="s">
-        <v>858</v>
+        <v>368</v>
       </c>
       <c r="D146" t="s">
-        <v>857</v>
+        <v>369</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>388</v>
+        <v>856</v>
       </c>
       <c r="C147" t="s">
-        <v>393</v>
+        <v>858</v>
       </c>
       <c r="D147" t="s">
-        <v>392</v>
+        <v>857</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>853</v>
-      </c>
-      <c r="B148" t="s">
-        <v>849</v>
+        <v>388</v>
       </c>
       <c r="C148" t="s">
-        <v>850</v>
+        <v>393</v>
       </c>
       <c r="D148" t="s">
-        <v>851</v>
+        <v>392</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>373</v>
+        <v>853</v>
+      </c>
+      <c r="B149" t="s">
+        <v>849</v>
       </c>
       <c r="C149" t="s">
-        <v>377</v>
+        <v>850</v>
       </c>
       <c r="D149" t="s">
-        <v>410</v>
+        <v>851</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>855</v>
+        <v>373</v>
       </c>
       <c r="C150" t="s">
-        <v>854</v>
+        <v>377</v>
       </c>
       <c r="D150" t="s">
-        <v>852</v>
+        <v>410</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>389</v>
+        <v>855</v>
       </c>
       <c r="C151" t="s">
-        <v>390</v>
+        <v>854</v>
       </c>
       <c r="D151" t="s">
-        <v>391</v>
+        <v>852</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>374</v>
+        <v>389</v>
       </c>
       <c r="C152" t="s">
-        <v>757</v>
+        <v>390</v>
       </c>
       <c r="D152" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C153" t="s">
-        <v>380</v>
+        <v>757</v>
       </c>
       <c r="D153" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="C154" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D154" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C155" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="D155" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>498</v>
-      </c>
-      <c r="C156" s="9" t="s">
-        <v>499</v>
+        <v>376</v>
+      </c>
+      <c r="C156" t="s">
+        <v>381</v>
       </c>
       <c r="D156" t="s">
-        <v>500</v>
+        <v>382</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>416</v>
-      </c>
-      <c r="C157" t="s">
-        <v>417</v>
+        <v>498</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>499</v>
       </c>
       <c r="D157" t="s">
-        <v>418</v>
+        <v>500</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C158" t="s">
-        <v>474</v>
+        <v>417</v>
       </c>
       <c r="D158" t="s">
-        <v>472</v>
+        <v>418</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C159" t="s">
-        <v>420</v>
+        <v>474</v>
       </c>
       <c r="D159" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>504</v>
+        <v>421</v>
       </c>
       <c r="C160" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D160" t="s">
-        <v>426</v>
+        <v>473</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="C161" t="s">
-        <v>520</v>
+        <v>425</v>
       </c>
       <c r="D161" t="s">
-        <v>521</v>
+        <v>426</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>427</v>
+        <v>522</v>
       </c>
       <c r="C162" t="s">
-        <v>428</v>
+        <v>520</v>
       </c>
       <c r="D162" t="s">
-        <v>429</v>
+        <v>521</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>466</v>
+        <v>427</v>
       </c>
       <c r="C163" t="s">
-        <v>468</v>
+        <v>428</v>
       </c>
       <c r="D163" t="s">
-        <v>470</v>
+        <v>429</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C164" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D164" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="C165" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="D165" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>508</v>
+        <v>475</v>
       </c>
       <c r="C166" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D166" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>480</v>
+        <v>508</v>
       </c>
       <c r="C167" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="D167" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C168" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D168" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C169" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D169" t="s">
-        <v>515</v>
+        <v>486</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>501</v>
-      </c>
-      <c r="C170" s="9" t="s">
-        <v>502</v>
+        <v>484</v>
+      </c>
+      <c r="C170" t="s">
+        <v>487</v>
       </c>
       <c r="D170" t="s">
-        <v>503</v>
+        <v>515</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="D171" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D172" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D173" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>487</v>
+        <v>514</v>
       </c>
       <c r="D174" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>516</v>
+        <v>487</v>
       </c>
       <c r="D175" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>531</v>
+        <v>516</v>
       </c>
       <c r="D176" t="s">
-        <v>532</v>
+        <v>517</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="D177" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D178" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="D179" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="D180" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D181" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>564</v>
+        <v>546</v>
       </c>
       <c r="D182" t="s">
-        <v>565</v>
+        <v>547</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>550</v>
+        <v>564</v>
       </c>
       <c r="D183" t="s">
-        <v>552</v>
+        <v>565</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D184" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>560</v>
+        <v>549</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D185" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D186" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>555</v>
-      </c>
-      <c r="D187" s="9" t="s">
-        <v>555</v>
+        <v>558</v>
+      </c>
+      <c r="D187" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C188" s="9" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D188" s="9" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C189" s="9" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>568</v>
+        <v>556</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="C190" s="9" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>573</v>
+      </c>
+      <c r="C191" s="9" t="s">
+        <v>576</v>
+      </c>
+      <c r="D191" s="9" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>574</v>
       </c>
-      <c r="C191" s="9" t="s">
+      <c r="C192" s="9" t="s">
         <v>575</v>
       </c>
-      <c r="D191" s="9" t="s">
+      <c r="D192" s="9" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="3" t="s">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B192" s="3"/>
-      <c r="C192" s="3"/>
-      <c r="D192" s="3"/>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>672</v>
-      </c>
-      <c r="C193" t="s">
-        <v>673</v>
-      </c>
-      <c r="D193" t="s">
-        <v>674</v>
-      </c>
+      <c r="B193" s="3"/>
+      <c r="C193" s="3"/>
+      <c r="D193" s="3"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
       <c r="C194" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D194" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="C195" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D195" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>679</v>
-      </c>
-      <c r="C196" s="7" t="s">
-        <v>669</v>
-      </c>
-      <c r="D196" s="7" t="s">
-        <v>670</v>
+        <v>671</v>
+      </c>
+      <c r="C196" t="s">
+        <v>676</v>
+      </c>
+      <c r="D196" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>134</v>
-      </c>
-      <c r="B197" t="s">
-        <v>131</v>
-      </c>
-      <c r="C197" t="s">
-        <v>132</v>
-      </c>
-      <c r="D197" t="s">
-        <v>133</v>
+        <v>679</v>
+      </c>
+      <c r="C197" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="D197" s="7" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B198" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C198" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D198" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B199" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C199" t="s">
-        <v>661</v>
+        <v>144</v>
       </c>
       <c r="D199" t="s">
-        <v>662</v>
+        <v>145</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B200" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C200" t="s">
-        <v>143</v>
+        <v>661</v>
       </c>
       <c r="D200" t="s">
-        <v>142</v>
+        <v>662</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B201" t="s">
-        <v>139</v>
-      </c>
-      <c r="C201" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D201" s="7" t="s">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="C201" t="s">
+        <v>143</v>
+      </c>
+      <c r="D201" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>659</v>
-      </c>
-      <c r="C202" t="s">
-        <v>658</v>
-      </c>
-      <c r="D202" t="s">
-        <v>658</v>
+        <v>138</v>
+      </c>
+      <c r="B202" t="s">
+        <v>139</v>
+      </c>
+      <c r="C202" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D202" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C203" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="D203" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
+        <v>660</v>
+      </c>
+      <c r="C204" t="s">
+        <v>664</v>
+      </c>
+      <c r="D204" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
         <v>665</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C205" t="s">
         <v>666</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D205" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="6" t="s">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B205" s="6"/>
-      <c r="C205" s="6"/>
-      <c r="D205" s="6"/>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>45</v>
-      </c>
-      <c r="B206" t="s">
-        <v>8</v>
-      </c>
-      <c r="C206" t="s">
-        <v>46</v>
-      </c>
-      <c r="D206" t="s">
-        <v>47</v>
-      </c>
+      <c r="B206" s="6"/>
+      <c r="C206" s="6"/>
+      <c r="D206" s="6"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="B207" t="s">
         <v>8</v>
       </c>
       <c r="C207" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="D207" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>582</v>
+        <v>89</v>
+      </c>
+      <c r="B208" t="s">
+        <v>8</v>
       </c>
       <c r="C208" t="s">
-        <v>583</v>
+        <v>90</v>
       </c>
       <c r="D208" t="s">
-        <v>584</v>
+        <v>91</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C209" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D209" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>617</v>
+        <v>585</v>
       </c>
       <c r="C210" t="s">
-        <v>619</v>
+        <v>586</v>
       </c>
       <c r="D210" t="s">
-        <v>620</v>
+        <v>587</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C211" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="D211" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>772</v>
+        <v>618</v>
       </c>
       <c r="C212" t="s">
-        <v>773</v>
+        <v>622</v>
       </c>
       <c r="D212" t="s">
-        <v>774</v>
+        <v>621</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>48</v>
-      </c>
-      <c r="B213" t="s">
-        <v>8</v>
+        <v>772</v>
       </c>
       <c r="C213" t="s">
-        <v>49</v>
+        <v>773</v>
       </c>
       <c r="D213" t="s">
-        <v>50</v>
+        <v>774</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B214" t="s">
         <v>8</v>
       </c>
       <c r="C214" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D214" t="s">
-        <v>216</v>
+        <v>50</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>211</v>
+        <v>51</v>
       </c>
       <c r="B215" t="s">
         <v>8</v>
       </c>
       <c r="C215" t="s">
-        <v>212</v>
+        <v>52</v>
       </c>
       <c r="D215" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>334</v>
+        <v>211</v>
       </c>
       <c r="B216" t="s">
         <v>8</v>
       </c>
       <c r="C216" t="s">
-        <v>599</v>
+        <v>212</v>
       </c>
       <c r="D216" t="s">
-        <v>601</v>
+        <v>212</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>600</v>
+        <v>333</v>
       </c>
       <c r="C217" t="s">
-        <v>598</v>
+        <v>881</v>
       </c>
       <c r="D217" t="s">
-        <v>602</v>
+        <v>882</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>790</v>
+        <v>334</v>
+      </c>
+      <c r="B218" t="s">
+        <v>8</v>
       </c>
       <c r="C218" t="s">
-        <v>791</v>
+        <v>599</v>
       </c>
       <c r="D218" t="s">
-        <v>792</v>
+        <v>601</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>149</v>
-      </c>
-      <c r="B219" t="s">
-        <v>8</v>
+        <v>600</v>
       </c>
       <c r="C219" t="s">
-        <v>579</v>
+        <v>598</v>
       </c>
       <c r="D219" t="s">
-        <v>150</v>
+        <v>602</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>159</v>
-      </c>
-      <c r="B220" t="s">
-        <v>8</v>
+        <v>794</v>
       </c>
       <c r="C220" t="s">
-        <v>580</v>
+        <v>880</v>
       </c>
       <c r="D220" t="s">
-        <v>160</v>
+        <v>792</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>167</v>
-      </c>
-      <c r="B221" t="s">
-        <v>8</v>
+        <v>790</v>
       </c>
       <c r="C221" t="s">
-        <v>581</v>
+        <v>791</v>
       </c>
       <c r="D221" t="s">
-        <v>168</v>
+        <v>792</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>588</v>
+        <v>149</v>
       </c>
       <c r="B222" t="s">
         <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
       <c r="D222" t="s">
-        <v>590</v>
+        <v>150</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>595</v>
+        <v>159</v>
       </c>
       <c r="B223" t="s">
         <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>593</v>
+        <v>580</v>
       </c>
       <c r="D223" t="s">
-        <v>591</v>
+        <v>160</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>596</v>
+        <v>167</v>
       </c>
       <c r="B224" t="s">
         <v>8</v>
       </c>
       <c r="C224" t="s">
-        <v>594</v>
+        <v>581</v>
       </c>
       <c r="D224" t="s">
-        <v>592</v>
+        <v>168</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>148</v>
+        <v>588</v>
       </c>
       <c r="B225" t="s">
         <v>8</v>
       </c>
       <c r="C225" t="s">
-        <v>184</v>
+        <v>589</v>
       </c>
       <c r="D225" t="s">
-        <v>185</v>
+        <v>590</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>53</v>
+        <v>595</v>
       </c>
       <c r="B226" t="s">
         <v>8</v>
       </c>
       <c r="C226" t="s">
-        <v>54</v>
+        <v>593</v>
       </c>
       <c r="D226" t="s">
-        <v>55</v>
+        <v>591</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>156</v>
+        <v>596</v>
       </c>
       <c r="B227" t="s">
         <v>8</v>
       </c>
       <c r="C227" t="s">
-        <v>151</v>
+        <v>594</v>
       </c>
       <c r="D227" t="s">
-        <v>16</v>
+        <v>592</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B228" t="s">
         <v>8</v>
       </c>
       <c r="C228" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="D228" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B229" t="s">
         <v>8</v>
       </c>
       <c r="C229" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D229" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B230" t="s">
         <v>8</v>
       </c>
       <c r="C230" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D230" t="s">
-        <v>158</v>
+        <v>16</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B231" t="s">
         <v>8</v>
       </c>
       <c r="C231" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D231" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B232" t="s">
         <v>8</v>
       </c>
       <c r="C232" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D232" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B233" t="s">
         <v>8</v>
       </c>
       <c r="C233" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D233" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B234" t="s">
         <v>8</v>
       </c>
       <c r="C234" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D234" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>188</v>
+        <v>59</v>
       </c>
       <c r="B235" t="s">
         <v>8</v>
       </c>
       <c r="C235" t="s">
-        <v>186</v>
+        <v>60</v>
       </c>
       <c r="D235" t="s">
-        <v>187</v>
+        <v>61</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="B236" t="s">
         <v>8</v>
       </c>
       <c r="C236" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
       <c r="D236" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="B237" t="s">
         <v>8</v>
       </c>
       <c r="C237" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="D237" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>269</v>
+        <v>188</v>
+      </c>
+      <c r="B238" t="s">
+        <v>8</v>
       </c>
       <c r="C238" t="s">
-        <v>270</v>
+        <v>186</v>
       </c>
       <c r="D238" t="s">
-        <v>271</v>
+        <v>187</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>65</v>
+        <v>189</v>
       </c>
       <c r="B239" t="s">
         <v>8</v>
       </c>
       <c r="C239" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="D239" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>7</v>
+        <v>191</v>
       </c>
       <c r="B240" t="s">
         <v>8</v>
       </c>
       <c r="C240" t="s">
-        <v>9</v>
+        <v>192</v>
       </c>
       <c r="D240" t="s">
-        <v>10</v>
+        <v>193</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>422</v>
+        <v>269</v>
       </c>
       <c r="C241" t="s">
-        <v>423</v>
+        <v>270</v>
       </c>
       <c r="D241" t="s">
-        <v>424</v>
+        <v>271</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>194</v>
+        <v>65</v>
       </c>
       <c r="B242" t="s">
         <v>8</v>
       </c>
       <c r="C242" t="s">
-        <v>194</v>
+        <v>66</v>
       </c>
       <c r="D242" t="s">
-        <v>195</v>
+        <v>67</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>172</v>
+        <v>7</v>
       </c>
       <c r="B243" t="s">
-        <v>173</v>
+        <v>8</v>
       </c>
       <c r="C243" t="s">
-        <v>172</v>
+        <v>9</v>
       </c>
       <c r="D243" t="s">
-        <v>174</v>
+        <v>10</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>196</v>
-      </c>
-      <c r="B244" t="s">
-        <v>8</v>
+        <v>422</v>
       </c>
       <c r="C244" t="s">
-        <v>198</v>
+        <v>423</v>
       </c>
       <c r="D244" t="s">
-        <v>199</v>
+        <v>424</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B245" t="s">
-        <v>173</v>
+        <v>8</v>
       </c>
       <c r="C245" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D245" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
       <c r="B246" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
       <c r="C246" t="s">
-        <v>219</v>
+        <v>172</v>
       </c>
       <c r="D246" t="s">
-        <v>221</v>
+        <v>174</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
       <c r="B247" t="s">
-        <v>173</v>
+        <v>8</v>
       </c>
       <c r="C247" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
       <c r="D247" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B248" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
       <c r="C248" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D248" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="B249" t="s">
-        <v>173</v>
+        <v>8</v>
       </c>
       <c r="C249" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="D249" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>100</v>
+        <v>224</v>
       </c>
       <c r="B250" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
       <c r="C250" t="s">
-        <v>101</v>
+        <v>220</v>
       </c>
       <c r="D250" t="s">
-        <v>102</v>
+        <v>222</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B251" t="s">
         <v>8</v>
       </c>
       <c r="C251" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D251" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>14</v>
+        <v>206</v>
       </c>
       <c r="B252" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
       <c r="C252" t="s">
-        <v>15</v>
+        <v>208</v>
       </c>
       <c r="D252" t="s">
-        <v>16</v>
+        <v>210</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>370</v>
+        <v>100</v>
+      </c>
+      <c r="B253" t="s">
+        <v>8</v>
       </c>
       <c r="C253" t="s">
-        <v>371</v>
+        <v>101</v>
       </c>
       <c r="D253" t="s">
-        <v>372</v>
+        <v>102</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>488</v>
+        <v>202</v>
+      </c>
+      <c r="B254" t="s">
+        <v>8</v>
       </c>
       <c r="C254" t="s">
-        <v>489</v>
+        <v>203</v>
       </c>
       <c r="D254" t="s">
-        <v>490</v>
+        <v>204</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>411</v>
+        <v>14</v>
       </c>
       <c r="B255" t="s">
-        <v>301</v>
+        <v>8</v>
       </c>
       <c r="C255" t="s">
-        <v>302</v>
+        <v>15</v>
       </c>
       <c r="D255" t="s">
-        <v>303</v>
+        <v>16</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>430</v>
+        <v>370</v>
       </c>
       <c r="C256" t="s">
-        <v>442</v>
+        <v>371</v>
       </c>
       <c r="D256" t="s">
-        <v>454</v>
+        <v>372</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>431</v>
+        <v>488</v>
       </c>
       <c r="C257" t="s">
-        <v>443</v>
+        <v>489</v>
       </c>
       <c r="D257" t="s">
-        <v>455</v>
+        <v>490</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>432</v>
+        <v>411</v>
+      </c>
+      <c r="B258" t="s">
+        <v>301</v>
       </c>
       <c r="C258" t="s">
-        <v>444</v>
+        <v>302</v>
       </c>
       <c r="D258" t="s">
-        <v>456</v>
+        <v>303</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C259" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D259" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C260" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D260" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C261" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D261" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C262" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D262" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C263" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D263" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C264" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D264" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C265" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D265" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C266" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D266" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C267" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D267" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>493</v>
+        <v>439</v>
       </c>
       <c r="C268" t="s">
-        <v>492</v>
+        <v>451</v>
       </c>
       <c r="D268" t="s">
-        <v>491</v>
+        <v>463</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>569</v>
+        <v>440</v>
       </c>
       <c r="C269" t="s">
-        <v>2</v>
+        <v>452</v>
       </c>
       <c r="D269" t="s">
-        <v>570</v>
+        <v>464</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>571</v>
+        <v>441</v>
       </c>
       <c r="C270" t="s">
-        <v>572</v>
+        <v>453</v>
       </c>
       <c r="D270" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A271" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B271" s="2"/>
-      <c r="C271" s="2"/>
-      <c r="D271" s="2"/>
+      <c r="A271" t="s">
+        <v>493</v>
+      </c>
+      <c r="C271" t="s">
+        <v>492</v>
+      </c>
+      <c r="D271" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>104</v>
-      </c>
-      <c r="B272" t="s">
-        <v>103</v>
+        <v>569</v>
       </c>
       <c r="C272" t="s">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="D272" t="s">
-        <v>122</v>
+        <v>570</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>121</v>
-      </c>
-      <c r="B273" t="s">
+        <v>571</v>
+      </c>
+      <c r="C273" t="s">
+        <v>572</v>
+      </c>
+      <c r="D273" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C273" t="s">
-        <v>124</v>
-      </c>
-      <c r="D273" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
-        <v>105</v>
-      </c>
-      <c r="B274" t="s">
-        <v>103</v>
-      </c>
-      <c r="C274" t="s">
-        <v>106</v>
-      </c>
-      <c r="D274" t="s">
-        <v>113</v>
-      </c>
+      <c r="B274" s="2"/>
+      <c r="C274" s="2"/>
+      <c r="D274" s="2"/>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B275" t="s">
         <v>103</v>
       </c>
       <c r="C275" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="D275" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="B276" t="s">
         <v>103</v>
       </c>
       <c r="C276" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D276" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B277" t="s">
         <v>103</v>
       </c>
       <c r="C277" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="D277" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B278" t="s">
         <v>103</v>
       </c>
       <c r="C278" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="D278" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B279" t="s">
         <v>103</v>
       </c>
       <c r="C279" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D279" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A280" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B280" s="3"/>
-      <c r="C280" s="3"/>
-      <c r="D280" s="3"/>
+      <c r="A280" t="s">
+        <v>114</v>
+      </c>
+      <c r="B280" t="s">
+        <v>103</v>
+      </c>
+      <c r="C280" t="s">
+        <v>126</v>
+      </c>
+      <c r="D280" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="B281" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C281" t="s">
-        <v>337</v>
+        <v>125</v>
       </c>
       <c r="D281" t="s">
-        <v>338</v>
+        <v>117</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>335</v>
+        <v>118</v>
       </c>
       <c r="B282" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C282" t="s">
-        <v>333</v>
+        <v>119</v>
       </c>
       <c r="D282" t="s">
-        <v>336</v>
+        <v>120</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
-        <v>147</v>
-      </c>
-      <c r="B283" t="s">
-        <v>69</v>
-      </c>
-      <c r="C283" t="s">
-        <v>339</v>
-      </c>
-      <c r="D283" t="s">
-        <v>340</v>
-      </c>
+      <c r="A283" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B283" s="3"/>
+      <c r="C283" s="3"/>
+      <c r="D283" s="3"/>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>341</v>
+        <v>68</v>
       </c>
       <c r="B284" t="s">
         <v>69</v>
       </c>
       <c r="C284" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D284" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>70</v>
+        <v>335</v>
       </c>
       <c r="B285" t="s">
         <v>69</v>
       </c>
       <c r="C285" t="s">
-        <v>71</v>
+        <v>333</v>
       </c>
       <c r="D285" t="s">
-        <v>72</v>
+        <v>336</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>603</v>
+        <v>147</v>
+      </c>
+      <c r="B286" t="s">
+        <v>69</v>
       </c>
       <c r="C286" t="s">
-        <v>597</v>
+        <v>339</v>
       </c>
       <c r="D286" t="s">
-        <v>604</v>
+        <v>340</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>614</v>
+        <v>341</v>
+      </c>
+      <c r="B287" t="s">
+        <v>69</v>
       </c>
       <c r="C287" t="s">
-        <v>615</v>
+        <v>342</v>
       </c>
       <c r="D287" t="s">
-        <v>616</v>
+        <v>343</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
+        <v>70</v>
+      </c>
+      <c r="B288" t="s">
+        <v>69</v>
+      </c>
+      <c r="C288" t="s">
+        <v>71</v>
+      </c>
+      <c r="D288" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>603</v>
+      </c>
+      <c r="C289" t="s">
+        <v>597</v>
+      </c>
+      <c r="D289" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>614</v>
+      </c>
+      <c r="C290" t="s">
+        <v>615</v>
+      </c>
+      <c r="D290" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
         <v>793</v>
       </c>
-      <c r="C288" t="s">
+      <c r="C291" t="s">
         <v>794</v>
       </c>
-      <c r="D288" t="s">
+      <c r="D291" t="s">
         <v>795</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C196" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
-    <hyperlink ref="D196" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
+    <hyperlink ref="C197" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
+    <hyperlink ref="D197" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
part way to making session specific cache if necessary.
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FFCAA9-74BA-4659-8CCE-F81DE17EA10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657A879D-C22C-4330-873A-C1DF2F3F95E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -2063,15 +2063,9 @@
     <t xml:space="preserve">The data, reports, and plots generated from this application are licenced under the Yukon Government's </t>
   </si>
   <si>
-    <t>Open Data Licence</t>
-  </si>
-  <si>
     <t xml:space="preserve">Les données, rapports et graphiques générés par cette application sont licenciés sous la </t>
   </si>
   <si>
-    <t>licence de données ouvertes du gouvernement du Yukon</t>
-  </si>
-  <si>
     <t>licence_url</t>
   </si>
   <si>
@@ -2754,6 +2748,12 @@
   </si>
   <si>
     <t>remove_subplot</t>
+  </si>
+  <si>
+    <t>Open Government Licence</t>
+  </si>
+  <si>
+    <t>licence de gouvernement ouvert du Yukon</t>
   </si>
 </sst>
 </file>
@@ -3693,7 +3693,7 @@
   <dimension ref="A1:D298"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="A199" sqref="A199:XFD199"/>
+      <selection activeCell="D202" sqref="D202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3749,7 +3749,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3760,7 +3760,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -3771,178 +3771,178 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B6" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C6" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D6" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C7" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B8" t="s">
+        <v>750</v>
+      </c>
+      <c r="C8" t="s">
+        <v>751</v>
+      </c>
+      <c r="D8" t="s">
         <v>752</v>
-      </c>
-      <c r="C8" t="s">
-        <v>753</v>
-      </c>
-      <c r="D8" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>690</v>
+      </c>
+      <c r="B9" t="s">
+        <v>728</v>
+      </c>
+      <c r="C9" t="s">
+        <v>691</v>
+      </c>
+      <c r="D9" t="s">
         <v>692</v>
-      </c>
-      <c r="B9" t="s">
-        <v>730</v>
-      </c>
-      <c r="C9" t="s">
-        <v>693</v>
-      </c>
-      <c r="D9" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B10" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C10" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="D10" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>698</v>
+      </c>
+      <c r="B11" t="s">
+        <v>727</v>
+      </c>
+      <c r="C11" t="s">
+        <v>699</v>
+      </c>
+      <c r="D11" t="s">
         <v>700</v>
-      </c>
-      <c r="B11" t="s">
-        <v>729</v>
-      </c>
-      <c r="C11" t="s">
-        <v>701</v>
-      </c>
-      <c r="D11" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>701</v>
+      </c>
+      <c r="B12" t="s">
+        <v>725</v>
+      </c>
+      <c r="C12" t="s">
+        <v>702</v>
+      </c>
+      <c r="D12" t="s">
         <v>703</v>
-      </c>
-      <c r="B12" t="s">
-        <v>727</v>
-      </c>
-      <c r="C12" t="s">
-        <v>704</v>
-      </c>
-      <c r="D12" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>706</v>
+      </c>
+      <c r="B13" t="s">
+        <v>726</v>
+      </c>
+      <c r="C13" t="s">
+        <v>707</v>
+      </c>
+      <c r="D13" t="s">
         <v>708</v>
-      </c>
-      <c r="B13" t="s">
-        <v>728</v>
-      </c>
-      <c r="C13" t="s">
-        <v>709</v>
-      </c>
-      <c r="D13" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B14" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C14" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D14" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B15" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C15" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D15" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B16" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C16" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D16" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B17" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C17" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D17" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B18" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C18" t="s">
         <v>42</v>
@@ -3953,38 +3953,38 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B19" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C19" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="D19" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B20" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C20" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D20" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B21" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
@@ -3995,52 +3995,52 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>735</v>
+      </c>
+      <c r="B22" t="s">
+        <v>741</v>
+      </c>
+      <c r="C22" t="s">
         <v>737</v>
       </c>
-      <c r="B22" t="s">
-        <v>743</v>
-      </c>
-      <c r="C22" t="s">
-        <v>739</v>
-      </c>
       <c r="D22" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>736</v>
+      </c>
+      <c r="B23" t="s">
+        <v>742</v>
+      </c>
+      <c r="C23" t="s">
         <v>738</v>
       </c>
-      <c r="B23" t="s">
-        <v>744</v>
-      </c>
-      <c r="C23" t="s">
-        <v>740</v>
-      </c>
       <c r="D23" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B24" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C24" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D24" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B25" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C25" t="s">
         <v>129</v>
@@ -4051,16 +4051,16 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B26" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C26" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="D26" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4093,10 +4093,10 @@
         <v>648</v>
       </c>
       <c r="C29" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4121,122 +4121,122 @@
         <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="D31" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>858</v>
+      </c>
+      <c r="B32" t="s">
         <v>860</v>
       </c>
-      <c r="B32" t="s">
-        <v>862</v>
-      </c>
       <c r="C32" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="D32" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="B33" t="s">
+        <v>860</v>
+      </c>
+      <c r="C33" t="s">
+        <v>861</v>
+      </c>
+      <c r="D33" t="s">
         <v>862</v>
-      </c>
-      <c r="C33" t="s">
-        <v>863</v>
-      </c>
-      <c r="D33" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="B34" t="s">
         <v>226</v>
       </c>
       <c r="C34" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="D34" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="B35" t="s">
         <v>226</v>
       </c>
       <c r="C35" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="D35" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B36" t="s">
         <v>226</v>
       </c>
       <c r="C36" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="D36" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="B37" t="s">
         <v>226</v>
       </c>
       <c r="C37" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D37" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B38" t="s">
         <v>226</v>
       </c>
       <c r="C38" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="D38" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="B39" t="s">
         <v>226</v>
       </c>
       <c r="C39" t="s">
+        <v>776</v>
+      </c>
+      <c r="D39" t="s">
         <v>778</v>
-      </c>
-      <c r="D39" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4523,7 +4523,7 @@
         <v>236</v>
       </c>
       <c r="C61" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="D61" t="s">
         <v>235</v>
@@ -4534,7 +4534,7 @@
         <v>637</v>
       </c>
       <c r="C62" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="D62" t="s">
         <v>638</v>
@@ -4576,10 +4576,10 @@
         <v>243</v>
       </c>
       <c r="C65" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D65" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4590,10 +4590,10 @@
         <v>243</v>
       </c>
       <c r="C66" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D66" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4604,7 +4604,7 @@
         <v>244</v>
       </c>
       <c r="C67" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="D67" t="s">
         <v>247</v>
@@ -4632,10 +4632,10 @@
         <v>244</v>
       </c>
       <c r="C69" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D69" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -4654,41 +4654,41 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>881</v>
+      </c>
+      <c r="C71" t="s">
+        <v>882</v>
+      </c>
+      <c r="D71" t="s">
         <v>883</v>
-      </c>
-      <c r="C71" t="s">
-        <v>884</v>
-      </c>
-      <c r="D71" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>797</v>
+      </c>
+      <c r="B72" t="s">
         <v>799</v>
       </c>
-      <c r="B72" t="s">
-        <v>801</v>
-      </c>
       <c r="C72" t="s">
+        <v>800</v>
+      </c>
+      <c r="D72" t="s">
         <v>802</v>
-      </c>
-      <c r="D72" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B73" t="s">
+        <v>799</v>
+      </c>
+      <c r="C73" t="s">
         <v>801</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>803</v>
-      </c>
-      <c r="D73" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -4777,164 +4777,164 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>757</v>
+      </c>
+      <c r="B80" t="s">
+        <v>758</v>
+      </c>
+      <c r="C80" t="s">
         <v>759</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>760</v>
-      </c>
-      <c r="C80" t="s">
-        <v>761</v>
-      </c>
-      <c r="D80" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B81" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C81" t="s">
+        <v>762</v>
+      </c>
+      <c r="D81" t="s">
         <v>764</v>
-      </c>
-      <c r="D81" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B82" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C82" t="s">
+        <v>763</v>
+      </c>
+      <c r="D82" t="s">
         <v>765</v>
-      </c>
-      <c r="D82" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>767</v>
+      </c>
+      <c r="B83" t="s">
+        <v>758</v>
+      </c>
+      <c r="C83" t="s">
+        <v>768</v>
+      </c>
+      <c r="D83" t="s">
         <v>769</v>
-      </c>
-      <c r="B83" t="s">
-        <v>760</v>
-      </c>
-      <c r="C83" t="s">
-        <v>770</v>
-      </c>
-      <c r="D83" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B84" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C84" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D84" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B85" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C85" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="D85" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B86" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C86" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="D86" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B87" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C87" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D87" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>816</v>
+      </c>
+      <c r="B88" t="s">
+        <v>758</v>
+      </c>
+      <c r="C88" t="s">
+        <v>817</v>
+      </c>
+      <c r="D88" t="s">
         <v>818</v>
-      </c>
-      <c r="B88" t="s">
-        <v>760</v>
-      </c>
-      <c r="C88" t="s">
-        <v>819</v>
-      </c>
-      <c r="D88" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>819</v>
+      </c>
+      <c r="B89" t="s">
+        <v>758</v>
+      </c>
+      <c r="C89" t="s">
+        <v>820</v>
+      </c>
+      <c r="D89" t="s">
         <v>821</v>
-      </c>
-      <c r="B89" t="s">
-        <v>760</v>
-      </c>
-      <c r="C89" t="s">
-        <v>822</v>
-      </c>
-      <c r="D89" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>825</v>
+      </c>
+      <c r="C90" t="s">
+        <v>826</v>
+      </c>
+      <c r="D90" t="s">
         <v>827</v>
-      </c>
-      <c r="C90" t="s">
-        <v>828</v>
-      </c>
-      <c r="D90" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>822</v>
+      </c>
+      <c r="C91" t="s">
+        <v>823</v>
+      </c>
+      <c r="D91" t="s">
         <v>824</v>
-      </c>
-      <c r="C91" t="s">
-        <v>825</v>
-      </c>
-      <c r="D91" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -5067,13 +5067,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C102" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="D102" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -5100,13 +5100,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>785</v>
+      </c>
+      <c r="C105" t="s">
+        <v>786</v>
+      </c>
+      <c r="D105" t="s">
         <v>787</v>
-      </c>
-      <c r="C105" t="s">
-        <v>788</v>
-      </c>
-      <c r="D105" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -5125,24 +5125,24 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>775</v>
+      </c>
+      <c r="C107" t="s">
+        <v>776</v>
+      </c>
+      <c r="D107" t="s">
         <v>777</v>
-      </c>
-      <c r="C107" t="s">
-        <v>778</v>
-      </c>
-      <c r="D107" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C108" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="D108" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -5156,12 +5156,12 @@
         <v>630</v>
       </c>
       <c r="D109" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B110" t="s">
         <v>643</v>
@@ -5175,16 +5175,16 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>837</v>
+      </c>
+      <c r="B111" t="s">
+        <v>838</v>
+      </c>
+      <c r="C111" t="s">
         <v>839</v>
       </c>
-      <c r="B111" t="s">
-        <v>840</v>
-      </c>
-      <c r="C111" t="s">
-        <v>841</v>
-      </c>
       <c r="D111" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -5217,35 +5217,35 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C114" t="s">
+        <v>780</v>
+      </c>
+      <c r="D114" t="s">
         <v>782</v>
-      </c>
-      <c r="D114" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C115" t="s">
+        <v>781</v>
+      </c>
+      <c r="D115" t="s">
         <v>783</v>
-      </c>
-      <c r="D115" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C116" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="D116" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -5278,10 +5278,10 @@
         <v>81</v>
       </c>
       <c r="C119" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="D119" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -5292,10 +5292,10 @@
         <v>81</v>
       </c>
       <c r="C120" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="D120" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -5607,13 +5607,13 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>854</v>
+      </c>
+      <c r="C147" t="s">
         <v>856</v>
       </c>
-      <c r="C147" t="s">
-        <v>858</v>
-      </c>
       <c r="D147" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -5629,16 +5629,16 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="B149" t="s">
+        <v>847</v>
+      </c>
+      <c r="C149" t="s">
+        <v>848</v>
+      </c>
+      <c r="D149" t="s">
         <v>849</v>
-      </c>
-      <c r="C149" t="s">
-        <v>850</v>
-      </c>
-      <c r="D149" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5654,13 +5654,13 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C151" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="D151" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -5679,7 +5679,7 @@
         <v>374</v>
       </c>
       <c r="C153" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D153" t="s">
         <v>378</v>
@@ -6116,68 +6116,68 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>884</v>
+      </c>
+      <c r="C193" s="9" t="s">
         <v>886</v>
       </c>
-      <c r="C193" s="9" t="s">
+      <c r="D193" s="9" t="s">
         <v>888</v>
-      </c>
-      <c r="D193" s="9" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
+        <v>893</v>
+      </c>
+      <c r="C194" s="9" t="s">
         <v>895</v>
       </c>
-      <c r="C194" s="9" t="s">
-        <v>897</v>
-      </c>
       <c r="D194" s="9" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
+        <v>894</v>
+      </c>
+      <c r="C195" s="9" t="s">
         <v>896</v>
       </c>
-      <c r="C195" s="9" t="s">
-        <v>898</v>
-      </c>
       <c r="D195" s="9" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
+        <v>885</v>
+      </c>
+      <c r="C196" s="9" t="s">
         <v>887</v>
       </c>
-      <c r="C196" s="9" t="s">
+      <c r="D196" s="9" t="s">
         <v>889</v>
-      </c>
-      <c r="D196" s="9" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -6207,7 +6207,7 @@
         <v>675</v>
       </c>
       <c r="D201" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -6215,15 +6215,15 @@
         <v>671</v>
       </c>
       <c r="C202" t="s">
-        <v>676</v>
+        <v>905</v>
       </c>
       <c r="D202" t="s">
-        <v>678</v>
+        <v>906</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C203" s="7" t="s">
         <v>669</v>
@@ -6417,13 +6417,13 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
+        <v>770</v>
+      </c>
+      <c r="C219" t="s">
+        <v>771</v>
+      </c>
+      <c r="D219" t="s">
         <v>772</v>
-      </c>
-      <c r="C219" t="s">
-        <v>773</v>
-      </c>
-      <c r="D219" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -6473,10 +6473,10 @@
         <v>333</v>
       </c>
       <c r="C223" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D223" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -6506,24 +6506,24 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C226" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="D226" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
+        <v>788</v>
+      </c>
+      <c r="C227" t="s">
+        <v>789</v>
+      </c>
+      <c r="D227" t="s">
         <v>790</v>
-      </c>
-      <c r="C227" t="s">
-        <v>791</v>
-      </c>
-      <c r="D227" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -7034,13 +7034,13 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
+        <v>890</v>
+      </c>
+      <c r="C265" t="s">
+        <v>891</v>
+      </c>
+      <c r="D265" t="s">
         <v>892</v>
-      </c>
-      <c r="C265" t="s">
-        <v>893</v>
-      </c>
-      <c r="D265" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
@@ -7430,13 +7430,13 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
+        <v>791</v>
+      </c>
+      <c r="C298" t="s">
+        <v>792</v>
+      </c>
+      <c r="D298" t="s">
         <v>793</v>
-      </c>
-      <c r="C298" t="s">
-        <v>794</v>
-      </c>
-      <c r="D298" t="s">
-        <v>795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed function calls in getSpatial and initial comit for raster vis shiny page
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esniede\Documents\github\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05570B2E-2768-4366-BF37-E182AEE3CF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D446A202-8823-431F-95FC-1FF4F308A62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="910">
   <si>
     <t>id</t>
   </si>
@@ -2754,6 +2754,15 @@
   </si>
   <si>
     <t>Explorateur des données sur l’eau du Yukon</t>
+  </si>
+  <si>
+    <t>mapsNavRasterTitle</t>
+  </si>
+  <si>
+    <t>Rasters</t>
+  </si>
+  <si>
+    <t>maps_raster</t>
   </si>
 </sst>
 </file>
@@ -3690,10 +3699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D298"/>
+  <dimension ref="A1:D299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3813,1550 +3822,1550 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>688</v>
+        <v>909</v>
       </c>
       <c r="B9" t="s">
-        <v>726</v>
+        <v>907</v>
       </c>
       <c r="C9" t="s">
-        <v>689</v>
+        <v>908</v>
       </c>
       <c r="D9" t="s">
-        <v>690</v>
+        <v>908</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="B10" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="C10" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="D10" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="B11" t="s">
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="C11" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="D11" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="B12" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="C12" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="D12" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="B13" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C13" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D13" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="B14" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="C14" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
       <c r="D14" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B15" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C15" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D15" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B16" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C16" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D16" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B17" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C17" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D17" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>680</v>
+        <v>710</v>
       </c>
       <c r="B18" t="s">
-        <v>728</v>
+        <v>719</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>717</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>718</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>702</v>
+        <v>680</v>
       </c>
       <c r="B19" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C19" t="s">
-        <v>694</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>695</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B20" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C20" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="D20" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>681</v>
+        <v>703</v>
       </c>
       <c r="B21" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>697</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>698</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>733</v>
+        <v>681</v>
       </c>
       <c r="B22" t="s">
-        <v>739</v>
+        <v>732</v>
       </c>
       <c r="C22" t="s">
-        <v>735</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>738</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B23" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C23" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D23" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>684</v>
+        <v>734</v>
       </c>
       <c r="B24" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C24" t="s">
-        <v>685</v>
+        <v>736</v>
       </c>
       <c r="D24" t="s">
-        <v>685</v>
+        <v>737</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="B25" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C25" t="s">
-        <v>129</v>
+        <v>685</v>
       </c>
       <c r="D25" t="s">
-        <v>130</v>
+        <v>685</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>692</v>
+      </c>
+      <c r="B26" t="s">
+        <v>741</v>
+      </c>
+      <c r="C26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>693</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>743</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>686</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>645</v>
-      </c>
-      <c r="B28" t="s">
-        <v>646</v>
-      </c>
-      <c r="C28" t="s">
-        <v>648</v>
-      </c>
-      <c r="D28" t="s">
-        <v>649</v>
-      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B29" t="s">
         <v>646</v>
       </c>
       <c r="C29" t="s">
-        <v>843</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>844</v>
+        <v>648</v>
+      </c>
+      <c r="D29" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>647</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>646</v>
       </c>
       <c r="C30" t="s">
-        <v>521</v>
-      </c>
-      <c r="D30" t="s">
-        <v>522</v>
+        <v>843</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>844</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>842</v>
+        <v>521</v>
       </c>
       <c r="D31" t="s">
-        <v>841</v>
+        <v>522</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>856</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>858</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>857</v>
+        <v>842</v>
       </c>
       <c r="D32" t="s">
-        <v>861</v>
+        <v>841</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B33" t="s">
         <v>858</v>
       </c>
       <c r="C33" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="D33" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>862</v>
+        <v>855</v>
       </c>
       <c r="B34" t="s">
-        <v>226</v>
+        <v>858</v>
       </c>
       <c r="C34" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="D34" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="B35" t="s">
         <v>226</v>
       </c>
       <c r="C35" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="D35" t="s">
-        <v>869</v>
+        <v>864</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>865</v>
+        <v>870</v>
       </c>
       <c r="B36" t="s">
         <v>226</v>
       </c>
       <c r="C36" t="s">
-        <v>779</v>
+        <v>871</v>
       </c>
       <c r="D36" t="s">
-        <v>780</v>
+        <v>869</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B37" t="s">
         <v>226</v>
       </c>
       <c r="C37" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="D37" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B38" t="s">
         <v>226</v>
       </c>
       <c r="C38" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="D38" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B39" t="s">
         <v>226</v>
       </c>
       <c r="C39" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="D39" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>868</v>
       </c>
       <c r="B40" t="s">
-        <v>22</v>
+        <v>226</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>774</v>
       </c>
       <c r="D40" t="s">
-        <v>24</v>
+        <v>776</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
         <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D41" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B43" t="s">
         <v>29</v>
       </c>
       <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" t="s">
         <v>33</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>276</v>
-      </c>
-      <c r="B45" t="s">
-        <v>278</v>
-      </c>
-      <c r="C45" t="s">
-        <v>523</v>
-      </c>
-      <c r="D45" t="s">
-        <v>524</v>
-      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B46" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C46" t="s">
-        <v>282</v>
+        <v>523</v>
       </c>
       <c r="D46" t="s">
-        <v>283</v>
+        <v>524</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B47" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C47" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D47" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B48" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C48" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="D48" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B49" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C49" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="D49" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B50" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C50" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="D50" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B51" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C51" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="D51" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>525</v>
+        <v>292</v>
       </c>
       <c r="B52" t="s">
         <v>294</v>
       </c>
       <c r="C52" t="s">
-        <v>526</v>
+        <v>290</v>
       </c>
       <c r="D52" t="s">
-        <v>527</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>304</v>
+        <v>525</v>
       </c>
       <c r="B53" t="s">
         <v>294</v>
       </c>
       <c r="C53" t="s">
-        <v>305</v>
+        <v>526</v>
       </c>
       <c r="D53" t="s">
-        <v>306</v>
+        <v>527</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>304</v>
+      </c>
+      <c r="B54" t="s">
+        <v>294</v>
+      </c>
+      <c r="C54" t="s">
+        <v>305</v>
+      </c>
+      <c r="D54" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>307</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>301</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>308</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>35</v>
-      </c>
-      <c r="B56" t="s">
-        <v>36</v>
-      </c>
-      <c r="C56" t="s">
-        <v>146</v>
-      </c>
-      <c r="D56" t="s">
-        <v>37</v>
-      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
+        <v>146</v>
+      </c>
+      <c r="D57" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>38</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>39</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>40</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>227</v>
-      </c>
-      <c r="B59" t="s">
-        <v>225</v>
-      </c>
-      <c r="C59" t="s">
-        <v>232</v>
-      </c>
-      <c r="D59" t="s">
-        <v>233</v>
-      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>227</v>
       </c>
       <c r="B60" t="s">
-        <v>179</v>
+        <v>225</v>
       </c>
       <c r="C60" t="s">
-        <v>74</v>
+        <v>232</v>
       </c>
       <c r="D60" t="s">
-        <v>75</v>
+        <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>234</v>
+        <v>73</v>
       </c>
       <c r="B61" t="s">
-        <v>236</v>
+        <v>179</v>
       </c>
       <c r="C61" t="s">
-        <v>832</v>
+        <v>74</v>
       </c>
       <c r="D61" t="s">
-        <v>235</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>635</v>
+        <v>234</v>
+      </c>
+      <c r="B62" t="s">
+        <v>236</v>
       </c>
       <c r="C62" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D62" t="s">
-        <v>636</v>
+        <v>235</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>240</v>
-      </c>
-      <c r="B63" t="s">
-        <v>242</v>
+        <v>635</v>
       </c>
       <c r="C63" t="s">
-        <v>241</v>
+        <v>833</v>
       </c>
       <c r="D63" t="s">
-        <v>265</v>
+        <v>636</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B64" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C64" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D64" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B65" t="s">
         <v>243</v>
       </c>
       <c r="C65" t="s">
-        <v>828</v>
+        <v>246</v>
       </c>
       <c r="D65" t="s">
-        <v>831</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B66" t="s">
         <v>243</v>
       </c>
       <c r="C66" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D66" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>631</v>
+        <v>239</v>
       </c>
       <c r="B67" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C67" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
       <c r="D67" t="s">
-        <v>247</v>
+        <v>830</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B68" t="s">
         <v>244</v>
       </c>
       <c r="C68" t="s">
-        <v>633</v>
+        <v>834</v>
       </c>
       <c r="D68" t="s">
-        <v>634</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>264</v>
+        <v>632</v>
       </c>
       <c r="B69" t="s">
         <v>244</v>
       </c>
       <c r="C69" t="s">
-        <v>826</v>
+        <v>633</v>
       </c>
       <c r="D69" t="s">
-        <v>827</v>
+        <v>634</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="B70" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C70" t="s">
-        <v>249</v>
+        <v>826</v>
       </c>
       <c r="D70" t="s">
-        <v>250</v>
+        <v>827</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>879</v>
+        <v>248</v>
+      </c>
+      <c r="B71" t="s">
+        <v>242</v>
       </c>
       <c r="C71" t="s">
-        <v>880</v>
+        <v>249</v>
       </c>
       <c r="D71" t="s">
-        <v>881</v>
+        <v>250</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>795</v>
-      </c>
-      <c r="B72" t="s">
-        <v>797</v>
+        <v>879</v>
       </c>
       <c r="C72" t="s">
-        <v>798</v>
+        <v>880</v>
       </c>
       <c r="D72" t="s">
-        <v>800</v>
+        <v>881</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B73" t="s">
         <v>797</v>
       </c>
       <c r="C73" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D73" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>252</v>
+        <v>796</v>
       </c>
       <c r="B74" t="s">
-        <v>242</v>
+        <v>797</v>
       </c>
       <c r="C74" t="s">
-        <v>253</v>
+        <v>799</v>
       </c>
       <c r="D74" t="s">
-        <v>254</v>
+        <v>801</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="B75" t="s">
         <v>242</v>
       </c>
       <c r="C75" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="D75" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="B76" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C76" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="D76" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B77" t="s">
         <v>243</v>
       </c>
       <c r="C77" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D77" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B78" t="s">
         <v>243</v>
       </c>
       <c r="C78" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D78" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B79" t="s">
-        <v>273</v>
+        <v>243</v>
       </c>
       <c r="C79" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="D79" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>755</v>
+        <v>272</v>
       </c>
       <c r="B80" t="s">
-        <v>756</v>
+        <v>273</v>
       </c>
       <c r="C80" t="s">
-        <v>757</v>
+        <v>274</v>
       </c>
       <c r="D80" t="s">
-        <v>758</v>
+        <v>275</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B81" t="s">
         <v>756</v>
       </c>
       <c r="C81" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="D81" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="B82" t="s">
         <v>756</v>
       </c>
       <c r="C82" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D82" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B83" t="s">
         <v>756</v>
       </c>
       <c r="C83" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="D83" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>804</v>
+        <v>765</v>
       </c>
       <c r="B84" t="s">
         <v>756</v>
       </c>
       <c r="C84" t="s">
-        <v>807</v>
+        <v>766</v>
       </c>
       <c r="D84" t="s">
-        <v>808</v>
+        <v>767</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B85" t="s">
         <v>756</v>
       </c>
       <c r="C85" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
       <c r="D85" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="B86" t="s">
         <v>756</v>
       </c>
       <c r="C86" t="s">
-        <v>802</v>
+        <v>812</v>
       </c>
       <c r="D86" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B87" t="s">
         <v>756</v>
       </c>
       <c r="C87" t="s">
-        <v>813</v>
+        <v>802</v>
       </c>
       <c r="D87" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="B88" t="s">
         <v>756</v>
       </c>
       <c r="C88" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="D88" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="B89" t="s">
         <v>756</v>
       </c>
       <c r="C89" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="D89" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>823</v>
+        <v>817</v>
+      </c>
+      <c r="B90" t="s">
+        <v>756</v>
       </c>
       <c r="C90" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="D90" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>823</v>
+      </c>
+      <c r="C91" t="s">
+        <v>824</v>
+      </c>
+      <c r="D91" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>820</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C92" t="s">
         <v>821</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D92" t="s">
         <v>822</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B92" s="8"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>603</v>
-      </c>
-      <c r="C93" t="s">
-        <v>604</v>
-      </c>
-      <c r="D93" t="s">
-        <v>605</v>
-      </c>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>621</v>
+        <v>603</v>
       </c>
       <c r="C94" t="s">
-        <v>622</v>
+        <v>604</v>
       </c>
       <c r="D94" t="s">
-        <v>623</v>
+        <v>605</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>606</v>
-      </c>
-      <c r="B95" t="s">
-        <v>643</v>
+        <v>621</v>
       </c>
       <c r="C95" t="s">
-        <v>607</v>
+        <v>622</v>
       </c>
       <c r="D95" t="s">
-        <v>608</v>
+        <v>623</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="B96" t="s">
         <v>643</v>
       </c>
       <c r="C96" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="D96" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>177</v>
+        <v>609</v>
       </c>
       <c r="B97" t="s">
-        <v>178</v>
+        <v>643</v>
       </c>
       <c r="C97" t="s">
-        <v>76</v>
+        <v>610</v>
       </c>
       <c r="D97" t="s">
-        <v>77</v>
+        <v>611</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="B98" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C98" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="D98" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>175</v>
+        <v>62</v>
       </c>
       <c r="B99" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C99" t="s">
-        <v>182</v>
+        <v>63</v>
       </c>
       <c r="D99" t="s">
-        <v>183</v>
+        <v>64</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>213</v>
+        <v>175</v>
       </c>
       <c r="B100" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="C100" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
       <c r="D100" t="s">
-        <v>218</v>
+        <v>183</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B101" t="s">
         <v>214</v>
       </c>
       <c r="C101" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="D101" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>677</v>
+        <v>215</v>
+      </c>
+      <c r="B102" t="s">
+        <v>214</v>
       </c>
       <c r="C102" t="s">
-        <v>678</v>
+        <v>231</v>
       </c>
       <c r="D102" t="s">
-        <v>676</v>
+        <v>231</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>653</v>
+        <v>677</v>
       </c>
       <c r="C103" t="s">
-        <v>654</v>
+        <v>678</v>
       </c>
       <c r="D103" t="s">
-        <v>655</v>
+        <v>676</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="C104" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="D104" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>783</v>
+        <v>650</v>
       </c>
       <c r="C105" t="s">
-        <v>784</v>
+        <v>651</v>
       </c>
       <c r="D105" t="s">
-        <v>785</v>
+        <v>652</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>637</v>
-      </c>
-      <c r="B106" t="s">
-        <v>642</v>
+        <v>783</v>
       </c>
       <c r="C106" t="s">
-        <v>639</v>
+        <v>784</v>
       </c>
       <c r="D106" t="s">
-        <v>638</v>
+        <v>785</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>773</v>
+        <v>637</v>
+      </c>
+      <c r="B107" t="s">
+        <v>642</v>
       </c>
       <c r="C107" t="s">
-        <v>774</v>
+        <v>639</v>
       </c>
       <c r="D107" t="s">
-        <v>775</v>
+        <v>638</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>782</v>
+        <v>773</v>
       </c>
       <c r="C108" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D108" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>627</v>
-      </c>
-      <c r="B109" t="s">
-        <v>640</v>
+        <v>782</v>
       </c>
       <c r="C109" t="s">
-        <v>628</v>
+        <v>777</v>
       </c>
       <c r="D109" t="s">
-        <v>839</v>
+        <v>776</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>838</v>
+        <v>627</v>
       </c>
       <c r="B110" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C110" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D110" t="s">
-        <v>630</v>
+        <v>839</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c r="B111" t="s">
-        <v>836</v>
+        <v>641</v>
       </c>
       <c r="C111" t="s">
-        <v>837</v>
+        <v>629</v>
       </c>
       <c r="D111" t="s">
-        <v>840</v>
+        <v>630</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>624</v>
+        <v>835</v>
       </c>
       <c r="B112" t="s">
-        <v>226</v>
+        <v>836</v>
       </c>
       <c r="C112" t="s">
-        <v>625</v>
+        <v>837</v>
       </c>
       <c r="D112" t="s">
-        <v>626</v>
+        <v>840</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>228</v>
+        <v>624</v>
       </c>
       <c r="B113" t="s">
         <v>226</v>
       </c>
       <c r="C113" t="s">
-        <v>229</v>
+        <v>625</v>
       </c>
       <c r="D113" t="s">
-        <v>230</v>
+        <v>626</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>771</v>
+        <v>228</v>
+      </c>
+      <c r="B114" t="s">
+        <v>226</v>
       </c>
       <c r="C114" t="s">
-        <v>778</v>
+        <v>229</v>
       </c>
       <c r="D114" t="s">
-        <v>781</v>
+        <v>230</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C115" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D115" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>772</v>
+      </c>
+      <c r="C116" t="s">
+        <v>779</v>
+      </c>
+      <c r="D116" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>794</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C117" t="s">
         <v>792</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D117" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="4" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B117" s="4"/>
-      <c r="C117" s="4"/>
-      <c r="D117" s="4"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>78</v>
-      </c>
-      <c r="B118" t="s">
-        <v>79</v>
-      </c>
-      <c r="C118" t="s">
-        <v>83</v>
-      </c>
-      <c r="D118" t="s">
-        <v>84</v>
-      </c>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B119" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C119" t="s">
-        <v>872</v>
+        <v>83</v>
       </c>
       <c r="D119" t="s">
-        <v>873</v>
+        <v>84</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B120" t="s">
         <v>81</v>
       </c>
       <c r="C120" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="D120" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B121" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C121" t="s">
-        <v>98</v>
+        <v>874</v>
       </c>
       <c r="D121" t="s">
-        <v>251</v>
+        <v>875</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>97</v>
+      </c>
+      <c r="B122" t="s">
+        <v>79</v>
+      </c>
+      <c r="C122" t="s">
+        <v>98</v>
+      </c>
+      <c r="D122" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>85</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>86</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C123" t="s">
         <v>87</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D123" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="B123" s="5"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>311</v>
-      </c>
-      <c r="B124" t="s">
-        <v>310</v>
-      </c>
-      <c r="C124" t="s">
-        <v>316</v>
-      </c>
-      <c r="D124" t="s">
-        <v>317</v>
-      </c>
+      <c r="B124" s="5"/>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B125" t="s">
         <v>310</v>
       </c>
       <c r="C125" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D125" t="s">
         <v>317</v>
@@ -5364,1163 +5373,1166 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B126" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C126" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D126" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B127" t="s">
         <v>313</v>
       </c>
       <c r="C127" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D127" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>407</v>
+        <v>320</v>
+      </c>
+      <c r="B128" t="s">
+        <v>313</v>
       </c>
       <c r="C128" t="s">
-        <v>408</v>
+        <v>321</v>
       </c>
       <c r="D128" t="s">
-        <v>409</v>
+        <v>322</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>323</v>
+        <v>407</v>
       </c>
       <c r="C129" t="s">
-        <v>325</v>
+        <v>408</v>
       </c>
       <c r="D129" t="s">
-        <v>324</v>
+        <v>409</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>400</v>
+        <v>323</v>
       </c>
       <c r="C130" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D130" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C131" t="s">
-        <v>405</v>
+        <v>326</v>
       </c>
       <c r="D131" t="s">
-        <v>406</v>
+        <v>327</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C132" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D132" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>328</v>
+        <v>402</v>
       </c>
       <c r="C133" t="s">
-        <v>330</v>
+        <v>404</v>
       </c>
       <c r="D133" t="s">
-        <v>329</v>
+        <v>403</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>344</v>
-      </c>
-      <c r="B134" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
       <c r="C134" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="D134" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>394</v>
+        <v>344</v>
+      </c>
+      <c r="B135" t="s">
+        <v>345</v>
       </c>
       <c r="C135" t="s">
-        <v>396</v>
+        <v>346</v>
       </c>
       <c r="D135" t="s">
-        <v>398</v>
+        <v>347</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C136" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D136" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>348</v>
-      </c>
-      <c r="B137" t="s">
-        <v>349</v>
+        <v>395</v>
       </c>
       <c r="C137" t="s">
-        <v>350</v>
+        <v>397</v>
       </c>
       <c r="D137" t="s">
-        <v>351</v>
+        <v>399</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>412</v>
+        <v>348</v>
+      </c>
+      <c r="B138" t="s">
+        <v>349</v>
       </c>
       <c r="C138" t="s">
-        <v>386</v>
+        <v>350</v>
       </c>
       <c r="D138" t="s">
-        <v>387</v>
+        <v>351</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C139" t="s">
-        <v>414</v>
+        <v>386</v>
       </c>
       <c r="D139" t="s">
-        <v>415</v>
+        <v>387</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>331</v>
+        <v>413</v>
       </c>
       <c r="C140" t="s">
-        <v>360</v>
+        <v>414</v>
       </c>
       <c r="D140" t="s">
-        <v>332</v>
+        <v>415</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
       <c r="C141" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="D141" t="s">
-        <v>353</v>
+        <v>332</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C142" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D142" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C143" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D143" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C144" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D144" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C145" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D145" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C146" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D146" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>852</v>
+        <v>367</v>
       </c>
       <c r="C147" t="s">
-        <v>854</v>
+        <v>368</v>
       </c>
       <c r="D147" t="s">
-        <v>853</v>
+        <v>369</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>388</v>
+        <v>852</v>
       </c>
       <c r="C148" t="s">
-        <v>393</v>
+        <v>854</v>
       </c>
       <c r="D148" t="s">
-        <v>392</v>
+        <v>853</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>849</v>
-      </c>
-      <c r="B149" t="s">
-        <v>845</v>
+        <v>388</v>
       </c>
       <c r="C149" t="s">
-        <v>846</v>
+        <v>393</v>
       </c>
       <c r="D149" t="s">
-        <v>847</v>
+        <v>392</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>373</v>
+        <v>849</v>
+      </c>
+      <c r="B150" t="s">
+        <v>845</v>
       </c>
       <c r="C150" t="s">
-        <v>377</v>
+        <v>846</v>
       </c>
       <c r="D150" t="s">
-        <v>410</v>
+        <v>847</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>851</v>
+        <v>373</v>
       </c>
       <c r="C151" t="s">
-        <v>850</v>
+        <v>377</v>
       </c>
       <c r="D151" t="s">
-        <v>848</v>
+        <v>410</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>389</v>
+        <v>851</v>
       </c>
       <c r="C152" t="s">
-        <v>390</v>
+        <v>850</v>
       </c>
       <c r="D152" t="s">
-        <v>391</v>
+        <v>848</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>374</v>
+        <v>389</v>
       </c>
       <c r="C153" t="s">
-        <v>753</v>
+        <v>390</v>
       </c>
       <c r="D153" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C154" t="s">
-        <v>380</v>
+        <v>753</v>
       </c>
       <c r="D154" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="C155" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D155" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C156" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="D156" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>496</v>
-      </c>
-      <c r="C157" s="9" t="s">
-        <v>497</v>
+        <v>376</v>
+      </c>
+      <c r="C157" t="s">
+        <v>381</v>
       </c>
       <c r="D157" t="s">
-        <v>498</v>
+        <v>382</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>416</v>
-      </c>
-      <c r="C158" t="s">
-        <v>417</v>
+        <v>496</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>497</v>
       </c>
       <c r="D158" t="s">
-        <v>418</v>
+        <v>498</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C159" t="s">
-        <v>474</v>
+        <v>417</v>
       </c>
       <c r="D159" t="s">
-        <v>472</v>
+        <v>418</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C160" t="s">
-        <v>420</v>
+        <v>474</v>
       </c>
       <c r="D160" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>502</v>
+        <v>421</v>
       </c>
       <c r="C161" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D161" t="s">
-        <v>426</v>
+        <v>473</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>520</v>
+        <v>502</v>
       </c>
       <c r="C162" t="s">
-        <v>518</v>
+        <v>425</v>
       </c>
       <c r="D162" t="s">
-        <v>519</v>
+        <v>426</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>427</v>
+        <v>520</v>
       </c>
       <c r="C163" t="s">
-        <v>428</v>
+        <v>518</v>
       </c>
       <c r="D163" t="s">
-        <v>429</v>
+        <v>519</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>466</v>
+        <v>427</v>
       </c>
       <c r="C164" t="s">
-        <v>468</v>
+        <v>428</v>
       </c>
       <c r="D164" t="s">
-        <v>470</v>
+        <v>429</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C165" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D165" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="C166" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="D166" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>506</v>
+        <v>475</v>
       </c>
       <c r="C167" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D167" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>480</v>
+        <v>506</v>
       </c>
       <c r="C168" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="D168" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C169" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D169" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C170" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D170" t="s">
-        <v>513</v>
+        <v>486</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>499</v>
-      </c>
-      <c r="C171" s="9" t="s">
-        <v>500</v>
+        <v>484</v>
+      </c>
+      <c r="C171" t="s">
+        <v>487</v>
       </c>
       <c r="D171" t="s">
-        <v>501</v>
+        <v>513</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="D172" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D173" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D174" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>487</v>
+        <v>512</v>
       </c>
       <c r="D175" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="D176" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>528</v>
+        <v>517</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>529</v>
+        <v>514</v>
       </c>
       <c r="D177" t="s">
-        <v>530</v>
+        <v>515</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="D178" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D179" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="D180" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="D181" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D182" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>562</v>
+        <v>544</v>
       </c>
       <c r="D183" t="s">
-        <v>563</v>
+        <v>545</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>548</v>
+        <v>562</v>
       </c>
       <c r="D184" t="s">
-        <v>550</v>
+        <v>563</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D185" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D186" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="D187" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C188" s="9" t="s">
-        <v>553</v>
-      </c>
-      <c r="D188" s="9" t="s">
-        <v>553</v>
+        <v>556</v>
+      </c>
+      <c r="D188" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C189" s="9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C190" s="9" t="s">
-        <v>565</v>
+        <v>554</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>566</v>
+        <v>554</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="C191" s="9" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C192" s="9" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="D192" s="9" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>882</v>
+        <v>572</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>884</v>
+        <v>573</v>
       </c>
       <c r="D193" s="9" t="s">
-        <v>886</v>
+        <v>576</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>891</v>
+        <v>882</v>
       </c>
       <c r="C194" s="9" t="s">
-        <v>893</v>
+        <v>884</v>
       </c>
       <c r="D194" s="9" t="s">
-        <v>899</v>
+        <v>886</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D195" s="9" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>883</v>
+        <v>892</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>885</v>
+        <v>894</v>
       </c>
       <c r="D196" s="9" t="s">
-        <v>887</v>
+        <v>900</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>901</v>
+        <v>883</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>895</v>
+        <v>885</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>898</v>
+        <v>887</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
+        <v>901</v>
+      </c>
+      <c r="C198" s="9" t="s">
+        <v>895</v>
+      </c>
+      <c r="D198" s="9" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
         <v>902</v>
       </c>
-      <c r="C198" s="9" t="s">
+      <c r="C199" s="9" t="s">
         <v>896</v>
       </c>
-      <c r="D198" s="9" t="s">
+      <c r="D199" s="9" t="s">
         <v>897</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="3" t="s">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B199" s="3"/>
-      <c r="C199" s="3"/>
-      <c r="D199" s="3"/>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>670</v>
-      </c>
-      <c r="C200" t="s">
-        <v>671</v>
-      </c>
-      <c r="D200" t="s">
-        <v>672</v>
-      </c>
+      <c r="B200" s="3"/>
+      <c r="C200" s="3"/>
+      <c r="D200" s="3"/>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c r="C201" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D201" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="C202" t="s">
-        <v>903</v>
+        <v>673</v>
       </c>
       <c r="D202" t="s">
-        <v>904</v>
+        <v>674</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>675</v>
-      </c>
-      <c r="C203" s="7" t="s">
-        <v>667</v>
-      </c>
-      <c r="D203" s="7" t="s">
-        <v>668</v>
+        <v>669</v>
+      </c>
+      <c r="C203" t="s">
+        <v>903</v>
+      </c>
+      <c r="D203" t="s">
+        <v>904</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>134</v>
-      </c>
-      <c r="B204" t="s">
-        <v>131</v>
-      </c>
-      <c r="C204" t="s">
-        <v>132</v>
-      </c>
-      <c r="D204" t="s">
-        <v>133</v>
+        <v>675</v>
+      </c>
+      <c r="C204" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="D204" s="7" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B205" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C205" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D205" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B206" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C206" t="s">
-        <v>659</v>
+        <v>144</v>
       </c>
       <c r="D206" t="s">
-        <v>660</v>
+        <v>145</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B207" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C207" t="s">
-        <v>143</v>
+        <v>659</v>
       </c>
       <c r="D207" t="s">
-        <v>142</v>
+        <v>660</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B208" t="s">
-        <v>139</v>
-      </c>
-      <c r="C208" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D208" s="7" t="s">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="C208" t="s">
+        <v>143</v>
+      </c>
+      <c r="D208" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>657</v>
-      </c>
-      <c r="C209" t="s">
-        <v>656</v>
-      </c>
-      <c r="D209" t="s">
-        <v>656</v>
+        <v>138</v>
+      </c>
+      <c r="B209" t="s">
+        <v>139</v>
+      </c>
+      <c r="C209" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D209" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C210" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="D210" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
+        <v>658</v>
+      </c>
+      <c r="C211" t="s">
+        <v>662</v>
+      </c>
+      <c r="D211" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>663</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C212" t="s">
         <v>664</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D212" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="6" t="s">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B212" s="6"/>
-      <c r="C212" s="6"/>
-      <c r="D212" s="6"/>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>45</v>
-      </c>
-      <c r="B213" t="s">
-        <v>8</v>
-      </c>
-      <c r="C213" t="s">
-        <v>46</v>
-      </c>
-      <c r="D213" t="s">
-        <v>47</v>
-      </c>
+      <c r="B213" s="6"/>
+      <c r="C213" s="6"/>
+      <c r="D213" s="6"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="B214" t="s">
         <v>8</v>
       </c>
       <c r="C214" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="D214" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>580</v>
+        <v>89</v>
+      </c>
+      <c r="B215" t="s">
+        <v>8</v>
       </c>
       <c r="C215" t="s">
-        <v>581</v>
+        <v>90</v>
       </c>
       <c r="D215" t="s">
-        <v>582</v>
+        <v>91</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C216" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D216" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>615</v>
+        <v>583</v>
       </c>
       <c r="C217" t="s">
-        <v>617</v>
+        <v>584</v>
       </c>
       <c r="D217" t="s">
-        <v>618</v>
+        <v>585</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C218" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="D218" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>768</v>
+        <v>616</v>
       </c>
       <c r="C219" t="s">
-        <v>769</v>
+        <v>620</v>
       </c>
       <c r="D219" t="s">
-        <v>770</v>
+        <v>619</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>48</v>
-      </c>
-      <c r="B220" t="s">
-        <v>8</v>
+        <v>768</v>
       </c>
       <c r="C220" t="s">
-        <v>49</v>
+        <v>769</v>
       </c>
       <c r="D220" t="s">
-        <v>50</v>
+        <v>770</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B221" t="s">
         <v>8</v>
       </c>
       <c r="C221" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D221" t="s">
-        <v>216</v>
+        <v>50</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>211</v>
+        <v>51</v>
       </c>
       <c r="B222" t="s">
         <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>212</v>
+        <v>52</v>
       </c>
       <c r="D222" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>333</v>
+        <v>211</v>
+      </c>
+      <c r="B223" t="s">
+        <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>877</v>
+        <v>212</v>
       </c>
       <c r="D223" t="s">
-        <v>878</v>
+        <v>212</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>334</v>
-      </c>
-      <c r="B224" t="s">
-        <v>8</v>
+        <v>333</v>
       </c>
       <c r="C224" t="s">
-        <v>597</v>
+        <v>877</v>
       </c>
       <c r="D224" t="s">
-        <v>599</v>
+        <v>878</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>598</v>
+        <v>334</v>
+      </c>
+      <c r="B225" t="s">
+        <v>8</v>
       </c>
       <c r="C225" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D225" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>790</v>
+        <v>598</v>
       </c>
       <c r="C226" t="s">
-        <v>876</v>
+        <v>596</v>
       </c>
       <c r="D226" t="s">
-        <v>788</v>
+        <v>600</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
       <c r="C227" t="s">
-        <v>787</v>
+        <v>876</v>
       </c>
       <c r="D227" t="s">
         <v>788</v>
@@ -6528,922 +6540,933 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>149</v>
-      </c>
-      <c r="B228" t="s">
-        <v>8</v>
+        <v>786</v>
       </c>
       <c r="C228" t="s">
-        <v>577</v>
+        <v>787</v>
       </c>
       <c r="D228" t="s">
-        <v>150</v>
+        <v>788</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B229" t="s">
         <v>8</v>
       </c>
       <c r="C229" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D229" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B230" t="s">
         <v>8</v>
       </c>
       <c r="C230" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D230" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>586</v>
+        <v>167</v>
       </c>
       <c r="B231" t="s">
         <v>8</v>
       </c>
       <c r="C231" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="D231" t="s">
-        <v>588</v>
+        <v>168</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="B232" t="s">
         <v>8</v>
       </c>
       <c r="C232" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D232" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B233" t="s">
         <v>8</v>
       </c>
       <c r="C233" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D233" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>148</v>
+        <v>594</v>
       </c>
       <c r="B234" t="s">
         <v>8</v>
       </c>
       <c r="C234" t="s">
-        <v>184</v>
+        <v>592</v>
       </c>
       <c r="D234" t="s">
-        <v>185</v>
+        <v>590</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>53</v>
+        <v>148</v>
       </c>
       <c r="B235" t="s">
         <v>8</v>
       </c>
       <c r="C235" t="s">
-        <v>54</v>
+        <v>184</v>
       </c>
       <c r="D235" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>156</v>
+        <v>53</v>
       </c>
       <c r="B236" t="s">
         <v>8</v>
       </c>
       <c r="C236" t="s">
-        <v>151</v>
+        <v>54</v>
       </c>
       <c r="D236" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B237" t="s">
         <v>8</v>
       </c>
       <c r="C237" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D237" t="s">
-        <v>163</v>
+        <v>16</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>56</v>
+        <v>161</v>
       </c>
       <c r="B238" t="s">
         <v>8</v>
       </c>
       <c r="C238" t="s">
-        <v>57</v>
+        <v>162</v>
       </c>
       <c r="D238" t="s">
-        <v>58</v>
+        <v>163</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="B239" t="s">
         <v>8</v>
       </c>
       <c r="C239" t="s">
-        <v>157</v>
+        <v>57</v>
       </c>
       <c r="D239" t="s">
-        <v>158</v>
+        <v>58</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B240" t="s">
         <v>8</v>
       </c>
       <c r="C240" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D240" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>59</v>
+        <v>164</v>
       </c>
       <c r="B241" t="s">
         <v>8</v>
       </c>
       <c r="C241" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="D241" t="s">
-        <v>61</v>
+        <v>166</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>154</v>
+        <v>59</v>
       </c>
       <c r="B242" t="s">
         <v>8</v>
       </c>
       <c r="C242" t="s">
-        <v>152</v>
+        <v>60</v>
       </c>
       <c r="D242" t="s">
-        <v>153</v>
+        <v>61</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="B243" t="s">
         <v>8</v>
       </c>
       <c r="C243" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="D243" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="B244" t="s">
         <v>8</v>
       </c>
       <c r="C244" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="D244" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B245" t="s">
         <v>8</v>
       </c>
       <c r="C245" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D245" t="s">
-        <v>99</v>
+        <v>187</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B246" t="s">
         <v>8</v>
       </c>
       <c r="C246" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D246" t="s">
-        <v>193</v>
+        <v>99</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>269</v>
+        <v>191</v>
+      </c>
+      <c r="B247" t="s">
+        <v>8</v>
       </c>
       <c r="C247" t="s">
-        <v>270</v>
+        <v>192</v>
       </c>
       <c r="D247" t="s">
-        <v>271</v>
+        <v>193</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>65</v>
-      </c>
-      <c r="B248" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="C248" t="s">
-        <v>66</v>
+        <v>270</v>
       </c>
       <c r="D248" t="s">
-        <v>67</v>
+        <v>271</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B249" t="s">
         <v>8</v>
       </c>
       <c r="C249" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D249" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>422</v>
+        <v>7</v>
+      </c>
+      <c r="B250" t="s">
+        <v>8</v>
       </c>
       <c r="C250" t="s">
-        <v>423</v>
+        <v>9</v>
       </c>
       <c r="D250" t="s">
-        <v>424</v>
+        <v>10</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>194</v>
-      </c>
-      <c r="B251" t="s">
-        <v>8</v>
+        <v>422</v>
       </c>
       <c r="C251" t="s">
-        <v>194</v>
+        <v>423</v>
       </c>
       <c r="D251" t="s">
-        <v>195</v>
+        <v>424</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="B252" t="s">
-        <v>173</v>
+        <v>8</v>
       </c>
       <c r="C252" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="D252" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="B253" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
       <c r="C253" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="D253" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B254" t="s">
-        <v>173</v>
+        <v>8</v>
       </c>
       <c r="C254" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D254" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
       <c r="B255" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
       <c r="C255" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="D255" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B256" t="s">
-        <v>173</v>
+        <v>8</v>
       </c>
       <c r="C256" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D256" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="B257" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
       <c r="C257" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="D257" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B258" t="s">
-        <v>173</v>
+        <v>8</v>
       </c>
       <c r="C258" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D258" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="B259" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
       <c r="C259" t="s">
-        <v>101</v>
+        <v>208</v>
       </c>
       <c r="D259" t="s">
-        <v>102</v>
+        <v>210</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>202</v>
+        <v>100</v>
       </c>
       <c r="B260" t="s">
         <v>8</v>
       </c>
       <c r="C260" t="s">
-        <v>203</v>
+        <v>101</v>
       </c>
       <c r="D260" t="s">
-        <v>204</v>
+        <v>102</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>14</v>
+        <v>202</v>
       </c>
       <c r="B261" t="s">
         <v>8</v>
       </c>
       <c r="C261" t="s">
-        <v>15</v>
+        <v>203</v>
       </c>
       <c r="D261" t="s">
-        <v>16</v>
+        <v>204</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>370</v>
+        <v>14</v>
+      </c>
+      <c r="B262" t="s">
+        <v>8</v>
       </c>
       <c r="C262" t="s">
-        <v>371</v>
+        <v>15</v>
       </c>
       <c r="D262" t="s">
-        <v>372</v>
+        <v>16</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>488</v>
+        <v>370</v>
       </c>
       <c r="C263" t="s">
-        <v>489</v>
+        <v>371</v>
       </c>
       <c r="D263" t="s">
-        <v>490</v>
+        <v>372</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>411</v>
-      </c>
-      <c r="B264" t="s">
-        <v>301</v>
+        <v>488</v>
       </c>
       <c r="C264" t="s">
-        <v>302</v>
+        <v>489</v>
       </c>
       <c r="D264" t="s">
-        <v>303</v>
+        <v>490</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>888</v>
+        <v>411</v>
+      </c>
+      <c r="B265" t="s">
+        <v>301</v>
       </c>
       <c r="C265" t="s">
-        <v>889</v>
+        <v>302</v>
       </c>
       <c r="D265" t="s">
-        <v>890</v>
+        <v>303</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>430</v>
+        <v>888</v>
       </c>
       <c r="C266" t="s">
-        <v>442</v>
+        <v>889</v>
       </c>
       <c r="D266" t="s">
-        <v>454</v>
+        <v>890</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C267" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D267" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C268" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D268" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C269" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D269" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C270" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D270" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C271" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D271" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C272" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D272" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C273" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D273" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C274" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D274" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C275" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D275" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C276" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D276" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C277" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D277" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>493</v>
+        <v>441</v>
       </c>
       <c r="C278" t="s">
-        <v>492</v>
+        <v>453</v>
       </c>
       <c r="D278" t="s">
-        <v>491</v>
+        <v>465</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>567</v>
+        <v>493</v>
       </c>
       <c r="C279" t="s">
-        <v>2</v>
+        <v>492</v>
       </c>
       <c r="D279" t="s">
-        <v>568</v>
+        <v>491</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
+        <v>567</v>
+      </c>
+      <c r="C280" t="s">
+        <v>2</v>
+      </c>
+      <c r="D280" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
         <v>569</v>
       </c>
-      <c r="C280" t="s">
+      <c r="C281" t="s">
         <v>570</v>
       </c>
-      <c r="D280" t="s">
+      <c r="D281" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A281" s="2" t="s">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B281" s="2"/>
-      <c r="C281" s="2"/>
-      <c r="D281" s="2"/>
-    </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
-        <v>104</v>
-      </c>
-      <c r="B282" t="s">
-        <v>103</v>
-      </c>
-      <c r="C282" t="s">
-        <v>123</v>
-      </c>
-      <c r="D282" t="s">
-        <v>122</v>
-      </c>
+      <c r="B282" s="2"/>
+      <c r="C282" s="2"/>
+      <c r="D282" s="2"/>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B283" t="s">
         <v>103</v>
       </c>
       <c r="C283" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D283" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B284" t="s">
         <v>103</v>
       </c>
       <c r="C284" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="D284" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B285" t="s">
         <v>103</v>
       </c>
       <c r="C285" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D285" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B286" t="s">
         <v>103</v>
       </c>
       <c r="C286" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D286" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B287" t="s">
         <v>103</v>
       </c>
       <c r="C287" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="D287" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B288" t="s">
         <v>103</v>
       </c>
       <c r="C288" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D288" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B289" t="s">
         <v>103</v>
       </c>
       <c r="C289" t="s">
+        <v>125</v>
+      </c>
+      <c r="D289" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>118</v>
+      </c>
+      <c r="B290" t="s">
+        <v>103</v>
+      </c>
+      <c r="C290" t="s">
         <v>119</v>
       </c>
-      <c r="D289" t="s">
+      <c r="D290" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A290" s="3" t="s">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B290" s="3"/>
-      <c r="C290" s="3"/>
-      <c r="D290" s="3"/>
-    </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>68</v>
-      </c>
-      <c r="B291" t="s">
-        <v>69</v>
-      </c>
-      <c r="C291" t="s">
-        <v>337</v>
-      </c>
-      <c r="D291" t="s">
-        <v>338</v>
-      </c>
+      <c r="B291" s="3"/>
+      <c r="C291" s="3"/>
+      <c r="D291" s="3"/>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>335</v>
+        <v>68</v>
       </c>
       <c r="B292" t="s">
         <v>69</v>
       </c>
       <c r="C292" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="D292" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>147</v>
+        <v>335</v>
       </c>
       <c r="B293" t="s">
         <v>69</v>
       </c>
       <c r="C293" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D293" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>341</v>
+        <v>147</v>
       </c>
       <c r="B294" t="s">
         <v>69</v>
       </c>
       <c r="C294" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D294" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>70</v>
+        <v>341</v>
       </c>
       <c r="B295" t="s">
         <v>69</v>
       </c>
       <c r="C295" t="s">
-        <v>71</v>
+        <v>342</v>
       </c>
       <c r="D295" t="s">
-        <v>72</v>
+        <v>343</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>601</v>
+        <v>70</v>
+      </c>
+      <c r="B296" t="s">
+        <v>69</v>
       </c>
       <c r="C296" t="s">
-        <v>595</v>
+        <v>71</v>
       </c>
       <c r="D296" t="s">
-        <v>602</v>
+        <v>72</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
       <c r="C297" t="s">
-        <v>613</v>
+        <v>595</v>
       </c>
       <c r="D297" t="s">
-        <v>614</v>
+        <v>602</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
+        <v>612</v>
+      </c>
+      <c r="C298" t="s">
+        <v>613</v>
+      </c>
+      <c r="D298" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
         <v>789</v>
       </c>
-      <c r="C298" t="s">
+      <c r="C299" t="s">
         <v>790</v>
       </c>
-      <c r="D298" t="s">
+      <c r="D299" t="s">
         <v>791</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C203" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
-    <hyperlink ref="D203" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
+    <hyperlink ref="C204" r:id="rId1" xr:uid="{CB807EE8-4E64-458B-BFA9-49A30A20AF1C}"/>
+    <hyperlink ref="D204" r:id="rId2" xr:uid="{24CEF538-6755-4741-89D5-FE4173EF0886}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Apply brand standards to buttons
</commit_message>
<xml_diff>
--- a/inst/apps/YGwater/translations.xlsx
+++ b/inst/apps/YGwater/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\YGwater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05570B2E-2768-4366-BF37-E182AEE3CF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C984F05-496E-460B-98C6-D5A3F15B56C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -1598,12 +1598,6 @@
     <t>gen_no_loc</t>
   </si>
   <si>
-    <t>Welcome to the Yukon Water Data Explorer! 🌧️🌊🌤️</t>
-  </si>
-  <si>
-    <t>Bienvenue à l'explorateur de données sur l'eau du Yukon! 🌧️🌊🌤️</t>
-  </si>
-  <si>
     <t>Log in to add/modify data and administer assets.</t>
   </si>
   <si>
@@ -2282,12 +2276,6 @@
     <t>mapsNavParamsTitle</t>
   </si>
   <si>
-    <t>Parameter value</t>
-  </si>
-  <si>
-    <t>Valeures de paramètres</t>
-  </si>
-  <si>
     <t>maps_locs</t>
   </si>
   <si>
@@ -2558,12 +2546,6 @@
     <t>séries temporelles</t>
   </si>
   <si>
-    <t>Plongez dans le monde de l'hydrologie, de la météorologie et de la chimie de l'eau avec le département de l'environment du gouvernement du Yukon. Notre mission? Mettre les données à portée de main, en alignement avec l'initiative de Gouvernement Ouvert pour la transparence, l'engagement des citoyens et l'incitation à la recherche créative. 📊 📈 Explorez les données en temps réel comme jamais auparavant, disponibles sous entente de nos limitations de responsabilité.</t>
-  </si>
-  <si>
-    <t>Dive into the world of hydrology, meteorology, and water chemistry with the Yukon Department of Environment's Water Resources Branch. Our mission? To bring data to your fingertips, aligning with the Open Government initiative for transparency, citizen empowerment, and sparking research creativity. 📊 📈 Explore real-time data like never before, made available under the terms of our limitations of liability.</t>
-  </si>
-  <si>
     <t>&lt;br&gt;We're now in the internal user testing phase. To enter your feedback please navigate to the &lt;b&gt;'Feedback'&lt;/b&gt; tab using the top navigation menu!&lt;br&gt;&lt;br&gt;Some application pieces will continue to be improved during this testing phase, notably the addition of missing French translations, the addition of some filters and user interface improvements to the plotting modules/tabs, and fixes to new bugs.</t>
   </si>
   <si>
@@ -2754,6 +2736,24 @@
   </si>
   <si>
     <t>Explorateur des données sur l’eau du Yukon</t>
+  </si>
+  <si>
+    <t>Current/past conditions</t>
+  </si>
+  <si>
+    <t>Conditions présentes/historiques</t>
+  </si>
+  <si>
+    <t>Welcome to the Yukon Water Data Explorer!</t>
+  </si>
+  <si>
+    <t>Bienvenue à l'explorateur de données sur l'eau du Yukon!</t>
+  </si>
+  <si>
+    <t>Dive into the world of hydrology, meteorology, and water chemistry with the Yukon Department of Environment's Water Resources Branch.&lt;br&gt;&lt;br&gt;Our mission? To bring data to your fingertips, aligning with the Open Government initiative for transparency, citizen empowerment, and sparking research creativity. Explore our historic and real-time data, made available under the terms of our limitation of liability.</t>
+  </si>
+  <si>
+    <t>Plongez dans le monde de l'hydrologie, de la météorologie et de la chimie de l'eau avec le département de l'environment du gouvernement du Yukon. &lt;br&gt;&lt;br&gt;Notre mission? Mettre les données à portée de main, en alignement avec l'initiative de Gouvernement Ouvert pour la transparence, l'engagement des citoyens et l'incitation à la recherche créative. Explorez nos données historiques et courantes comme jamais auparavant, disponibles sous entente de nos limitations de responsabilité.</t>
   </si>
 </sst>
 </file>
@@ -3692,8 +3692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D298"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3741,15 +3741,15 @@
         <v>495</v>
       </c>
       <c r="C3" t="s">
-        <v>905</v>
+        <v>899</v>
       </c>
       <c r="D3" t="s">
-        <v>906</v>
+        <v>900</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3760,7 +3760,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -3771,178 +3771,178 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B6" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C6" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D6" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="B7" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C7" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="D7" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B8" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C8" t="s">
-        <v>749</v>
+        <v>901</v>
       </c>
       <c r="D8" t="s">
-        <v>750</v>
+        <v>902</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>686</v>
+      </c>
+      <c r="B9" t="s">
+        <v>724</v>
+      </c>
+      <c r="C9" t="s">
+        <v>687</v>
+      </c>
+      <c r="D9" t="s">
         <v>688</v>
-      </c>
-      <c r="B9" t="s">
-        <v>726</v>
-      </c>
-      <c r="C9" t="s">
-        <v>689</v>
-      </c>
-      <c r="D9" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B10" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="C10" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="D10" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>694</v>
+      </c>
+      <c r="B11" t="s">
+        <v>723</v>
+      </c>
+      <c r="C11" t="s">
+        <v>695</v>
+      </c>
+      <c r="D11" t="s">
         <v>696</v>
-      </c>
-      <c r="B11" t="s">
-        <v>725</v>
-      </c>
-      <c r="C11" t="s">
-        <v>697</v>
-      </c>
-      <c r="D11" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>697</v>
+      </c>
+      <c r="B12" t="s">
+        <v>721</v>
+      </c>
+      <c r="C12" t="s">
+        <v>698</v>
+      </c>
+      <c r="D12" t="s">
         <v>699</v>
-      </c>
-      <c r="B12" t="s">
-        <v>723</v>
-      </c>
-      <c r="C12" t="s">
-        <v>700</v>
-      </c>
-      <c r="D12" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>702</v>
+      </c>
+      <c r="B13" t="s">
+        <v>722</v>
+      </c>
+      <c r="C13" t="s">
+        <v>703</v>
+      </c>
+      <c r="D13" t="s">
         <v>704</v>
-      </c>
-      <c r="B13" t="s">
-        <v>724</v>
-      </c>
-      <c r="C13" t="s">
-        <v>705</v>
-      </c>
-      <c r="D13" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B14" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C14" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D14" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B15" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C15" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D15" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B16" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C16" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D16" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B17" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C17" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D17" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B18" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C18" t="s">
         <v>42</v>
@@ -3953,38 +3953,38 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B19" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C19" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="D19" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B20" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C20" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="D20" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B21" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
@@ -3995,52 +3995,52 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>731</v>
+      </c>
+      <c r="B22" t="s">
+        <v>737</v>
+      </c>
+      <c r="C22" t="s">
         <v>733</v>
       </c>
-      <c r="B22" t="s">
-        <v>739</v>
-      </c>
-      <c r="C22" t="s">
-        <v>735</v>
-      </c>
       <c r="D22" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>732</v>
+      </c>
+      <c r="B23" t="s">
+        <v>738</v>
+      </c>
+      <c r="C23" t="s">
         <v>734</v>
       </c>
-      <c r="B23" t="s">
-        <v>740</v>
-      </c>
-      <c r="C23" t="s">
-        <v>736</v>
-      </c>
       <c r="D23" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B24" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C24" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D24" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B25" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C25" t="s">
         <v>129</v>
@@ -4051,21 +4051,21 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B26" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C26" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D26" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4073,30 +4073,30 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B28" t="s">
+        <v>644</v>
+      </c>
+      <c r="C28" t="s">
         <v>646</v>
       </c>
-      <c r="C28" t="s">
-        <v>648</v>
-      </c>
       <c r="D28" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B29" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C29" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4107,10 +4107,10 @@
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>521</v>
+        <v>903</v>
       </c>
       <c r="D30" t="s">
-        <v>522</v>
+        <v>904</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4121,122 +4121,122 @@
         <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>842</v>
+        <v>905</v>
       </c>
       <c r="D31" t="s">
-        <v>841</v>
+        <v>906</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
       <c r="B32" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="C32" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="D32" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="B33" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="C33" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="D33" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="B34" t="s">
         <v>226</v>
       </c>
       <c r="C34" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="D34" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="B35" t="s">
         <v>226</v>
       </c>
       <c r="C35" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="D35" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="B36" t="s">
         <v>226</v>
       </c>
       <c r="C36" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="D36" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>866</v>
+        <v>860</v>
       </c>
       <c r="B37" t="s">
         <v>226</v>
       </c>
       <c r="C37" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="D37" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
       <c r="B38" t="s">
         <v>226</v>
       </c>
       <c r="C38" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D38" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="B39" t="s">
         <v>226</v>
       </c>
       <c r="C39" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="D39" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4311,10 +4311,10 @@
         <v>278</v>
       </c>
       <c r="C45" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D45" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4403,16 +4403,16 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B52" t="s">
         <v>294</v>
       </c>
       <c r="C52" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D52" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4523,7 +4523,7 @@
         <v>236</v>
       </c>
       <c r="C61" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="D61" t="s">
         <v>235</v>
@@ -4531,13 +4531,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C62" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="D62" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4576,10 +4576,10 @@
         <v>243</v>
       </c>
       <c r="C65" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="D65" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4590,21 +4590,21 @@
         <v>243</v>
       </c>
       <c r="C66" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="D66" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B67" t="s">
         <v>244</v>
       </c>
       <c r="C67" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="D67" t="s">
         <v>247</v>
@@ -4612,16 +4612,16 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B68" t="s">
         <v>244</v>
       </c>
       <c r="C68" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D68" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4632,10 +4632,10 @@
         <v>244</v>
       </c>
       <c r="C69" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="D69" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -4654,41 +4654,41 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
       <c r="C71" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="D71" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="B72" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="C72" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="D72" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="B73" t="s">
+        <v>793</v>
+      </c>
+      <c r="C73" t="s">
+        <v>795</v>
+      </c>
+      <c r="D73" t="s">
         <v>797</v>
-      </c>
-      <c r="C73" t="s">
-        <v>799</v>
-      </c>
-      <c r="D73" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -4777,164 +4777,164 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="B80" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="C80" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="D80" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B81" t="s">
+        <v>752</v>
+      </c>
+      <c r="C81" t="s">
         <v>756</v>
       </c>
-      <c r="C81" t="s">
-        <v>760</v>
-      </c>
       <c r="D81" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="B82" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="C82" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D82" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="B83" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="C83" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="D83" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>800</v>
+      </c>
+      <c r="B84" t="s">
+        <v>752</v>
+      </c>
+      <c r="C84" t="s">
+        <v>803</v>
+      </c>
+      <c r="D84" t="s">
         <v>804</v>
-      </c>
-      <c r="B84" t="s">
-        <v>756</v>
-      </c>
-      <c r="C84" t="s">
-        <v>807</v>
-      </c>
-      <c r="D84" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>801</v>
+      </c>
+      <c r="B85" t="s">
+        <v>752</v>
+      </c>
+      <c r="C85" t="s">
+        <v>808</v>
+      </c>
+      <c r="D85" t="s">
         <v>805</v>
-      </c>
-      <c r="B85" t="s">
-        <v>756</v>
-      </c>
-      <c r="C85" t="s">
-        <v>812</v>
-      </c>
-      <c r="D85" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B86" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="C86" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="D86" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B87" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="C87" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D87" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B88" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="C88" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="D88" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="B89" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="C89" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="D89" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C90" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D90" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C91" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="D91" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4947,52 +4947,52 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>601</v>
+      </c>
+      <c r="C93" t="s">
+        <v>602</v>
+      </c>
+      <c r="D93" t="s">
         <v>603</v>
-      </c>
-      <c r="C93" t="s">
-        <v>604</v>
-      </c>
-      <c r="D93" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>619</v>
+      </c>
+      <c r="C94" t="s">
+        <v>620</v>
+      </c>
+      <c r="D94" t="s">
         <v>621</v>
-      </c>
-      <c r="C94" t="s">
-        <v>622</v>
-      </c>
-      <c r="D94" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>604</v>
+      </c>
+      <c r="B95" t="s">
+        <v>641</v>
+      </c>
+      <c r="C95" t="s">
+        <v>605</v>
+      </c>
+      <c r="D95" t="s">
         <v>606</v>
-      </c>
-      <c r="B95" t="s">
-        <v>643</v>
-      </c>
-      <c r="C95" t="s">
-        <v>607</v>
-      </c>
-      <c r="D95" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>607</v>
+      </c>
+      <c r="B96" t="s">
+        <v>641</v>
+      </c>
+      <c r="C96" t="s">
+        <v>608</v>
+      </c>
+      <c r="D96" t="s">
         <v>609</v>
-      </c>
-      <c r="B96" t="s">
-        <v>643</v>
-      </c>
-      <c r="C96" t="s">
-        <v>610</v>
-      </c>
-      <c r="D96" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -5067,138 +5067,138 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C102" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D102" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>651</v>
+      </c>
+      <c r="C103" t="s">
+        <v>652</v>
+      </c>
+      <c r="D103" t="s">
         <v>653</v>
-      </c>
-      <c r="C103" t="s">
-        <v>654</v>
-      </c>
-      <c r="D103" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>648</v>
+      </c>
+      <c r="C104" t="s">
+        <v>649</v>
+      </c>
+      <c r="D104" t="s">
         <v>650</v>
-      </c>
-      <c r="C104" t="s">
-        <v>651</v>
-      </c>
-      <c r="D104" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C105" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="D105" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>635</v>
+      </c>
+      <c r="B106" t="s">
+        <v>640</v>
+      </c>
+      <c r="C106" t="s">
         <v>637</v>
       </c>
-      <c r="B106" t="s">
-        <v>642</v>
-      </c>
-      <c r="C106" t="s">
-        <v>639</v>
-      </c>
       <c r="D106" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="C107" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="D107" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="C108" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D108" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B109" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C109" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D109" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="B110" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C110" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D110" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="B111" t="s">
+        <v>832</v>
+      </c>
+      <c r="C111" t="s">
+        <v>833</v>
+      </c>
+      <c r="D111" t="s">
         <v>836</v>
-      </c>
-      <c r="C111" t="s">
-        <v>837</v>
-      </c>
-      <c r="D111" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B112" t="s">
         <v>226</v>
       </c>
       <c r="C112" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D112" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -5217,35 +5217,35 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C114" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="D114" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="C115" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="D115" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="C116" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="D116" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -5278,10 +5278,10 @@
         <v>81</v>
       </c>
       <c r="C119" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="D119" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -5292,10 +5292,10 @@
         <v>81</v>
       </c>
       <c r="C120" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
       <c r="D120" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -5607,13 +5607,13 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>852</v>
+        <v>846</v>
       </c>
       <c r="C147" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="D147" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -5629,16 +5629,16 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>849</v>
+        <v>843</v>
       </c>
       <c r="B149" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="C149" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
       <c r="D149" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5654,13 +5654,13 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>851</v>
+        <v>845</v>
       </c>
       <c r="C151" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="D151" t="s">
-        <v>848</v>
+        <v>842</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -5679,7 +5679,7 @@
         <v>374</v>
       </c>
       <c r="C153" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="D153" t="s">
         <v>378</v>
@@ -5940,244 +5940,244 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>526</v>
+      </c>
+      <c r="C177" s="9" t="s">
+        <v>527</v>
+      </c>
+      <c r="D177" t="s">
         <v>528</v>
-      </c>
-      <c r="C177" s="9" t="s">
-        <v>529</v>
-      </c>
-      <c r="D177" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>529</v>
+      </c>
+      <c r="C178" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="D178" t="s">
         <v>531</v>
-      </c>
-      <c r="C178" s="9" t="s">
-        <v>535</v>
-      </c>
-      <c r="D178" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>530</v>
+      </c>
+      <c r="C179" s="9" t="s">
         <v>532</v>
       </c>
-      <c r="C179" s="9" t="s">
-        <v>534</v>
-      </c>
       <c r="D179" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D180" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
+        <v>535</v>
+      </c>
+      <c r="C181" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="C181" s="9" t="s">
-        <v>539</v>
-      </c>
       <c r="D181" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>541</v>
+      </c>
+      <c r="C182" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="D182" t="s">
         <v>543</v>
-      </c>
-      <c r="C182" s="9" t="s">
-        <v>544</v>
-      </c>
-      <c r="D182" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D183" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>544</v>
+      </c>
+      <c r="C184" s="9" t="s">
         <v>546</v>
       </c>
-      <c r="C184" s="9" t="s">
+      <c r="D184" t="s">
         <v>548</v>
-      </c>
-      <c r="D184" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>545</v>
+      </c>
+      <c r="C185" s="9" t="s">
         <v>547</v>
       </c>
-      <c r="C185" s="9" t="s">
+      <c r="D185" t="s">
         <v>549</v>
-      </c>
-      <c r="D185" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D186" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D187" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C188" s="9" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D188" s="9" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C189" s="9" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>562</v>
+      </c>
+      <c r="C190" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="D190" s="9" t="s">
         <v>564</v>
-      </c>
-      <c r="C190" s="9" t="s">
-        <v>565</v>
-      </c>
-      <c r="D190" s="9" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C191" s="9" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C192" s="9" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D192" s="9" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="D193" s="9" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="C194" s="9" t="s">
+        <v>887</v>
+      </c>
+      <c r="D194" s="9" t="s">
         <v>893</v>
-      </c>
-      <c r="D194" s="9" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="C195" s="9" t="s">
+        <v>888</v>
+      </c>
+      <c r="D195" s="9" t="s">
         <v>894</v>
-      </c>
-      <c r="D195" s="9" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="D196" s="9" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>898</v>
+        <v>892</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>902</v>
+        <v>896</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>897</v>
+        <v>891</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -6190,46 +6190,46 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
+        <v>668</v>
+      </c>
+      <c r="C200" t="s">
+        <v>669</v>
+      </c>
+      <c r="D200" t="s">
         <v>670</v>
-      </c>
-      <c r="C200" t="s">
-        <v>671</v>
-      </c>
-      <c r="D200" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C201" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D201" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C202" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="D202" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C203" s="7" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D203" s="7" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -6268,10 +6268,10 @@
         <v>131</v>
       </c>
       <c r="C206" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D206" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -6304,35 +6304,35 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C209" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D209" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C210" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D210" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
+        <v>661</v>
+      </c>
+      <c r="C211" t="s">
+        <v>662</v>
+      </c>
+      <c r="D211" t="s">
         <v>663</v>
-      </c>
-      <c r="C211" t="s">
-        <v>664</v>
-      </c>
-      <c r="D211" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -6373,57 +6373,57 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
+        <v>578</v>
+      </c>
+      <c r="C215" t="s">
+        <v>579</v>
+      </c>
+      <c r="D215" t="s">
         <v>580</v>
-      </c>
-      <c r="C215" t="s">
-        <v>581</v>
-      </c>
-      <c r="D215" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
+        <v>581</v>
+      </c>
+      <c r="C216" t="s">
+        <v>582</v>
+      </c>
+      <c r="D216" t="s">
         <v>583</v>
-      </c>
-      <c r="C216" t="s">
-        <v>584</v>
-      </c>
-      <c r="D216" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
+        <v>613</v>
+      </c>
+      <c r="C217" t="s">
         <v>615</v>
       </c>
-      <c r="C217" t="s">
-        <v>617</v>
-      </c>
       <c r="D217" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C218" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D218" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="C219" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="D219" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -6473,10 +6473,10 @@
         <v>333</v>
       </c>
       <c r="C223" t="s">
-        <v>877</v>
+        <v>871</v>
       </c>
       <c r="D223" t="s">
-        <v>878</v>
+        <v>872</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -6487,43 +6487,43 @@
         <v>8</v>
       </c>
       <c r="C224" t="s">
+        <v>595</v>
+      </c>
+      <c r="D224" t="s">
         <v>597</v>
-      </c>
-      <c r="D224" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
+        <v>596</v>
+      </c>
+      <c r="C225" t="s">
+        <v>594</v>
+      </c>
+      <c r="D225" t="s">
         <v>598</v>
-      </c>
-      <c r="C225" t="s">
-        <v>596</v>
-      </c>
-      <c r="D225" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="C226" t="s">
-        <v>876</v>
+        <v>870</v>
       </c>
       <c r="D226" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="C227" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="D227" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -6534,7 +6534,7 @@
         <v>8</v>
       </c>
       <c r="C228" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D228" t="s">
         <v>150</v>
@@ -6548,7 +6548,7 @@
         <v>8</v>
       </c>
       <c r="C229" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D229" t="s">
         <v>160</v>
@@ -6562,7 +6562,7 @@
         <v>8</v>
       </c>
       <c r="C230" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D230" t="s">
         <v>168</v>
@@ -6570,44 +6570,44 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B231" t="s">
         <v>8</v>
       </c>
       <c r="C231" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D231" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B232" t="s">
         <v>8</v>
       </c>
       <c r="C232" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D232" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B233" t="s">
         <v>8</v>
       </c>
       <c r="C233" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D233" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -7034,13 +7034,13 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>888</v>
+        <v>882</v>
       </c>
       <c r="C265" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="D265" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
@@ -7188,21 +7188,21 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C279" t="s">
         <v>2</v>
       </c>
       <c r="D279" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C280" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D280" t="s">
         <v>3</v>
@@ -7408,35 +7408,35 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C296" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D296" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
+        <v>610</v>
+      </c>
+      <c r="C297" t="s">
+        <v>611</v>
+      </c>
+      <c r="D297" t="s">
         <v>612</v>
-      </c>
-      <c r="C297" t="s">
-        <v>613</v>
-      </c>
-      <c r="D297" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="C298" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="D298" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
     </row>
   </sheetData>

</xml_diff>